<commit_message>
v1.0.8 - Create, Modify & Delete records in outside DB
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE43FE64-411D-4A35-AB98-8946360E60D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5325F4E4-8634-463C-A37E-0216E78A1646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="331">
   <si>
     <t>TEC_ID</t>
   </si>
@@ -1023,6 +1023,12 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>BanColombia S.A.</t>
+  </si>
+  <si>
+    <t>Une compagnie en Colombie</t>
   </si>
 </sst>
 </file>
@@ -1455,8 +1461,10 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:Q234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="B220" sqref="B220"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <pane ySplit="600" topLeftCell="A216" activePane="bottomLeft"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomLeft" activeCell="O227" sqref="O227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,8 +1474,8 @@
     <col min="3" max="3" width="6.5703125" style="13" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="52.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="94.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.5703125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="50.7109375" style="16" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -11032,17 +11040,19 @@
         <v>1</v>
       </c>
       <c r="K225" s="6">
-        <v>45275.5391319444</v>
+        <v>45276.4154050926</v>
       </c>
       <c r="L225" s="18" t="b">
         <v>0</v>
       </c>
       <c r="M225" s="18"/>
       <c r="N225" t="b">
-        <v>0</v>
-      </c>
-      <c r="O225" s="16" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="O225" s="16" t="inlineStr">
+        <is>
+          <t>v1.0.8</t>
+        </is>
       </c>
       <c r="P225" s="12"/>
     </row>
@@ -11118,14 +11128,14 @@
         <v>1</v>
       </c>
       <c r="K227" s="6">
-        <v>45275.7156597222</v>
+        <v>45276.4120023148</v>
       </c>
       <c r="L227" s="18" t="b">
         <v>0</v>
       </c>
       <c r="M227" s="18"/>
       <c r="N227" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O227" s="16" t="s">
         <v>318</v>
@@ -11161,16 +11171,18 @@
         <v>1</v>
       </c>
       <c r="K228" s="6">
-        <v>45275.814837963</v>
+        <v>45276.415625</v>
       </c>
       <c r="L228" s="1" t="b">
         <v>0</v>
       </c>
       <c r="N228" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O228" s="22" t="s">
-        <v>318</v>
+        <v>1</v>
+      </c>
+      <c r="O228" s="22" t="inlineStr">
+        <is>
+          <t>v1.0.8</t>
+        </is>
       </c>
     </row>
     <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="229">
@@ -11202,16 +11214,18 @@
         <v>1</v>
       </c>
       <c r="K229" s="6">
-        <v>45275.815150463</v>
+        <v>45276.4153009259</v>
       </c>
       <c r="L229" s="1" t="b">
         <v>0</v>
       </c>
       <c r="N229" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O229" s="22" t="s">
-        <v>318</v>
+        <v>1</v>
+      </c>
+      <c r="O229" s="22" t="inlineStr">
+        <is>
+          <t>v1.0.8</t>
+        </is>
       </c>
     </row>
     <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="230">
@@ -11230,20 +11244,24 @@
       <c r="E230" s="1">
         <v>199</v>
       </c>
-      <c r="F230" s="22" t="s">
-        <v>320</v>
-      </c>
-      <c r="G230" s="22" t="s">
-        <v>307</v>
+      <c r="F230" s="22" t="inlineStr">
+        <is>
+          <t>Autodesk, Inc.</t>
+        </is>
+      </c>
+      <c r="G230" s="22" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
       </c>
       <c r="H230" s="7">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="J230" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K230" s="6">
-        <v>45275.8157060185</v>
+        <v>45276.4157291667</v>
       </c>
       <c r="L230" s="1" t="b">
         <v>0</v>
@@ -11251,8 +11269,10 @@
       <c r="N230" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="O230" s="22" t="s">
-        <v>318</v>
+      <c r="O230" s="22" t="inlineStr">
+        <is>
+          <t>v1.0.8</t>
+        </is>
       </c>
     </row>
     <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="231">
@@ -11312,29 +11332,35 @@
       <c r="E232" s="1">
         <v>1396</v>
       </c>
-      <c r="F232" s="22" t="s">
-        <v>324</v>
-      </c>
-      <c r="G232" s="22" t="s">
-        <v>325</v>
+      <c r="F232" s="22" t="inlineStr">
+        <is>
+          <t>Pepsico, Inc.</t>
+        </is>
+      </c>
+      <c r="G232" s="22" t="inlineStr">
+        <is>
+          <t>Un bon pepsi si ce test fonctionne</t>
+        </is>
       </c>
       <c r="H232" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J232" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K232" s="6">
-        <v>45276.3596180556</v>
+        <v>45276.4187962963</v>
       </c>
       <c r="L232" s="1" t="b">
         <v>0</v>
       </c>
       <c r="N232" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O232" s="22" t="s">
-        <v>323</v>
+        <v>1</v>
+      </c>
+      <c r="O232" s="22" t="inlineStr">
+        <is>
+          <t>v1.0.8</t>
+        </is>
       </c>
     </row>
     <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="233">
@@ -11353,15 +11379,11 @@
       <c r="E233" s="1">
         <v>277</v>
       </c>
-      <c r="F233" s="22" t="inlineStr">
-        <is>
-          <t>BMC Software, Inc.</t>
-        </is>
-      </c>
-      <c r="G233" s="22" t="inlineStr">
-        <is>
-          <t>Compagnie intéressante</t>
-        </is>
+      <c r="F233" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="G233" s="22" t="s">
+        <v>327</v>
       </c>
       <c r="H233" s="23">
         <v>1.5</v>
@@ -11378,26 +11400,22 @@
       <c r="N233" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="O233" s="22" t="inlineStr">
-        <is>
-          <t>v1.0.7</t>
-        </is>
+      <c r="O233" s="22" t="s">
+        <v>323</v>
       </c>
       <c r="Q233" s="22" t="s">
         <v>328</v>
       </c>
     </row>
-    <row outlineLevel="0" r="234">
+    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="234">
       <c r="A234" s="22">
         <v>234</v>
       </c>
       <c r="B234" s="22">
         <v>4</v>
       </c>
-      <c r="C234" s="22" t="inlineStr">
-        <is>
-          <t>RMV</t>
-        </is>
+      <c r="C234" s="22" t="s">
+        <v>21</v>
       </c>
       <c r="D234" s="5">
         <v>45276</v>
@@ -11412,11 +11430,11 @@
       </c>
       <c r="G234" s="22" t="inlineStr">
         <is>
-          <t>Une compganie en Colombie</t>
+          <t>Une compagnie en Colombie</t>
         </is>
       </c>
       <c r="H234" s="22">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I234" s="22" t="inlineStr">
         <is>
@@ -11427,7 +11445,7 @@
         <v>1</v>
       </c>
       <c r="K234" s="5">
-        <v>45276.3983564815</v>
+        <v>45276.418587963</v>
       </c>
       <c r="L234" s="22" t="b">
         <v>0</v>
@@ -11437,13 +11455,11 @@
       </c>
       <c r="O234" s="22" t="inlineStr">
         <is>
-          <t>v1.0.7</t>
+          <t>v1.0.8</t>
         </is>
       </c>
-      <c r="Q234" s="22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q234" s="22" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.1.0 - TEC fonctionne bien
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -1459,7 +1459,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:Q234"/>
+  <dimension ref="A1:Q241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <pane ySplit="600" topLeftCell="A216" activePane="bottomLeft"/>
@@ -11379,20 +11379,24 @@
       <c r="E233" s="1">
         <v>277</v>
       </c>
-      <c r="F233" s="22" t="s">
-        <v>326</v>
-      </c>
-      <c r="G233" s="22" t="s">
-        <v>327</v>
+      <c r="F233" s="22" t="inlineStr">
+        <is>
+          <t>BMC Software, Inc.</t>
+        </is>
+      </c>
+      <c r="G233" s="22" t="inlineStr">
+        <is>
+          <t>Compagnie intéressante</t>
+        </is>
       </c>
       <c r="H233" s="23">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="J233" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K233" s="6">
-        <v>45276.3977430556</v>
+        <v>45276.547962963</v>
       </c>
       <c r="L233" s="1" t="b">
         <v>0</v>
@@ -11400,8 +11404,10 @@
       <c r="N233" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="O233" s="22" t="s">
-        <v>323</v>
+      <c r="O233" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.0</t>
+        </is>
       </c>
       <c r="Q233" s="22" t="s">
         <v>328</v>
@@ -11434,7 +11440,7 @@
         </is>
       </c>
       <c r="H234" s="22">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="I234" s="22" t="inlineStr">
         <is>
@@ -11445,7 +11451,7 @@
         <v>1</v>
       </c>
       <c r="K234" s="5">
-        <v>45276.418587963</v>
+        <v>45276.5418518518</v>
       </c>
       <c r="L234" s="22" t="b">
         <v>0</v>
@@ -11455,11 +11461,384 @@
       </c>
       <c r="O234" s="22" t="inlineStr">
         <is>
-          <t>v1.0.8</t>
+          <t>v1.1.0</t>
         </is>
       </c>
       <c r="Q234" s="22" t="s">
         <v>328</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="235">
+      <c r="A235" s="22">
+        <v>235</v>
+      </c>
+      <c r="B235" s="22">
+        <v>1</v>
+      </c>
+      <c r="C235" s="22" t="inlineStr">
+        <is>
+          <t>GC</t>
+        </is>
+      </c>
+      <c r="D235" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E235" s="22">
+        <v>369</v>
+      </c>
+      <c r="F235" s="22" t="inlineStr">
+        <is>
+          <t>CDW Corporation</t>
+        </is>
+      </c>
+      <c r="G235" s="22" t="inlineStr">
+        <is>
+          <t>CDW Corporation</t>
+        </is>
+      </c>
+      <c r="H235" s="22">
+        <v>1</v>
+      </c>
+      <c r="J235" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K235" s="5">
+        <v>45276.511099537</v>
+      </c>
+      <c r="L235" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N235" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O235" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.0</t>
+        </is>
+      </c>
+      <c r="Q235" s="22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="236">
+      <c r="A236" s="22">
+        <v>236</v>
+      </c>
+      <c r="B236" s="22">
+        <v>1</v>
+      </c>
+      <c r="C236" s="22" t="inlineStr">
+        <is>
+          <t>GC</t>
+        </is>
+      </c>
+      <c r="D236" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E236" s="22">
+        <v>1757</v>
+      </c>
+      <c r="F236" s="22" t="inlineStr">
+        <is>
+          <t>Telefonica Moviles S.A.</t>
+        </is>
+      </c>
+      <c r="G236" s="22" t="inlineStr">
+        <is>
+          <t>Telefonica</t>
+        </is>
+      </c>
+      <c r="H236" s="22">
+        <v>2</v>
+      </c>
+      <c r="I236" s="22" t="inlineStr">
+        <is>
+          <t>Telefonica</t>
+        </is>
+      </c>
+      <c r="J236" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K236" s="5">
+        <v>45276.5113657407</v>
+      </c>
+      <c r="L236" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N236" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O236" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.0</t>
+        </is>
+      </c>
+      <c r="Q236" s="22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="237">
+      <c r="A237" s="22">
+        <v>237</v>
+      </c>
+      <c r="B237" s="22">
+        <v>2</v>
+      </c>
+      <c r="C237" s="22" t="inlineStr">
+        <is>
+          <t>VG</t>
+        </is>
+      </c>
+      <c r="D237" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E237" s="22">
+        <v>570</v>
+      </c>
+      <c r="F237" s="22" t="inlineStr">
+        <is>
+          <t>Digital Insight Corporation</t>
+        </is>
+      </c>
+      <c r="G237" s="22" t="inlineStr">
+        <is>
+          <t>Test du 16 décembre</t>
+        </is>
+      </c>
+      <c r="H237" s="22">
+        <v>1</v>
+      </c>
+      <c r="J237" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K237" s="5">
+        <v>45276.5118287037</v>
+      </c>
+      <c r="L237" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N237" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O237" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.0</t>
+        </is>
+      </c>
+      <c r="Q237" s="22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="238">
+      <c r="A238" s="22">
+        <v>238</v>
+      </c>
+      <c r="B238" s="22">
+        <v>2</v>
+      </c>
+      <c r="C238" s="22" t="inlineStr">
+        <is>
+          <t>VG</t>
+        </is>
+      </c>
+      <c r="D238" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E238" s="22">
+        <v>1263</v>
+      </c>
+      <c r="F238" s="22" t="inlineStr">
+        <is>
+          <t>Networks Associates, Inc.</t>
+        </is>
+      </c>
+      <c r="G238" s="22" t="inlineStr">
+        <is>
+          <t>Test du 16 décembre</t>
+        </is>
+      </c>
+      <c r="H238" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="J238" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K238" s="5">
+        <v>45276.512037037</v>
+      </c>
+      <c r="L238" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N238" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O238" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.0</t>
+        </is>
+      </c>
+      <c r="Q238" s="22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="239">
+      <c r="A239" s="22">
+        <v>239</v>
+      </c>
+      <c r="B239" s="22">
+        <v>2</v>
+      </c>
+      <c r="C239" s="22" t="inlineStr">
+        <is>
+          <t>VG</t>
+        </is>
+      </c>
+      <c r="D239" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E239" s="22">
+        <v>1232</v>
+      </c>
+      <c r="F239" s="22" t="inlineStr">
+        <is>
+          <t>Murphy Oil Corporation</t>
+        </is>
+      </c>
+      <c r="G239" s="22" t="inlineStr">
+        <is>
+          <t>Test du 16 décembre</t>
+        </is>
+      </c>
+      <c r="H239" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="J239" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K239" s="5">
+        <v>45276.5126041667</v>
+      </c>
+      <c r="L239" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N239" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O239" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.0</t>
+        </is>
+      </c>
+      <c r="Q239" s="22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="240">
+      <c r="A240" s="22">
+        <v>240</v>
+      </c>
+      <c r="B240" s="22">
+        <v>3</v>
+      </c>
+      <c r="C240" s="22" t="inlineStr">
+        <is>
+          <t>MFP</t>
+        </is>
+      </c>
+      <c r="D240" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E240" s="22">
+        <v>95</v>
+      </c>
+      <c r="F240" s="22" t="inlineStr">
+        <is>
+          <t>Altria Group</t>
+        </is>
+      </c>
+      <c r="H240" s="22">
+        <v>3</v>
+      </c>
+      <c r="J240" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K240" s="5">
+        <v>45276.5128472222</v>
+      </c>
+      <c r="L240" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N240" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O240" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.0</t>
+        </is>
+      </c>
+      <c r="Q240" s="22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="241">
+      <c r="A241" s="22">
+        <v>241</v>
+      </c>
+      <c r="B241" s="22">
+        <v>4</v>
+      </c>
+      <c r="C241" s="22" t="inlineStr">
+        <is>
+          <t>RMV</t>
+        </is>
+      </c>
+      <c r="D241" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E241" s="22">
+        <v>1554</v>
+      </c>
+      <c r="F241" s="22" t="inlineStr">
+        <is>
+          <t>Royal Caribbean Cruises Ltd.</t>
+        </is>
+      </c>
+      <c r="G241" s="22" t="inlineStr">
+        <is>
+          <t>Un beau voyage</t>
+        </is>
+      </c>
+      <c r="H241" s="22">
+        <v>2</v>
+      </c>
+      <c r="J241" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K241" s="5">
+        <v>45276.5477662037</v>
+      </c>
+      <c r="L241" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N241" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O241" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.1.1 - Ménage de code + Préparation pour FACTURE
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5325F4E4-8634-463C-A37E-0216E78A1646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F254C9A0-985C-4493-BC5C-1C39D7B494A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="339">
   <si>
     <t>TEC_ID</t>
   </si>
@@ -1001,9 +1001,6 @@
     <t>Autodesk, Inc.</t>
   </si>
   <si>
-    <t>BD_Row</t>
-  </si>
-  <si>
     <t>Meilleur test de la journée ;-)</t>
   </si>
   <si>
@@ -1022,13 +1019,40 @@
     <t>Compagnie intéressante</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>BanColombia S.A.</t>
   </si>
   <si>
     <t>Une compagnie en Colombie</t>
+  </si>
+  <si>
+    <t>v1.0.8</t>
+  </si>
+  <si>
+    <t>v1.1.0</t>
+  </si>
+  <si>
+    <t>CDW Corporation</t>
+  </si>
+  <si>
+    <t>Telefonica Moviles S.A.</t>
+  </si>
+  <si>
+    <t>Telefonica</t>
+  </si>
+  <si>
+    <t>Digital Insight Corporation</t>
+  </si>
+  <si>
+    <t>Test du 16 décembre</t>
+  </si>
+  <si>
+    <t>Murphy Oil Corporation</t>
+  </si>
+  <si>
+    <t>Altria Group</t>
+  </si>
+  <si>
+    <t>Un beau voyage</t>
   </si>
 </sst>
 </file>
@@ -1459,11 +1483,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:Q241"/>
+  <dimension ref="A1:P246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <pane ySplit="600" topLeftCell="A216" activePane="bottomLeft"/>
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <pane ySplit="600" topLeftCell="A216"/>
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
       <selection pane="bottomLeft" activeCell="O227" sqref="O227"/>
     </sheetView>
   </sheetViews>
@@ -1485,10 +1509,9 @@
     <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1537,11 +1560,8 @@
       <c r="P1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="17" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
       <c r="A2" s="9">
         <v>2</v>
       </c>
@@ -1585,7 +1605,7 @@
       <c r="O2" s="14"/>
       <c r="P2" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
       <c r="A3" s="9">
         <v>3</v>
       </c>
@@ -1629,7 +1649,7 @@
       <c r="O3" s="14"/>
       <c r="P3" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
       <c r="A4" s="9">
         <v>4</v>
       </c>
@@ -1671,7 +1691,7 @@
       <c r="O4" s="14"/>
       <c r="P4" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
       <c r="A5" s="9">
         <v>5</v>
       </c>
@@ -1715,7 +1735,7 @@
       <c r="O5" s="14"/>
       <c r="P5" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="6">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="6">
       <c r="A6" s="9">
         <v>6</v>
       </c>
@@ -1759,7 +1779,7 @@
       <c r="O6" s="14"/>
       <c r="P6" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="7">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="7">
       <c r="A7" s="9">
         <v>7</v>
       </c>
@@ -1803,7 +1823,7 @@
       <c r="O7" s="14"/>
       <c r="P7" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="8">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="8">
       <c r="A8" s="9">
         <v>8</v>
       </c>
@@ -1847,7 +1867,7 @@
       <c r="O8" s="14"/>
       <c r="P8" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="9">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="9">
       <c r="A9" s="9">
         <v>9</v>
       </c>
@@ -1889,7 +1909,7 @@
       <c r="O9" s="14"/>
       <c r="P9" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="10">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="10">
       <c r="A10" s="9">
         <v>10</v>
       </c>
@@ -1933,7 +1953,7 @@
       <c r="O10" s="14"/>
       <c r="P10" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="11">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="11">
       <c r="A11" s="9">
         <v>11</v>
       </c>
@@ -1977,7 +1997,7 @@
       <c r="O11" s="14"/>
       <c r="P11" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="12">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="12">
       <c r="A12" s="9">
         <v>12</v>
       </c>
@@ -2019,7 +2039,7 @@
       <c r="O12" s="14"/>
       <c r="P12" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="13">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="13">
       <c r="A13" s="9">
         <v>13</v>
       </c>
@@ -2063,7 +2083,7 @@
       <c r="O13" s="14"/>
       <c r="P13" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="14">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="14">
       <c r="A14" s="9">
         <v>14</v>
       </c>
@@ -2107,7 +2127,7 @@
       <c r="O14" s="14"/>
       <c r="P14" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="15">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="15">
       <c r="A15" s="9">
         <v>15</v>
       </c>
@@ -2151,7 +2171,7 @@
       <c r="O15" s="14"/>
       <c r="P15" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="16">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="16">
       <c r="A16" s="9">
         <v>16</v>
       </c>
@@ -11010,7 +11030,7 @@
       </c>
       <c r="P224" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="225">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="225">
       <c r="A225" s="9">
         <v>225</v>
       </c>
@@ -11049,14 +11069,12 @@
       <c r="N225" t="b">
         <v>1</v>
       </c>
-      <c r="O225" s="16" t="inlineStr">
-        <is>
-          <t>v1.0.8</t>
-        </is>
+      <c r="O225" s="16" t="s">
+        <v>329</v>
       </c>
       <c r="P225" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="226">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="226">
       <c r="A226" s="9">
         <v>226</v>
       </c>
@@ -11100,7 +11118,7 @@
       </c>
       <c r="P226" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="227">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="227">
       <c r="A227" s="9">
         <v>227</v>
       </c>
@@ -11142,7 +11160,7 @@
       </c>
       <c r="P227" s="12"/>
     </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="228">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="228">
       <c r="A228" s="1">
         <v>228</v>
       </c>
@@ -11179,13 +11197,11 @@
       <c r="N228" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="O228" s="22" t="inlineStr">
-        <is>
-          <t>v1.0.8</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="229">
+      <c r="O228" s="22" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="229">
       <c r="A229" s="1">
         <v>229</v>
       </c>
@@ -11222,13 +11238,11 @@
       <c r="N229" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="O229" s="22" t="inlineStr">
-        <is>
-          <t>v1.0.8</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="230">
+      <c r="O229" s="22" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="230">
       <c r="A230" s="1">
         <v>230</v>
       </c>
@@ -11244,15 +11258,11 @@
       <c r="E230" s="1">
         <v>199</v>
       </c>
-      <c r="F230" s="22" t="inlineStr">
-        <is>
-          <t>Autodesk, Inc.</t>
-        </is>
-      </c>
-      <c r="G230" s="22" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
+      <c r="F230" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="G230" s="22" t="s">
+        <v>307</v>
       </c>
       <c r="H230" s="7">
         <v>1.25</v>
@@ -11269,13 +11279,11 @@
       <c r="N230" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="O230" s="22" t="inlineStr">
-        <is>
-          <t>v1.0.8</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="231">
+      <c r="O230" s="22" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="231">
       <c r="A231" s="1">
         <v>231</v>
       </c>
@@ -11295,7 +11303,7 @@
         <v>195</v>
       </c>
       <c r="G231" s="22" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H231" s="1">
         <v>0.75</v>
@@ -11313,10 +11321,10 @@
         <v>0</v>
       </c>
       <c r="O231" s="22" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="232">
+        <v>322</v>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="232">
       <c r="A232" s="1">
         <v>232</v>
       </c>
@@ -11332,15 +11340,11 @@
       <c r="E232" s="1">
         <v>1396</v>
       </c>
-      <c r="F232" s="22" t="inlineStr">
-        <is>
-          <t>Pepsico, Inc.</t>
-        </is>
-      </c>
-      <c r="G232" s="22" t="inlineStr">
-        <is>
-          <t>Un bon pepsi si ce test fonctionne</t>
-        </is>
+      <c r="F232" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="G232" s="22" t="s">
+        <v>324</v>
       </c>
       <c r="H232" s="23">
         <v>2</v>
@@ -11357,13 +11361,11 @@
       <c r="N232" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="O232" s="22" t="inlineStr">
-        <is>
-          <t>v1.0.8</t>
-        </is>
-      </c>
-    </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="233">
+      <c r="O232" s="22" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="233">
       <c r="A233" s="1">
         <v>233</v>
       </c>
@@ -11393,10 +11395,10 @@
         <v>2.5</v>
       </c>
       <c r="J233" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K233" s="6">
-        <v>45276.547962963</v>
+        <v>45276.6225</v>
       </c>
       <c r="L233" s="1" t="b">
         <v>0</v>
@@ -11406,14 +11408,11 @@
       </c>
       <c r="O233" s="22" t="inlineStr">
         <is>
-          <t>v1.1.0</t>
+          <t>v1.1.1</t>
         </is>
       </c>
-      <c r="Q233" s="22" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row spans="1:17" x14ac:dyDescent="0.25" outlineLevel="0" r="234">
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="234">
       <c r="A234" s="22">
         <v>234</v>
       </c>
@@ -11440,7 +11439,7 @@
         </is>
       </c>
       <c r="H234" s="22">
-        <v>3.5</v>
+        <v>1.75</v>
       </c>
       <c r="I234" s="22" t="inlineStr">
         <is>
@@ -11448,10 +11447,10 @@
         </is>
       </c>
       <c r="J234" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K234" s="5">
-        <v>45276.5418518518</v>
+        <v>45276.6221990741</v>
       </c>
       <c r="L234" s="22" t="b">
         <v>0</v>
@@ -11461,24 +11460,19 @@
       </c>
       <c r="O234" s="22" t="inlineStr">
         <is>
-          <t>v1.1.0</t>
+          <t>v1.1.1</t>
         </is>
       </c>
-      <c r="Q234" s="22" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="235">
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="235">
       <c r="A235" s="22">
         <v>235</v>
       </c>
       <c r="B235" s="22">
         <v>1</v>
       </c>
-      <c r="C235" s="22" t="inlineStr">
-        <is>
-          <t>GC</t>
-        </is>
+      <c r="C235" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="D235" s="5">
         <v>45276</v>
@@ -11486,15 +11480,11 @@
       <c r="E235" s="22">
         <v>369</v>
       </c>
-      <c r="F235" s="22" t="inlineStr">
-        <is>
-          <t>CDW Corporation</t>
-        </is>
-      </c>
-      <c r="G235" s="22" t="inlineStr">
-        <is>
-          <t>CDW Corporation</t>
-        </is>
+      <c r="F235" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="G235" s="22" t="s">
+        <v>331</v>
       </c>
       <c r="H235" s="22">
         <v>1</v>
@@ -11511,28 +11501,19 @@
       <c r="N235" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="O235" s="22" t="inlineStr">
-        <is>
-          <t>v1.1.0</t>
-        </is>
-      </c>
-      <c r="Q235" s="22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="236">
+      <c r="O235" s="22" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="236">
       <c r="A236" s="22">
         <v>236</v>
       </c>
       <c r="B236" s="22">
         <v>1</v>
       </c>
-      <c r="C236" s="22" t="inlineStr">
-        <is>
-          <t>GC</t>
-        </is>
+      <c r="C236" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="D236" s="5">
         <v>45276</v>
@@ -11540,23 +11521,17 @@
       <c r="E236" s="22">
         <v>1757</v>
       </c>
-      <c r="F236" s="22" t="inlineStr">
-        <is>
-          <t>Telefonica Moviles S.A.</t>
-        </is>
-      </c>
-      <c r="G236" s="22" t="inlineStr">
-        <is>
-          <t>Telefonica</t>
-        </is>
+      <c r="F236" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="G236" s="22" t="s">
+        <v>333</v>
       </c>
       <c r="H236" s="22">
         <v>2</v>
       </c>
-      <c r="I236" s="22" t="inlineStr">
-        <is>
-          <t>Telefonica</t>
-        </is>
+      <c r="I236" s="22" t="s">
+        <v>333</v>
       </c>
       <c r="J236" s="22" t="b">
         <v>1</v>
@@ -11570,28 +11545,19 @@
       <c r="N236" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="O236" s="22" t="inlineStr">
-        <is>
-          <t>v1.1.0</t>
-        </is>
-      </c>
-      <c r="Q236" s="22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="237">
+      <c r="O236" s="22" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="237">
       <c r="A237" s="22">
         <v>237</v>
       </c>
       <c r="B237" s="22">
         <v>2</v>
       </c>
-      <c r="C237" s="22" t="inlineStr">
-        <is>
-          <t>VG</t>
-        </is>
+      <c r="C237" s="22" t="s">
+        <v>247</v>
       </c>
       <c r="D237" s="5">
         <v>45276</v>
@@ -11599,15 +11565,11 @@
       <c r="E237" s="22">
         <v>570</v>
       </c>
-      <c r="F237" s="22" t="inlineStr">
-        <is>
-          <t>Digital Insight Corporation</t>
-        </is>
-      </c>
-      <c r="G237" s="22" t="inlineStr">
-        <is>
-          <t>Test du 16 décembre</t>
-        </is>
+      <c r="F237" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="G237" s="22" t="s">
+        <v>335</v>
       </c>
       <c r="H237" s="22">
         <v>1</v>
@@ -11624,28 +11586,19 @@
       <c r="N237" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="O237" s="22" t="inlineStr">
-        <is>
-          <t>v1.1.0</t>
-        </is>
-      </c>
-      <c r="Q237" s="22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="238">
+      <c r="O237" s="22" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="238">
       <c r="A238" s="22">
         <v>238</v>
       </c>
       <c r="B238" s="22">
         <v>2</v>
       </c>
-      <c r="C238" s="22" t="inlineStr">
-        <is>
-          <t>VG</t>
-        </is>
+      <c r="C238" s="22" t="s">
+        <v>247</v>
       </c>
       <c r="D238" s="5">
         <v>45276</v>
@@ -11664,13 +11617,13 @@
         </is>
       </c>
       <c r="H238" s="22">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="J238" s="22" t="b">
         <v>1</v>
       </c>
       <c r="K238" s="5">
-        <v>45276.512037037</v>
+        <v>45276.594525463</v>
       </c>
       <c r="L238" s="22" t="b">
         <v>0</v>
@@ -11680,26 +11633,19 @@
       </c>
       <c r="O238" s="22" t="inlineStr">
         <is>
-          <t>v1.1.0</t>
+          <t>v1.1.1</t>
         </is>
       </c>
-      <c r="Q238" s="22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="239">
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="239">
       <c r="A239" s="22">
         <v>239</v>
       </c>
       <c r="B239" s="22">
         <v>2</v>
       </c>
-      <c r="C239" s="22" t="inlineStr">
-        <is>
-          <t>VG</t>
-        </is>
+      <c r="C239" s="22" t="s">
+        <v>247</v>
       </c>
       <c r="D239" s="5">
         <v>45276</v>
@@ -11718,13 +11664,13 @@
         </is>
       </c>
       <c r="H239" s="22">
-        <v>0.75</v>
+        <v>3.75</v>
       </c>
       <c r="J239" s="22" t="b">
         <v>0</v>
       </c>
       <c r="K239" s="5">
-        <v>45276.5126041667</v>
+        <v>45276.5943981481</v>
       </c>
       <c r="L239" s="22" t="b">
         <v>0</v>
@@ -11734,26 +11680,19 @@
       </c>
       <c r="O239" s="22" t="inlineStr">
         <is>
-          <t>v1.1.0</t>
+          <t>v1.1.1</t>
         </is>
       </c>
-      <c r="Q239" s="22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="240">
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="240">
       <c r="A240" s="22">
         <v>240</v>
       </c>
       <c r="B240" s="22">
         <v>3</v>
       </c>
-      <c r="C240" s="22" t="inlineStr">
-        <is>
-          <t>MFP</t>
-        </is>
+      <c r="C240" s="22" t="s">
+        <v>59</v>
       </c>
       <c r="D240" s="5">
         <v>45276</v>
@@ -11761,10 +11700,8 @@
       <c r="E240" s="22">
         <v>95</v>
       </c>
-      <c r="F240" s="22" t="inlineStr">
-        <is>
-          <t>Altria Group</t>
-        </is>
+      <c r="F240" s="22" t="s">
+        <v>337</v>
       </c>
       <c r="H240" s="22">
         <v>3</v>
@@ -11781,63 +11718,293 @@
       <c r="N240" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="O240" s="22" t="inlineStr">
-        <is>
-          <t>v1.1.0</t>
-        </is>
-      </c>
-      <c r="Q240" s="22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="241">
+      <c r="O240" s="22" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row spans="1:15" x14ac:dyDescent="0.25" outlineLevel="0" r="241">
       <c r="A241" s="22">
         <v>241</v>
       </c>
       <c r="B241" s="22">
         <v>4</v>
       </c>
-      <c r="C241" s="22" t="inlineStr">
+      <c r="C241" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D241" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E241" s="22">
+        <v>1554</v>
+      </c>
+      <c r="F241" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="G241" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="H241" s="22">
+        <v>2</v>
+      </c>
+      <c r="J241" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K241" s="5">
+        <v>45276.5477662037</v>
+      </c>
+      <c r="L241" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N241" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O241" s="22" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="242">
+      <c r="A242" s="22">
+        <v>242</v>
+      </c>
+      <c r="B242" s="22">
+        <v>4</v>
+      </c>
+      <c r="C242" s="22" t="inlineStr">
         <is>
           <t>RMV</t>
         </is>
       </c>
-      <c r="D241" s="5">
+      <c r="D242" s="5">
         <v>45276</v>
       </c>
-      <c r="E241" s="22">
-        <v>1554</v>
-      </c>
-      <c r="F241" s="22" t="inlineStr">
+      <c r="E242" s="22">
+        <v>1222</v>
+      </c>
+      <c r="F242" s="22" t="inlineStr">
         <is>
-          <t>Royal Caribbean Cruises Ltd.</t>
+          <t>Monsieur Robert M. Vigneault</t>
         </is>
       </c>
-      <c r="G241" s="22" t="inlineStr">
+      <c r="G242" s="22" t="inlineStr">
         <is>
-          <t>Un beau voyage</t>
+          <t>Test avec le meilleur client en ville</t>
         </is>
       </c>
-      <c r="H241" s="22">
-        <v>2</v>
-      </c>
-      <c r="J241" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="K241" s="5">
-        <v>45276.5477662037</v>
-      </c>
-      <c r="L241" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="N241" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="O241" s="22" t="inlineStr">
+      <c r="H242" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="J242" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K242" s="5">
+        <v>45276.622650463</v>
+      </c>
+      <c r="L242" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N242" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O242" s="22" t="inlineStr">
         <is>
-          <t>v1.1.0</t>
+          <t>v1.1.1</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="243">
+      <c r="A243" s="22">
+        <v>243</v>
+      </c>
+      <c r="B243" s="22">
+        <v>4</v>
+      </c>
+      <c r="C243" s="22" t="inlineStr">
+        <is>
+          <t>RMV</t>
+        </is>
+      </c>
+      <c r="D243" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E243" s="22">
+        <v>1134</v>
+      </c>
+      <c r="F243" s="22" t="inlineStr">
+        <is>
+          <t>Marie Guay, experte en RH</t>
+        </is>
+      </c>
+      <c r="G243" s="22" t="inlineStr">
+        <is>
+          <t>Autre test</t>
+        </is>
+      </c>
+      <c r="H243" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="J243" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K243" s="5">
+        <v>45276.6227662037</v>
+      </c>
+      <c r="L243" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N243" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O243" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.1</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="244">
+      <c r="A244" s="22">
+        <v>244</v>
+      </c>
+      <c r="B244" s="22">
+        <v>4</v>
+      </c>
+      <c r="C244" s="22" t="inlineStr">
+        <is>
+          <t>RMV</t>
+        </is>
+      </c>
+      <c r="D244" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E244" s="22">
+        <v>1134</v>
+      </c>
+      <c r="F244" s="22" t="inlineStr">
+        <is>
+          <t>Marie Guay, experte en RH</t>
+        </is>
+      </c>
+      <c r="G244" s="22" t="inlineStr">
+        <is>
+          <t>Autre test</t>
+        </is>
+      </c>
+      <c r="H244" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="J244" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K244" s="5">
+        <v>45276.6228472222</v>
+      </c>
+      <c r="L244" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N244" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O244" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.1</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="245">
+      <c r="A245" s="22">
+        <v>245</v>
+      </c>
+      <c r="B245" s="22">
+        <v>4</v>
+      </c>
+      <c r="C245" s="22" t="inlineStr">
+        <is>
+          <t>RMV</t>
+        </is>
+      </c>
+      <c r="D245" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E245" s="22">
+        <v>241</v>
+      </c>
+      <c r="F245" s="22" t="inlineStr">
+        <is>
+          <t>BCE, Inc.</t>
+        </is>
+      </c>
+      <c r="G245" s="22" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="H245" s="22">
+        <v>1</v>
+      </c>
+      <c r="J245" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K245" s="5">
+        <v>45276.6058912037</v>
+      </c>
+      <c r="L245" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N245" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O245" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.1</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="246">
+      <c r="A246" s="22">
+        <v>246</v>
+      </c>
+      <c r="B246" s="22">
+        <v>4</v>
+      </c>
+      <c r="C246" s="22" t="inlineStr">
+        <is>
+          <t>RMV</t>
+        </is>
+      </c>
+      <c r="D246" s="5">
+        <v>45276</v>
+      </c>
+      <c r="E246" s="22">
+        <v>229</v>
+      </c>
+      <c r="F246" s="22" t="inlineStr">
+        <is>
+          <t>Bank of New York Company, Inc. (The)</t>
+        </is>
+      </c>
+      <c r="G246" s="22" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="H246" s="22">
+        <v>1</v>
+      </c>
+      <c r="J246" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K246" s="5">
+        <v>45276.6220601852</v>
+      </c>
+      <c r="L246" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N246" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O246" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.1.2 - Début de l'intégration de Facture
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -11893,10 +11893,10 @@
         <v>0.5</v>
       </c>
       <c r="J244" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K244" s="5">
-        <v>45276.6228472222</v>
+        <v>45276.7048726852</v>
       </c>
       <c r="L244" s="22" t="b">
         <v>0</v>
@@ -11906,7 +11906,7 @@
       </c>
       <c r="O244" s="22" t="inlineStr">
         <is>
-          <t>v1.1.1</t>
+          <t>v1.1.2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.1.9.8 - Démonstration à Guillaume
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -1696,11 +1696,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:P246"/>
+  <dimension ref="A1:P247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" rightToLeft="false">
       <pane ySplit="600" topLeftCell="A216"/>
       <selection sqref="A1:P1"/>
       <selection pane="bottomLeft" activeCell="O227" sqref="O227"/>
@@ -1726,7 +1726,7 @@
     <col min="16" max="16" width="10.140625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
       <c r="A2" s="9">
         <v>2</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="6">
-        <v>44976.765347222201</v>
+        <v>44976.7653472222</v>
       </c>
       <c r="L2" s="18" t="b">
         <v>0</v>
@@ -1820,7 +1820,7 @@
       <c r="O2" s="14"/>
       <c r="P2" s="12"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
       <c r="A3" s="9">
         <v>3</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="6">
-        <v>44979.379212963002</v>
+        <v>44979.379212963</v>
       </c>
       <c r="L3" s="18" t="b">
         <v>0</v>
@@ -1864,7 +1864,7 @@
       <c r="O3" s="14"/>
       <c r="P3" s="12"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
       <c r="A4" s="9">
         <v>4</v>
       </c>
@@ -1906,7 +1906,7 @@
       <c r="O4" s="14"/>
       <c r="P4" s="12"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
       <c r="A5" s="9">
         <v>5</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="6">
-        <v>44979.390057870398</v>
+        <v>44979.3900578704</v>
       </c>
       <c r="L5" s="18" t="b">
         <v>0</v>
@@ -1950,7 +1950,7 @@
       <c r="O5" s="14"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="6">
       <c r="A6" s="9">
         <v>6</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="6">
-        <v>44979.393460648098</v>
+        <v>44979.3934606481</v>
       </c>
       <c r="L6" s="18" t="b">
         <v>0</v>
@@ -1994,7 +1994,7 @@
       <c r="O6" s="14"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="7">
       <c r="A7" s="9">
         <v>7</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="6">
-        <v>44979.413668981499</v>
+        <v>44979.4136689815</v>
       </c>
       <c r="L7" s="18" t="b">
         <v>0</v>
@@ -2038,7 +2038,7 @@
       <c r="O7" s="14"/>
       <c r="P7" s="12"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="8">
       <c r="A8" s="9">
         <v>8</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="6">
-        <v>44979.414583333302</v>
+        <v>44979.4145833333</v>
       </c>
       <c r="L8" s="18" t="s">
         <v>51</v>
@@ -2082,7 +2082,7 @@
       <c r="O8" s="14"/>
       <c r="P8" s="12"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="9">
       <c r="A9" s="9">
         <v>9</v>
       </c>
@@ -2124,7 +2124,7 @@
       <c r="O9" s="14"/>
       <c r="P9" s="12"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="10">
       <c r="A10" s="9">
         <v>10</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="6">
-        <v>44979.429293981499</v>
+        <v>44979.4292939815</v>
       </c>
       <c r="L10" s="18" t="b">
         <v>0</v>
@@ -2168,7 +2168,7 @@
       <c r="O10" s="14"/>
       <c r="P10" s="12"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="11">
       <c r="A11" s="9">
         <v>11</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>1</v>
       </c>
       <c r="K11" s="6">
-        <v>44979.433402777802</v>
+        <v>44979.4334027778</v>
       </c>
       <c r="L11" s="18" t="b">
         <v>0</v>
@@ -2212,7 +2212,7 @@
       <c r="O11" s="14"/>
       <c r="P11" s="12"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="12">
       <c r="A12" s="9">
         <v>12</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="6">
-        <v>44979.437129629601</v>
+        <v>44979.4371296296</v>
       </c>
       <c r="L12" s="18" t="b">
         <v>0</v>
@@ -2254,7 +2254,7 @@
       <c r="O12" s="14"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="13">
       <c r="A13" s="9">
         <v>13</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="6">
-        <v>44979.437465277799</v>
+        <v>44979.4374652778</v>
       </c>
       <c r="L13" s="18" t="b">
         <v>0</v>
@@ -2298,7 +2298,7 @@
       <c r="O13" s="14"/>
       <c r="P13" s="12"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="14">
       <c r="A14" s="9">
         <v>14</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="O14" s="14"/>
       <c r="P14" s="12"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="15">
       <c r="A15" s="9">
         <v>15</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>1</v>
       </c>
       <c r="K15" s="6">
-        <v>44979.439270833303</v>
+        <v>44979.4392708333</v>
       </c>
       <c r="L15" s="18" t="b">
         <v>0</v>
@@ -2386,7 +2386,7 @@
       <c r="O15" s="14"/>
       <c r="P15" s="12"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="16">
       <c r="A16" s="9">
         <v>16</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>65</v>
       </c>
       <c r="K16" s="6">
-        <v>44979.445138888899</v>
+        <v>44979.4451388889</v>
       </c>
       <c r="L16" s="18" t="s">
         <v>51</v>
@@ -2430,7 +2430,7 @@
       <c r="O16" s="14"/>
       <c r="P16" s="12"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="17">
       <c r="A17" s="9">
         <v>17</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="6">
-        <v>44979.445787037002</v>
+        <v>44979.445787037</v>
       </c>
       <c r="L17" s="18" t="b">
         <v>0</v>
@@ -2474,7 +2474,7 @@
       <c r="O17" s="14"/>
       <c r="P17" s="12"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="18">
       <c r="A18" s="9">
         <v>18</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>1</v>
       </c>
       <c r="K18" s="6">
-        <v>44979.446041666699</v>
+        <v>44979.4460416667</v>
       </c>
       <c r="L18" s="18" t="b">
         <v>0</v>
@@ -2514,7 +2514,7 @@
       <c r="O18" s="14"/>
       <c r="P18" s="12"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="19">
       <c r="A19" s="9">
         <v>19</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="6">
-        <v>44979.446192129602</v>
+        <v>44979.4461921296</v>
       </c>
       <c r="L19" s="18" t="b">
         <v>0</v>
@@ -2556,7 +2556,7 @@
       <c r="O19" s="14"/>
       <c r="P19" s="12"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="20">
       <c r="A20" s="9">
         <v>20</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>65</v>
       </c>
       <c r="K20" s="6">
-        <v>44980.429861111101</v>
+        <v>44980.4298611111</v>
       </c>
       <c r="L20" s="18" t="s">
         <v>51</v>
@@ -2598,7 +2598,7 @@
       <c r="O20" s="14"/>
       <c r="P20" s="12"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="21">
       <c r="A21" s="9">
         <v>21</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>1</v>
       </c>
       <c r="K21" s="6">
-        <v>44980.526597222197</v>
+        <v>44980.5265972222</v>
       </c>
       <c r="L21" s="18" t="b">
         <v>0</v>
@@ -2640,7 +2640,7 @@
       <c r="O21" s="14"/>
       <c r="P21" s="12"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="22">
       <c r="A22" s="9">
         <v>22</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>65</v>
       </c>
       <c r="K22" s="6">
-        <v>44980.527083333298</v>
+        <v>44980.5270833333</v>
       </c>
       <c r="L22" s="18" t="s">
         <v>51</v>
@@ -2682,7 +2682,7 @@
       <c r="O22" s="14"/>
       <c r="P22" s="12"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="23">
       <c r="A23" s="9">
         <v>23</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="6">
-        <v>44980.531087962998</v>
+        <v>44980.531087963</v>
       </c>
       <c r="L23" s="18" t="b">
         <v>0</v>
@@ -2724,7 +2724,7 @@
       <c r="O23" s="14"/>
       <c r="P23" s="12"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="24">
       <c r="A24" s="9">
         <v>24</v>
       </c>
@@ -2768,7 +2768,7 @@
       <c r="O24" s="14"/>
       <c r="P24" s="12"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="25">
       <c r="A25" s="9">
         <v>25</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="6">
-        <v>44980.893067129597</v>
+        <v>44980.8930671296</v>
       </c>
       <c r="L25" s="18" t="b">
         <v>0</v>
@@ -2812,7 +2812,7 @@
       <c r="O25" s="14"/>
       <c r="P25" s="12"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="26">
       <c r="A26" s="9">
         <v>26</v>
       </c>
@@ -2854,7 +2854,7 @@
       <c r="O26" s="14"/>
       <c r="P26" s="12"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="27">
       <c r="A27" s="9">
         <v>27</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="6">
-        <v>44981.441863425898</v>
+        <v>44981.4418634259</v>
       </c>
       <c r="L27" s="18" t="b">
         <v>0</v>
@@ -2896,7 +2896,7 @@
       <c r="O27" s="14"/>
       <c r="P27" s="12"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="28">
       <c r="A28" s="9">
         <v>28</v>
       </c>
@@ -2938,7 +2938,7 @@
       <c r="O28" s="14"/>
       <c r="P28" s="12"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="29">
       <c r="A29" s="9">
         <v>29</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>1</v>
       </c>
       <c r="K29" s="6">
-        <v>44981.448298611103</v>
+        <v>44981.4482986111</v>
       </c>
       <c r="L29" s="18" t="b">
         <v>0</v>
@@ -2980,7 +2980,7 @@
       <c r="O29" s="14"/>
       <c r="P29" s="12"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="30">
       <c r="A30" s="9">
         <v>30</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>1</v>
       </c>
       <c r="K30" s="6">
-        <v>44981.450335648202</v>
+        <v>44981.4503356482</v>
       </c>
       <c r="L30" s="18" t="b">
         <v>0</v>
@@ -3022,7 +3022,7 @@
       <c r="O30" s="14"/>
       <c r="P30" s="12"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="31">
       <c r="A31" s="9">
         <v>31</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>1</v>
       </c>
       <c r="K31" s="6">
-        <v>44981.469525462999</v>
+        <v>44981.469525463</v>
       </c>
       <c r="L31" s="18" t="b">
         <v>0</v>
@@ -3064,7 +3064,7 @@
       <c r="O31" s="14"/>
       <c r="P31" s="12"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="32">
       <c r="A32" s="9">
         <v>32</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>1</v>
       </c>
       <c r="K32" s="6">
-        <v>44981.475532407399</v>
+        <v>44981.4755324074</v>
       </c>
       <c r="L32" s="18" t="b">
         <v>0</v>
@@ -3108,7 +3108,7 @@
       <c r="O32" s="14"/>
       <c r="P32" s="12"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="33">
       <c r="A33" s="9">
         <v>33</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>1</v>
       </c>
       <c r="K33" s="6">
-        <v>44981.478599536997</v>
+        <v>44981.478599537</v>
       </c>
       <c r="L33" s="18" t="b">
         <v>0</v>
@@ -3150,7 +3150,7 @@
       <c r="O33" s="14"/>
       <c r="P33" s="12"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="34">
       <c r="A34" s="9">
         <v>34</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>1</v>
       </c>
       <c r="K34" s="6">
-        <v>44981.519988425898</v>
+        <v>44981.5199884259</v>
       </c>
       <c r="L34" s="18" t="b">
         <v>0</v>
@@ -3192,7 +3192,7 @@
       <c r="O34" s="14"/>
       <c r="P34" s="12"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="35">
       <c r="A35" s="9">
         <v>35</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>1</v>
       </c>
       <c r="K35" s="6">
-        <v>44981.522662037001</v>
+        <v>44981.522662037</v>
       </c>
       <c r="L35" s="18" t="b">
         <v>0</v>
@@ -3234,7 +3234,7 @@
       <c r="O35" s="14"/>
       <c r="P35" s="12"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="36">
       <c r="A36" s="9">
         <v>36</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>1</v>
       </c>
       <c r="K36" s="6">
-        <v>44981.524583333303</v>
+        <v>44981.5245833333</v>
       </c>
       <c r="L36" s="18" t="b">
         <v>0</v>
@@ -3276,7 +3276,7 @@
       <c r="O36" s="14"/>
       <c r="P36" s="12"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="37">
       <c r="A37" s="9">
         <v>37</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>1</v>
       </c>
       <c r="K37" s="6">
-        <v>44981.536736111098</v>
+        <v>44981.5367361111</v>
       </c>
       <c r="L37" s="18" t="b">
         <v>0</v>
@@ -3318,7 +3318,7 @@
       <c r="O37" s="14"/>
       <c r="P37" s="12"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="38">
       <c r="A38" s="9">
         <v>38</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>1</v>
       </c>
       <c r="K38" s="6">
-        <v>44981.538946759298</v>
+        <v>44981.5389467593</v>
       </c>
       <c r="L38" s="18" t="b">
         <v>0</v>
@@ -3360,7 +3360,7 @@
       <c r="O38" s="14"/>
       <c r="P38" s="12"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="39">
       <c r="A39" s="9">
         <v>39</v>
       </c>
@@ -3402,7 +3402,7 @@
       <c r="O39" s="14"/>
       <c r="P39" s="12"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="40">
       <c r="A40" s="9">
         <v>40</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>1</v>
       </c>
       <c r="K40" s="6">
-        <v>44981.561747685198</v>
+        <v>44981.5617476852</v>
       </c>
       <c r="L40" s="18" t="b">
         <v>0</v>
@@ -3444,7 +3444,7 @@
       <c r="O40" s="14"/>
       <c r="P40" s="12"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="41">
       <c r="A41" s="9">
         <v>41</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>1</v>
       </c>
       <c r="K41" s="6">
-        <v>44981.567627314798</v>
+        <v>44981.5676273148</v>
       </c>
       <c r="L41" s="18" t="b">
         <v>0</v>
@@ -3486,7 +3486,7 @@
       <c r="O41" s="14"/>
       <c r="P41" s="12"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="42">
       <c r="A42" s="9">
         <v>42</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>1</v>
       </c>
       <c r="K42" s="6">
-        <v>44981.623101851903</v>
+        <v>44981.6231018519</v>
       </c>
       <c r="L42" s="18" t="b">
         <v>0</v>
@@ -3530,7 +3530,7 @@
       <c r="O42" s="14"/>
       <c r="P42" s="12"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="43">
       <c r="A43" s="9">
         <v>43</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>1</v>
       </c>
       <c r="K43" s="6">
-        <v>44987.941435185203</v>
+        <v>44987.9414351852</v>
       </c>
       <c r="L43" s="18" t="b">
         <v>0</v>
@@ -3574,7 +3574,7 @@
       <c r="O43" s="14"/>
       <c r="P43" s="12"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="44">
       <c r="A44" s="9">
         <v>44</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>1</v>
       </c>
       <c r="K44" s="6">
-        <v>44987.941793981503</v>
+        <v>44987.9417939815</v>
       </c>
       <c r="L44" s="18" t="b">
         <v>0</v>
@@ -3616,7 +3616,7 @@
       <c r="O44" s="14"/>
       <c r="P44" s="12"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="45">
       <c r="A45" s="9">
         <v>45</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>1</v>
       </c>
       <c r="K45" s="6">
-        <v>44987.942037036999</v>
+        <v>44987.942037037</v>
       </c>
       <c r="L45" s="18" t="b">
         <v>0</v>
@@ -3658,7 +3658,7 @@
       <c r="O45" s="14"/>
       <c r="P45" s="12"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="46">
       <c r="A46" s="9">
         <v>46</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>1</v>
       </c>
       <c r="K46" s="6">
-        <v>44987.943229166704</v>
+        <v>44987.9432291667</v>
       </c>
       <c r="L46" s="18" t="b">
         <v>0</v>
@@ -3700,7 +3700,7 @@
       <c r="O46" s="14"/>
       <c r="P46" s="12"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="47">
       <c r="A47" s="9">
         <v>47</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>1</v>
       </c>
       <c r="K47" s="6">
-        <v>44988.359097222201</v>
+        <v>44988.3590972222</v>
       </c>
       <c r="L47" s="18" t="b">
         <v>0</v>
@@ -3742,7 +3742,7 @@
       <c r="O47" s="14"/>
       <c r="P47" s="12"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="48">
       <c r="A48" s="9">
         <v>48</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
       <c r="K48" s="6">
-        <v>45003.453194444402</v>
+        <v>45003.4531944444</v>
       </c>
       <c r="L48" s="18" t="b">
         <v>0</v>
@@ -3784,7 +3784,7 @@
       <c r="O48" s="14"/>
       <c r="P48" s="12"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="49">
       <c r="A49" s="9">
         <v>49</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>1</v>
       </c>
       <c r="K49" s="6">
-        <v>45003.453518518501</v>
+        <v>45003.4535185185</v>
       </c>
       <c r="L49" s="18" t="b">
         <v>0</v>
@@ -3826,7 +3826,7 @@
       <c r="O49" s="14"/>
       <c r="P49" s="12"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="50">
       <c r="A50" s="9">
         <v>50</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>1</v>
       </c>
       <c r="K50" s="6">
-        <v>45004.731134259302</v>
+        <v>45004.7311342593</v>
       </c>
       <c r="L50" s="18" t="b">
         <v>0</v>
@@ -3868,7 +3868,7 @@
       <c r="O50" s="14"/>
       <c r="P50" s="12"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="51">
       <c r="A51" s="9">
         <v>51</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>1</v>
       </c>
       <c r="K51" s="6">
-        <v>45005.433055555601</v>
+        <v>45005.4330555556</v>
       </c>
       <c r="L51" s="18" t="b">
         <v>0</v>
@@ -3910,7 +3910,7 @@
       <c r="O51" s="14"/>
       <c r="P51" s="12"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="52">
       <c r="A52" s="9">
         <v>52</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>1</v>
       </c>
       <c r="K52" s="6">
-        <v>45005.629942129599</v>
+        <v>45005.6299421296</v>
       </c>
       <c r="L52" s="18" t="b">
         <v>0</v>
@@ -3952,7 +3952,7 @@
       <c r="O52" s="14"/>
       <c r="P52" s="12"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="53">
       <c r="A53" s="9">
         <v>53</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>1</v>
       </c>
       <c r="K53" s="6">
-        <v>45005.645393518498</v>
+        <v>45005.6453935185</v>
       </c>
       <c r="L53" s="18" t="b">
         <v>0</v>
@@ -3994,7 +3994,7 @@
       <c r="O53" s="14"/>
       <c r="P53" s="12"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="54">
       <c r="A54" s="9">
         <v>54</v>
       </c>
@@ -4036,7 +4036,7 @@
       <c r="O54" s="14"/>
       <c r="P54" s="12"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="55">
       <c r="A55" s="9">
         <v>55</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>65</v>
       </c>
       <c r="K55" s="6">
-        <v>45006.319386574098</v>
+        <v>45006.3193865741</v>
       </c>
       <c r="L55" s="18" t="s">
         <v>51</v>
@@ -4078,7 +4078,7 @@
       <c r="O55" s="14"/>
       <c r="P55" s="12"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="56">
       <c r="A56" s="9">
         <v>56</v>
       </c>
@@ -4120,7 +4120,7 @@
       <c r="O56" s="14"/>
       <c r="P56" s="12"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="57">
       <c r="A57" s="9">
         <v>57</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="6">
-        <v>45006.328726851898</v>
+        <v>45006.3287268519</v>
       </c>
       <c r="L57" s="18" t="b">
         <v>0</v>
@@ -4162,7 +4162,7 @@
       <c r="O57" s="14"/>
       <c r="P57" s="12"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="58">
       <c r="A58" s="9">
         <v>58</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>1</v>
       </c>
       <c r="K58" s="6">
-        <v>45006.328912037003</v>
+        <v>45006.328912037</v>
       </c>
       <c r="L58" s="18" t="b">
         <v>0</v>
@@ -4204,7 +4204,7 @@
       <c r="O58" s="14"/>
       <c r="P58" s="12"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="59">
       <c r="A59" s="9">
         <v>59</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>1</v>
       </c>
       <c r="K59" s="6">
-        <v>45006.353715277801</v>
+        <v>45006.3537152778</v>
       </c>
       <c r="L59" s="18" t="b">
         <v>0</v>
@@ -4246,7 +4246,7 @@
       <c r="O59" s="14"/>
       <c r="P59" s="12"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="60">
       <c r="A60" s="9">
         <v>60</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>1</v>
       </c>
       <c r="K60" s="6">
-        <v>45006.360671296301</v>
+        <v>45006.3606712963</v>
       </c>
       <c r="L60" s="18" t="b">
         <v>0</v>
@@ -4288,7 +4288,7 @@
       <c r="O60" s="14"/>
       <c r="P60" s="12"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="61">
       <c r="A61" s="9">
         <v>61</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>1</v>
       </c>
       <c r="K61" s="6">
-        <v>45006.382627314801</v>
+        <v>45006.3826273148</v>
       </c>
       <c r="L61" s="18" t="b">
         <v>0</v>
@@ -4330,7 +4330,7 @@
       <c r="O61" s="14"/>
       <c r="P61" s="12"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="62">
       <c r="A62" s="9">
         <v>62</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>1</v>
       </c>
       <c r="K62" s="6">
-        <v>45006.390879629602</v>
+        <v>45006.3908796296</v>
       </c>
       <c r="L62" s="18" t="b">
         <v>0</v>
@@ -4374,7 +4374,7 @@
       <c r="O62" s="14"/>
       <c r="P62" s="12"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="63">
       <c r="A63" s="9">
         <v>63</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>1</v>
       </c>
       <c r="K63" s="6">
-        <v>45006.419502314799</v>
+        <v>45006.4195023148</v>
       </c>
       <c r="L63" s="18" t="b">
         <v>0</v>
@@ -4416,7 +4416,7 @@
       <c r="O63" s="14"/>
       <c r="P63" s="12"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="64">
       <c r="A64" s="9">
         <v>64</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>1</v>
       </c>
       <c r="K64" s="6">
-        <v>45006.436261574097</v>
+        <v>45006.4362615741</v>
       </c>
       <c r="L64" s="18" t="b">
         <v>0</v>
@@ -4458,7 +4458,7 @@
       <c r="O64" s="14"/>
       <c r="P64" s="12"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="65">
       <c r="A65" s="9">
         <v>65</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>1</v>
       </c>
       <c r="K65" s="6">
-        <v>45006.437523148103</v>
+        <v>45006.4375231481</v>
       </c>
       <c r="L65" s="18" t="b">
         <v>0</v>
@@ -4500,7 +4500,7 @@
       <c r="O65" s="14"/>
       <c r="P65" s="12"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="66">
       <c r="A66" s="9">
         <v>66</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>1</v>
       </c>
       <c r="K66" s="6">
-        <v>45006.437824074099</v>
+        <v>45006.4378240741</v>
       </c>
       <c r="L66" s="18" t="b">
         <v>0</v>
@@ -4542,7 +4542,7 @@
       <c r="O66" s="14"/>
       <c r="P66" s="12"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="67">
       <c r="A67" s="9">
         <v>67</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>1</v>
       </c>
       <c r="K67" s="6">
-        <v>45006.438090277799</v>
+        <v>45006.4380902778</v>
       </c>
       <c r="L67" s="18" t="b">
         <v>0</v>
@@ -4584,7 +4584,7 @@
       <c r="O67" s="14"/>
       <c r="P67" s="12"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="68">
       <c r="A68" s="9">
         <v>68</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>1</v>
       </c>
       <c r="K68" s="6">
-        <v>45006.438750000001</v>
+        <v>45006.43875</v>
       </c>
       <c r="L68" s="18" t="b">
         <v>0</v>
@@ -4626,7 +4626,7 @@
       <c r="O68" s="14"/>
       <c r="P68" s="12"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="69">
       <c r="A69" s="9">
         <v>69</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>1</v>
       </c>
       <c r="K69" s="6">
-        <v>45006.439062500001</v>
+        <v>45006.4390625</v>
       </c>
       <c r="L69" s="18" t="b">
         <v>0</v>
@@ -4668,7 +4668,7 @@
       <c r="O69" s="14"/>
       <c r="P69" s="12"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="70">
       <c r="A70" s="9">
         <v>70</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>1</v>
       </c>
       <c r="K70" s="6">
-        <v>45006.440173611103</v>
+        <v>45006.4401736111</v>
       </c>
       <c r="L70" s="18" t="b">
         <v>0</v>
@@ -4710,7 +4710,7 @@
       <c r="O70" s="14"/>
       <c r="P70" s="12"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="71">
       <c r="A71" s="9">
         <v>71</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>1</v>
       </c>
       <c r="K71" s="6">
-        <v>45006.472696759301</v>
+        <v>45006.4726967593</v>
       </c>
       <c r="L71" s="18" t="b">
         <v>0</v>
@@ -4752,7 +4752,7 @@
       <c r="O71" s="14"/>
       <c r="P71" s="12"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="72">
       <c r="A72" s="9">
         <v>72</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>1</v>
       </c>
       <c r="K72" s="6">
-        <v>45006.473784722199</v>
+        <v>45006.4737847222</v>
       </c>
       <c r="L72" s="18" t="b">
         <v>0</v>
@@ -4794,7 +4794,7 @@
       <c r="O72" s="14"/>
       <c r="P72" s="12"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="73">
       <c r="A73" s="9">
         <v>73</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>1</v>
       </c>
       <c r="K73" s="6">
-        <v>45006.474016203698</v>
+        <v>45006.4740162037</v>
       </c>
       <c r="L73" s="18" t="b">
         <v>0</v>
@@ -4836,7 +4836,7 @@
       <c r="O73" s="14"/>
       <c r="P73" s="12"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="74">
       <c r="A74" s="9">
         <v>74</v>
       </c>
@@ -4878,7 +4878,7 @@
       <c r="O74" s="14"/>
       <c r="P74" s="12"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="75">
       <c r="A75" s="9">
         <v>75</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>1</v>
       </c>
       <c r="K75" s="6">
-        <v>45006.475092592598</v>
+        <v>45006.4750925926</v>
       </c>
       <c r="L75" s="18" t="b">
         <v>0</v>
@@ -4918,7 +4918,7 @@
       <c r="O75" s="14"/>
       <c r="P75" s="12"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="76">
       <c r="A76" s="9">
         <v>76</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>1</v>
       </c>
       <c r="K76" s="6">
-        <v>45006.483124999999</v>
+        <v>45006.483125</v>
       </c>
       <c r="L76" s="18" t="b">
         <v>0</v>
@@ -4958,7 +4958,7 @@
       <c r="O76" s="14"/>
       <c r="P76" s="12"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="77">
       <c r="A77" s="9">
         <v>77</v>
       </c>
@@ -5000,7 +5000,7 @@
       <c r="O77" s="14"/>
       <c r="P77" s="12"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="78">
       <c r="A78" s="9">
         <v>78</v>
       </c>
@@ -5030,7 +5030,7 @@
         <v>1</v>
       </c>
       <c r="K78" s="6">
-        <v>45006.487939814797</v>
+        <v>45006.4879398148</v>
       </c>
       <c r="L78" s="18" t="b">
         <v>0</v>
@@ -5042,7 +5042,7 @@
       <c r="O78" s="14"/>
       <c r="P78" s="12"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="79">
       <c r="A79" s="9">
         <v>79</v>
       </c>
@@ -5070,7 +5070,7 @@
       <c r="I79" s="14"/>
       <c r="J79" s="18"/>
       <c r="K79" s="6">
-        <v>45006.488333333298</v>
+        <v>45006.4883333333</v>
       </c>
       <c r="L79" s="18" t="b">
         <v>0</v>
@@ -5082,7 +5082,7 @@
       <c r="O79" s="14"/>
       <c r="P79" s="12"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="80">
       <c r="A80" s="9">
         <v>80</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>1</v>
       </c>
       <c r="K80" s="6">
-        <v>45006.493657407402</v>
+        <v>45006.4936574074</v>
       </c>
       <c r="L80" s="18" t="b">
         <v>0</v>
@@ -5124,7 +5124,7 @@
       <c r="O80" s="14"/>
       <c r="P80" s="12"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="81">
       <c r="A81" s="9">
         <v>81</v>
       </c>
@@ -5166,7 +5166,7 @@
       <c r="O81" s="14"/>
       <c r="P81" s="12"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="82">
       <c r="A82" s="9">
         <v>82</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>1</v>
       </c>
       <c r="K82" s="6">
-        <v>45006.545081018499</v>
+        <v>45006.5450810185</v>
       </c>
       <c r="L82" s="18" t="b">
         <v>0</v>
@@ -5208,7 +5208,7 @@
       <c r="O82" s="14"/>
       <c r="P82" s="12"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="83">
       <c r="A83" s="9">
         <v>83</v>
       </c>
@@ -5238,7 +5238,7 @@
         <v>1</v>
       </c>
       <c r="K83" s="6">
-        <v>45006.557372685202</v>
+        <v>45006.5573726852</v>
       </c>
       <c r="L83" s="18" t="b">
         <v>0</v>
@@ -5250,7 +5250,7 @@
       <c r="O83" s="14"/>
       <c r="P83" s="12"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="84">
       <c r="A84" s="9">
         <v>84</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>1</v>
       </c>
       <c r="K84" s="6">
-        <v>45006.559016203697</v>
+        <v>45006.5590162037</v>
       </c>
       <c r="L84" s="18" t="b">
         <v>0</v>
@@ -5292,7 +5292,7 @@
       <c r="O84" s="14"/>
       <c r="P84" s="12"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="85">
       <c r="A85" s="9">
         <v>85</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>1</v>
       </c>
       <c r="K85" s="6">
-        <v>45006.559641203698</v>
+        <v>45006.5596412037</v>
       </c>
       <c r="L85" s="18" t="b">
         <v>0</v>
@@ -5334,7 +5334,7 @@
       <c r="O85" s="14"/>
       <c r="P85" s="12"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="86">
       <c r="A86" s="9">
         <v>86</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>1</v>
       </c>
       <c r="K86" s="6">
-        <v>45006.577060185198</v>
+        <v>45006.5770601852</v>
       </c>
       <c r="L86" s="18" t="b">
         <v>0</v>
@@ -5374,7 +5374,7 @@
       <c r="O86" s="14"/>
       <c r="P86" s="12"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="87">
       <c r="A87" s="9">
         <v>87</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>1</v>
       </c>
       <c r="K87" s="6">
-        <v>45006.577199074098</v>
+        <v>45006.5771990741</v>
       </c>
       <c r="L87" s="18" t="b">
         <v>0</v>
@@ -5416,7 +5416,7 @@
       <c r="O87" s="14"/>
       <c r="P87" s="12"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="88">
       <c r="A88" s="9">
         <v>88</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="6">
-        <v>45006.577696759297</v>
+        <v>45006.5776967593</v>
       </c>
       <c r="L88" s="18" t="b">
         <v>0</v>
@@ -5458,7 +5458,7 @@
       <c r="O88" s="14"/>
       <c r="P88" s="12"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="89">
       <c r="A89" s="9">
         <v>89</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>1</v>
       </c>
       <c r="K89" s="6">
-        <v>45007.360069444403</v>
+        <v>45007.3600694444</v>
       </c>
       <c r="L89" s="18" t="b">
         <v>0</v>
@@ -5500,7 +5500,7 @@
       <c r="O89" s="14"/>
       <c r="P89" s="12"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="90">
       <c r="A90" s="9">
         <v>90</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>1</v>
       </c>
       <c r="K90" s="6">
-        <v>45007.479652777802</v>
+        <v>45007.4796527778</v>
       </c>
       <c r="L90" s="18" t="b">
         <v>0</v>
@@ -5542,7 +5542,7 @@
       <c r="O90" s="14"/>
       <c r="P90" s="12"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="91">
       <c r="A91" s="9">
         <v>91</v>
       </c>
@@ -5572,7 +5572,7 @@
         <v>1</v>
       </c>
       <c r="K91" s="6">
-        <v>45007.743148148104</v>
+        <v>45007.7431481481</v>
       </c>
       <c r="L91" s="18" t="b">
         <v>0</v>
@@ -5584,7 +5584,7 @@
       <c r="O91" s="14"/>
       <c r="P91" s="12"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="92">
       <c r="A92" s="9">
         <v>92</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>1</v>
       </c>
       <c r="K92" s="6">
-        <v>45007.748680555596</v>
+        <v>45007.7486805556</v>
       </c>
       <c r="L92" s="18" t="b">
         <v>0</v>
@@ -5626,7 +5626,7 @@
       <c r="O92" s="14"/>
       <c r="P92" s="12"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="93">
       <c r="A93" s="9">
         <v>93</v>
       </c>
@@ -5658,7 +5658,7 @@
         <v>1</v>
       </c>
       <c r="K93" s="6">
-        <v>45007.783877314803</v>
+        <v>45007.7838773148</v>
       </c>
       <c r="L93" s="18" t="b">
         <v>0</v>
@@ -5670,7 +5670,7 @@
       <c r="O93" s="14"/>
       <c r="P93" s="12"/>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="94">
       <c r="A94" s="9">
         <v>94</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>1</v>
       </c>
       <c r="K94" s="6">
-        <v>45007.784224536997</v>
+        <v>45007.784224537</v>
       </c>
       <c r="L94" s="18" t="b">
         <v>0</v>
@@ -5712,7 +5712,7 @@
       <c r="O94" s="14"/>
       <c r="P94" s="12"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="95">
       <c r="A95" s="9">
         <v>95</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>1</v>
       </c>
       <c r="K95" s="6">
-        <v>45007.784652777802</v>
+        <v>45007.7846527778</v>
       </c>
       <c r="L95" s="18" t="b">
         <v>0</v>
@@ -5754,7 +5754,7 @@
       <c r="O95" s="14"/>
       <c r="P95" s="12"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="96">
       <c r="A96" s="9">
         <v>96</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>1</v>
       </c>
       <c r="K96" s="6">
-        <v>45008.690810185202</v>
+        <v>45008.6908101852</v>
       </c>
       <c r="L96" s="18" t="b">
         <v>0</v>
@@ -5796,7 +5796,7 @@
       <c r="O96" s="14"/>
       <c r="P96" s="12"/>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="97">
       <c r="A97" s="9">
         <v>97</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>1</v>
       </c>
       <c r="K97" s="6">
-        <v>45008.713206018503</v>
+        <v>45008.7132060185</v>
       </c>
       <c r="L97" s="18" t="b">
         <v>0</v>
@@ -5838,7 +5838,7 @@
       <c r="O97" s="14"/>
       <c r="P97" s="12"/>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="98">
       <c r="A98" s="9">
         <v>98</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>1</v>
       </c>
       <c r="K98" s="6">
-        <v>45008.716041666703</v>
+        <v>45008.7160416667</v>
       </c>
       <c r="L98" s="18" t="b">
         <v>0</v>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="P98" s="12"/>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="99">
       <c r="A99" s="9">
         <v>99</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>1</v>
       </c>
       <c r="K99" s="6">
-        <v>45008.717870370398</v>
+        <v>45008.7178703704</v>
       </c>
       <c r="L99" s="18" t="b">
         <v>0</v>
@@ -5920,7 +5920,7 @@
       </c>
       <c r="P99" s="12"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="100">
       <c r="A100" s="9">
         <v>100</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>1</v>
       </c>
       <c r="K100" s="6">
-        <v>45008.718692129602</v>
+        <v>45008.7186921296</v>
       </c>
       <c r="L100" s="18" t="b">
         <v>0</v>
@@ -5961,7 +5961,7 @@
       </c>
       <c r="P100" s="12"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="101">
       <c r="A101" s="9">
         <v>101</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>65</v>
       </c>
       <c r="K101" s="6">
-        <v>45009.360347222202</v>
+        <v>45009.3603472222</v>
       </c>
       <c r="L101" s="18" t="s">
         <v>51</v>
@@ -6003,7 +6003,7 @@
       <c r="O101" s="14"/>
       <c r="P101" s="12"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="102">
       <c r="A102" s="9">
         <v>102</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>1</v>
       </c>
       <c r="K102" s="6">
-        <v>45010.410451388903</v>
+        <v>45010.4104513889</v>
       </c>
       <c r="L102" s="18" t="b">
         <v>0</v>
@@ -6044,7 +6044,7 @@
       </c>
       <c r="P102" s="12"/>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="103">
       <c r="A103" s="9">
         <v>103</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>1</v>
       </c>
       <c r="K103" s="6">
-        <v>45010.437974537002</v>
+        <v>45010.437974537</v>
       </c>
       <c r="L103" s="18" t="b">
         <v>0</v>
@@ -6085,7 +6085,7 @@
       </c>
       <c r="P103" s="12"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="104">
       <c r="A104" s="9">
         <v>104</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>1</v>
       </c>
       <c r="K104" s="6">
-        <v>45010.438148148103</v>
+        <v>45010.4381481481</v>
       </c>
       <c r="L104" s="18" t="b">
         <v>0</v>
@@ -6126,7 +6126,7 @@
       </c>
       <c r="P104" s="12"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="105">
       <c r="A105" s="9">
         <v>105</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>1</v>
       </c>
       <c r="K105" s="6">
-        <v>45010.439699074101</v>
+        <v>45010.4396990741</v>
       </c>
       <c r="L105" s="18" t="b">
         <v>0</v>
@@ -6167,7 +6167,7 @@
       </c>
       <c r="P105" s="12"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="106">
       <c r="A106" s="9">
         <v>106</v>
       </c>
@@ -6208,7 +6208,7 @@
       </c>
       <c r="P106" s="12"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="107">
       <c r="A107" s="9">
         <v>107</v>
       </c>
@@ -6238,7 +6238,7 @@
         <v>1</v>
       </c>
       <c r="K107" s="6">
-        <v>45010.554745370398</v>
+        <v>45010.5547453704</v>
       </c>
       <c r="L107" s="18" t="b">
         <v>0</v>
@@ -6249,7 +6249,7 @@
       </c>
       <c r="P107" s="12"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="108">
       <c r="A108" s="9">
         <v>108</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>1</v>
       </c>
       <c r="K108" s="6">
-        <v>45011.814490740697</v>
+        <v>45011.8144907407</v>
       </c>
       <c r="L108" s="18" t="b">
         <v>0</v>
@@ -6290,7 +6290,7 @@
       </c>
       <c r="P108" s="12"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="109">
       <c r="A109" s="9">
         <v>109</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>1</v>
       </c>
       <c r="K109" s="6">
-        <v>45011.841840277797</v>
+        <v>45011.8418402778</v>
       </c>
       <c r="L109" s="18" t="b">
         <v>0</v>
@@ -6331,7 +6331,7 @@
       </c>
       <c r="P109" s="12"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="110">
       <c r="A110" s="9">
         <v>110</v>
       </c>
@@ -6361,7 +6361,7 @@
         <v>1</v>
       </c>
       <c r="K110" s="6">
-        <v>45012.440081018503</v>
+        <v>45012.4400810185</v>
       </c>
       <c r="L110" s="18" t="b">
         <v>0</v>
@@ -6372,7 +6372,7 @@
       </c>
       <c r="P110" s="12"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="111">
       <c r="A111" s="9">
         <v>111</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>65</v>
       </c>
       <c r="K111" s="6">
-        <v>45012.895972222199</v>
+        <v>45012.8959722222</v>
       </c>
       <c r="L111" s="18" t="s">
         <v>51</v>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="P111" s="12"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="112">
       <c r="A112" s="9">
         <v>112</v>
       </c>
@@ -6454,7 +6454,7 @@
       </c>
       <c r="P112" s="12"/>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="113">
       <c r="A113" s="9">
         <v>113</v>
       </c>
@@ -6484,7 +6484,7 @@
         <v>65</v>
       </c>
       <c r="K113" s="6">
-        <v>45012.906909722202</v>
+        <v>45012.9069097222</v>
       </c>
       <c r="L113" s="18" t="s">
         <v>51</v>
@@ -6495,7 +6495,7 @@
       </c>
       <c r="P113" s="12"/>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="114">
       <c r="A114" s="9">
         <v>114</v>
       </c>
@@ -6525,7 +6525,7 @@
         <v>1</v>
       </c>
       <c r="K114" s="6">
-        <v>45012.945370370398</v>
+        <v>45012.9453703704</v>
       </c>
       <c r="L114" s="18" t="b">
         <v>0</v>
@@ -6536,7 +6536,7 @@
       </c>
       <c r="P114" s="12"/>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="115">
       <c r="A115" s="9">
         <v>115</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="6">
-        <v>45012.974618055603</v>
+        <v>45012.9746180556</v>
       </c>
       <c r="L115" s="18" t="b">
         <v>0</v>
@@ -6579,7 +6579,7 @@
       </c>
       <c r="P115" s="12"/>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="116">
       <c r="A116" s="9">
         <v>116</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>1</v>
       </c>
       <c r="K116" s="6">
-        <v>45012.975543981498</v>
+        <v>45012.9755439815</v>
       </c>
       <c r="L116" s="18" t="b">
         <v>0</v>
@@ -6620,7 +6620,7 @@
       </c>
       <c r="P116" s="12"/>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="117">
       <c r="A117" s="9">
         <v>117</v>
       </c>
@@ -6661,7 +6661,7 @@
       </c>
       <c r="P117" s="12"/>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="118">
       <c r="A118" s="9">
         <v>118</v>
       </c>
@@ -6691,7 +6691,7 @@
         <v>1</v>
       </c>
       <c r="K118" s="6">
-        <v>45012.997291666703</v>
+        <v>45012.9972916667</v>
       </c>
       <c r="L118" s="18" t="b">
         <v>0</v>
@@ -6702,7 +6702,7 @@
       </c>
       <c r="P118" s="12"/>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="119">
       <c r="A119" s="9">
         <v>119</v>
       </c>
@@ -6732,7 +6732,7 @@
         <v>1</v>
       </c>
       <c r="K119" s="6">
-        <v>45012.998761574097</v>
+        <v>45012.9987615741</v>
       </c>
       <c r="L119" s="18" t="b">
         <v>0</v>
@@ -6743,7 +6743,7 @@
       </c>
       <c r="P119" s="12"/>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="120">
       <c r="A120" s="9">
         <v>120</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>1</v>
       </c>
       <c r="K120" s="6">
-        <v>45012.999085648102</v>
+        <v>45012.9990856481</v>
       </c>
       <c r="L120" s="18" t="b">
         <v>0</v>
@@ -6784,7 +6784,7 @@
       </c>
       <c r="P120" s="12"/>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="121">
       <c r="A121" s="9">
         <v>121</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>1</v>
       </c>
       <c r="K121" s="6">
-        <v>45012.999178240701</v>
+        <v>45012.9991782407</v>
       </c>
       <c r="L121" s="18" t="b">
         <v>0</v>
@@ -6825,7 +6825,7 @@
       </c>
       <c r="P121" s="12"/>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="122">
       <c r="A122" s="9">
         <v>122</v>
       </c>
@@ -6855,7 +6855,7 @@
         <v>1</v>
       </c>
       <c r="K122" s="6">
-        <v>45013.008564814802</v>
+        <v>45013.0085648148</v>
       </c>
       <c r="L122" s="18" t="b">
         <v>0</v>
@@ -6866,7 +6866,7 @@
       </c>
       <c r="P122" s="12"/>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="123">
       <c r="A123" s="9">
         <v>123</v>
       </c>
@@ -6896,7 +6896,7 @@
         <v>1</v>
       </c>
       <c r="K123" s="6">
-        <v>45013.008703703701</v>
+        <v>45013.0087037037</v>
       </c>
       <c r="L123" s="18" t="b">
         <v>0</v>
@@ -6907,7 +6907,7 @@
       </c>
       <c r="P123" s="12"/>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="124">
       <c r="A124" s="9">
         <v>124</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>65</v>
       </c>
       <c r="K124" s="6">
-        <v>45013.009259259299</v>
+        <v>45013.0092592593</v>
       </c>
       <c r="L124" s="18" t="s">
         <v>51</v>
@@ -6948,7 +6948,7 @@
       </c>
       <c r="P124" s="12"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="125">
       <c r="A125" s="9">
         <v>125</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>1</v>
       </c>
       <c r="K125" s="6">
-        <v>45013.010439814803</v>
+        <v>45013.0104398148</v>
       </c>
       <c r="L125" s="18" t="b">
         <v>0</v>
@@ -6989,7 +6989,7 @@
       </c>
       <c r="P125" s="12"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="126">
       <c r="A126" s="9">
         <v>126</v>
       </c>
@@ -7019,7 +7019,7 @@
         <v>1</v>
       </c>
       <c r="K126" s="6">
-        <v>45013.010567129597</v>
+        <v>45013.0105671296</v>
       </c>
       <c r="L126" s="18" t="b">
         <v>0</v>
@@ -7030,7 +7030,7 @@
       </c>
       <c r="P126" s="12"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="127">
       <c r="A127" s="9">
         <v>127</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>1</v>
       </c>
       <c r="K127" s="6">
-        <v>45013.010740740698</v>
+        <v>45013.0107407407</v>
       </c>
       <c r="L127" s="18" t="b">
         <v>0</v>
@@ -7071,7 +7071,7 @@
       </c>
       <c r="P127" s="12"/>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="128">
       <c r="A128" s="9">
         <v>128</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>65</v>
       </c>
       <c r="K128" s="6">
-        <v>45013.014340277798</v>
+        <v>45013.0143402778</v>
       </c>
       <c r="L128" s="18" t="s">
         <v>51</v>
@@ -7112,7 +7112,7 @@
       </c>
       <c r="P128" s="12"/>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="129">
       <c r="A129" s="9">
         <v>129</v>
       </c>
@@ -7153,7 +7153,7 @@
       </c>
       <c r="P129" s="12"/>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="130">
       <c r="A130" s="9">
         <v>130</v>
       </c>
@@ -7183,7 +7183,7 @@
         <v>1</v>
       </c>
       <c r="K130" s="6">
-        <v>45013.014675925901</v>
+        <v>45013.0146759259</v>
       </c>
       <c r="L130" s="18" t="b">
         <v>0</v>
@@ -7194,7 +7194,7 @@
       </c>
       <c r="P130" s="12"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="131">
       <c r="A131" s="9">
         <v>131</v>
       </c>
@@ -7224,7 +7224,7 @@
         <v>1</v>
       </c>
       <c r="K131" s="6">
-        <v>45013.016145833302</v>
+        <v>45013.0161458333</v>
       </c>
       <c r="L131" s="18" t="b">
         <v>0</v>
@@ -7235,7 +7235,7 @@
       </c>
       <c r="P131" s="12"/>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="132">
       <c r="A132" s="9">
         <v>132</v>
       </c>
@@ -7265,7 +7265,7 @@
         <v>1</v>
       </c>
       <c r="K132" s="6">
-        <v>45013.016400462999</v>
+        <v>45013.016400463</v>
       </c>
       <c r="L132" s="18" t="b">
         <v>0</v>
@@ -7276,7 +7276,7 @@
       </c>
       <c r="P132" s="12"/>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="133">
       <c r="A133" s="9">
         <v>133</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>1</v>
       </c>
       <c r="K133" s="6">
-        <v>45013.725219907399</v>
+        <v>45013.7252199074</v>
       </c>
       <c r="L133" s="18" t="b">
         <v>0</v>
@@ -7317,7 +7317,7 @@
       </c>
       <c r="P133" s="12"/>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="134">
       <c r="A134" s="9">
         <v>134</v>
       </c>
@@ -7358,7 +7358,7 @@
       </c>
       <c r="P134" s="12"/>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="135">
       <c r="A135" s="9">
         <v>135</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>1</v>
       </c>
       <c r="K135" s="6">
-        <v>45019.587534722203</v>
+        <v>45019.5875347222</v>
       </c>
       <c r="L135" s="18" t="b">
         <v>0</v>
@@ -7399,7 +7399,7 @@
       </c>
       <c r="P135" s="12"/>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="136">
       <c r="A136" s="9">
         <v>136</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>1</v>
       </c>
       <c r="K136" s="6">
-        <v>45019.587777777801</v>
+        <v>45019.5877777778</v>
       </c>
       <c r="L136" s="18" t="b">
         <v>0</v>
@@ -7440,7 +7440,7 @@
       </c>
       <c r="P136" s="12"/>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="137">
       <c r="A137" s="9">
         <v>137</v>
       </c>
@@ -7481,7 +7481,7 @@
       </c>
       <c r="P137" s="12"/>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="138">
       <c r="A138" s="9">
         <v>138</v>
       </c>
@@ -7511,7 +7511,7 @@
         <v>1</v>
       </c>
       <c r="K138" s="6">
-        <v>45020.886458333298</v>
+        <v>45020.8864583333</v>
       </c>
       <c r="L138" s="18" t="b">
         <v>0</v>
@@ -7522,7 +7522,7 @@
       </c>
       <c r="P138" s="12"/>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="139">
       <c r="A139" s="9">
         <v>139</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>1</v>
       </c>
       <c r="K139" s="6">
-        <v>45020.886956018498</v>
+        <v>45020.8869560185</v>
       </c>
       <c r="L139" s="18" t="b">
         <v>0</v>
@@ -7563,7 +7563,7 @@
       </c>
       <c r="P139" s="12"/>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="140">
       <c r="A140" s="9">
         <v>140</v>
       </c>
@@ -7593,7 +7593,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="6">
-        <v>45021.320138888899</v>
+        <v>45021.3201388889</v>
       </c>
       <c r="L140" s="18" t="b">
         <v>0</v>
@@ -7604,7 +7604,7 @@
       </c>
       <c r="P140" s="12"/>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="141">
       <c r="A141" s="9">
         <v>141</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>1</v>
       </c>
       <c r="K141" s="6">
-        <v>45021.347268518497</v>
+        <v>45021.3472685185</v>
       </c>
       <c r="L141" s="18" t="b">
         <v>0</v>
@@ -7645,7 +7645,7 @@
       </c>
       <c r="P141" s="12"/>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="142">
       <c r="A142" s="9">
         <v>142</v>
       </c>
@@ -7675,7 +7675,7 @@
         <v>1</v>
       </c>
       <c r="K142" s="6">
-        <v>45021.348298611098</v>
+        <v>45021.3482986111</v>
       </c>
       <c r="L142" s="18" t="b">
         <v>0</v>
@@ -7686,7 +7686,7 @@
       </c>
       <c r="P142" s="12"/>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="143">
       <c r="A143" s="9">
         <v>143</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>1</v>
       </c>
       <c r="K143" s="6">
-        <v>45021.397905092599</v>
+        <v>45021.3979050926</v>
       </c>
       <c r="L143" s="18" t="b">
         <v>0</v>
@@ -7727,7 +7727,7 @@
       </c>
       <c r="P143" s="12"/>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="144">
       <c r="A144" s="9">
         <v>144</v>
       </c>
@@ -7768,7 +7768,7 @@
       </c>
       <c r="P144" s="12"/>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="145">
       <c r="A145" s="9">
         <v>145</v>
       </c>
@@ -7798,7 +7798,7 @@
         <v>1</v>
       </c>
       <c r="K145" s="6">
-        <v>45021.932916666701</v>
+        <v>45021.9329166667</v>
       </c>
       <c r="L145" s="18" t="b">
         <v>0</v>
@@ -7809,7 +7809,7 @@
       </c>
       <c r="P145" s="12"/>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="146">
       <c r="A146" s="9">
         <v>146</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>1</v>
       </c>
       <c r="K146" s="6">
-        <v>45021.984050925901</v>
+        <v>45021.9840509259</v>
       </c>
       <c r="L146" s="18" t="b">
         <v>0</v>
@@ -7850,7 +7850,7 @@
       </c>
       <c r="P146" s="12"/>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="147">
       <c r="A147" s="9">
         <v>147</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>1</v>
       </c>
       <c r="K147" s="6">
-        <v>45022.383969907401</v>
+        <v>45022.3839699074</v>
       </c>
       <c r="L147" s="18" t="b">
         <v>0</v>
@@ -7891,7 +7891,7 @@
       </c>
       <c r="P147" s="12"/>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="148">
       <c r="A148" s="9">
         <v>148</v>
       </c>
@@ -7921,7 +7921,7 @@
         <v>1</v>
       </c>
       <c r="K148" s="6">
-        <v>45022.384421296301</v>
+        <v>45022.3844212963</v>
       </c>
       <c r="L148" s="18" t="b">
         <v>0</v>
@@ -7932,7 +7932,7 @@
       </c>
       <c r="P148" s="12"/>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="149">
       <c r="A149" s="9">
         <v>149</v>
       </c>
@@ -7962,7 +7962,7 @@
         <v>1</v>
       </c>
       <c r="K149" s="6">
-        <v>45022.385682870401</v>
+        <v>45022.3856828704</v>
       </c>
       <c r="L149" s="18" t="b">
         <v>0</v>
@@ -7973,7 +7973,7 @@
       </c>
       <c r="P149" s="12"/>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="150">
       <c r="A150" s="9">
         <v>150</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>1</v>
       </c>
       <c r="K150" s="6">
-        <v>45022.390694444402</v>
+        <v>45022.3906944444</v>
       </c>
       <c r="L150" s="18" t="b">
         <v>0</v>
@@ -8014,7 +8014,7 @@
       </c>
       <c r="P150" s="12"/>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="151">
       <c r="A151" s="9">
         <v>151</v>
       </c>
@@ -8046,7 +8046,7 @@
         <v>65</v>
       </c>
       <c r="K151" s="6">
-        <v>45022.394189814797</v>
+        <v>45022.3941898148</v>
       </c>
       <c r="L151" s="18" t="s">
         <v>51</v>
@@ -8057,7 +8057,7 @@
       </c>
       <c r="P151" s="12"/>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="152">
       <c r="A152" s="9">
         <v>152</v>
       </c>
@@ -8087,7 +8087,7 @@
         <v>1</v>
       </c>
       <c r="K152" s="6">
-        <v>45022.409745370402</v>
+        <v>45022.4097453704</v>
       </c>
       <c r="L152" s="18" t="b">
         <v>0</v>
@@ -8098,7 +8098,7 @@
       </c>
       <c r="P152" s="12"/>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="153">
       <c r="A153" s="9">
         <v>153</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>1</v>
       </c>
       <c r="K153" s="6">
-        <v>45022.409976851799</v>
+        <v>45022.4099768518</v>
       </c>
       <c r="L153" s="18" t="b">
         <v>0</v>
@@ -8139,7 +8139,7 @@
       </c>
       <c r="P153" s="12"/>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="154">
       <c r="A154" s="9">
         <v>154</v>
       </c>
@@ -8180,7 +8180,7 @@
       </c>
       <c r="P154" s="12"/>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="155">
       <c r="A155" s="9">
         <v>155</v>
       </c>
@@ -8210,7 +8210,7 @@
         <v>65</v>
       </c>
       <c r="K155" s="6">
-        <v>45022.452488425901</v>
+        <v>45022.4524884259</v>
       </c>
       <c r="L155" s="18" t="s">
         <v>51</v>
@@ -8221,7 +8221,7 @@
       </c>
       <c r="P155" s="12"/>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="156">
       <c r="A156" s="9">
         <v>156</v>
       </c>
@@ -8251,7 +8251,7 @@
         <v>1</v>
       </c>
       <c r="K156" s="6">
-        <v>45022.460381944402</v>
+        <v>45022.4603819444</v>
       </c>
       <c r="L156" s="18" t="b">
         <v>0</v>
@@ -8262,7 +8262,7 @@
       </c>
       <c r="P156" s="12"/>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="157">
       <c r="A157" s="9">
         <v>157</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>1</v>
       </c>
       <c r="K157" s="6">
-        <v>45022.678726851896</v>
+        <v>45022.6787268519</v>
       </c>
       <c r="L157" s="18" t="b">
         <v>0</v>
@@ -8303,7 +8303,7 @@
       </c>
       <c r="P157" s="12"/>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="158">
       <c r="A158" s="9">
         <v>158</v>
       </c>
@@ -8344,7 +8344,7 @@
       </c>
       <c r="P158" s="12"/>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="159">
       <c r="A159" s="9">
         <v>159</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>1</v>
       </c>
       <c r="K159" s="6">
-        <v>45022.682002314803</v>
+        <v>45022.6820023148</v>
       </c>
       <c r="L159" s="18" t="b">
         <v>0</v>
@@ -8385,7 +8385,7 @@
       </c>
       <c r="P159" s="12"/>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="160">
       <c r="A160" s="9">
         <v>160</v>
       </c>
@@ -8415,7 +8415,7 @@
         <v>65</v>
       </c>
       <c r="K160" s="6">
-        <v>45022.686874999999</v>
+        <v>45022.686875</v>
       </c>
       <c r="L160" s="18" t="s">
         <v>51</v>
@@ -8426,7 +8426,7 @@
       </c>
       <c r="P160" s="12"/>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="161">
       <c r="A161" s="9">
         <v>161</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v>65</v>
       </c>
       <c r="K161" s="6">
-        <v>45022.690787036998</v>
+        <v>45022.690787037</v>
       </c>
       <c r="L161" s="18" t="s">
         <v>51</v>
@@ -8467,7 +8467,7 @@
       </c>
       <c r="P161" s="12"/>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="162">
       <c r="A162" s="9">
         <v>162</v>
       </c>
@@ -8508,7 +8508,7 @@
       </c>
       <c r="P162" s="12"/>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="163">
       <c r="A163" s="9">
         <v>163</v>
       </c>
@@ -8538,7 +8538,7 @@
         <v>1</v>
       </c>
       <c r="K163" s="6">
-        <v>45022.694826388899</v>
+        <v>45022.6948263889</v>
       </c>
       <c r="L163" s="18" t="b">
         <v>0</v>
@@ -8549,7 +8549,7 @@
       </c>
       <c r="P163" s="12"/>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="164">
       <c r="A164" s="9">
         <v>164</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>1</v>
       </c>
       <c r="K164" s="6">
-        <v>45022.694826388899</v>
+        <v>45022.6948263889</v>
       </c>
       <c r="L164" s="18" t="b">
         <v>0</v>
@@ -8590,7 +8590,7 @@
       </c>
       <c r="P164" s="12"/>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="165">
       <c r="A165" s="9">
         <v>165</v>
       </c>
@@ -8631,7 +8631,7 @@
       </c>
       <c r="P165" s="12"/>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="166">
       <c r="A166" s="9">
         <v>166</v>
       </c>
@@ -8672,7 +8672,7 @@
       </c>
       <c r="P166" s="12"/>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="167">
       <c r="A167" s="9">
         <v>167</v>
       </c>
@@ -8713,7 +8713,7 @@
       </c>
       <c r="P167" s="12"/>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="168">
       <c r="A168" s="9">
         <v>168</v>
       </c>
@@ -8743,7 +8743,7 @@
         <v>1</v>
       </c>
       <c r="K168" s="6">
-        <v>45025.467060185198</v>
+        <v>45025.4670601852</v>
       </c>
       <c r="L168" s="18" t="b">
         <v>0</v>
@@ -8754,7 +8754,7 @@
       </c>
       <c r="P168" s="12"/>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="169">
       <c r="A169" s="9">
         <v>169</v>
       </c>
@@ -8786,7 +8786,7 @@
         <v>1</v>
       </c>
       <c r="K169" s="6">
-        <v>45084.457824074103</v>
+        <v>45084.4578240741</v>
       </c>
       <c r="L169" s="18" t="b">
         <v>0</v>
@@ -8797,7 +8797,7 @@
       </c>
       <c r="P169" s="12"/>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="170">
       <c r="A170" s="9">
         <v>170</v>
       </c>
@@ -8829,7 +8829,7 @@
         <v>1</v>
       </c>
       <c r="K170" s="6">
-        <v>45120.613877314798</v>
+        <v>45120.6138773148</v>
       </c>
       <c r="L170" s="18" t="b">
         <v>0</v>
@@ -8840,7 +8840,7 @@
       </c>
       <c r="P170" s="12"/>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="171">
       <c r="A171" s="9">
         <v>171</v>
       </c>
@@ -8872,7 +8872,7 @@
         <v>1</v>
       </c>
       <c r="K171" s="6">
-        <v>45120.620127314804</v>
+        <v>45120.6201273148</v>
       </c>
       <c r="L171" s="18" t="b">
         <v>0</v>
@@ -8883,7 +8883,7 @@
       </c>
       <c r="P171" s="12"/>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="172">
       <c r="A172" s="9">
         <v>172</v>
       </c>
@@ -8915,7 +8915,7 @@
         <v>1</v>
       </c>
       <c r="K172" s="6">
-        <v>45259.640601851897</v>
+        <v>45259.6406018519</v>
       </c>
       <c r="L172" s="18" t="b">
         <v>0</v>
@@ -8929,7 +8929,7 @@
       </c>
       <c r="P172" s="12"/>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="173">
       <c r="A173" s="9">
         <v>173</v>
       </c>
@@ -8961,7 +8961,7 @@
         <v>1</v>
       </c>
       <c r="K173" s="6">
-        <v>45259.657118055598</v>
+        <v>45259.6571180556</v>
       </c>
       <c r="L173" s="18" t="b">
         <v>0</v>
@@ -8975,7 +8975,7 @@
       </c>
       <c r="P173" s="12"/>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="174">
       <c r="A174" s="9">
         <v>174</v>
       </c>
@@ -9007,7 +9007,7 @@
         <v>1</v>
       </c>
       <c r="K174" s="6">
-        <v>45259.661562499998</v>
+        <v>45259.6615625</v>
       </c>
       <c r="L174" s="18" t="b">
         <v>0</v>
@@ -9021,7 +9021,7 @@
       </c>
       <c r="P174" s="12"/>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="175">
       <c r="A175" s="9">
         <v>175</v>
       </c>
@@ -9053,7 +9053,7 @@
         <v>1</v>
       </c>
       <c r="K175" s="6">
-        <v>45259.665451388901</v>
+        <v>45259.6654513889</v>
       </c>
       <c r="L175" s="18" t="b">
         <v>0</v>
@@ -9067,7 +9067,7 @@
       </c>
       <c r="P175" s="12"/>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="176">
       <c r="A176" s="9">
         <v>176</v>
       </c>
@@ -9099,7 +9099,7 @@
         <v>1</v>
       </c>
       <c r="K176" s="6">
-        <v>45274.508854166699</v>
+        <v>45274.5088541667</v>
       </c>
       <c r="L176" s="18" t="b">
         <v>0</v>
@@ -9113,7 +9113,7 @@
       </c>
       <c r="P176" s="12"/>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="177">
       <c r="A177" s="9">
         <v>177</v>
       </c>
@@ -9145,7 +9145,7 @@
         <v>1</v>
       </c>
       <c r="K177" s="6">
-        <v>45274.521157407398</v>
+        <v>45274.5211574074</v>
       </c>
       <c r="L177" s="18" t="b">
         <v>0</v>
@@ -9159,7 +9159,7 @@
       </c>
       <c r="P177" s="12"/>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="178">
       <c r="A178" s="9">
         <v>178</v>
       </c>
@@ -9205,7 +9205,7 @@
       </c>
       <c r="P178" s="12"/>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="179">
       <c r="A179" s="9">
         <v>179</v>
       </c>
@@ -9237,7 +9237,7 @@
         <v>1</v>
       </c>
       <c r="K179" s="6">
-        <v>45259.671840277799</v>
+        <v>45259.6718402778</v>
       </c>
       <c r="L179" s="18" t="b">
         <v>0</v>
@@ -9251,7 +9251,7 @@
       </c>
       <c r="P179" s="12"/>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="180">
       <c r="A180" s="9">
         <v>180</v>
       </c>
@@ -9297,7 +9297,7 @@
       </c>
       <c r="P180" s="12"/>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="181">
       <c r="A181" s="9">
         <v>181</v>
       </c>
@@ -9329,7 +9329,7 @@
         <v>1</v>
       </c>
       <c r="K181" s="6">
-        <v>45259.688136574099</v>
+        <v>45259.6881365741</v>
       </c>
       <c r="L181" s="18" t="b">
         <v>0</v>
@@ -9343,7 +9343,7 @@
       </c>
       <c r="P181" s="12"/>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="182">
       <c r="A182" s="9">
         <v>182</v>
       </c>
@@ -9373,7 +9373,7 @@
         <v>1</v>
       </c>
       <c r="K182" s="6">
-        <v>45260.006180555603</v>
+        <v>45260.0061805556</v>
       </c>
       <c r="L182" s="18" t="b">
         <v>0</v>
@@ -9387,7 +9387,7 @@
       </c>
       <c r="P182" s="12"/>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="183">
       <c r="A183" s="9">
         <v>183</v>
       </c>
@@ -9417,7 +9417,7 @@
         <v>1</v>
       </c>
       <c r="K183" s="6">
-        <v>45260.010891203703</v>
+        <v>45260.0108912037</v>
       </c>
       <c r="L183" s="18" t="b">
         <v>0</v>
@@ -9431,7 +9431,7 @@
       </c>
       <c r="P183" s="12"/>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="184">
       <c r="A184" s="9">
         <v>184</v>
       </c>
@@ -9461,7 +9461,7 @@
         <v>1</v>
       </c>
       <c r="K184" s="6">
-        <v>45260.016539351898</v>
+        <v>45260.0165393519</v>
       </c>
       <c r="L184" s="18" t="b">
         <v>0</v>
@@ -9475,7 +9475,7 @@
       </c>
       <c r="P184" s="12"/>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="185">
       <c r="A185" s="9">
         <v>185</v>
       </c>
@@ -9501,13 +9501,13 @@
         <v>104</v>
       </c>
       <c r="I185" s="14">
-        <v>45274.500486111101</v>
+        <v>45274.5004861111</v>
       </c>
       <c r="J185" t="b">
         <v>1</v>
       </c>
       <c r="K185" s="6">
-        <v>45260.027037036998</v>
+        <v>45260.027037037</v>
       </c>
       <c r="L185" s="18" t="b">
         <v>0</v>
@@ -9521,7 +9521,7 @@
       </c>
       <c r="P185" s="12"/>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="186">
       <c r="A186" s="9">
         <v>186</v>
       </c>
@@ -9553,7 +9553,7 @@
         <v>1</v>
       </c>
       <c r="K186" s="6">
-        <v>45260.029594907399</v>
+        <v>45260.0295949074</v>
       </c>
       <c r="L186" s="18" t="b">
         <v>0</v>
@@ -9567,7 +9567,7 @@
       </c>
       <c r="P186" s="12"/>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="187">
       <c r="A187" s="9">
         <v>187</v>
       </c>
@@ -9599,7 +9599,7 @@
         <v>1</v>
       </c>
       <c r="K187" s="6">
-        <v>45261.071990740696</v>
+        <v>45261.0719907407</v>
       </c>
       <c r="L187" s="18" t="b">
         <v>0</v>
@@ -9613,7 +9613,7 @@
       </c>
       <c r="P187" s="12"/>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="188">
       <c r="A188" s="9">
         <v>188</v>
       </c>
@@ -9645,7 +9645,7 @@
         <v>1</v>
       </c>
       <c r="K188" s="6">
-        <v>45261.072662036997</v>
+        <v>45261.072662037</v>
       </c>
       <c r="L188" s="18" t="b">
         <v>0</v>
@@ -9659,7 +9659,7 @@
       </c>
       <c r="P188" s="12"/>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="189">
       <c r="A189" s="9">
         <v>189</v>
       </c>
@@ -9691,7 +9691,7 @@
         <v>1</v>
       </c>
       <c r="K189" s="6">
-        <v>45261.076516203699</v>
+        <v>45261.0765162037</v>
       </c>
       <c r="L189" s="18" t="b">
         <v>0</v>
@@ -9705,7 +9705,7 @@
       </c>
       <c r="P189" s="12"/>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="190">
       <c r="A190" s="9">
         <v>190</v>
       </c>
@@ -9747,7 +9747,7 @@
       </c>
       <c r="P190" s="12"/>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="191">
       <c r="A191" s="9">
         <v>191</v>
       </c>
@@ -9775,7 +9775,7 @@
         <v>1</v>
       </c>
       <c r="K191" s="6">
-        <v>45261.077303240701</v>
+        <v>45261.0773032407</v>
       </c>
       <c r="L191" s="18" t="b">
         <v>0</v>
@@ -9789,7 +9789,7 @@
       </c>
       <c r="P191" s="12"/>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="192">
       <c r="A192" s="9">
         <v>192</v>
       </c>
@@ -9817,7 +9817,7 @@
         <v>1</v>
       </c>
       <c r="K192" s="6">
-        <v>45261.083263888897</v>
+        <v>45261.0832638889</v>
       </c>
       <c r="L192" s="18" t="b">
         <v>0</v>
@@ -9831,7 +9831,7 @@
       </c>
       <c r="P192" s="12"/>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="193">
       <c r="A193" s="9">
         <v>193</v>
       </c>
@@ -9859,7 +9859,7 @@
         <v>1</v>
       </c>
       <c r="K193" s="6">
-        <v>45261.086990740703</v>
+        <v>45261.0869907407</v>
       </c>
       <c r="L193" s="18" t="b">
         <v>0</v>
@@ -9873,7 +9873,7 @@
       </c>
       <c r="P193" s="12"/>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="194">
       <c r="A194" s="9">
         <v>194</v>
       </c>
@@ -9903,7 +9903,7 @@
         <v>1</v>
       </c>
       <c r="K194" s="6">
-        <v>45261.101226851897</v>
+        <v>45261.1012268519</v>
       </c>
       <c r="L194" s="18" t="b">
         <v>0</v>
@@ -9917,7 +9917,7 @@
       </c>
       <c r="P194" s="12"/>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="195">
       <c r="A195" s="9">
         <v>195</v>
       </c>
@@ -9947,7 +9947,7 @@
         <v>1</v>
       </c>
       <c r="K195" s="6">
-        <v>45261.101736111101</v>
+        <v>45261.1017361111</v>
       </c>
       <c r="L195" s="18" t="b">
         <v>0</v>
@@ -9961,7 +9961,7 @@
       </c>
       <c r="P195" s="12"/>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="196">
       <c r="A196" s="9">
         <v>196</v>
       </c>
@@ -9993,7 +9993,7 @@
         <v>1</v>
       </c>
       <c r="K196" s="6">
-        <v>45261.385486111103</v>
+        <v>45261.3854861111</v>
       </c>
       <c r="L196" t="b">
         <v>0</v>
@@ -10007,7 +10007,7 @@
       </c>
       <c r="P196" s="12"/>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="197">
       <c r="A197" s="9">
         <v>197</v>
       </c>
@@ -10037,7 +10037,7 @@
         <v>1</v>
       </c>
       <c r="K197" s="6">
-        <v>45261.369560185201</v>
+        <v>45261.3695601852</v>
       </c>
       <c r="L197" s="18" t="b">
         <v>0</v>
@@ -10051,7 +10051,7 @@
       </c>
       <c r="P197" s="12"/>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="198">
       <c r="A198" s="9">
         <v>198</v>
       </c>
@@ -10083,7 +10083,7 @@
         <v>1</v>
       </c>
       <c r="K198" s="6">
-        <v>45261.370555555601</v>
+        <v>45261.3705555556</v>
       </c>
       <c r="L198" s="18" t="b">
         <v>0</v>
@@ -10097,7 +10097,7 @@
       </c>
       <c r="P198" s="12"/>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="199">
       <c r="A199" s="9">
         <v>199</v>
       </c>
@@ -10127,7 +10127,7 @@
         <v>1</v>
       </c>
       <c r="K199" s="6">
-        <v>45261.397777777798</v>
+        <v>45261.3977777778</v>
       </c>
       <c r="L199" s="18" t="b">
         <v>0</v>
@@ -10141,7 +10141,7 @@
       </c>
       <c r="P199" s="12"/>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="200">
       <c r="A200" s="9">
         <v>200</v>
       </c>
@@ -10171,7 +10171,7 @@
         <v>1</v>
       </c>
       <c r="K200" s="6">
-        <v>45262.574467592603</v>
+        <v>45262.5744675926</v>
       </c>
       <c r="L200" s="18" t="b">
         <v>0</v>
@@ -10185,7 +10185,7 @@
       </c>
       <c r="P200" s="12"/>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="201">
       <c r="A201" s="9">
         <v>201</v>
       </c>
@@ -10215,7 +10215,7 @@
         <v>1</v>
       </c>
       <c r="K201" s="6">
-        <v>45274.489675925899</v>
+        <v>45274.4896759259</v>
       </c>
       <c r="L201" s="18" t="b">
         <v>0</v>
@@ -10229,7 +10229,7 @@
       </c>
       <c r="P201" s="12"/>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="202">
       <c r="A202" s="9">
         <v>202</v>
       </c>
@@ -10259,7 +10259,7 @@
         <v>1</v>
       </c>
       <c r="K202" s="6">
-        <v>45274.522037037001</v>
+        <v>45274.522037037</v>
       </c>
       <c r="L202" s="18" t="b">
         <v>0</v>
@@ -10273,7 +10273,7 @@
       </c>
       <c r="P202" s="12"/>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="203">
       <c r="A203" s="9">
         <v>203</v>
       </c>
@@ -10317,7 +10317,7 @@
       </c>
       <c r="P203" s="12"/>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="204">
       <c r="A204" s="9">
         <v>204</v>
       </c>
@@ -10347,7 +10347,7 @@
         <v>1</v>
       </c>
       <c r="K204" s="6">
-        <v>45274.495266203703</v>
+        <v>45274.4952662037</v>
       </c>
       <c r="L204" s="18" t="b">
         <v>0</v>
@@ -10361,7 +10361,7 @@
       </c>
       <c r="P204" s="12"/>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="205">
       <c r="A205" s="9">
         <v>205</v>
       </c>
@@ -10393,7 +10393,7 @@
         <v>1</v>
       </c>
       <c r="K205" s="6">
-        <v>45274.531458333302</v>
+        <v>45274.5314583333</v>
       </c>
       <c r="L205" s="18" t="b">
         <v>0</v>
@@ -10407,7 +10407,7 @@
       </c>
       <c r="P205" s="12"/>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="206">
       <c r="A206" s="9">
         <v>206</v>
       </c>
@@ -10437,7 +10437,7 @@
         <v>1</v>
       </c>
       <c r="K206" s="6">
-        <v>45274.533599536997</v>
+        <v>45274.533599537</v>
       </c>
       <c r="L206" s="18" t="b">
         <v>0</v>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="P206" s="12"/>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="207">
       <c r="A207" s="9">
         <v>207</v>
       </c>
@@ -10481,7 +10481,7 @@
         <v>1</v>
       </c>
       <c r="K207" s="6">
-        <v>45274.536157407398</v>
+        <v>45274.5361574074</v>
       </c>
       <c r="L207" s="18" t="b">
         <v>0</v>
@@ -10495,7 +10495,7 @@
       </c>
       <c r="P207" s="12"/>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="208">
       <c r="A208" s="9">
         <v>208</v>
       </c>
@@ -10525,7 +10525,7 @@
         <v>1</v>
       </c>
       <c r="K208" s="6">
-        <v>45275.299328703702</v>
+        <v>45275.2993287037</v>
       </c>
       <c r="L208" s="18" t="b">
         <v>0</v>
@@ -10539,7 +10539,7 @@
       </c>
       <c r="P208" s="12"/>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="209">
       <c r="A209" s="9">
         <v>209</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>1</v>
       </c>
       <c r="K209" s="6">
-        <v>45275.299699074101</v>
+        <v>45275.2996990741</v>
       </c>
       <c r="L209" s="18" t="b">
         <v>0</v>
@@ -10583,7 +10583,7 @@
       </c>
       <c r="P209" s="12"/>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="210">
       <c r="A210" s="9">
         <v>210</v>
       </c>
@@ -10613,7 +10613,7 @@
         <v>1</v>
       </c>
       <c r="K210" s="6">
-        <v>45275.306145833303</v>
+        <v>45275.3061458333</v>
       </c>
       <c r="L210" s="18" t="b">
         <v>0</v>
@@ -10627,7 +10627,7 @@
       </c>
       <c r="P210" s="12"/>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="211">
       <c r="A211" s="9">
         <v>211</v>
       </c>
@@ -10657,7 +10657,7 @@
         <v>1</v>
       </c>
       <c r="K211" s="6">
-        <v>45275.299942129597</v>
+        <v>45275.2999421296</v>
       </c>
       <c r="L211" s="18" t="b">
         <v>0</v>
@@ -10671,7 +10671,7 @@
       </c>
       <c r="P211" s="12"/>
     </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="212">
       <c r="A212" s="9">
         <v>212</v>
       </c>
@@ -10701,7 +10701,7 @@
         <v>1</v>
       </c>
       <c r="K212" s="6">
-        <v>45275.300034722197</v>
+        <v>45275.3000347222</v>
       </c>
       <c r="L212" s="18" t="b">
         <v>0</v>
@@ -10715,7 +10715,7 @@
       </c>
       <c r="P212" s="12"/>
     </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="213">
       <c r="A213" s="9">
         <v>213</v>
       </c>
@@ -10745,7 +10745,7 @@
         <v>1</v>
       </c>
       <c r="K213" s="6">
-        <v>45275.300127314797</v>
+        <v>45275.3001273148</v>
       </c>
       <c r="L213" s="18" t="b">
         <v>0</v>
@@ -10759,7 +10759,7 @@
       </c>
       <c r="P213" s="12"/>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="214">
       <c r="A214" s="9">
         <v>214</v>
       </c>
@@ -10789,7 +10789,7 @@
         <v>1</v>
       </c>
       <c r="K214" s="6">
-        <v>45275.305937500001</v>
+        <v>45275.3059375</v>
       </c>
       <c r="L214" s="18" t="b">
         <v>0</v>
@@ -10803,7 +10803,7 @@
       </c>
       <c r="P214" s="12"/>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="215">
       <c r="A215" s="9">
         <v>215</v>
       </c>
@@ -10833,7 +10833,7 @@
         <v>1</v>
       </c>
       <c r="K215" s="6">
-        <v>45275.305821759299</v>
+        <v>45275.3058217593</v>
       </c>
       <c r="L215" s="18" t="b">
         <v>0</v>
@@ -10847,7 +10847,7 @@
       </c>
       <c r="P215" s="12"/>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="216">
       <c r="A216" s="9">
         <v>216</v>
       </c>
@@ -10891,7 +10891,7 @@
       </c>
       <c r="P216" s="12"/>
     </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="217">
       <c r="A217" s="9">
         <v>217</v>
       </c>
@@ -10935,7 +10935,7 @@
       </c>
       <c r="P217" s="12"/>
     </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="218">
       <c r="A218" s="9">
         <v>218</v>
       </c>
@@ -10965,7 +10965,7 @@
         <v>1</v>
       </c>
       <c r="K218" s="6">
-        <v>45275.335289351897</v>
+        <v>45275.3352893519</v>
       </c>
       <c r="L218" s="18" t="b">
         <v>0</v>
@@ -10979,7 +10979,7 @@
       </c>
       <c r="P218" s="12"/>
     </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="219">
       <c r="A219" s="9">
         <v>219</v>
       </c>
@@ -11009,7 +11009,7 @@
         <v>1</v>
       </c>
       <c r="K219" s="6">
-        <v>45275.336921296301</v>
+        <v>45275.3369212963</v>
       </c>
       <c r="L219" s="18" t="b">
         <v>0</v>
@@ -11023,7 +11023,7 @@
       </c>
       <c r="P219" s="12"/>
     </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="220">
       <c r="A220" s="9">
         <v>220</v>
       </c>
@@ -11053,7 +11053,7 @@
         <v>1</v>
       </c>
       <c r="K220" s="6">
-        <v>45275.460428240702</v>
+        <v>45275.4604282407</v>
       </c>
       <c r="L220" s="18" t="b">
         <v>0</v>
@@ -11067,7 +11067,7 @@
       </c>
       <c r="P220" s="12"/>
     </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="221">
       <c r="A221" s="9">
         <v>221</v>
       </c>
@@ -11097,7 +11097,7 @@
         <v>1</v>
       </c>
       <c r="K221" s="6">
-        <v>45275.461006944402</v>
+        <v>45275.4610069444</v>
       </c>
       <c r="L221" s="18" t="b">
         <v>0</v>
@@ -11111,7 +11111,7 @@
       </c>
       <c r="P221" s="12"/>
     </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="222">
       <c r="A222" s="9">
         <v>222</v>
       </c>
@@ -11143,7 +11143,7 @@
         <v>1</v>
       </c>
       <c r="K222" s="6">
-        <v>45275.466168981497</v>
+        <v>45275.4661689815</v>
       </c>
       <c r="L222" s="18" t="b">
         <v>0</v>
@@ -11157,7 +11157,7 @@
       </c>
       <c r="P222" s="12"/>
     </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="223">
       <c r="A223" s="9">
         <v>223</v>
       </c>
@@ -11187,7 +11187,7 @@
         <v>1</v>
       </c>
       <c r="K223" s="6">
-        <v>45275.536249999997</v>
+        <v>45275.53625</v>
       </c>
       <c r="L223" s="18" t="b">
         <v>0</v>
@@ -11201,7 +11201,7 @@
       </c>
       <c r="P223" s="12"/>
     </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="224">
       <c r="A224" s="9">
         <v>224</v>
       </c>
@@ -11231,7 +11231,7 @@
         <v>0</v>
       </c>
       <c r="K224" s="6">
-        <v>45275.537731481498</v>
+        <v>45275.5377314815</v>
       </c>
       <c r="L224" s="18" t="b">
         <v>0</v>
@@ -11245,7 +11245,7 @@
       </c>
       <c r="P224" s="12"/>
     </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="225">
       <c r="A225" s="9">
         <v>225</v>
       </c>
@@ -11275,7 +11275,7 @@
         <v>1</v>
       </c>
       <c r="K225" s="6">
-        <v>45276.415405092601</v>
+        <v>45276.4154050926</v>
       </c>
       <c r="L225" s="18" t="b">
         <v>0</v>
@@ -11289,7 +11289,7 @@
       </c>
       <c r="P225" s="12"/>
     </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="226">
       <c r="A226" s="9">
         <v>226</v>
       </c>
@@ -11319,7 +11319,7 @@
         <v>1</v>
       </c>
       <c r="K226" s="6">
-        <v>45275.560624999998</v>
+        <v>45275.560625</v>
       </c>
       <c r="L226" s="18" t="b">
         <v>0</v>
@@ -11333,7 +11333,7 @@
       </c>
       <c r="P226" s="12"/>
     </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="227">
       <c r="A227" s="9">
         <v>227</v>
       </c>
@@ -11361,7 +11361,7 @@
         <v>1</v>
       </c>
       <c r="K227" s="6">
-        <v>45276.412002314799</v>
+        <v>45276.4120023148</v>
       </c>
       <c r="L227" s="18" t="b">
         <v>0</v>
@@ -11375,7 +11375,7 @@
       </c>
       <c r="P227" s="12"/>
     </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="228">
       <c r="A228" s="1">
         <v>228</v>
       </c>
@@ -11404,7 +11404,7 @@
         <v>1</v>
       </c>
       <c r="K228" s="6">
-        <v>45276.415625000001</v>
+        <v>45276.415625</v>
       </c>
       <c r="L228" s="1" t="b">
         <v>0</v>
@@ -11416,7 +11416,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="229">
       <c r="A229" s="1">
         <v>229</v>
       </c>
@@ -11445,7 +11445,7 @@
         <v>1</v>
       </c>
       <c r="K229" s="6">
-        <v>45276.415300925903</v>
+        <v>45276.4153009259</v>
       </c>
       <c r="L229" s="1" t="b">
         <v>0</v>
@@ -11457,7 +11457,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="230">
       <c r="A230" s="1">
         <v>230</v>
       </c>
@@ -11498,7 +11498,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="231">
       <c r="A231" s="1">
         <v>231</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="232">
       <c r="A232" s="1">
         <v>232</v>
       </c>
@@ -11568,7 +11568,7 @@
         <v>1</v>
       </c>
       <c r="K232" s="6">
-        <v>45276.418796296297</v>
+        <v>45276.4187962963</v>
       </c>
       <c r="L232" s="1" t="b">
         <v>0</v>
@@ -11580,7 +11580,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="233">
       <c r="A233" s="1">
         <v>233</v>
       </c>
@@ -11609,7 +11609,7 @@
         <v>0</v>
       </c>
       <c r="K233" s="6">
-        <v>45276.622499999998</v>
+        <v>45276.6225</v>
       </c>
       <c r="L233" s="1" t="b">
         <v>0</v>
@@ -11621,7 +11621,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="234">
       <c r="A234" s="22">
         <v>234</v>
       </c>
@@ -11653,7 +11653,7 @@
         <v>0</v>
       </c>
       <c r="K234" s="5">
-        <v>45276.622199074103</v>
+        <v>45276.6221990741</v>
       </c>
       <c r="L234" s="22" t="b">
         <v>0</v>
@@ -11665,7 +11665,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="235">
       <c r="A235" s="22">
         <v>235</v>
       </c>
@@ -11694,7 +11694,7 @@
         <v>1</v>
       </c>
       <c r="K235" s="5">
-        <v>45276.511099536998</v>
+        <v>45276.511099537</v>
       </c>
       <c r="L235" s="22" t="b">
         <v>0</v>
@@ -11706,7 +11706,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="236">
       <c r="A236" s="22">
         <v>236</v>
       </c>
@@ -11738,7 +11738,7 @@
         <v>1</v>
       </c>
       <c r="K236" s="5">
-        <v>45276.511365740698</v>
+        <v>45276.5113657407</v>
       </c>
       <c r="L236" s="22" t="b">
         <v>0</v>
@@ -11750,7 +11750,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="237">
       <c r="A237" s="22">
         <v>237</v>
       </c>
@@ -11779,7 +11779,7 @@
         <v>1</v>
       </c>
       <c r="K237" s="5">
-        <v>45276.511828703697</v>
+        <v>45276.5118287037</v>
       </c>
       <c r="L237" s="22" t="b">
         <v>0</v>
@@ -11791,7 +11791,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="238">
       <c r="A238" s="22">
         <v>238</v>
       </c>
@@ -11820,7 +11820,7 @@
         <v>1</v>
       </c>
       <c r="K238" s="5">
-        <v>45276.594525462999</v>
+        <v>45276.594525463</v>
       </c>
       <c r="L238" s="22" t="b">
         <v>0</v>
@@ -11832,7 +11832,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="239">
       <c r="A239" s="22">
         <v>239</v>
       </c>
@@ -11848,20 +11848,24 @@
       <c r="E239" s="22">
         <v>1232</v>
       </c>
-      <c r="F239" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="G239" s="22" t="s">
-        <v>335</v>
+      <c r="F239" s="22" t="inlineStr">
+        <is>
+          <t>Murphy Oil Corporation</t>
+        </is>
+      </c>
+      <c r="G239" s="22" t="inlineStr">
+        <is>
+          <t>Test du 16 décembre</t>
+        </is>
       </c>
       <c r="H239" s="22">
         <v>3.75</v>
       </c>
       <c r="J239" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K239" s="5">
-        <v>45276.594398148103</v>
+        <v>45282.4237268519</v>
       </c>
       <c r="L239" s="22" t="b">
         <v>0</v>
@@ -11869,11 +11873,13 @@
       <c r="N239" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="O239" s="22" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O239" s="22" t="inlineStr">
+        <is>
+          <t>v1.1.9.7</t>
+        </is>
+      </c>
+    </row>
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="240">
       <c r="A240" s="22">
         <v>240</v>
       </c>
@@ -11899,7 +11905,7 @@
         <v>1</v>
       </c>
       <c r="K240" s="5">
-        <v>45276.512847222199</v>
+        <v>45276.5128472222</v>
       </c>
       <c r="L240" s="22" t="b">
         <v>0</v>
@@ -11911,7 +11917,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
+    <row spans="1:15" x14ac:dyDescent="0.25" outlineLevel="0" r="241">
       <c r="A241" s="22">
         <v>241</v>
       </c>
@@ -11940,7 +11946,7 @@
         <v>1</v>
       </c>
       <c r="K241" s="5">
-        <v>45276.547766203701</v>
+        <v>45276.5477662037</v>
       </c>
       <c r="L241" s="22" t="b">
         <v>0</v>
@@ -11952,7 +11958,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
+    <row spans="1:15" x14ac:dyDescent="0.25" outlineLevel="0" r="242">
       <c r="A242" s="22">
         <v>242</v>
       </c>
@@ -11981,7 +11987,7 @@
         <v>0</v>
       </c>
       <c r="K242" s="5">
-        <v>45276.622650463003</v>
+        <v>45276.622650463</v>
       </c>
       <c r="L242" s="22" t="b">
         <v>0</v>
@@ -11993,7 +11999,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
+    <row spans="1:15" x14ac:dyDescent="0.25" outlineLevel="0" r="243">
       <c r="A243" s="22">
         <v>243</v>
       </c>
@@ -12022,7 +12028,7 @@
         <v>1</v>
       </c>
       <c r="K243" s="5">
-        <v>45276.622766203698</v>
+        <v>45276.6227662037</v>
       </c>
       <c r="L243" s="22" t="b">
         <v>0</v>
@@ -12034,7 +12040,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
+    <row spans="1:15" x14ac:dyDescent="0.25" outlineLevel="0" r="244">
       <c r="A244" s="22">
         <v>244</v>
       </c>
@@ -12063,7 +12069,7 @@
         <v>0</v>
       </c>
       <c r="K244" s="5">
-        <v>45276.704872685201</v>
+        <v>45276.7048726852</v>
       </c>
       <c r="L244" s="22" t="b">
         <v>0</v>
@@ -12075,7 +12081,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
+    <row spans="1:15" x14ac:dyDescent="0.25" outlineLevel="0" r="245">
       <c r="A245" s="22">
         <v>245</v>
       </c>
@@ -12104,7 +12110,7 @@
         <v>1</v>
       </c>
       <c r="K245" s="5">
-        <v>45276.605891203697</v>
+        <v>45276.6058912037</v>
       </c>
       <c r="L245" s="22" t="b">
         <v>0</v>
@@ -12116,7 +12122,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
+    <row spans="1:15" x14ac:dyDescent="0.25" outlineLevel="0" r="246">
       <c r="A246" s="22">
         <v>246</v>
       </c>
@@ -12145,7 +12151,7 @@
         <v>1</v>
       </c>
       <c r="K246" s="5">
-        <v>45276.622060185196</v>
+        <v>45276.6220601852</v>
       </c>
       <c r="L246" s="22" t="b">
         <v>0</v>
@@ -12155,6 +12161,55 @@
       </c>
       <c r="O246" s="22" t="s">
         <v>339</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="247">
+      <c r="A247" s="30">
+        <v>247</v>
+      </c>
+      <c r="B247" s="30">
+        <v>2</v>
+      </c>
+      <c r="C247" s="30" t="inlineStr">
+        <is>
+          <t>VG</t>
+        </is>
+      </c>
+      <c r="D247" s="32">
+        <v>45276</v>
+      </c>
+      <c r="E247" s="30">
+        <v>2</v>
+      </c>
+      <c r="F247" s="30" t="inlineStr">
+        <is>
+          <t>3Com Corporation</t>
+        </is>
+      </c>
+      <c r="G247" s="30" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="H247" s="30">
+        <v>2.5</v>
+      </c>
+      <c r="J247" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K247" s="32">
+        <v>45282.4241898148</v>
+      </c>
+      <c r="L247" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N247" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O247" s="30" t="inlineStr">
+        <is>
+          <t>v1.1.9.7</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024-01-05 @ 13:31 - Still working in G/L module
J/E is now working
The format in 'GCF_BD_Sortie is still to be corrected
More tests are required
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F79563-8D7D-49C6-9953-014FF09BA457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B12E31-ACFE-4BBE-9C58-3E59DC6F995A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <definedName name="Inv_ID">OFFSET([1]Factures!$A$3,1,,COUNTA([1]Factures!$A$3:$A$99958)-1,1)</definedName>
     <definedName name="MonthStart">#REF!</definedName>
     <definedName name="nrClients">OFFSET([1]clientsImportés!$B$2,,,COUNTA([1]clientsImportés!$B$2:$B$9999))</definedName>
-    <definedName name="nrJE_All">OFFSET(GLTrans!#REF!,,,COUNTA(GLTrans!$C$2:$C$999548))</definedName>
+    <definedName name="nrJE_All">OFFSET(GLTrans!#REF!,,,COUNTA(GLTrans!$C$2:$C$417))</definedName>
     <definedName name="nrPlanComptable">OFFSET([2]wshAdmin!$T$10,,,COUNTA([2]wshAdmin!$T:$T)-1,4)</definedName>
     <definedName name="nrServices">OFFSET([1]Services!$B$4,,,COUNTA([1]Services!$B$4:$B$999))</definedName>
     <definedName name="PlanComptable">OFFSET([2]wshAdmin!$T1048576:$T9989,,,COUNTA([2]wshAdmin!$T:$T)-1,4)</definedName>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="538">
   <si>
     <t>TEC_ID</t>
   </si>
@@ -1676,6 +1676,21 @@
   </si>
   <si>
     <t>No_Compte</t>
+  </si>
+  <si>
+    <t>1er 25,00 $</t>
+  </si>
+  <si>
+    <t>2ème 25,00 $</t>
+  </si>
+  <si>
+    <t>3ème 25,00 $</t>
+  </si>
+  <si>
+    <t>Dernier 25,00 $</t>
+  </si>
+  <si>
+    <t>Test d'intégration</t>
   </si>
 </sst>
 </file>
@@ -2536,7 +2551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="234">
+  <cellXfs count="233">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3068,6 +3083,13 @@
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3080,33 +3102,19 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire 2" xfId="1" xr:uid="{7066D7D9-A0C5-4744-AD1B-CDB1C4228FB1}"/>
@@ -25498,14 +25506,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ADD6A68-0236-43C2-BFF9-CD5F2E02CF02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{5ADD6A68-0236-43C2-BFF9-CD5F2E02CF02}">
   <sheetPr codeName="wshGLFACTrans"/>
-  <dimension ref="A1:M437"/>
+  <dimension ref="C1:L425"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="825" topLeftCell="A389" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <pane ySplit="825" topLeftCell="A401" activePane="bottomLeft"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="H411" sqref="H411"/>
+      <selection pane="bottomLeft" activeCell="H420" sqref="H420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25521,7 +25529,7 @@
     <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
       <c r="C1" s="37" t="s">
         <v>531</v>
       </c>
@@ -25553,7 +25561,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
       <c r="C2" s="42">
         <v>1</v>
       </c>
@@ -25582,7 +25590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="3:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row spans="3:12" ht="15.75" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
       <c r="C3" s="42">
         <v>1</v>
       </c>
@@ -25611,7 +25619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="4">
       <c r="C4" s="42">
         <v>1</v>
       </c>
@@ -25634,7 +25642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="5">
       <c r="C5" s="42">
         <v>1</v>
       </c>
@@ -25653,7 +25661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="6">
       <c r="C6" s="42">
         <v>2</v>
       </c>
@@ -25682,7 +25690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="7">
       <c r="C7" s="42">
         <v>2</v>
       </c>
@@ -25711,7 +25719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="8">
       <c r="C8" s="42">
         <v>2</v>
       </c>
@@ -25732,7 +25740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="9">
       <c r="C9" s="42">
         <v>2</v>
       </c>
@@ -25751,7 +25759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="10">
       <c r="C10" s="42">
         <v>3</v>
       </c>
@@ -25780,7 +25788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="11">
       <c r="C11" s="42">
         <v>3</v>
       </c>
@@ -25809,7 +25817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="12">
       <c r="C12" s="42">
         <v>3</v>
       </c>
@@ -25834,7 +25842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="13">
       <c r="C13" s="42">
         <v>3</v>
       </c>
@@ -25852,7 +25860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="14">
       <c r="C14" s="42">
         <v>4</v>
       </c>
@@ -25881,7 +25889,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="15">
       <c r="C15" s="42">
         <v>4</v>
       </c>
@@ -25910,7 +25918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="16">
       <c r="C16" s="42">
         <v>4</v>
       </c>
@@ -25930,7 +25938,7 @@
         <v>415</v>
       </c>
       <c r="I16" s="56">
-        <v>570.91999999999996</v>
+        <v>570.92</v>
       </c>
       <c r="J16" s="56"/>
       <c r="K16" s="61"/>
@@ -25939,7 +25947,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="17">
       <c r="C17" s="42">
         <v>4</v>
       </c>
@@ -25968,7 +25976,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="18">
       <c r="C18" s="42">
         <v>4</v>
       </c>
@@ -25997,7 +26005,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="19">
       <c r="C19" s="42">
         <v>4</v>
       </c>
@@ -26022,7 +26030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="20">
       <c r="C20" s="42">
         <v>4</v>
       </c>
@@ -26044,7 +26052,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="21">
       <c r="C21" s="42">
         <v>5</v>
       </c>
@@ -26073,7 +26081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="22">
       <c r="C22" s="42">
         <v>5</v>
       </c>
@@ -26102,7 +26110,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="23">
       <c r="C23" s="42">
         <v>5</v>
       </c>
@@ -26131,7 +26139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="24">
       <c r="C24" s="42">
         <v>5</v>
       </c>
@@ -26160,7 +26168,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="25">
       <c r="C25" s="42">
         <v>5</v>
       </c>
@@ -26189,7 +26197,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="26">
       <c r="C26" s="42">
         <v>5</v>
       </c>
@@ -26218,7 +26226,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="27">
       <c r="C27" s="42">
         <v>5</v>
       </c>
@@ -26247,7 +26255,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="28">
       <c r="C28" s="42">
         <v>5</v>
       </c>
@@ -26276,7 +26284,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="29">
       <c r="C29" s="42">
         <v>5</v>
       </c>
@@ -26301,7 +26309,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="30">
       <c r="C30" s="42">
         <v>5</v>
       </c>
@@ -26324,7 +26332,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="31">
       <c r="C31" s="42">
         <v>6</v>
       </c>
@@ -26353,7 +26361,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="32">
       <c r="C32" s="42">
         <v>6</v>
       </c>
@@ -26382,7 +26390,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="33">
       <c r="C33" s="42">
         <v>6</v>
       </c>
@@ -26411,7 +26419,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="34">
       <c r="C34" s="42">
         <v>6</v>
       </c>
@@ -26440,7 +26448,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="35">
       <c r="C35" s="42">
         <v>6</v>
       </c>
@@ -26469,7 +26477,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="36">
       <c r="C36" s="42">
         <v>6</v>
       </c>
@@ -26498,7 +26506,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="37">
       <c r="C37" s="42">
         <v>6</v>
       </c>
@@ -26527,7 +26535,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="38">
       <c r="C38" s="42">
         <v>6</v>
       </c>
@@ -26556,7 +26564,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="39">
       <c r="C39" s="42">
         <v>6</v>
       </c>
@@ -26581,7 +26589,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="40">
       <c r="C40" s="42">
         <v>6</v>
       </c>
@@ -26600,7 +26608,7 @@
       <c r="J40" s="34"/>
       <c r="L40" s="42"/>
     </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="41">
       <c r="C41" s="42">
         <v>7</v>
       </c>
@@ -26629,7 +26637,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="42">
       <c r="C42" s="42">
         <v>7</v>
       </c>
@@ -26658,7 +26666,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="43">
       <c r="C43" s="42">
         <v>7</v>
       </c>
@@ -26687,7 +26695,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="44">
       <c r="C44" s="42">
         <v>7</v>
       </c>
@@ -26716,7 +26724,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="45">
       <c r="C45" s="42">
         <v>7</v>
       </c>
@@ -26745,7 +26753,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="46">
       <c r="C46" s="42">
         <v>7</v>
       </c>
@@ -26774,7 +26782,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="47">
       <c r="C47" s="42">
         <v>7</v>
       </c>
@@ -26795,7 +26803,7 @@
       </c>
       <c r="I47" s="56"/>
       <c r="J47" s="56">
-        <v>67.680000000000007</v>
+        <v>67.68</v>
       </c>
       <c r="K47" s="61"/>
       <c r="L47" s="42">
@@ -26803,7 +26811,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="48">
       <c r="C48" s="42">
         <v>7</v>
       </c>
@@ -26832,7 +26840,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="49">
       <c r="C49" s="42">
         <v>7</v>
       </c>
@@ -26857,7 +26865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="50">
       <c r="C50" s="42">
         <v>7</v>
       </c>
@@ -26879,7 +26887,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="51">
       <c r="C51" s="42">
         <v>8</v>
       </c>
@@ -26899,7 +26907,7 @@
         <v>402</v>
       </c>
       <c r="I51" s="48">
-        <v>1248.6300000000001</v>
+        <v>1248.63</v>
       </c>
       <c r="J51" s="48"/>
       <c r="K51" s="50"/>
@@ -26908,7 +26916,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="52">
       <c r="C52" s="42">
         <v>8</v>
       </c>
@@ -26937,7 +26945,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="53">
       <c r="C53" s="42">
         <v>8</v>
       </c>
@@ -26966,7 +26974,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="54">
       <c r="C54" s="42">
         <v>8</v>
       </c>
@@ -26995,7 +27003,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="55">
       <c r="C55" s="42">
         <v>8</v>
       </c>
@@ -27024,7 +27032,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="56">
       <c r="C56" s="42">
         <v>8</v>
       </c>
@@ -27053,7 +27061,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="57">
       <c r="C57" s="42">
         <v>8</v>
       </c>
@@ -27082,7 +27090,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="58">
       <c r="C58" s="42">
         <v>8</v>
       </c>
@@ -27107,7 +27115,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="59">
       <c r="C59" s="42">
         <v>8</v>
       </c>
@@ -27129,7 +27137,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="60">
       <c r="C60" s="42">
         <v>9</v>
       </c>
@@ -27149,7 +27157,7 @@
         <v>399</v>
       </c>
       <c r="I60" s="48">
-        <v>1248.6300000000001</v>
+        <v>1248.63</v>
       </c>
       <c r="J60" s="48"/>
       <c r="K60" s="50"/>
@@ -27158,7 +27166,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="61">
       <c r="C61" s="42">
         <v>9</v>
       </c>
@@ -27179,7 +27187,7 @@
       </c>
       <c r="I61" s="56"/>
       <c r="J61" s="56">
-        <v>1248.6300000000001</v>
+        <v>1248.63</v>
       </c>
       <c r="K61" s="61"/>
       <c r="L61" s="42">
@@ -27187,7 +27195,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="62">
       <c r="C62" s="42">
         <v>9</v>
       </c>
@@ -27212,7 +27220,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="63">
       <c r="C63" s="42">
         <v>9</v>
       </c>
@@ -27234,7 +27242,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="64">
       <c r="C64" s="42">
         <v>10</v>
       </c>
@@ -27263,7 +27271,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="65">
       <c r="C65" s="42">
         <v>10</v>
       </c>
@@ -27292,7 +27300,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="66">
       <c r="C66" s="42">
         <v>10</v>
       </c>
@@ -27317,7 +27325,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="67">
       <c r="C67" s="42">
         <v>10</v>
       </c>
@@ -27332,7 +27340,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="68">
       <c r="C68" s="42">
         <v>11</v>
       </c>
@@ -27361,7 +27369,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="69">
       <c r="C69" s="42">
         <v>11</v>
       </c>
@@ -27390,7 +27398,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="70">
       <c r="C70" s="42">
         <v>11</v>
       </c>
@@ -27415,7 +27423,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="71">
       <c r="C71" s="42">
         <v>11</v>
       </c>
@@ -27437,7 +27445,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="72">
       <c r="C72" s="42">
         <v>12</v>
       </c>
@@ -27464,7 +27472,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="73">
       <c r="C73" s="42">
         <v>12</v>
       </c>
@@ -27491,7 +27499,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="74">
       <c r="C74" s="42">
         <v>12</v>
       </c>
@@ -27518,7 +27526,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="75">
       <c r="C75" s="42">
         <v>12</v>
       </c>
@@ -27537,7 +27545,7 @@
       </c>
       <c r="I75" s="56"/>
       <c r="J75" s="56">
-        <v>4585.3999999999996</v>
+        <v>4585.4</v>
       </c>
       <c r="K75" s="61"/>
       <c r="L75" s="42">
@@ -27545,7 +27553,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="76">
       <c r="C76" s="42">
         <v>12</v>
       </c>
@@ -27568,7 +27576,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="77">
       <c r="C77" s="42">
         <v>12</v>
       </c>
@@ -27588,7 +27596,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="78">
       <c r="C78" s="42">
         <v>13</v>
       </c>
@@ -27617,7 +27625,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="79">
       <c r="C79" s="42">
         <v>13</v>
       </c>
@@ -27646,7 +27654,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="80">
       <c r="C80" s="42">
         <v>13</v>
       </c>
@@ -27675,7 +27683,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="81">
       <c r="C81" s="42">
         <v>13</v>
       </c>
@@ -27704,7 +27712,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="82">
       <c r="C82" s="42">
         <v>13</v>
       </c>
@@ -27729,7 +27737,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="83">
       <c r="C83" s="42">
         <v>13</v>
       </c>
@@ -27751,7 +27759,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="84">
       <c r="C84" s="42">
         <v>14</v>
       </c>
@@ -27771,7 +27779,7 @@
         <v>402</v>
       </c>
       <c r="I84" s="48">
-        <v>1034.9100000000001</v>
+        <v>1034.91</v>
       </c>
       <c r="J84" s="48"/>
       <c r="K84" s="50"/>
@@ -27780,7 +27788,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="85">
       <c r="C85" s="42">
         <v>14</v>
       </c>
@@ -27809,7 +27817,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="86">
       <c r="C86" s="42">
         <v>14</v>
       </c>
@@ -27830,7 +27838,7 @@
       </c>
       <c r="I86" s="56"/>
       <c r="J86" s="56">
-        <v>153.72999999999999</v>
+        <v>153.73</v>
       </c>
       <c r="K86" s="61"/>
       <c r="L86" s="42">
@@ -27838,7 +27846,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="87">
       <c r="C87" s="42">
         <v>14</v>
       </c>
@@ -27867,7 +27875,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="88">
       <c r="C88" s="42">
         <v>14</v>
       </c>
@@ -27896,7 +27904,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="89">
       <c r="C89" s="42">
         <v>14</v>
       </c>
@@ -27925,7 +27933,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="90">
       <c r="C90" s="42">
         <v>14</v>
       </c>
@@ -27954,7 +27962,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="91">
       <c r="C91" s="42">
         <v>14</v>
       </c>
@@ -27983,7 +27991,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="92">
       <c r="C92" s="42">
         <v>14</v>
       </c>
@@ -28008,7 +28016,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="93">
       <c r="C93" s="42">
         <v>14</v>
       </c>
@@ -28030,7 +28038,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="94">
       <c r="C94" s="42">
         <v>15</v>
       </c>
@@ -28059,7 +28067,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="95">
       <c r="C95" s="42">
         <v>15</v>
       </c>
@@ -28088,7 +28096,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="96">
       <c r="C96" s="42">
         <v>15</v>
       </c>
@@ -28117,7 +28125,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="97">
       <c r="C97" s="42">
         <v>15</v>
       </c>
@@ -28146,7 +28154,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="98">
       <c r="C98" s="42">
         <v>15</v>
       </c>
@@ -28175,7 +28183,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="99">
       <c r="C99" s="42">
         <v>15</v>
       </c>
@@ -28204,7 +28212,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="100">
       <c r="C100" s="42">
         <v>15</v>
       </c>
@@ -28233,7 +28241,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="101">
       <c r="C101" s="42">
         <v>15</v>
       </c>
@@ -28264,7 +28272,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="102">
       <c r="C102" s="42">
         <v>15</v>
       </c>
@@ -28289,7 +28297,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="103">
       <c r="C103" s="42">
         <v>15</v>
       </c>
@@ -28311,7 +28319,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="104" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="104">
       <c r="C104" s="42">
         <v>16</v>
       </c>
@@ -28331,7 +28339,7 @@
         <v>399</v>
       </c>
       <c r="I104" s="48">
-        <v>1034.9100000000001</v>
+        <v>1034.91</v>
       </c>
       <c r="J104" s="48"/>
       <c r="K104" s="50"/>
@@ -28340,7 +28348,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="105">
       <c r="C105" s="42">
         <v>16</v>
       </c>
@@ -28361,7 +28369,7 @@
       </c>
       <c r="I105" s="56"/>
       <c r="J105" s="56">
-        <v>1034.9100000000001</v>
+        <v>1034.91</v>
       </c>
       <c r="K105" s="61"/>
       <c r="L105" s="42">
@@ -28369,7 +28377,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="106" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="106">
       <c r="C106" s="42">
         <v>16</v>
       </c>
@@ -28394,7 +28402,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="107">
       <c r="C107" s="42">
         <v>16</v>
       </c>
@@ -28416,7 +28424,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="108" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="108">
       <c r="C108" s="42">
         <v>17</v>
       </c>
@@ -28447,7 +28455,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="109" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="109">
       <c r="C109" s="42">
         <v>17</v>
       </c>
@@ -28478,7 +28486,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="110">
       <c r="C110" s="42">
         <v>17</v>
       </c>
@@ -28503,7 +28511,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="111">
       <c r="C111" s="42">
         <v>17</v>
       </c>
@@ -28525,7 +28533,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="112" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="112">
       <c r="C112" s="42">
         <v>18</v>
       </c>
@@ -28554,7 +28562,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="113" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="113">
       <c r="C113" s="42">
         <v>18</v>
       </c>
@@ -28583,7 +28591,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="114" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="114">
       <c r="C114" s="42">
         <v>18</v>
       </c>
@@ -28612,7 +28620,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="115" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="115">
       <c r="C115" s="42">
         <v>18</v>
       </c>
@@ -28641,7 +28649,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="116" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="116">
       <c r="C116" s="42">
         <v>18</v>
       </c>
@@ -28666,7 +28674,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="117" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="117">
       <c r="C117" s="42">
         <v>18</v>
       </c>
@@ -28688,7 +28696,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="118" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="118">
       <c r="C118" s="42">
         <v>19</v>
       </c>
@@ -28717,7 +28725,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="119" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="119">
       <c r="C119" s="42">
         <v>19</v>
       </c>
@@ -28746,7 +28754,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="120">
       <c r="C120" s="42">
         <v>19</v>
       </c>
@@ -28771,7 +28779,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="121">
       <c r="C121" s="42">
         <v>19</v>
       </c>
@@ -28793,7 +28801,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="122" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="122">
       <c r="C122" s="42">
         <v>20</v>
       </c>
@@ -28822,7 +28830,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="123" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="123">
       <c r="C123" s="42">
         <v>20</v>
       </c>
@@ -28851,7 +28859,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="124" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="124">
       <c r="C124" s="42">
         <v>20</v>
       </c>
@@ -28876,7 +28884,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="125">
       <c r="C125" s="42">
         <v>20</v>
       </c>
@@ -28898,7 +28906,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="126" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="126">
       <c r="C126" s="42">
         <v>21</v>
       </c>
@@ -28927,7 +28935,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="127">
       <c r="C127" s="42">
         <v>21</v>
       </c>
@@ -28956,7 +28964,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="128" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="128">
       <c r="C128" s="42">
         <v>21</v>
       </c>
@@ -28981,7 +28989,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="129" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="129">
       <c r="C129" s="42">
         <v>21</v>
       </c>
@@ -29003,7 +29011,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="130" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="130">
       <c r="C130" s="42">
         <v>22</v>
       </c>
@@ -29034,7 +29042,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="131" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="131">
       <c r="C131" s="42">
         <v>22</v>
       </c>
@@ -29063,7 +29071,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="132" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="132">
       <c r="C132" s="42">
         <v>22</v>
       </c>
@@ -29088,7 +29096,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="133" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="133">
       <c r="C133" s="42">
         <v>22</v>
       </c>
@@ -29110,7 +29118,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="134" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="134">
       <c r="C134" s="42">
         <v>23</v>
       </c>
@@ -29130,7 +29138,7 @@
         <v>399</v>
       </c>
       <c r="I134" s="111">
-        <v>159.94999999999999</v>
+        <v>159.95</v>
       </c>
       <c r="J134" s="111"/>
       <c r="K134" s="112"/>
@@ -29139,7 +29147,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="135">
       <c r="C135" s="42">
         <v>23</v>
       </c>
@@ -29160,7 +29168,7 @@
       </c>
       <c r="I135" s="118"/>
       <c r="J135" s="118">
-        <v>149.94999999999999</v>
+        <v>149.95</v>
       </c>
       <c r="K135" s="119"/>
       <c r="L135" s="42">
@@ -29168,7 +29176,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="136" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="136">
       <c r="C136" s="42">
         <v>23</v>
       </c>
@@ -29197,7 +29205,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="137" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="137">
       <c r="C137" s="42">
         <v>23</v>
       </c>
@@ -29226,7 +29234,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="138">
       <c r="C138" s="42">
         <v>23</v>
       </c>
@@ -29251,7 +29259,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="139" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="139">
       <c r="C139" s="42">
         <v>23</v>
       </c>
@@ -29273,7 +29281,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="140">
       <c r="C140" s="42">
         <v>24</v>
       </c>
@@ -29302,7 +29310,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="141" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="141">
       <c r="C141" s="42">
         <v>24</v>
       </c>
@@ -29331,7 +29339,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="142" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="142">
       <c r="C142" s="42">
         <v>24</v>
       </c>
@@ -29356,7 +29364,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="143" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="143">
       <c r="C143" s="42">
         <v>24</v>
       </c>
@@ -29378,7 +29386,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="144" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="144">
       <c r="C144" s="42">
         <v>25</v>
       </c>
@@ -29407,7 +29415,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="145" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="145">
       <c r="C145" s="42">
         <v>25</v>
       </c>
@@ -29436,7 +29444,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="146" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="146">
       <c r="C146" s="42">
         <v>25</v>
       </c>
@@ -29461,7 +29469,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="147">
       <c r="C147" s="42">
         <v>25</v>
       </c>
@@ -29483,7 +29491,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="148" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="148">
       <c r="C148" s="42">
         <v>26</v>
       </c>
@@ -29512,7 +29520,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="149" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="149">
       <c r="C149" s="42">
         <v>26</v>
       </c>
@@ -29541,7 +29549,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="150" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="150">
       <c r="C150" s="42">
         <v>26</v>
       </c>
@@ -29566,7 +29574,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="151" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="151">
       <c r="C151" s="42">
         <v>26</v>
       </c>
@@ -29588,7 +29596,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="152" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="152">
       <c r="C152" s="42">
         <v>27</v>
       </c>
@@ -29617,7 +29625,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="153" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="153">
       <c r="C153" s="42">
         <v>27</v>
       </c>
@@ -29646,7 +29654,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="154" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="154">
       <c r="C154" s="42">
         <v>27</v>
       </c>
@@ -29671,7 +29679,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="155" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="155">
       <c r="C155" s="42">
         <v>27</v>
       </c>
@@ -29693,7 +29701,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="156" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="156">
       <c r="C156" s="42">
         <v>28</v>
       </c>
@@ -29722,7 +29730,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="157" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="157">
       <c r="C157" s="42">
         <v>28</v>
       </c>
@@ -29751,7 +29759,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="158" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="158">
       <c r="C158" s="42">
         <v>28</v>
       </c>
@@ -29776,7 +29784,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="159" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="159">
       <c r="C159" s="42">
         <v>28</v>
       </c>
@@ -29798,7 +29806,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="160" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="160">
       <c r="C160" s="42">
         <v>29</v>
       </c>
@@ -29818,7 +29826,7 @@
         <v>402</v>
       </c>
       <c r="I160" s="136">
-        <v>2157.0700000000002</v>
+        <v>2157.07</v>
       </c>
       <c r="J160" s="136"/>
       <c r="K160" s="137"/>
@@ -29827,7 +29835,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="161" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="161">
       <c r="C161" s="42">
         <v>29</v>
       </c>
@@ -29856,7 +29864,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="162" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="162">
       <c r="C162" s="42">
         <v>29</v>
       </c>
@@ -29885,7 +29893,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="163">
       <c r="C163" s="42">
         <v>29</v>
       </c>
@@ -29914,7 +29922,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="164" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="164">
       <c r="C164" s="42">
         <v>29</v>
       </c>
@@ -29943,7 +29951,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="165" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="165">
       <c r="C165" s="42">
         <v>29</v>
       </c>
@@ -29972,7 +29980,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="166" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="166">
       <c r="C166" s="42">
         <v>29</v>
       </c>
@@ -30001,7 +30009,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="167" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="167">
       <c r="C167" s="42">
         <v>29</v>
       </c>
@@ -30030,7 +30038,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="168" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="168">
       <c r="C168" s="42">
         <v>29</v>
       </c>
@@ -30055,7 +30063,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="169" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="169">
       <c r="C169" s="42">
         <v>29</v>
       </c>
@@ -30078,7 +30086,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="170" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="170">
       <c r="C170" s="42">
         <v>30</v>
       </c>
@@ -30107,7 +30115,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="171" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="171">
       <c r="C171" s="42">
         <v>30</v>
       </c>
@@ -30136,7 +30144,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="172" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="172">
       <c r="C172" s="42">
         <v>30</v>
       </c>
@@ -30165,7 +30173,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="173" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="173">
       <c r="C173" s="42">
         <v>30</v>
       </c>
@@ -30194,7 +30202,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="174" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="174">
       <c r="C174" s="42">
         <v>30</v>
       </c>
@@ -30223,7 +30231,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="175" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="175">
       <c r="C175" s="42">
         <v>30</v>
       </c>
@@ -30252,7 +30260,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="176" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="176">
       <c r="C176" s="42">
         <v>30</v>
       </c>
@@ -30281,7 +30289,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="177" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="177">
       <c r="C177" s="42">
         <v>30</v>
       </c>
@@ -30310,7 +30318,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="178" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="178">
       <c r="C178" s="42">
         <v>30</v>
       </c>
@@ -30335,7 +30343,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="179" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="179">
       <c r="C179" s="42">
         <v>30</v>
       </c>
@@ -30357,7 +30365,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="180" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="180">
       <c r="C180" s="42">
         <v>31</v>
       </c>
@@ -30386,7 +30394,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="181" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="181">
       <c r="C181" s="42">
         <v>31</v>
       </c>
@@ -30415,7 +30423,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="182" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="182">
       <c r="C182" s="42">
         <v>31</v>
       </c>
@@ -30440,7 +30448,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="183" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="183">
       <c r="C183" s="42">
         <v>31</v>
       </c>
@@ -30463,7 +30471,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="184" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="184">
       <c r="C184" s="42">
         <v>32</v>
       </c>
@@ -30492,7 +30500,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="185" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="185">
       <c r="C185" s="42">
         <v>32</v>
       </c>
@@ -30521,7 +30529,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="186" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="186">
       <c r="C186" s="42">
         <v>32</v>
       </c>
@@ -30546,7 +30554,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="187" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="187">
       <c r="C187" s="42">
         <v>32</v>
       </c>
@@ -30568,7 +30576,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="188" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="188">
       <c r="C188" s="42">
         <v>33</v>
       </c>
@@ -30597,7 +30605,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="189" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="189">
       <c r="C189" s="42">
         <v>33</v>
       </c>
@@ -30628,7 +30636,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="190" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="190">
       <c r="C190" s="42">
         <v>33</v>
       </c>
@@ -30653,7 +30661,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="191" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="191">
       <c r="C191" s="42">
         <v>33</v>
       </c>
@@ -30675,7 +30683,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="192" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="192">
       <c r="C192" s="42">
         <v>34</v>
       </c>
@@ -30704,7 +30712,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="193" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="193">
       <c r="C193" s="42">
         <v>34</v>
       </c>
@@ -30733,7 +30741,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="194" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="194">
       <c r="C194" s="42">
         <v>34</v>
       </c>
@@ -30758,7 +30766,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="195" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="195">
       <c r="C195" s="42">
         <v>34</v>
       </c>
@@ -30780,7 +30788,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="196" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="196">
       <c r="C196" s="42">
         <v>35</v>
       </c>
@@ -30809,7 +30817,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="197">
       <c r="C197" s="42">
         <v>35</v>
       </c>
@@ -30838,7 +30846,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="198" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="198">
       <c r="C198" s="42">
         <v>35</v>
       </c>
@@ -30863,7 +30871,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="199" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="199">
       <c r="C199" s="42">
         <v>35</v>
       </c>
@@ -30885,7 +30893,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="200" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="200">
       <c r="C200" s="42">
         <v>36</v>
       </c>
@@ -30912,7 +30920,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="201" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="201">
       <c r="C201" s="42">
         <v>36</v>
       </c>
@@ -30939,7 +30947,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="202" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="202">
       <c r="C202" s="42">
         <v>36</v>
       </c>
@@ -30962,7 +30970,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="203" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="203">
       <c r="C203" s="42">
         <v>36</v>
       </c>
@@ -30982,7 +30990,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="204" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="204">
       <c r="C204" s="42">
         <v>37</v>
       </c>
@@ -31011,7 +31019,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="205" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="205">
       <c r="C205" s="42">
         <v>37</v>
       </c>
@@ -31040,7 +31048,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="206" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="206">
       <c r="C206" s="42">
         <v>37</v>
       </c>
@@ -31065,7 +31073,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="207" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="207">
       <c r="C207" s="42">
         <v>37</v>
       </c>
@@ -31087,7 +31095,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="208" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="208">
       <c r="C208" s="42">
         <v>38</v>
       </c>
@@ -31116,7 +31124,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="209" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="209">
       <c r="C209" s="42">
         <v>38</v>
       </c>
@@ -31145,7 +31153,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="210" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="210">
       <c r="C210" s="42">
         <v>38</v>
       </c>
@@ -31170,7 +31178,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="211" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="211">
       <c r="C211" s="42">
         <v>38</v>
       </c>
@@ -31193,7 +31201,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="212" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="212">
       <c r="C212" s="42">
         <v>39</v>
       </c>
@@ -31222,7 +31230,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="213" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="213">
       <c r="C213" s="42">
         <v>39</v>
       </c>
@@ -31251,7 +31259,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="214" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="214">
       <c r="C214" s="42">
         <v>39</v>
       </c>
@@ -31276,7 +31284,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="215" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="215">
       <c r="C215" s="42">
         <v>39</v>
       </c>
@@ -31299,7 +31307,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="216" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="216">
       <c r="C216" s="42">
         <v>40</v>
       </c>
@@ -31328,7 +31336,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="217" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="217">
       <c r="C217" s="42">
         <v>40</v>
       </c>
@@ -31357,7 +31365,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="218" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="218">
       <c r="C218" s="42">
         <v>40</v>
       </c>
@@ -31378,7 +31386,7 @@
       </c>
       <c r="I218" s="34"/>
       <c r="J218" s="34">
-        <v>33.950000000000003</v>
+        <v>33.95</v>
       </c>
       <c r="K218" s="176"/>
       <c r="L218" s="42">
@@ -31386,7 +31394,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="219" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="219">
       <c r="C219" s="42">
         <v>40</v>
       </c>
@@ -31411,7 +31419,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="220" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="220">
       <c r="C220" s="42">
         <v>40</v>
       </c>
@@ -31433,7 +31441,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="221" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="221">
       <c r="C221" s="42">
         <v>41</v>
       </c>
@@ -31462,7 +31470,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="222" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="222">
       <c r="C222" s="42">
         <v>41</v>
       </c>
@@ -31491,7 +31499,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="223" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="223">
       <c r="C223" s="42">
         <v>41</v>
       </c>
@@ -31516,7 +31524,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="224" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="224">
       <c r="C224" s="42">
         <v>41</v>
       </c>
@@ -31538,7 +31546,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="225" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="225">
       <c r="C225" s="42">
         <v>42</v>
       </c>
@@ -31567,7 +31575,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="226" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="226">
       <c r="C226" s="42">
         <v>42</v>
       </c>
@@ -31596,7 +31604,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="227" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="227">
       <c r="C227" s="42">
         <v>42</v>
       </c>
@@ -31621,7 +31629,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="228" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="228">
       <c r="C228" s="42">
         <v>42</v>
       </c>
@@ -31643,7 +31651,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="229" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="229">
       <c r="C229" s="42">
         <v>43</v>
       </c>
@@ -31672,7 +31680,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="230" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="230">
       <c r="C230" s="42">
         <v>43</v>
       </c>
@@ -31701,7 +31709,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="231" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="231">
       <c r="C231" s="42">
         <v>43</v>
       </c>
@@ -31726,7 +31734,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="232" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="232">
       <c r="C232" s="42">
         <v>43</v>
       </c>
@@ -31748,7 +31756,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="233" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="233">
       <c r="C233" s="42">
         <v>44</v>
       </c>
@@ -31777,7 +31785,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="234" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="234">
       <c r="C234" s="42">
         <v>44</v>
       </c>
@@ -31806,7 +31814,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="235" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="235">
       <c r="C235" s="42">
         <v>44</v>
       </c>
@@ -31831,7 +31839,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="236" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="236">
       <c r="C236" s="42">
         <v>44</v>
       </c>
@@ -31853,7 +31861,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="237" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="237">
       <c r="C237" s="42">
         <v>45</v>
       </c>
@@ -31882,7 +31890,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="238" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="238">
       <c r="C238" s="42">
         <v>45</v>
       </c>
@@ -31911,7 +31919,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="239" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="239">
       <c r="C239" s="42">
         <v>45</v>
       </c>
@@ -31940,7 +31948,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="240" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="240">
       <c r="C240" s="42">
         <v>45</v>
       </c>
@@ -31969,7 +31977,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="241" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="241">
       <c r="C241" s="42">
         <v>45</v>
       </c>
@@ -31994,7 +32002,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="242" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="242">
       <c r="C242" s="42">
         <v>45</v>
       </c>
@@ -32016,7 +32024,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="243" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="243">
       <c r="C243" s="42">
         <v>46</v>
       </c>
@@ -32036,7 +32044,7 @@
         <v>469</v>
       </c>
       <c r="I243" s="158">
-        <v>9.9499999999999993</v>
+        <v>9.95</v>
       </c>
       <c r="J243" s="158"/>
       <c r="K243" s="174"/>
@@ -32045,7 +32053,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="244" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="244">
       <c r="C244" s="42">
         <v>46</v>
       </c>
@@ -32066,7 +32074,7 @@
       </c>
       <c r="I244" s="34"/>
       <c r="J244" s="34">
-        <v>9.9499999999999993</v>
+        <v>9.95</v>
       </c>
       <c r="K244" s="176"/>
       <c r="L244" s="42">
@@ -32074,7 +32082,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="245" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="245">
       <c r="C245" s="42">
         <v>46</v>
       </c>
@@ -32099,7 +32107,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="246" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="246">
       <c r="C246" s="42">
         <v>46</v>
       </c>
@@ -32121,7 +32129,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="247" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="247">
       <c r="C247" s="42">
         <v>47</v>
       </c>
@@ -32148,7 +32156,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="248" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="248">
       <c r="C248" s="42">
         <v>47</v>
       </c>
@@ -32175,7 +32183,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="249" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="249">
       <c r="C249" s="42">
         <v>47</v>
       </c>
@@ -32198,7 +32206,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="250" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="250">
       <c r="C250" s="42">
         <v>47</v>
       </c>
@@ -32218,7 +32226,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="251" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="251">
       <c r="C251" s="42">
         <v>48</v>
       </c>
@@ -32245,7 +32253,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="252" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="252">
       <c r="C252" s="42">
         <v>48</v>
       </c>
@@ -32272,7 +32280,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="253" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="253">
       <c r="C253" s="42">
         <v>48</v>
       </c>
@@ -32299,7 +32307,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="254" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="254">
       <c r="C254" s="42">
         <v>48</v>
       </c>
@@ -32326,7 +32334,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="255" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="255">
       <c r="C255" s="42">
         <v>48</v>
       </c>
@@ -32353,7 +32361,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="256" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="256">
       <c r="C256" s="42">
         <v>48</v>
       </c>
@@ -32376,7 +32384,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="257" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="257">
       <c r="C257" s="42">
         <v>48</v>
       </c>
@@ -32396,7 +32404,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="258" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="258">
       <c r="C258" s="42">
         <v>49</v>
       </c>
@@ -32425,7 +32433,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="259" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="259">
       <c r="C259" s="42">
         <v>49</v>
       </c>
@@ -32454,7 +32462,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="260" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="260">
       <c r="C260" s="42">
         <v>49</v>
       </c>
@@ -32483,7 +32491,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="261" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="261">
       <c r="C261" s="42">
         <v>49</v>
       </c>
@@ -32512,7 +32520,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="262" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="262">
       <c r="C262" s="42">
         <v>49</v>
       </c>
@@ -32537,7 +32545,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="263" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="263">
       <c r="C263" s="42">
         <v>49</v>
       </c>
@@ -32559,7 +32567,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="264" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="264">
       <c r="C264" s="42">
         <v>50</v>
       </c>
@@ -32588,7 +32596,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="265" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="265">
       <c r="C265" s="42">
         <v>50</v>
       </c>
@@ -32617,7 +32625,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="266" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="266">
       <c r="C266" s="42">
         <v>50</v>
       </c>
@@ -32646,7 +32654,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="267" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="267">
       <c r="C267" s="42">
         <v>50</v>
       </c>
@@ -32675,7 +32683,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="268" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="268">
       <c r="C268" s="42">
         <v>50</v>
       </c>
@@ -32700,7 +32708,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="269" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="269">
       <c r="C269" s="42">
         <v>50</v>
       </c>
@@ -32722,7 +32730,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="270" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="270">
       <c r="C270" s="42">
         <v>51</v>
       </c>
@@ -32751,7 +32759,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="271" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="271">
       <c r="C271" s="42">
         <v>51</v>
       </c>
@@ -32780,7 +32788,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="272" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="272">
       <c r="C272" s="42">
         <v>51</v>
       </c>
@@ -32805,7 +32813,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="273" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="273">
       <c r="C273" s="42">
         <v>51</v>
       </c>
@@ -32827,7 +32835,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="274" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="274">
       <c r="C274" s="42">
         <v>52</v>
       </c>
@@ -32847,7 +32855,7 @@
         <v>514</v>
       </c>
       <c r="I274" s="158">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="J274" s="158"/>
       <c r="K274" s="174"/>
@@ -32856,7 +32864,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="275" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="275">
       <c r="C275" s="42">
         <v>52</v>
       </c>
@@ -32885,7 +32893,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="276" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="276">
       <c r="C276" s="42">
         <v>52</v>
       </c>
@@ -32914,7 +32922,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="277" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="277">
       <c r="C277" s="42">
         <v>52</v>
       </c>
@@ -32945,7 +32953,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="278" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="278">
       <c r="C278" s="42">
         <v>52</v>
       </c>
@@ -32970,7 +32978,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="279" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="279">
       <c r="C279" s="42">
         <v>52</v>
       </c>
@@ -32992,7 +33000,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="280" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="280">
       <c r="C280" s="42">
         <v>53</v>
       </c>
@@ -33010,7 +33018,7 @@
         <v>514</v>
       </c>
       <c r="I280" s="158">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="J280" s="158"/>
       <c r="K280" s="174"/>
@@ -33019,7 +33027,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="281" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="281">
       <c r="C281" s="42">
         <v>53</v>
       </c>
@@ -33046,7 +33054,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="282" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="282">
       <c r="C282" s="42">
         <v>53</v>
       </c>
@@ -33073,7 +33081,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="283" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="283">
       <c r="C283" s="42">
         <v>53</v>
       </c>
@@ -33102,7 +33110,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="284" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="284">
       <c r="C284" s="42">
         <v>53</v>
       </c>
@@ -33125,7 +33133,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="285" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="285">
       <c r="C285" s="42">
         <v>53</v>
       </c>
@@ -33145,7 +33153,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="286" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="286">
       <c r="C286" s="42">
         <v>54</v>
       </c>
@@ -33163,7 +33171,7 @@
         <v>514</v>
       </c>
       <c r="I286" s="158">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="J286" s="158"/>
       <c r="K286" s="174"/>
@@ -33172,7 +33180,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="287" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="287">
       <c r="C287" s="42">
         <v>54</v>
       </c>
@@ -33199,7 +33207,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="288" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="288">
       <c r="C288" s="42">
         <v>54</v>
       </c>
@@ -33226,7 +33234,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="289" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="289">
       <c r="C289" s="42">
         <v>54</v>
       </c>
@@ -33255,7 +33263,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="290" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="290">
       <c r="C290" s="42">
         <v>54</v>
       </c>
@@ -33278,7 +33286,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="291" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="291">
       <c r="C291" s="42">
         <v>54</v>
       </c>
@@ -33298,7 +33306,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="292" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="292">
       <c r="C292" s="42">
         <v>55</v>
       </c>
@@ -33316,7 +33324,7 @@
         <v>514</v>
       </c>
       <c r="I292" s="158">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="J292" s="158"/>
       <c r="K292" s="174"/>
@@ -33325,7 +33333,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="293" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="293">
       <c r="C293" s="42">
         <v>55</v>
       </c>
@@ -33352,7 +33360,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="294" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="294">
       <c r="C294" s="42">
         <v>55</v>
       </c>
@@ -33379,7 +33387,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="295" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="295">
       <c r="C295" s="42">
         <v>55</v>
       </c>
@@ -33408,7 +33416,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="296" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="296">
       <c r="C296" s="42">
         <v>55</v>
       </c>
@@ -33431,7 +33439,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="297" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="297">
       <c r="C297" s="42">
         <v>55</v>
       </c>
@@ -33451,7 +33459,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="298" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="298">
       <c r="C298" s="42">
         <v>56</v>
       </c>
@@ -33478,7 +33486,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="299" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="299">
       <c r="C299" s="42">
         <v>56</v>
       </c>
@@ -33505,7 +33513,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="300" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="300">
       <c r="C300" s="42">
         <v>56</v>
       </c>
@@ -33528,7 +33536,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="301" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="301">
       <c r="C301" s="42">
         <v>56</v>
       </c>
@@ -33548,7 +33556,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="302" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="302">
       <c r="C302" s="42">
         <v>57</v>
       </c>
@@ -33575,7 +33583,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="303" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="303">
       <c r="C303" s="42">
         <v>57</v>
       </c>
@@ -33602,7 +33610,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="304" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="304">
       <c r="C304" s="42">
         <v>57</v>
       </c>
@@ -33629,7 +33637,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="305" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="305">
       <c r="C305" s="42">
         <v>57</v>
       </c>
@@ -33656,7 +33664,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="306" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="306">
       <c r="C306" s="42">
         <v>57</v>
       </c>
@@ -33683,7 +33691,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="307" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="307">
       <c r="C307" s="42">
         <v>57</v>
       </c>
@@ -33706,7 +33714,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="308" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="308">
       <c r="C308" s="42">
         <v>57</v>
       </c>
@@ -33726,7 +33734,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="309" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="309">
       <c r="C309" s="42">
         <v>58</v>
       </c>
@@ -33753,7 +33761,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="310" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="310">
       <c r="C310" s="42">
         <v>58</v>
       </c>
@@ -33780,7 +33788,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="311" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="311">
       <c r="C311" s="42">
         <v>58</v>
       </c>
@@ -33807,7 +33815,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="312" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="312">
       <c r="C312" s="42">
         <v>58</v>
       </c>
@@ -33834,7 +33842,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="313" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="313">
       <c r="C313" s="42">
         <v>58</v>
       </c>
@@ -33857,7 +33865,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="314" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="314">
       <c r="C314" s="42">
         <v>58</v>
       </c>
@@ -33877,7 +33885,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="315" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="315">
       <c r="C315" s="42">
         <v>59</v>
       </c>
@@ -33904,7 +33912,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="316" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="316">
       <c r="C316" s="42">
         <v>59</v>
       </c>
@@ -33931,7 +33939,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="317" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="317">
       <c r="C317" s="42">
         <v>59</v>
       </c>
@@ -33958,7 +33966,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="318" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="318">
       <c r="C318" s="42">
         <v>59</v>
       </c>
@@ -33985,7 +33993,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="319" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="319">
       <c r="C319" s="42">
         <v>59</v>
       </c>
@@ -34008,7 +34016,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="320" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="320">
       <c r="C320" s="42">
         <v>59</v>
       </c>
@@ -34028,7 +34036,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="321" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="321">
       <c r="C321" s="42">
         <v>60</v>
       </c>
@@ -34046,7 +34054,7 @@
         <v>514</v>
       </c>
       <c r="I321" s="158">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="J321" s="158"/>
       <c r="K321" s="174"/>
@@ -34055,7 +34063,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="322" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="322">
       <c r="C322" s="42">
         <v>60</v>
       </c>
@@ -34082,7 +34090,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="323" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="323">
       <c r="C323" s="42">
         <v>60</v>
       </c>
@@ -34109,7 +34117,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="324" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="324">
       <c r="C324" s="42">
         <v>60</v>
       </c>
@@ -34138,7 +34146,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="325" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="325">
       <c r="C325" s="42">
         <v>60</v>
       </c>
@@ -34161,7 +34169,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="326" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="326">
       <c r="C326" s="42">
         <v>60</v>
       </c>
@@ -34181,7 +34189,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="327" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="327">
       <c r="C327" s="42">
         <v>61</v>
       </c>
@@ -34208,7 +34216,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="328" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="328">
       <c r="C328" s="42">
         <v>61</v>
       </c>
@@ -34235,7 +34243,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="329" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="329">
       <c r="C329" s="42">
         <v>61</v>
       </c>
@@ -34262,7 +34270,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="330" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="330">
       <c r="C330" s="42">
         <v>61</v>
       </c>
@@ -34289,7 +34297,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="331" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="331">
       <c r="C331" s="42">
         <v>61</v>
       </c>
@@ -34316,7 +34324,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="332" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="332">
       <c r="C332" s="42">
         <v>61</v>
       </c>
@@ -34339,7 +34347,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="333" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="333">
       <c r="C333" s="42">
         <v>61</v>
       </c>
@@ -34359,7 +34367,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="334" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="334">
       <c r="C334" s="42">
         <v>62</v>
       </c>
@@ -34386,7 +34394,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="335" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="335">
       <c r="C335" s="42">
         <v>62</v>
       </c>
@@ -34413,7 +34421,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="336" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="336">
       <c r="C336" s="42">
         <v>62</v>
       </c>
@@ -34440,7 +34448,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="337" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="337">
       <c r="C337" s="42">
         <v>62</v>
       </c>
@@ -34467,7 +34475,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="338" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="338">
       <c r="C338" s="42">
         <v>62</v>
       </c>
@@ -34490,7 +34498,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="339" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="339">
       <c r="C339" s="42">
         <v>62</v>
       </c>
@@ -34510,7 +34518,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="340" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="340">
       <c r="C340" s="42">
         <v>63</v>
       </c>
@@ -34537,7 +34545,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="341" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="341">
       <c r="C341" s="42">
         <v>63</v>
       </c>
@@ -34564,7 +34572,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="342" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="342">
       <c r="C342" s="42">
         <v>63</v>
       </c>
@@ -34591,7 +34599,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="343" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="343">
       <c r="C343" s="42">
         <v>63</v>
       </c>
@@ -34618,7 +34626,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="344" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="344">
       <c r="C344" s="42">
         <v>63</v>
       </c>
@@ -34641,7 +34649,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="345" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="345">
       <c r="C345" s="42">
         <v>63</v>
       </c>
@@ -34661,7 +34669,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="346" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="346">
       <c r="C346" s="42">
         <v>64</v>
       </c>
@@ -34690,7 +34698,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="347" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="347">
       <c r="C347" s="42">
         <v>64</v>
       </c>
@@ -34719,7 +34727,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="348" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="348">
       <c r="C348" s="42">
         <v>64</v>
       </c>
@@ -34748,7 +34756,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="349" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="349">
       <c r="C349" s="42">
         <v>64</v>
       </c>
@@ -34777,7 +34785,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="350" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="350">
       <c r="C350" s="42">
         <v>64</v>
       </c>
@@ -34806,7 +34814,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="351" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="351">
       <c r="C351" s="42">
         <v>64</v>
       </c>
@@ -34835,7 +34843,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="352" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="352">
       <c r="C352" s="42">
         <v>64</v>
       </c>
@@ -34860,7 +34868,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="353" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="353">
       <c r="C353" s="42">
         <v>64</v>
       </c>
@@ -34882,7 +34890,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="354" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="354">
       <c r="C354" s="42">
         <v>65</v>
       </c>
@@ -34909,7 +34917,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="355" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="355">
       <c r="C355" s="42">
         <v>65</v>
       </c>
@@ -34936,7 +34944,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="356" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="356">
       <c r="C356" s="42">
         <v>65</v>
       </c>
@@ -34963,7 +34971,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="357" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="357">
       <c r="C357" s="42">
         <v>65</v>
       </c>
@@ -34990,7 +34998,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="358" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="358">
       <c r="C358" s="42">
         <v>65</v>
       </c>
@@ -35013,7 +35021,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="359" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="359">
       <c r="C359" s="42">
         <v>65</v>
       </c>
@@ -35033,7 +35041,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="360" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="360">
       <c r="C360" s="42">
         <v>66</v>
       </c>
@@ -35062,7 +35070,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="361" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="361">
       <c r="C361" s="42">
         <v>66</v>
       </c>
@@ -35091,7 +35099,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="362" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="362">
       <c r="C362" s="42">
         <v>66</v>
       </c>
@@ -35116,7 +35124,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="363" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="363">
       <c r="C363" s="42">
         <v>66</v>
       </c>
@@ -35138,7 +35146,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="364" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="364">
       <c r="C364" s="42">
         <v>67</v>
       </c>
@@ -35167,7 +35175,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="365" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="365">
       <c r="C365" s="42">
         <v>67</v>
       </c>
@@ -35194,7 +35202,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="366" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="366">
       <c r="C366" s="42">
         <v>67</v>
       </c>
@@ -35217,7 +35225,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="367" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="367">
       <c r="C367" s="42">
         <v>67</v>
       </c>
@@ -35237,7 +35245,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="368" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="368">
       <c r="C368" s="42">
         <v>68</v>
       </c>
@@ -35266,7 +35274,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="369" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="369">
       <c r="C369" s="42">
         <v>68</v>
       </c>
@@ -35295,7 +35303,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="370" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="370">
       <c r="C370" s="42">
         <v>68</v>
       </c>
@@ -35324,7 +35332,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="371" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="371">
       <c r="C371" s="42">
         <v>68</v>
       </c>
@@ -35345,7 +35353,7 @@
       </c>
       <c r="I371" s="34"/>
       <c r="J371" s="34">
-        <v>37.409999999999997</v>
+        <v>37.41</v>
       </c>
       <c r="K371" s="209"/>
       <c r="L371" s="42">
@@ -35353,7 +35361,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="372" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="372">
       <c r="C372" s="42">
         <v>68</v>
       </c>
@@ -35367,18 +35375,18 @@
         <v>486</v>
       </c>
       <c r="G372" s="210"/>
-      <c r="H372" s="219" t="s">
+      <c r="H372" s="222" t="s">
         <v>526</v>
       </c>
-      <c r="I372" s="219"/>
-      <c r="J372" s="219"/>
-      <c r="K372" s="220"/>
+      <c r="I372" s="222"/>
+      <c r="J372" s="222"/>
+      <c r="K372" s="223"/>
       <c r="L372" s="42">
         <f>ROW()</f>
         <v>372</v>
       </c>
     </row>
-    <row r="373" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="373">
       <c r="C373" s="42">
         <v>68</v>
       </c>
@@ -35396,7 +35404,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="374" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="374">
       <c r="C374" s="42">
         <v>69</v>
       </c>
@@ -35425,7 +35433,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="375" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="375">
       <c r="C375" s="42">
         <v>69</v>
       </c>
@@ -35454,7 +35462,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="376" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="376">
       <c r="C376" s="42">
         <v>69</v>
       </c>
@@ -35483,7 +35491,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="377" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="377">
       <c r="C377" s="42">
         <v>69</v>
       </c>
@@ -35512,7 +35520,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="378" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="378">
       <c r="C378" s="42">
         <v>69</v>
       </c>
@@ -35541,7 +35549,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="379" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="379">
       <c r="C379" s="42">
         <v>69</v>
       </c>
@@ -35570,7 +35578,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="380" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="380">
       <c r="C380" s="42">
         <v>69</v>
       </c>
@@ -35599,7 +35607,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="381" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="381">
       <c r="C381" s="42">
         <v>69</v>
       </c>
@@ -35613,18 +35621,18 @@
         <v>486</v>
       </c>
       <c r="G381" s="210"/>
-      <c r="H381" s="219" t="s">
+      <c r="H381" s="222" t="s">
         <v>527</v>
       </c>
-      <c r="I381" s="219"/>
-      <c r="J381" s="219"/>
-      <c r="K381" s="220"/>
+      <c r="I381" s="222"/>
+      <c r="J381" s="222"/>
+      <c r="K381" s="223"/>
       <c r="L381" s="42">
         <f>ROW()</f>
         <v>381</v>
       </c>
     </row>
-    <row r="382" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="382">
       <c r="C382" s="42">
         <v>69</v>
       </c>
@@ -35640,7 +35648,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="383" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="383">
       <c r="C383" s="42">
         <v>70</v>
       </c>
@@ -35669,7 +35677,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="384" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="384">
       <c r="C384" s="42">
         <v>70</v>
       </c>
@@ -35698,7 +35706,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="385" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="385">
       <c r="C385" s="42">
         <v>70</v>
       </c>
@@ -35727,7 +35735,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="386" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="386">
       <c r="C386" s="42">
         <v>70</v>
       </c>
@@ -35756,7 +35764,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="387" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="387">
       <c r="C387" s="42">
         <v>70</v>
       </c>
@@ -35785,7 +35793,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="388" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="388">
       <c r="C388" s="42">
         <v>70</v>
       </c>
@@ -35814,7 +35822,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="389" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="389">
       <c r="C389" s="42">
         <v>70</v>
       </c>
@@ -35843,7 +35851,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="390" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="390">
       <c r="C390" s="42">
         <v>70</v>
       </c>
@@ -35857,18 +35865,18 @@
         <v>486</v>
       </c>
       <c r="G390" s="183"/>
-      <c r="H390" s="221" t="s">
+      <c r="H390" s="224" t="s">
         <v>528</v>
       </c>
-      <c r="I390" s="221"/>
-      <c r="J390" s="221"/>
-      <c r="K390" s="222"/>
+      <c r="I390" s="224"/>
+      <c r="J390" s="224"/>
+      <c r="K390" s="225"/>
       <c r="L390" s="42">
         <f>ROW()</f>
         <v>390</v>
       </c>
     </row>
-    <row r="391" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="391">
       <c r="C391" s="42">
         <v>70</v>
       </c>
@@ -35886,7 +35894,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="392" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="392">
       <c r="C392" s="42">
         <v>71</v>
       </c>
@@ -35915,7 +35923,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="393" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="393">
       <c r="C393" s="42">
         <v>71</v>
       </c>
@@ -35944,7 +35952,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="394" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="394">
       <c r="C394" s="42">
         <v>71</v>
       </c>
@@ -35973,7 +35981,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="395" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="395">
       <c r="C395" s="42">
         <v>71</v>
       </c>
@@ -36002,7 +36010,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="396" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="396">
       <c r="C396" s="42">
         <v>71</v>
       </c>
@@ -36031,7 +36039,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="397" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="397">
       <c r="C397" s="42">
         <v>71</v>
       </c>
@@ -36060,7 +36068,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="398" spans="3:12" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="398">
       <c r="C398" s="42">
         <v>71</v>
       </c>
@@ -36089,7 +36097,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="399" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="399">
       <c r="C399" s="42">
         <v>71</v>
       </c>
@@ -36103,18 +36111,18 @@
         <v>486</v>
       </c>
       <c r="G399" s="183"/>
-      <c r="H399" s="221" t="s">
+      <c r="H399" s="224" t="s">
         <v>529</v>
       </c>
-      <c r="I399" s="221"/>
-      <c r="J399" s="221"/>
-      <c r="K399" s="222"/>
+      <c r="I399" s="224"/>
+      <c r="J399" s="224"/>
+      <c r="K399" s="225"/>
       <c r="L399" s="42">
         <f>ROW()</f>
         <v>399</v>
       </c>
     </row>
-    <row r="400" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="400">
       <c r="C400" s="42">
         <v>71</v>
       </c>
@@ -36132,7 +36140,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="401" spans="1:13" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="401">
       <c r="C401" s="42">
         <v>72</v>
       </c>
@@ -36161,7 +36169,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="402" spans="1:13" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="402">
       <c r="C402" s="42">
         <v>72</v>
       </c>
@@ -36190,7 +36198,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="403" spans="1:13" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="403">
       <c r="C403" s="42">
         <v>72</v>
       </c>
@@ -36219,7 +36227,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="404" spans="1:13" x14ac:dyDescent="0.25">
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="404">
       <c r="C404" s="42">
         <v>72</v>
       </c>
@@ -36248,7 +36256,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="405" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="405">
       <c r="C405" s="42">
         <v>72</v>
       </c>
@@ -36262,18 +36270,18 @@
         <v>486</v>
       </c>
       <c r="G405" s="183"/>
-      <c r="H405" s="221" t="s">
+      <c r="H405" s="224" t="s">
         <v>530</v>
       </c>
-      <c r="I405" s="221"/>
-      <c r="J405" s="221"/>
-      <c r="K405" s="222"/>
+      <c r="I405" s="224"/>
+      <c r="J405" s="224"/>
+      <c r="K405" s="225"/>
       <c r="L405" s="42">
         <f>ROW()</f>
         <v>405</v>
       </c>
     </row>
-    <row r="406" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="406">
       <c r="C406" s="42">
         <v>72</v>
       </c>
@@ -36291,9 +36299,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="407" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A407" s="223"/>
-      <c r="B407" s="223"/>
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="407">
       <c r="C407" s="42">
         <v>73</v>
       </c>
@@ -36303,16 +36309,16 @@
       <c r="E407" s="205">
         <v>73</v>
       </c>
-      <c r="F407" s="227" t="s">
+      <c r="F407" s="219" t="s">
         <v>307</v>
       </c>
       <c r="G407" s="205">
         <v>1000</v>
       </c>
-      <c r="H407" s="227" t="s">
+      <c r="H407" s="219" t="s">
         <v>399</v>
       </c>
-      <c r="I407" s="228">
+      <c r="I407" s="187">
         <v>125</v>
       </c>
       <c r="J407" s="198"/>
@@ -36321,31 +36327,27 @@
         <f>ROW()</f>
         <v>407</v>
       </c>
-      <c r="M407" s="223"/>
-    </row>
-    <row r="408" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A408" s="223"/>
-      <c r="B408" s="223"/>
+    </row>
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="408">
       <c r="C408" s="42">
         <v>73</v>
       </c>
-      <c r="D408" s="229">
+      <c r="D408" s="220">
         <v>45294</v>
       </c>
-      <c r="E408" s="230">
+      <c r="E408" s="71">
         <v>73</v>
       </c>
-      <c r="F408" s="231" t="s">
+      <c r="F408" s="106" t="s">
         <v>307</v>
       </c>
-      <c r="G408" s="224">
+      <c r="G408" s="1">
         <v>5013</v>
       </c>
-      <c r="H408" s="225" t="s">
+      <c r="H408" s="22" t="s">
         <v>469</v>
       </c>
-      <c r="I408" s="223"/>
-      <c r="J408" s="226">
+      <c r="J408" s="186">
         <v>125</v>
       </c>
       <c r="K408" s="209"/>
@@ -36353,11 +36355,8 @@
         <f>ROW()</f>
         <v>408</v>
       </c>
-      <c r="M408" s="223"/>
-    </row>
-    <row r="409" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A409" s="223"/>
-      <c r="B409" s="223"/>
+    </row>
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="409">
       <c r="C409" s="42">
         <v>73</v>
       </c>
@@ -36367,185 +36366,428 @@
       <c r="E409" s="216">
         <v>73</v>
       </c>
-      <c r="F409" s="232" t="s">
+      <c r="F409" s="221" t="s">
         <v>307</v>
       </c>
       <c r="G409" s="210"/>
-      <c r="H409" s="219" t="s">
+      <c r="H409" s="222" t="s">
         <v>64</v>
       </c>
-      <c r="I409" s="219"/>
-      <c r="J409" s="219"/>
-      <c r="K409" s="220"/>
+      <c r="I409" s="222"/>
+      <c r="J409" s="222"/>
+      <c r="K409" s="223"/>
       <c r="L409" s="42">
         <f>ROW()</f>
         <v>409</v>
       </c>
-      <c r="M409" s="223"/>
-    </row>
-    <row r="410" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A410" s="223"/>
-      <c r="B410" s="223"/>
+    </row>
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="410">
       <c r="C410" s="42">
         <v>73</v>
       </c>
-      <c r="D410" s="233">
+      <c r="D410" s="217">
         <v>45294</v>
       </c>
-      <c r="E410" s="230">
+      <c r="E410" s="71">
         <v>73</v>
       </c>
-      <c r="F410" s="231" t="s">
+      <c r="F410" s="106" t="s">
         <v>307</v>
       </c>
-      <c r="G410" s="224"/>
-      <c r="H410" s="223"/>
-      <c r="I410" s="223"/>
-      <c r="J410" s="223"/>
-      <c r="K410" s="223"/>
       <c r="L410" s="42">
         <f>ROW()</f>
         <v>410</v>
       </c>
-      <c r="M410" s="223"/>
-    </row>
-    <row r="411" spans="1:13" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C411" s="224"/>
-      <c r="E411" s="224"/>
-      <c r="G411" s="224"/>
-    </row>
-    <row r="412" spans="1:13" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C412" s="224"/>
-      <c r="E412" s="224"/>
-      <c r="G412" s="224"/>
-    </row>
-    <row r="413" spans="1:13" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C413" s="224"/>
-      <c r="E413" s="224"/>
-      <c r="G413" s="224"/>
-    </row>
-    <row r="414" spans="1:13" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C414" s="224"/>
-      <c r="E414" s="224"/>
-      <c r="G414" s="224"/>
-    </row>
-    <row r="415" spans="1:13" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C415" s="224"/>
-      <c r="E415" s="224"/>
-      <c r="G415" s="224"/>
-    </row>
-    <row r="416" spans="1:13" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C416" s="224"/>
-      <c r="E416" s="224"/>
-      <c r="G416" s="224"/>
-    </row>
-    <row r="417" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C417" s="224"/>
-      <c r="E417" s="224"/>
-      <c r="G417" s="224"/>
-    </row>
-    <row r="418" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C418" s="224"/>
-      <c r="E418" s="224"/>
-      <c r="G418" s="224"/>
-    </row>
-    <row r="419" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C419" s="224"/>
-      <c r="E419" s="224"/>
-      <c r="G419" s="224"/>
-    </row>
-    <row r="420" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C420" s="224"/>
-      <c r="E420" s="224"/>
-      <c r="G420" s="224"/>
-    </row>
-    <row r="421" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C421" s="224"/>
-      <c r="E421" s="224"/>
-      <c r="G421" s="224"/>
-    </row>
-    <row r="422" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C422" s="224"/>
-      <c r="E422" s="224"/>
-      <c r="G422" s="224"/>
-    </row>
-    <row r="423" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C423" s="224"/>
-      <c r="E423" s="224"/>
-      <c r="G423" s="224"/>
-    </row>
-    <row r="424" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C424" s="224"/>
-      <c r="E424" s="224"/>
-      <c r="G424" s="224"/>
-    </row>
-    <row r="425" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C425" s="224"/>
-      <c r="E425" s="224"/>
-      <c r="G425" s="224"/>
-    </row>
-    <row r="426" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C426" s="224"/>
-      <c r="E426" s="224"/>
-      <c r="G426" s="224"/>
-    </row>
-    <row r="427" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C427" s="224"/>
-      <c r="E427" s="224"/>
-      <c r="G427" s="224"/>
-    </row>
-    <row r="428" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C428" s="224"/>
-      <c r="E428" s="224"/>
-      <c r="G428" s="224"/>
-    </row>
-    <row r="429" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C429" s="224"/>
-      <c r="E429" s="224"/>
-      <c r="G429" s="224"/>
-    </row>
-    <row r="430" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C430" s="224"/>
-      <c r="E430" s="224"/>
-      <c r="G430" s="224"/>
-    </row>
-    <row r="431" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C431" s="224"/>
-      <c r="E431" s="224"/>
-      <c r="G431" s="224"/>
-    </row>
-    <row r="432" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C432" s="224"/>
-      <c r="E432" s="224"/>
-      <c r="G432" s="224"/>
-    </row>
-    <row r="433" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C433" s="224"/>
-      <c r="E433" s="224"/>
-      <c r="G433" s="224"/>
-    </row>
-    <row r="434" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C434" s="224"/>
-      <c r="E434" s="224"/>
-      <c r="G434" s="224"/>
-    </row>
-    <row r="435" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C435" s="224"/>
-      <c r="E435" s="224"/>
-      <c r="G435" s="224"/>
-    </row>
-    <row r="436" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C436" s="224"/>
-      <c r="E436" s="224"/>
-      <c r="G436" s="224"/>
-    </row>
-    <row r="437" spans="3:7" s="223" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C437" s="224"/>
-      <c r="E437" s="224"/>
-      <c r="G437" s="224"/>
+    </row>
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="411">
+      <c r="C411" s="42">
+        <v>74</v>
+      </c>
+      <c r="D411" s="218">
+        <v>45296</v>
+      </c>
+      <c r="E411" s="157">
+        <v>74</v>
+      </c>
+      <c r="F411" s="157" t="s">
+        <v>64</v>
+      </c>
+      <c r="G411" s="157" t="s">
+        <v>401</v>
+      </c>
+      <c r="H411" s="157" t="s">
+        <v>399</v>
+      </c>
+      <c r="I411" s="187">
+        <v>100</v>
+      </c>
+      <c r="J411" s="159"/>
+      <c r="K411" s="174"/>
+      <c r="L411" s="42">
+        <f>ROW()</f>
+        <v>411</v>
+      </c>
+    </row>
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="412">
+      <c r="C412" s="42">
+        <v>74</v>
+      </c>
+      <c r="D412" s="229">
+        <v>45296</v>
+      </c>
+      <c r="E412" s="230">
+        <v>74</v>
+      </c>
+      <c r="F412" s="230" t="s">
+        <v>64</v>
+      </c>
+      <c r="G412" s="226" t="s">
+        <v>468</v>
+      </c>
+      <c r="H412" s="226" t="s">
+        <v>469</v>
+      </c>
+      <c r="I412" s="227"/>
+      <c r="J412" s="186">
+        <v>25</v>
+      </c>
+      <c r="K412" s="228" t="s">
+        <v>533</v>
+      </c>
+      <c r="L412" s="42">
+        <f>ROW()</f>
+        <v>412</v>
+      </c>
+    </row>
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="413">
+      <c r="C413" s="42">
+        <v>74</v>
+      </c>
+      <c r="D413" s="229">
+        <v>45296</v>
+      </c>
+      <c r="E413" s="230">
+        <v>74</v>
+      </c>
+      <c r="F413" s="230" t="s">
+        <v>64</v>
+      </c>
+      <c r="G413" s="226" t="s">
+        <v>468</v>
+      </c>
+      <c r="H413" s="226" t="s">
+        <v>469</v>
+      </c>
+      <c r="I413" s="227"/>
+      <c r="J413" s="186">
+        <v>25</v>
+      </c>
+      <c r="K413" s="228" t="s">
+        <v>534</v>
+      </c>
+      <c r="L413" s="42">
+        <f>ROW()</f>
+        <v>413</v>
+      </c>
+    </row>
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="414">
+      <c r="C414" s="42">
+        <v>74</v>
+      </c>
+      <c r="D414" s="229">
+        <v>45296</v>
+      </c>
+      <c r="E414" s="230">
+        <v>74</v>
+      </c>
+      <c r="F414" s="230" t="s">
+        <v>64</v>
+      </c>
+      <c r="G414" s="226" t="s">
+        <v>468</v>
+      </c>
+      <c r="H414" s="226" t="s">
+        <v>469</v>
+      </c>
+      <c r="I414" s="227"/>
+      <c r="J414" s="186">
+        <v>25</v>
+      </c>
+      <c r="K414" s="228" t="s">
+        <v>535</v>
+      </c>
+      <c r="L414" s="42">
+        <f>ROW()</f>
+        <v>414</v>
+      </c>
+    </row>
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="415">
+      <c r="C415" s="42">
+        <v>74</v>
+      </c>
+      <c r="D415" s="229">
+        <v>45296</v>
+      </c>
+      <c r="E415" s="230">
+        <v>74</v>
+      </c>
+      <c r="F415" s="230" t="s">
+        <v>64</v>
+      </c>
+      <c r="G415" s="226" t="s">
+        <v>468</v>
+      </c>
+      <c r="H415" s="226" t="s">
+        <v>469</v>
+      </c>
+      <c r="I415" s="227"/>
+      <c r="J415" s="186">
+        <v>25</v>
+      </c>
+      <c r="K415" s="228" t="s">
+        <v>536</v>
+      </c>
+      <c r="L415" s="42">
+        <f>ROW()</f>
+        <v>415</v>
+      </c>
+    </row>
+    <row spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3" outlineLevel="0" r="416">
+      <c r="C416" s="42">
+        <v>74</v>
+      </c>
+      <c r="D416" s="231">
+        <v>45296</v>
+      </c>
+      <c r="E416" s="202">
+        <v>74</v>
+      </c>
+      <c r="F416" s="202" t="s">
+        <v>64</v>
+      </c>
+      <c r="G416" s="183"/>
+      <c r="H416" s="222" t="s">
+        <v>537</v>
+      </c>
+      <c r="I416" s="222"/>
+      <c r="J416" s="222"/>
+      <c r="K416" s="223"/>
+      <c r="L416" s="42">
+        <f>ROW()</f>
+        <v>416</v>
+      </c>
+    </row>
+    <row spans="3:12" x14ac:dyDescent="0.25" outlineLevel="0" r="417">
+      <c r="C417" s="42">
+        <v>74</v>
+      </c>
+      <c r="D417" s="232">
+        <v>45296</v>
+      </c>
+      <c r="E417" s="230">
+        <v>74</v>
+      </c>
+      <c r="F417" s="230" t="s">
+        <v>64</v>
+      </c>
+      <c r="L417" s="42">
+        <f>ROW()</f>
+        <v>417</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="418">
+      <c r="C418" s="228">
+        <v>75</v>
+      </c>
+      <c r="D418" s="218">
+        <v>45296</v>
+      </c>
+      <c r="E418" s="228">
+        <v>75</v>
+      </c>
+      <c r="F418" s="228" t="inlineStr">
+        <is>
+          <t>TEST # 2</t>
+        </is>
+      </c>
+      <c r="G418" s="228" t="inlineStr">
+        <is>
+          <t>5013</t>
+        </is>
+      </c>
+      <c r="H418" s="228" t="inlineStr">
+        <is>
+          <t>Frais financiers</t>
+        </is>
+      </c>
+      <c r="I418" s="23">
+        <v>25</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="419">
+      <c r="C419" s="228">
+        <v>75</v>
+      </c>
+      <c r="D419" s="218">
+        <v>45296</v>
+      </c>
+      <c r="E419" s="228">
+        <v>75</v>
+      </c>
+      <c r="F419" s="228" t="inlineStr">
+        <is>
+          <t>TEST # 2</t>
+        </is>
+      </c>
+      <c r="G419" s="228" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H419" s="228" t="inlineStr">
+        <is>
+          <t>Encaisse</t>
+        </is>
+      </c>
+      <c r="J419" s="23">
+        <v>25</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="420">
+      <c r="C420" s="228">
+        <v>75</v>
+      </c>
+      <c r="D420" s="218">
+        <v>45296</v>
+      </c>
+      <c r="E420" s="228">
+        <v>75</v>
+      </c>
+      <c r="F420" s="228" t="inlineStr">
+        <is>
+          <t>TEST # 2</t>
+        </is>
+      </c>
+      <c r="H420" s="228" t="inlineStr">
+        <is>
+          <t>Autre test requis</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="421">
+      <c r="C421" s="228">
+        <v>75</v>
+      </c>
+      <c r="D421" s="218">
+        <v>45296</v>
+      </c>
+      <c r="E421" s="228">
+        <v>75</v>
+      </c>
+      <c r="F421" s="228" t="inlineStr">
+        <is>
+          <t>TEST # 2</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="422">
+      <c r="C422" s="228">
+        <v>76</v>
+      </c>
+      <c r="D422" s="218">
+        <v>45291</v>
+      </c>
+      <c r="E422" s="228">
+        <v>76</v>
+      </c>
+      <c r="F422" s="228" t="inlineStr">
+        <is>
+          <t>Test # 3</t>
+        </is>
+      </c>
+      <c r="G422" s="228" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H422" s="228" t="inlineStr">
+        <is>
+          <t>Encaisse</t>
+        </is>
+      </c>
+      <c r="I422" s="23">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="423">
+      <c r="C423" s="228">
+        <v>76</v>
+      </c>
+      <c r="D423" s="218">
+        <v>45291</v>
+      </c>
+      <c r="E423" s="228">
+        <v>76</v>
+      </c>
+      <c r="F423" s="228" t="inlineStr">
+        <is>
+          <t>Test # 3</t>
+        </is>
+      </c>
+      <c r="G423" s="228" t="inlineStr">
+        <is>
+          <t>5013</t>
+        </is>
+      </c>
+      <c r="H423" s="228" t="inlineStr">
+        <is>
+          <t>Frais financiers</t>
+        </is>
+      </c>
+      <c r="J423" s="23">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="424">
+      <c r="C424" s="228">
+        <v>76</v>
+      </c>
+      <c r="D424" s="218">
+        <v>45291</v>
+      </c>
+      <c r="E424" s="228">
+        <v>76</v>
+      </c>
+      <c r="F424" s="228" t="inlineStr">
+        <is>
+          <t>Test # 3</t>
+        </is>
+      </c>
+      <c r="H424" s="228" t="inlineStr">
+        <is>
+          <t>Test en date du 31 décembre 2023</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="425">
+      <c r="C425" s="228">
+        <v>76</v>
+      </c>
+      <c r="D425" s="218">
+        <v>45291</v>
+      </c>
+      <c r="E425" s="228">
+        <v>76</v>
+      </c>
+      <c r="F425" s="228" t="inlineStr">
+        <is>
+          <t>Test # 3</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="H416:K416"/>
     <mergeCell ref="H409:K409"/>
     <mergeCell ref="H372:K372"/>
     <mergeCell ref="H381:K381"/>

</xml_diff>

<commit_message>
2024-01-10 - Avant de quitter en vacances
Fonctionnement du menu "MENU"
Ajout de l'option EXIT sur menu principal
Sortie contrôlée de l'application
Ménage
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B32BC38-3A1A-4713-890F-56EA820542C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8126002-B040-431B-B802-EAEF607A236A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2392" uniqueCount="566">
   <si>
     <t>TEC_ID</t>
   </si>
@@ -1734,6 +1734,24 @@
   </si>
   <si>
     <t>Entrée manuelle pour double vérifier mes tests</t>
+  </si>
+  <si>
+    <t>Après import du plan comptable</t>
+  </si>
+  <si>
+    <t>5007b</t>
+  </si>
+  <si>
+    <t>Électricité - B</t>
+  </si>
+  <si>
+    <t>Tests après ménage dans les NamedRanges</t>
+  </si>
+  <si>
+    <t>5006a</t>
+  </si>
+  <si>
+    <t>Logiciel informatiques</t>
   </si>
 </sst>
 </file>
@@ -13814,10 +13832,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{E0D58006-DE1D-488F-9BB7-8096C5818030}">
-  <dimension ref="A1:K402"/>
+  <sheetPr codeName="Feuil3"/>
+  <dimension ref="A1:K408"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="J407" sqref="J407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25714,92 +25733,254 @@
         <v>399</v>
       </c>
     </row>
-    <row outlineLevel="0" r="400">
-      <c r="A400" s="87">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="400">
+      <c r="A400" s="48">
         <v>89</v>
       </c>
-      <c r="B400" s="86">
+      <c r="B400" s="22">
         <v>45299</v>
       </c>
-      <c r="C400" s="87">
+      <c r="C400" s="1">
         <v>89</v>
       </c>
-      <c r="D400" s="87" t="inlineStr">
+      <c r="D400" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E400" s="14" t="s">
+        <v>560</v>
+      </c>
+      <c r="F400" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="G400" s="14" t="s">
+        <v>562</v>
+      </c>
+      <c r="H400" s="24">
+        <v>45.98</v>
+      </c>
+      <c r="I400" s="24"/>
+      <c r="K400" s="48">
+        <f>ROW()</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="401">
+      <c r="A401" s="48">
+        <v>89</v>
+      </c>
+      <c r="B401" s="31">
+        <v>45299</v>
+      </c>
+      <c r="C401" s="32">
+        <v>89</v>
+      </c>
+      <c r="D401" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E401" s="32" t="s">
+        <v>560</v>
+      </c>
+      <c r="F401" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G401" s="14" t="s">
+        <v>432</v>
+      </c>
+      <c r="H401" s="24"/>
+      <c r="I401" s="24">
+        <v>45.98</v>
+      </c>
+      <c r="K401" s="48">
+        <f>ROW()</f>
+        <v>401</v>
+      </c>
+    </row>
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="402">
+      <c r="A402" s="48">
+        <v>89</v>
+      </c>
+      <c r="B402" s="31">
+        <v>45299</v>
+      </c>
+      <c r="C402" s="32">
+        <v>89</v>
+      </c>
+      <c r="D402" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E402" s="32" t="s">
+        <v>560</v>
+      </c>
+      <c r="F402" s="1"/>
+      <c r="H402" s="24"/>
+      <c r="I402" s="24"/>
+      <c r="K402" s="48">
+        <f>ROW()</f>
+        <v>402</v>
+      </c>
+    </row>
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="403">
+      <c r="A403" s="48">
+        <v>90</v>
+      </c>
+      <c r="B403" s="22">
+        <v>45300</v>
+      </c>
+      <c r="C403" s="1">
+        <v>90</v>
+      </c>
+      <c r="E403" s="14" t="s">
+        <v>563</v>
+      </c>
+      <c r="F403" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="G403" s="14" t="s">
+        <v>565</v>
+      </c>
+      <c r="H403" s="24">
+        <v>259.95</v>
+      </c>
+      <c r="I403" s="24"/>
+      <c r="K403" s="48">
+        <f>ROW()</f>
+        <v>403</v>
+      </c>
+    </row>
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="404">
+      <c r="A404" s="48">
+        <v>90</v>
+      </c>
+      <c r="B404" s="31">
+        <v>45300</v>
+      </c>
+      <c r="C404" s="33">
+        <v>90</v>
+      </c>
+      <c r="D404" s="42"/>
+      <c r="E404" s="33" t="s">
+        <v>563</v>
+      </c>
+      <c r="F404" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="G404" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="H404" s="24"/>
+      <c r="I404" s="24">
+        <v>259.95</v>
+      </c>
+      <c r="K404" s="48">
+        <f>ROW()</f>
+        <v>404</v>
+      </c>
+    </row>
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="405">
+      <c r="A405" s="48">
+        <v>90</v>
+      </c>
+      <c r="B405" s="31">
+        <v>45300</v>
+      </c>
+      <c r="C405" s="33">
+        <v>90</v>
+      </c>
+      <c r="D405" s="42"/>
+      <c r="E405" s="33" t="s">
+        <v>563</v>
+      </c>
+      <c r="K405" s="48">
+        <f>ROW()</f>
+        <v>405</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="406">
+      <c r="A406" s="87">
+        <v>91</v>
+      </c>
+      <c r="B406" s="86">
+        <v>45301</v>
+      </c>
+      <c r="C406" s="87">
+        <v>91</v>
+      </c>
+      <c r="D406" s="87" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>Test mercredi</t>
         </is>
       </c>
-      <c r="E400" s="87" t="inlineStr">
+      <c r="E406" s="87" t="inlineStr">
         <is>
-          <t>Après import du plan comptable</t>
+          <t>Ceci est la description de l'entrée de journal</t>
         </is>
       </c>
-      <c r="F400" s="87" t="inlineStr">
+      <c r="F406" s="87" t="inlineStr">
         <is>
-          <t>5007b</t>
+          <t>1000</t>
         </is>
       </c>
-      <c r="G400" s="87" t="inlineStr">
+      <c r="G406" s="87" t="inlineStr">
         <is>
-          <t>Électricité - B</t>
+          <t>Encaisse</t>
         </is>
       </c>
-      <c r="H400" s="84">
-        <v>45.98</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="401">
-      <c r="A401" s="87">
-        <v>89</v>
-      </c>
-      <c r="B401" s="86">
-        <v>45299</v>
-      </c>
-      <c r="C401" s="87">
-        <v>89</v>
-      </c>
-      <c r="D401" s="87" t="inlineStr">
+      <c r="H406" s="84">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="407">
+      <c r="A407" s="87">
+        <v>91</v>
+      </c>
+      <c r="B407" s="86">
+        <v>45301</v>
+      </c>
+      <c r="C407" s="87">
+        <v>91</v>
+      </c>
+      <c r="D407" s="87" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>Test mercredi</t>
         </is>
       </c>
-      <c r="E401" s="87" t="inlineStr">
+      <c r="E407" s="87" t="inlineStr">
         <is>
-          <t>Après import du plan comptable</t>
+          <t>Ceci est la description de l'entrée de journal</t>
         </is>
       </c>
-      <c r="F401" s="87" t="inlineStr">
+      <c r="F407" s="87" t="inlineStr">
         <is>
-          <t>1230</t>
+          <t>5008</t>
         </is>
       </c>
-      <c r="G401" s="87" t="inlineStr">
+      <c r="G407" s="87" t="inlineStr">
         <is>
-          <t>Frais payés d'avance</t>
+          <t>Frais de communications</t>
         </is>
       </c>
-      <c r="I401" s="84">
-        <v>45.98</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="402">
-      <c r="A402" s="87">
-        <v>89</v>
-      </c>
-      <c r="B402" s="86">
-        <v>45299</v>
-      </c>
-      <c r="C402" s="87">
-        <v>89</v>
-      </c>
-      <c r="D402" s="87" t="inlineStr">
+      <c r="I407" s="84">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="408">
+      <c r="A408" s="87">
+        <v>91</v>
+      </c>
+      <c r="B408" s="86">
+        <v>45301</v>
+      </c>
+      <c r="C408" s="87">
+        <v>91</v>
+      </c>
+      <c r="D408" s="87" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>Test mercredi</t>
         </is>
       </c>
-      <c r="E402" s="87" t="inlineStr">
+      <c r="E408" s="87" t="inlineStr">
         <is>
-          <t>Après import du plan comptable</t>
+          <t>Ceci est la description de l'entrée de journal</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
2024-02-07 @ 07:16 - v1.5
Ajustements au DynamicNamedRange
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8126002-B040-431B-B802-EAEF607A236A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02C7260-3139-4A84-9B49-599471976072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEC" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2392" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2406" uniqueCount="570">
   <si>
     <t>TEC_ID</t>
   </si>
@@ -1752,6 +1752,18 @@
   </si>
   <si>
     <t>Logiciel informatiques</t>
+  </si>
+  <si>
+    <t>Test suite aux modifications dans les autres modules</t>
+  </si>
+  <si>
+    <t>v1.4</t>
+  </si>
+  <si>
+    <t>Test mercredi</t>
+  </si>
+  <si>
+    <t>Ceci est la description de l'entrée de journal</t>
   </si>
 </sst>
 </file>
@@ -1854,7 +1866,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1876,6 +1888,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1993,7 +2011,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2228,12 +2246,22 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire 2" xfId="1" xr:uid="{7066D7D9-A0C5-4744-AD1B-CDB1C4228FB1}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2525,12 +2553,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:P247"/>
+  <dimension ref="A1:P248"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="600" topLeftCell="A230" activePane="bottomLeft"/>
       <selection sqref="A1:P1"/>
-      <selection pane="bottomLeft" activeCell="A248" sqref="A248:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="G252" sqref="G252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13026,9 +13054,56 @@
         <v>390</v>
       </c>
     </row>
+    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>248</v>
+      </c>
+      <c r="B248" s="1">
+        <v>1</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D248" s="78">
+        <v>45328</v>
+      </c>
+      <c r="E248" s="90"/>
+      <c r="F248" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G248" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="H248" s="84">
+        <v>2</v>
+      </c>
+      <c r="J248" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K248" s="81">
+        <v>45328.7430439815</v>
+      </c>
+      <c r="L248" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="N248" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="O248" s="14" t="s">
+        <v>567</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:P247">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+    <cfRule type="expression" priority="4">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A248:P248">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
     <cfRule type="expression" priority="2">
@@ -13819,7 +13894,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:T12">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
     <cfRule type="expression" priority="2">
@@ -13831,11 +13906,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{E0D58006-DE1D-488F-9BB7-8096C5818030}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D58006-DE1D-488F-9BB7-8096C5818030}">
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:K408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0" rightToLeft="false">
+    <sheetView topLeftCell="A385" workbookViewId="0">
       <selection activeCell="J407" sqref="J407"/>
     </sheetView>
   </sheetViews>
@@ -13852,7 +13927,7 @@
     <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:11" ht="25.5" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>531</v>
       </c>
@@ -13887,7 +13962,7 @@
         <v>397</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="48">
         <v>1</v>
       </c>
@@ -13919,7 +13994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row spans="1:11" ht="15.75" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="48">
         <v>1</v>
       </c>
@@ -13951,7 +14026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="48">
         <v>1</v>
       </c>
@@ -13972,7 +14047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="48">
         <v>2</v>
       </c>
@@ -14004,7 +14079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="48">
         <v>2</v>
       </c>
@@ -14036,7 +14111,7 @@
         <v>6</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="48">
         <v>2</v>
       </c>
@@ -14055,7 +14130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="48">
         <v>3</v>
       </c>
@@ -14087,7 +14162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="48">
         <v>3</v>
       </c>
@@ -14119,7 +14194,7 @@
         <v>9</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48">
         <v>3</v>
       </c>
@@ -14139,7 +14214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="48">
         <v>4</v>
       </c>
@@ -14171,7 +14246,7 @@
         <v>11</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="48">
         <v>4</v>
       </c>
@@ -14203,7 +14278,7 @@
         <v>12</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="13">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="48">
         <v>4</v>
       </c>
@@ -14226,7 +14301,7 @@
         <v>415</v>
       </c>
       <c r="H13" s="24">
-        <v>570.92</v>
+        <v>570.91999999999996</v>
       </c>
       <c r="I13" s="24"/>
       <c r="J13" s="14"/>
@@ -14235,7 +14310,7 @@
         <v>13</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="14">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
         <v>4</v>
       </c>
@@ -14267,7 +14342,7 @@
         <v>14</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="48">
         <v>4</v>
       </c>
@@ -14299,7 +14374,7 @@
         <v>15</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="16">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="48">
         <v>4</v>
       </c>
@@ -14323,7 +14398,7 @@
         <v>16</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="17">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="48">
         <v>5</v>
       </c>
@@ -14355,7 +14430,7 @@
         <v>17</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="18">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="48">
         <v>5</v>
       </c>
@@ -14387,7 +14462,7 @@
         <v>18</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="19">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="48">
         <v>5</v>
       </c>
@@ -14419,7 +14494,7 @@
         <v>19</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="20">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="48">
         <v>5</v>
       </c>
@@ -14451,7 +14526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="21">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="48">
         <v>5</v>
       </c>
@@ -14483,7 +14558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="22">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="48">
         <v>5</v>
       </c>
@@ -14515,7 +14590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="23">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="48">
         <v>5</v>
       </c>
@@ -14547,7 +14622,7 @@
         <v>23</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="24">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="48">
         <v>5</v>
       </c>
@@ -14579,7 +14654,7 @@
         <v>24</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="48">
         <v>5</v>
       </c>
@@ -14603,7 +14678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="26">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="48">
         <v>6</v>
       </c>
@@ -14635,7 +14710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="27">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="48">
         <v>6</v>
       </c>
@@ -14667,7 +14742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="28">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="48">
         <v>6</v>
       </c>
@@ -14699,7 +14774,7 @@
         <v>28</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="29">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="48">
         <v>6</v>
       </c>
@@ -14731,7 +14806,7 @@
         <v>29</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="30">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="48">
         <v>6</v>
       </c>
@@ -14763,7 +14838,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="31">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="48">
         <v>6</v>
       </c>
@@ -14795,7 +14870,7 @@
         <v>31</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="32">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="48">
         <v>6</v>
       </c>
@@ -14827,7 +14902,7 @@
         <v>32</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="33">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="48">
         <v>6</v>
       </c>
@@ -14859,7 +14934,7 @@
         <v>33</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="34">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="48">
         <v>6</v>
       </c>
@@ -14883,7 +14958,7 @@
         <v>34</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="48">
         <v>7</v>
       </c>
@@ -14915,7 +14990,7 @@
         <v>35</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="36">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="48">
         <v>7</v>
       </c>
@@ -14947,7 +15022,7 @@
         <v>36</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="37">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="48">
         <v>7</v>
       </c>
@@ -14979,7 +15054,7 @@
         <v>37</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="38">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="48">
         <v>7</v>
       </c>
@@ -15011,7 +15086,7 @@
         <v>38</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="39">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="48">
         <v>7</v>
       </c>
@@ -15043,7 +15118,7 @@
         <v>39</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="40">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="48">
         <v>7</v>
       </c>
@@ -15075,7 +15150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="41">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="48">
         <v>7</v>
       </c>
@@ -15099,7 +15174,7 @@
       </c>
       <c r="H41" s="24"/>
       <c r="I41" s="24">
-        <v>67.68</v>
+        <v>67.680000000000007</v>
       </c>
       <c r="J41" s="14"/>
       <c r="K41" s="48">
@@ -15107,7 +15182,7 @@
         <v>41</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="42">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="48">
         <v>7</v>
       </c>
@@ -15139,7 +15214,7 @@
         <v>42</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="43">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="48">
         <v>7</v>
       </c>
@@ -15163,7 +15238,7 @@
         <v>43</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="44">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="48">
         <v>8</v>
       </c>
@@ -15186,7 +15261,7 @@
         <v>402</v>
       </c>
       <c r="H44" s="24">
-        <v>1248.63</v>
+        <v>1248.6300000000001</v>
       </c>
       <c r="I44" s="24"/>
       <c r="J44" s="14"/>
@@ -15195,7 +15270,7 @@
         <v>44</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="48">
         <v>8</v>
       </c>
@@ -15227,7 +15302,7 @@
         <v>45</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="46">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="48">
         <v>8</v>
       </c>
@@ -15259,7 +15334,7 @@
         <v>46</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="47">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="48">
         <v>8</v>
       </c>
@@ -15291,7 +15366,7 @@
         <v>47</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="48">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="48">
         <v>8</v>
       </c>
@@ -15323,7 +15398,7 @@
         <v>48</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="49">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="48">
         <v>8</v>
       </c>
@@ -15355,7 +15430,7 @@
         <v>49</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="50">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="48">
         <v>8</v>
       </c>
@@ -15387,7 +15462,7 @@
         <v>50</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="51">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="48">
         <v>8</v>
       </c>
@@ -15411,7 +15486,7 @@
         <v>51</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="52">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="48">
         <v>9</v>
       </c>
@@ -15434,7 +15509,7 @@
         <v>399</v>
       </c>
       <c r="H52" s="24">
-        <v>1248.63</v>
+        <v>1248.6300000000001</v>
       </c>
       <c r="I52" s="24"/>
       <c r="J52" s="14"/>
@@ -15443,7 +15518,7 @@
         <v>52</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="53">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="48">
         <v>9</v>
       </c>
@@ -15467,7 +15542,7 @@
       </c>
       <c r="H53" s="24"/>
       <c r="I53" s="24">
-        <v>1248.63</v>
+        <v>1248.6300000000001</v>
       </c>
       <c r="J53" s="14"/>
       <c r="K53" s="48">
@@ -15475,7 +15550,7 @@
         <v>53</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="54">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="48">
         <v>9</v>
       </c>
@@ -15499,7 +15574,7 @@
         <v>54</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="55">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="48">
         <v>10</v>
       </c>
@@ -15531,7 +15606,7 @@
         <v>55</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="56">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="48">
         <v>10</v>
       </c>
@@ -15563,7 +15638,7 @@
         <v>56</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="57">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="48">
         <v>10</v>
       </c>
@@ -15581,7 +15656,7 @@
         <v>67</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="58">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="48">
         <v>11</v>
       </c>
@@ -15613,7 +15688,7 @@
         <v>58</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="59">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="48">
         <v>11</v>
       </c>
@@ -15645,7 +15720,7 @@
         <v>59</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="60">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="48">
         <v>11</v>
       </c>
@@ -15669,7 +15744,7 @@
         <v>60</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="61">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="48">
         <v>12</v>
       </c>
@@ -15698,7 +15773,7 @@
         <v>61</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="62">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="48">
         <v>12</v>
       </c>
@@ -15728,7 +15803,7 @@
         <v>62</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="63">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="48">
         <v>12</v>
       </c>
@@ -15758,7 +15833,7 @@
         <v>63</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="64">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="48">
         <v>12</v>
       </c>
@@ -15780,7 +15855,7 @@
       </c>
       <c r="H64" s="24"/>
       <c r="I64" s="24">
-        <v>4585.4</v>
+        <v>4585.3999999999996</v>
       </c>
       <c r="J64" s="14"/>
       <c r="K64" s="48">
@@ -15788,7 +15863,7 @@
         <v>64</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="65">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="48">
         <v>12</v>
       </c>
@@ -15810,7 +15885,7 @@
         <v>65</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="66">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="48">
         <v>13</v>
       </c>
@@ -15842,7 +15917,7 @@
         <v>66</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="67">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="48">
         <v>13</v>
       </c>
@@ -15874,7 +15949,7 @@
         <v>67</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="68">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="48">
         <v>13</v>
       </c>
@@ -15906,7 +15981,7 @@
         <v>68</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="69">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="48">
         <v>13</v>
       </c>
@@ -15938,7 +16013,7 @@
         <v>69</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="70">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="48">
         <v>13</v>
       </c>
@@ -15962,7 +16037,7 @@
         <v>70</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="71">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="48">
         <v>14</v>
       </c>
@@ -15985,7 +16060,7 @@
         <v>402</v>
       </c>
       <c r="H71" s="24">
-        <v>1034.91</v>
+        <v>1034.9100000000001</v>
       </c>
       <c r="I71" s="24"/>
       <c r="J71" s="14"/>
@@ -15994,7 +16069,7 @@
         <v>71</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="72">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="48">
         <v>14</v>
       </c>
@@ -16026,7 +16101,7 @@
         <v>72</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="73">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="48">
         <v>14</v>
       </c>
@@ -16050,7 +16125,7 @@
       </c>
       <c r="H73" s="24"/>
       <c r="I73" s="24">
-        <v>153.73</v>
+        <v>153.72999999999999</v>
       </c>
       <c r="J73" s="14"/>
       <c r="K73" s="48">
@@ -16058,7 +16133,7 @@
         <v>73</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="74">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="48">
         <v>14</v>
       </c>
@@ -16090,7 +16165,7 @@
         <v>74</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="75">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="48">
         <v>14</v>
       </c>
@@ -16122,7 +16197,7 @@
         <v>75</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="76">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="48">
         <v>14</v>
       </c>
@@ -16154,7 +16229,7 @@
         <v>76</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="77">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="48">
         <v>14</v>
       </c>
@@ -16186,7 +16261,7 @@
         <v>77</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="78">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="48">
         <v>14</v>
       </c>
@@ -16218,7 +16293,7 @@
         <v>78</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="79">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="48">
         <v>14</v>
       </c>
@@ -16242,7 +16317,7 @@
         <v>79</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="80">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="48">
         <v>15</v>
       </c>
@@ -16274,7 +16349,7 @@
         <v>80</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="81">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="48">
         <v>15</v>
       </c>
@@ -16306,7 +16381,7 @@
         <v>81</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="82">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="48">
         <v>15</v>
       </c>
@@ -16338,7 +16413,7 @@
         <v>82</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="83">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="48">
         <v>15</v>
       </c>
@@ -16370,7 +16445,7 @@
         <v>83</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="84">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="48">
         <v>15</v>
       </c>
@@ -16402,7 +16477,7 @@
         <v>84</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="85">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="48">
         <v>15</v>
       </c>
@@ -16434,7 +16509,7 @@
         <v>85</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="86">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="48">
         <v>15</v>
       </c>
@@ -16466,7 +16541,7 @@
         <v>86</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="87">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="48">
         <v>15</v>
       </c>
@@ -16500,7 +16575,7 @@
         <v>87</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="88">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="48">
         <v>15</v>
       </c>
@@ -16524,7 +16599,7 @@
         <v>88</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="89">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="48">
         <v>16</v>
       </c>
@@ -16547,7 +16622,7 @@
         <v>399</v>
       </c>
       <c r="H89" s="24">
-        <v>1034.91</v>
+        <v>1034.9100000000001</v>
       </c>
       <c r="I89" s="24"/>
       <c r="J89" s="14"/>
@@ -16556,7 +16631,7 @@
         <v>89</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="90">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="48">
         <v>16</v>
       </c>
@@ -16580,7 +16655,7 @@
       </c>
       <c r="H90" s="24"/>
       <c r="I90" s="24">
-        <v>1034.91</v>
+        <v>1034.9100000000001</v>
       </c>
       <c r="J90" s="14"/>
       <c r="K90" s="48">
@@ -16588,7 +16663,7 @@
         <v>90</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="91">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="48">
         <v>16</v>
       </c>
@@ -16612,7 +16687,7 @@
         <v>91</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="92">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="48">
         <v>17</v>
       </c>
@@ -16646,7 +16721,7 @@
         <v>92</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="93">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="48">
         <v>17</v>
       </c>
@@ -16680,7 +16755,7 @@
         <v>93</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="94">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="48">
         <v>17</v>
       </c>
@@ -16704,7 +16779,7 @@
         <v>94</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="95">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="48">
         <v>18</v>
       </c>
@@ -16736,7 +16811,7 @@
         <v>95</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="96">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="48">
         <v>18</v>
       </c>
@@ -16768,7 +16843,7 @@
         <v>96</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="97">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="48">
         <v>18</v>
       </c>
@@ -16800,7 +16875,7 @@
         <v>97</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="98">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="48">
         <v>18</v>
       </c>
@@ -16832,7 +16907,7 @@
         <v>98</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="99">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="48">
         <v>18</v>
       </c>
@@ -16856,7 +16931,7 @@
         <v>99</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="100">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="48">
         <v>19</v>
       </c>
@@ -16888,7 +16963,7 @@
         <v>100</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="101">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="48">
         <v>19</v>
       </c>
@@ -16920,7 +16995,7 @@
         <v>101</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="102">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="48">
         <v>19</v>
       </c>
@@ -16944,7 +17019,7 @@
         <v>102</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="103">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="48">
         <v>20</v>
       </c>
@@ -16976,7 +17051,7 @@
         <v>103</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="104">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="48">
         <v>20</v>
       </c>
@@ -17008,7 +17083,7 @@
         <v>104</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="105">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="48">
         <v>20</v>
       </c>
@@ -17032,7 +17107,7 @@
         <v>105</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="106">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="48">
         <v>21</v>
       </c>
@@ -17064,7 +17139,7 @@
         <v>106</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="107">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="48">
         <v>21</v>
       </c>
@@ -17096,7 +17171,7 @@
         <v>107</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="108">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="48">
         <v>21</v>
       </c>
@@ -17120,7 +17195,7 @@
         <v>108</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="109">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="48">
         <v>22</v>
       </c>
@@ -17154,7 +17229,7 @@
         <v>109</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="110">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="48">
         <v>22</v>
       </c>
@@ -17186,7 +17261,7 @@
         <v>110</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="111">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="48">
         <v>22</v>
       </c>
@@ -17210,7 +17285,7 @@
         <v>111</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="112">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="48">
         <v>23</v>
       </c>
@@ -17233,7 +17308,7 @@
         <v>399</v>
       </c>
       <c r="H112" s="24">
-        <v>159.95</v>
+        <v>159.94999999999999</v>
       </c>
       <c r="I112" s="24"/>
       <c r="J112" s="14"/>
@@ -17242,7 +17317,7 @@
         <v>112</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="113">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="48">
         <v>23</v>
       </c>
@@ -17266,7 +17341,7 @@
       </c>
       <c r="H113" s="24"/>
       <c r="I113" s="24">
-        <v>149.95</v>
+        <v>149.94999999999999</v>
       </c>
       <c r="J113" s="14"/>
       <c r="K113" s="48">
@@ -17274,7 +17349,7 @@
         <v>113</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="114">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="48">
         <v>23</v>
       </c>
@@ -17306,7 +17381,7 @@
         <v>114</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="115">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="48">
         <v>23</v>
       </c>
@@ -17338,7 +17413,7 @@
         <v>115</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="116">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="48">
         <v>23</v>
       </c>
@@ -17362,7 +17437,7 @@
         <v>116</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="117">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="48">
         <v>24</v>
       </c>
@@ -17394,7 +17469,7 @@
         <v>117</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="118">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="48">
         <v>24</v>
       </c>
@@ -17426,7 +17501,7 @@
         <v>118</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="119">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="48">
         <v>24</v>
       </c>
@@ -17450,7 +17525,7 @@
         <v>119</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="120">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="48">
         <v>25</v>
       </c>
@@ -17482,7 +17557,7 @@
         <v>120</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="121">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="48">
         <v>25</v>
       </c>
@@ -17514,7 +17589,7 @@
         <v>121</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="122">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="48">
         <v>25</v>
       </c>
@@ -17538,7 +17613,7 @@
         <v>122</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="123">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="48">
         <v>26</v>
       </c>
@@ -17570,7 +17645,7 @@
         <v>123</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="124">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="48">
         <v>26</v>
       </c>
@@ -17602,7 +17677,7 @@
         <v>124</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="125">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="48">
         <v>26</v>
       </c>
@@ -17626,7 +17701,7 @@
         <v>125</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="126">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="48">
         <v>27</v>
       </c>
@@ -17658,7 +17733,7 @@
         <v>126</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="127">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="48">
         <v>27</v>
       </c>
@@ -17690,7 +17765,7 @@
         <v>127</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="128">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="48">
         <v>27</v>
       </c>
@@ -17714,7 +17789,7 @@
         <v>128</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="129">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="48">
         <v>28</v>
       </c>
@@ -17746,7 +17821,7 @@
         <v>129</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="130">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="48">
         <v>28</v>
       </c>
@@ -17778,7 +17853,7 @@
         <v>130</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="131">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="48">
         <v>28</v>
       </c>
@@ -17802,7 +17877,7 @@
         <v>131</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="132">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="48">
         <v>29</v>
       </c>
@@ -17825,7 +17900,7 @@
         <v>402</v>
       </c>
       <c r="H132" s="24">
-        <v>2157.07</v>
+        <v>2157.0700000000002</v>
       </c>
       <c r="I132" s="24"/>
       <c r="J132" s="14"/>
@@ -17834,7 +17909,7 @@
         <v>132</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="133">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="48">
         <v>29</v>
       </c>
@@ -17866,7 +17941,7 @@
         <v>133</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="134">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="48">
         <v>29</v>
       </c>
@@ -17898,7 +17973,7 @@
         <v>134</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="135">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="48">
         <v>29</v>
       </c>
@@ -17930,7 +18005,7 @@
         <v>135</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="136">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="48">
         <v>29</v>
       </c>
@@ -17962,7 +18037,7 @@
         <v>136</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="137">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="48">
         <v>29</v>
       </c>
@@ -17994,7 +18069,7 @@
         <v>137</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="138">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="48">
         <v>29</v>
       </c>
@@ -18026,7 +18101,7 @@
         <v>138</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="139">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="48">
         <v>29</v>
       </c>
@@ -18058,7 +18133,7 @@
         <v>139</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="140">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="48">
         <v>29</v>
       </c>
@@ -18082,7 +18157,7 @@
         <v>140</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="141">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="48">
         <v>30</v>
       </c>
@@ -18114,7 +18189,7 @@
         <v>141</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="142">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="48">
         <v>30</v>
       </c>
@@ -18146,7 +18221,7 @@
         <v>142</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="143">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="48">
         <v>30</v>
       </c>
@@ -18178,7 +18253,7 @@
         <v>143</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="144">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="48">
         <v>30</v>
       </c>
@@ -18210,7 +18285,7 @@
         <v>144</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="145">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="48">
         <v>30</v>
       </c>
@@ -18242,7 +18317,7 @@
         <v>145</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="146">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="48">
         <v>30</v>
       </c>
@@ -18274,7 +18349,7 @@
         <v>146</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="147">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="48">
         <v>30</v>
       </c>
@@ -18306,7 +18381,7 @@
         <v>147</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="148">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="48">
         <v>30</v>
       </c>
@@ -18338,7 +18413,7 @@
         <v>148</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="149">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="48">
         <v>30</v>
       </c>
@@ -18362,7 +18437,7 @@
         <v>149</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="150">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="48">
         <v>31</v>
       </c>
@@ -18394,7 +18469,7 @@
         <v>150</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="151">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="48">
         <v>31</v>
       </c>
@@ -18426,7 +18501,7 @@
         <v>151</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="152">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="48">
         <v>31</v>
       </c>
@@ -18450,7 +18525,7 @@
         <v>152</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="153">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="48">
         <v>32</v>
       </c>
@@ -18482,7 +18557,7 @@
         <v>153</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="154">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="48">
         <v>32</v>
       </c>
@@ -18514,7 +18589,7 @@
         <v>154</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="155">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="48">
         <v>32</v>
       </c>
@@ -18538,7 +18613,7 @@
         <v>155</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="156">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="48">
         <v>33</v>
       </c>
@@ -18570,7 +18645,7 @@
         <v>156</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="157">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="48">
         <v>33</v>
       </c>
@@ -18604,7 +18679,7 @@
         <v>157</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="158">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="48">
         <v>33</v>
       </c>
@@ -18628,7 +18703,7 @@
         <v>158</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="159">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="48">
         <v>34</v>
       </c>
@@ -18660,7 +18735,7 @@
         <v>159</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="160">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="48">
         <v>34</v>
       </c>
@@ -18692,7 +18767,7 @@
         <v>160</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="161">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="48">
         <v>34</v>
       </c>
@@ -18716,7 +18791,7 @@
         <v>161</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="162">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="48">
         <v>35</v>
       </c>
@@ -18748,7 +18823,7 @@
         <v>162</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="163">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="48">
         <v>35</v>
       </c>
@@ -18780,7 +18855,7 @@
         <v>163</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="164">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="48">
         <v>35</v>
       </c>
@@ -18804,7 +18879,7 @@
         <v>164</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="165">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="48">
         <v>36</v>
       </c>
@@ -18833,7 +18908,7 @@
         <v>165</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="166">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="48">
         <v>36</v>
       </c>
@@ -18863,7 +18938,7 @@
         <v>166</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="167">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="48">
         <v>36</v>
       </c>
@@ -18885,7 +18960,7 @@
         <v>167</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="168">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="48">
         <v>37</v>
       </c>
@@ -18917,7 +18992,7 @@
         <v>168</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="169">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="48">
         <v>37</v>
       </c>
@@ -18949,7 +19024,7 @@
         <v>169</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="170">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="48">
         <v>37</v>
       </c>
@@ -18973,7 +19048,7 @@
         <v>170</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="171">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="48">
         <v>38</v>
       </c>
@@ -19005,7 +19080,7 @@
         <v>171</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="172">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="48">
         <v>38</v>
       </c>
@@ -19037,7 +19112,7 @@
         <v>172</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="173">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="48">
         <v>38</v>
       </c>
@@ -19061,7 +19136,7 @@
         <v>173</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="174">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="48">
         <v>39</v>
       </c>
@@ -19093,7 +19168,7 @@
         <v>174</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="175">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="48">
         <v>39</v>
       </c>
@@ -19125,7 +19200,7 @@
         <v>175</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="176">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="48">
         <v>39</v>
       </c>
@@ -19149,7 +19224,7 @@
         <v>176</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="177">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="48">
         <v>40</v>
       </c>
@@ -19181,7 +19256,7 @@
         <v>177</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="178">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="48">
         <v>40</v>
       </c>
@@ -19213,7 +19288,7 @@
         <v>178</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="179">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="48">
         <v>40</v>
       </c>
@@ -19237,7 +19312,7 @@
       </c>
       <c r="H179" s="24"/>
       <c r="I179" s="24">
-        <v>33.95</v>
+        <v>33.950000000000003</v>
       </c>
       <c r="J179" s="14"/>
       <c r="K179" s="48">
@@ -19245,7 +19320,7 @@
         <v>179</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="180">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="48">
         <v>40</v>
       </c>
@@ -19269,7 +19344,7 @@
         <v>180</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="181">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="48">
         <v>41</v>
       </c>
@@ -19301,7 +19376,7 @@
         <v>181</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="182">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="48">
         <v>41</v>
       </c>
@@ -19333,7 +19408,7 @@
         <v>182</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="183">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="48">
         <v>41</v>
       </c>
@@ -19357,7 +19432,7 @@
         <v>183</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="184">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="48">
         <v>42</v>
       </c>
@@ -19389,7 +19464,7 @@
         <v>184</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="185">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="48">
         <v>42</v>
       </c>
@@ -19421,7 +19496,7 @@
         <v>185</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="186">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="48">
         <v>42</v>
       </c>
@@ -19445,7 +19520,7 @@
         <v>186</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="187">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="48">
         <v>43</v>
       </c>
@@ -19477,7 +19552,7 @@
         <v>187</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="188">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="48">
         <v>43</v>
       </c>
@@ -19509,7 +19584,7 @@
         <v>188</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="189">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="48">
         <v>43</v>
       </c>
@@ -19533,7 +19608,7 @@
         <v>189</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="190">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="48">
         <v>44</v>
       </c>
@@ -19565,7 +19640,7 @@
         <v>190</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="191">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="48">
         <v>44</v>
       </c>
@@ -19597,7 +19672,7 @@
         <v>191</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="192">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="48">
         <v>44</v>
       </c>
@@ -19621,7 +19696,7 @@
         <v>192</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="193">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="48">
         <v>45</v>
       </c>
@@ -19653,7 +19728,7 @@
         <v>193</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="194">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="48">
         <v>45</v>
       </c>
@@ -19685,7 +19760,7 @@
         <v>194</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="195">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="48">
         <v>45</v>
       </c>
@@ -19717,7 +19792,7 @@
         <v>195</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="196">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="48">
         <v>45</v>
       </c>
@@ -19749,7 +19824,7 @@
         <v>196</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="197">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="48">
         <v>45</v>
       </c>
@@ -19773,7 +19848,7 @@
         <v>197</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="198">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="48">
         <v>46</v>
       </c>
@@ -19796,7 +19871,7 @@
         <v>469</v>
       </c>
       <c r="H198" s="24">
-        <v>9.95</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="I198" s="24"/>
       <c r="J198" s="14"/>
@@ -19805,7 +19880,7 @@
         <v>198</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="199">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="48">
         <v>46</v>
       </c>
@@ -19829,7 +19904,7 @@
       </c>
       <c r="H199" s="24"/>
       <c r="I199" s="24">
-        <v>9.95</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="J199" s="14"/>
       <c r="K199" s="48">
@@ -19837,7 +19912,7 @@
         <v>199</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="200">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="48">
         <v>46</v>
       </c>
@@ -19861,7 +19936,7 @@
         <v>200</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="201">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="48">
         <v>47</v>
       </c>
@@ -19890,7 +19965,7 @@
         <v>201</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="202">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="48">
         <v>47</v>
       </c>
@@ -19920,7 +19995,7 @@
         <v>202</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="203">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="48">
         <v>47</v>
       </c>
@@ -19942,7 +20017,7 @@
         <v>203</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="204">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="48">
         <v>48</v>
       </c>
@@ -19971,7 +20046,7 @@
         <v>204</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="205">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="48">
         <v>48</v>
       </c>
@@ -20001,7 +20076,7 @@
         <v>205</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="206">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="48">
         <v>48</v>
       </c>
@@ -20031,7 +20106,7 @@
         <v>206</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="207">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="48">
         <v>48</v>
       </c>
@@ -20061,7 +20136,7 @@
         <v>207</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="208">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="48">
         <v>48</v>
       </c>
@@ -20091,7 +20166,7 @@
         <v>208</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="209">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="48">
         <v>48</v>
       </c>
@@ -20113,7 +20188,7 @@
         <v>209</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="210">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="48">
         <v>49</v>
       </c>
@@ -20145,7 +20220,7 @@
         <v>210</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="211">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="48">
         <v>49</v>
       </c>
@@ -20177,7 +20252,7 @@
         <v>211</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="212">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="48">
         <v>49</v>
       </c>
@@ -20209,7 +20284,7 @@
         <v>212</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="213">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="48">
         <v>49</v>
       </c>
@@ -20241,7 +20316,7 @@
         <v>213</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="214">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="48">
         <v>49</v>
       </c>
@@ -20265,7 +20340,7 @@
         <v>214</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="215">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="48">
         <v>50</v>
       </c>
@@ -20297,7 +20372,7 @@
         <v>215</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="216">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="48">
         <v>50</v>
       </c>
@@ -20329,7 +20404,7 @@
         <v>216</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="217">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="48">
         <v>50</v>
       </c>
@@ -20361,7 +20436,7 @@
         <v>217</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="218">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="48">
         <v>50</v>
       </c>
@@ -20393,7 +20468,7 @@
         <v>218</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="219">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="48">
         <v>50</v>
       </c>
@@ -20417,7 +20492,7 @@
         <v>219</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="220">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="48">
         <v>51</v>
       </c>
@@ -20449,7 +20524,7 @@
         <v>220</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="221">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="48">
         <v>51</v>
       </c>
@@ -20481,7 +20556,7 @@
         <v>221</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="222">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="48">
         <v>51</v>
       </c>
@@ -20505,7 +20580,7 @@
         <v>222</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="223">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="48">
         <v>52</v>
       </c>
@@ -20528,7 +20603,7 @@
         <v>514</v>
       </c>
       <c r="H223" s="24">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I223" s="24"/>
       <c r="J223" s="14"/>
@@ -20537,7 +20612,7 @@
         <v>223</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="224">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="48">
         <v>52</v>
       </c>
@@ -20569,7 +20644,7 @@
         <v>224</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="225">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="48">
         <v>52</v>
       </c>
@@ -20601,7 +20676,7 @@
         <v>225</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="226">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="48">
         <v>52</v>
       </c>
@@ -20635,7 +20710,7 @@
         <v>226</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="227">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="48">
         <v>52</v>
       </c>
@@ -20659,7 +20734,7 @@
         <v>227</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="228">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="48">
         <v>53</v>
       </c>
@@ -20679,7 +20754,7 @@
         <v>514</v>
       </c>
       <c r="H228" s="24">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I228" s="24"/>
       <c r="J228" s="14"/>
@@ -20688,7 +20763,7 @@
         <v>228</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="229">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="48">
         <v>53</v>
       </c>
@@ -20718,7 +20793,7 @@
         <v>229</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="230">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="48">
         <v>53</v>
       </c>
@@ -20748,7 +20823,7 @@
         <v>230</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="231">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="48">
         <v>53</v>
       </c>
@@ -20780,7 +20855,7 @@
         <v>231</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="232">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="48">
         <v>53</v>
       </c>
@@ -20802,7 +20877,7 @@
         <v>232</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="233">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="48">
         <v>54</v>
       </c>
@@ -20822,7 +20897,7 @@
         <v>514</v>
       </c>
       <c r="H233" s="24">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I233" s="24"/>
       <c r="J233" s="14"/>
@@ -20831,7 +20906,7 @@
         <v>233</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="234">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="48">
         <v>54</v>
       </c>
@@ -20861,7 +20936,7 @@
         <v>234</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="235">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="48">
         <v>54</v>
       </c>
@@ -20891,7 +20966,7 @@
         <v>235</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="236">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="48">
         <v>54</v>
       </c>
@@ -20923,7 +20998,7 @@
         <v>236</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="237">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="48">
         <v>54</v>
       </c>
@@ -20945,7 +21020,7 @@
         <v>237</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="238">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="48">
         <v>55</v>
       </c>
@@ -20965,7 +21040,7 @@
         <v>514</v>
       </c>
       <c r="H238" s="24">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I238" s="24"/>
       <c r="J238" s="14"/>
@@ -20974,7 +21049,7 @@
         <v>238</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="239">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="48">
         <v>55</v>
       </c>
@@ -21004,7 +21079,7 @@
         <v>239</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="240">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="48">
         <v>55</v>
       </c>
@@ -21034,7 +21109,7 @@
         <v>240</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="241">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="48">
         <v>55</v>
       </c>
@@ -21066,7 +21141,7 @@
         <v>241</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="242">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="48">
         <v>55</v>
       </c>
@@ -21088,7 +21163,7 @@
         <v>242</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="243">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="48">
         <v>56</v>
       </c>
@@ -21117,7 +21192,7 @@
         <v>243</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="244">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="48">
         <v>56</v>
       </c>
@@ -21147,7 +21222,7 @@
         <v>244</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="245">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="48">
         <v>56</v>
       </c>
@@ -21169,7 +21244,7 @@
         <v>245</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="246">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="48">
         <v>57</v>
       </c>
@@ -21198,7 +21273,7 @@
         <v>246</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="247">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="48">
         <v>57</v>
       </c>
@@ -21228,7 +21303,7 @@
         <v>247</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="248">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="48">
         <v>57</v>
       </c>
@@ -21258,7 +21333,7 @@
         <v>248</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="249">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="48">
         <v>57</v>
       </c>
@@ -21288,7 +21363,7 @@
         <v>249</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="250">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="48">
         <v>57</v>
       </c>
@@ -21318,7 +21393,7 @@
         <v>250</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="251">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" s="48">
         <v>57</v>
       </c>
@@ -21340,7 +21415,7 @@
         <v>251</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="252">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" s="48">
         <v>58</v>
       </c>
@@ -21369,7 +21444,7 @@
         <v>252</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="253">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" s="48">
         <v>58</v>
       </c>
@@ -21399,7 +21474,7 @@
         <v>253</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="254">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="48">
         <v>58</v>
       </c>
@@ -21429,7 +21504,7 @@
         <v>254</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="255">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="48">
         <v>58</v>
       </c>
@@ -21459,7 +21534,7 @@
         <v>255</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="256">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" s="48">
         <v>58</v>
       </c>
@@ -21481,7 +21556,7 @@
         <v>256</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="257">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="48">
         <v>59</v>
       </c>
@@ -21510,7 +21585,7 @@
         <v>257</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="258">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="48">
         <v>59</v>
       </c>
@@ -21540,7 +21615,7 @@
         <v>258</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="259">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="48">
         <v>59</v>
       </c>
@@ -21570,7 +21645,7 @@
         <v>259</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="260">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="48">
         <v>59</v>
       </c>
@@ -21600,7 +21675,7 @@
         <v>260</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="261">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" s="48">
         <v>59</v>
       </c>
@@ -21622,7 +21697,7 @@
         <v>261</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="262">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="48">
         <v>60</v>
       </c>
@@ -21642,7 +21717,7 @@
         <v>514</v>
       </c>
       <c r="H262" s="24">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I262" s="24"/>
       <c r="J262" s="14"/>
@@ -21651,7 +21726,7 @@
         <v>262</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="263">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="48">
         <v>60</v>
       </c>
@@ -21681,7 +21756,7 @@
         <v>263</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="264">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="48">
         <v>60</v>
       </c>
@@ -21711,7 +21786,7 @@
         <v>264</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="265">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="48">
         <v>60</v>
       </c>
@@ -21743,7 +21818,7 @@
         <v>265</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="266">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="48">
         <v>60</v>
       </c>
@@ -21765,7 +21840,7 @@
         <v>266</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="267">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" s="48">
         <v>61</v>
       </c>
@@ -21794,7 +21869,7 @@
         <v>267</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="268">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" s="48">
         <v>61</v>
       </c>
@@ -21824,7 +21899,7 @@
         <v>268</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="269">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="48">
         <v>61</v>
       </c>
@@ -21854,7 +21929,7 @@
         <v>269</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="270">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="48">
         <v>61</v>
       </c>
@@ -21884,7 +21959,7 @@
         <v>270</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="271">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="48">
         <v>61</v>
       </c>
@@ -21914,7 +21989,7 @@
         <v>271</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="272">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="48">
         <v>61</v>
       </c>
@@ -21936,7 +22011,7 @@
         <v>272</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="273">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" s="48">
         <v>62</v>
       </c>
@@ -21965,7 +22040,7 @@
         <v>273</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="274">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="48">
         <v>62</v>
       </c>
@@ -21995,7 +22070,7 @@
         <v>274</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="275">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" s="48">
         <v>62</v>
       </c>
@@ -22025,7 +22100,7 @@
         <v>275</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="276">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="48">
         <v>62</v>
       </c>
@@ -22055,7 +22130,7 @@
         <v>276</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="277">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" s="48">
         <v>62</v>
       </c>
@@ -22077,7 +22152,7 @@
         <v>277</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="278">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="48">
         <v>63</v>
       </c>
@@ -22106,7 +22181,7 @@
         <v>278</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="279">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="48">
         <v>63</v>
       </c>
@@ -22136,7 +22211,7 @@
         <v>279</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="280">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="48">
         <v>63</v>
       </c>
@@ -22166,7 +22241,7 @@
         <v>280</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="281">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="48">
         <v>63</v>
       </c>
@@ -22196,7 +22271,7 @@
         <v>281</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="282">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="48">
         <v>63</v>
       </c>
@@ -22218,7 +22293,7 @@
         <v>282</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="283">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="48">
         <v>64</v>
       </c>
@@ -22250,7 +22325,7 @@
         <v>283</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="284">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="48">
         <v>64</v>
       </c>
@@ -22282,7 +22357,7 @@
         <v>284</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="285">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="48">
         <v>64</v>
       </c>
@@ -22314,7 +22389,7 @@
         <v>285</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="286">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" s="48">
         <v>64</v>
       </c>
@@ -22346,7 +22421,7 @@
         <v>286</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="287">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="48">
         <v>64</v>
       </c>
@@ -22378,7 +22453,7 @@
         <v>287</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="288">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" s="48">
         <v>64</v>
       </c>
@@ -22410,7 +22485,7 @@
         <v>288</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="289">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="48">
         <v>64</v>
       </c>
@@ -22434,7 +22509,7 @@
         <v>289</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="290">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" s="48">
         <v>65</v>
       </c>
@@ -22463,7 +22538,7 @@
         <v>290</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="291">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291" s="48">
         <v>65</v>
       </c>
@@ -22493,7 +22568,7 @@
         <v>291</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="292">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292" s="48">
         <v>65</v>
       </c>
@@ -22523,7 +22598,7 @@
         <v>292</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="293">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293" s="48">
         <v>65</v>
       </c>
@@ -22553,7 +22628,7 @@
         <v>293</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="294">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" s="48">
         <v>65</v>
       </c>
@@ -22575,7 +22650,7 @@
         <v>294</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="295">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A295" s="48">
         <v>66</v>
       </c>
@@ -22607,7 +22682,7 @@
         <v>295</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="296">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296" s="48">
         <v>66</v>
       </c>
@@ -22639,7 +22714,7 @@
         <v>296</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="297">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A297" s="48">
         <v>66</v>
       </c>
@@ -22663,7 +22738,7 @@
         <v>297</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="298">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" s="48">
         <v>67</v>
       </c>
@@ -22695,7 +22770,7 @@
         <v>298</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="299">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" s="48">
         <v>67</v>
       </c>
@@ -22725,7 +22800,7 @@
         <v>299</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="300">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" s="48">
         <v>67</v>
       </c>
@@ -22747,7 +22822,7 @@
         <v>300</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="301">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A301" s="48">
         <v>68</v>
       </c>
@@ -22779,7 +22854,7 @@
         <v>301</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="302">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" s="48">
         <v>68</v>
       </c>
@@ -22811,7 +22886,7 @@
         <v>302</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="303">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303" s="48">
         <v>68</v>
       </c>
@@ -22843,7 +22918,7 @@
         <v>303</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="304">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" s="48">
         <v>68</v>
       </c>
@@ -22867,7 +22942,7 @@
       </c>
       <c r="H304" s="24"/>
       <c r="I304" s="24">
-        <v>37.41</v>
+        <v>37.409999999999997</v>
       </c>
       <c r="J304" s="14"/>
       <c r="K304" s="48">
@@ -22875,7 +22950,7 @@
         <v>304</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="305">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305" s="48">
         <v>68</v>
       </c>
@@ -22899,7 +22974,7 @@
         <v>305</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="306">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="48">
         <v>69</v>
       </c>
@@ -22931,7 +23006,7 @@
         <v>306</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="307">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" s="48">
         <v>69</v>
       </c>
@@ -22963,7 +23038,7 @@
         <v>307</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="308">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="48">
         <v>69</v>
       </c>
@@ -22995,7 +23070,7 @@
         <v>308</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="309">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309" s="48">
         <v>69</v>
       </c>
@@ -23027,7 +23102,7 @@
         <v>309</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="310">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310" s="48">
         <v>69</v>
       </c>
@@ -23059,7 +23134,7 @@
         <v>310</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="311">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A311" s="48">
         <v>69</v>
       </c>
@@ -23091,7 +23166,7 @@
         <v>311</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="312">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A312" s="48">
         <v>69</v>
       </c>
@@ -23123,7 +23198,7 @@
         <v>312</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="313">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A313" s="48">
         <v>69</v>
       </c>
@@ -23145,7 +23220,7 @@
         <v>313</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="314">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314" s="48">
         <v>70</v>
       </c>
@@ -23177,7 +23252,7 @@
         <v>314</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="315">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A315" s="48">
         <v>70</v>
       </c>
@@ -23209,7 +23284,7 @@
         <v>315</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="316">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" s="48">
         <v>70</v>
       </c>
@@ -23241,7 +23316,7 @@
         <v>316</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="317">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="48">
         <v>70</v>
       </c>
@@ -23273,7 +23348,7 @@
         <v>317</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="318">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="48">
         <v>70</v>
       </c>
@@ -23305,7 +23380,7 @@
         <v>318</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="319">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" s="48">
         <v>70</v>
       </c>
@@ -23337,7 +23412,7 @@
         <v>319</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="320">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A320" s="48">
         <v>70</v>
       </c>
@@ -23369,7 +23444,7 @@
         <v>320</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="321">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" s="48">
         <v>70</v>
       </c>
@@ -23393,7 +23468,7 @@
         <v>321</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="322">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322" s="48">
         <v>71</v>
       </c>
@@ -23425,7 +23500,7 @@
         <v>322</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="323">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A323" s="48">
         <v>71</v>
       </c>
@@ -23457,7 +23532,7 @@
         <v>323</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="324">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" s="48">
         <v>71</v>
       </c>
@@ -23489,7 +23564,7 @@
         <v>324</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="325">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325" s="48">
         <v>71</v>
       </c>
@@ -23521,7 +23596,7 @@
         <v>325</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="326">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" s="48">
         <v>71</v>
       </c>
@@ -23553,7 +23628,7 @@
         <v>326</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="327">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="48">
         <v>71</v>
       </c>
@@ -23585,7 +23660,7 @@
         <v>327</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="328">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328" s="48">
         <v>71</v>
       </c>
@@ -23617,7 +23692,7 @@
         <v>328</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="329">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329" s="48">
         <v>71</v>
       </c>
@@ -23641,7 +23716,7 @@
         <v>329</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="330">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330" s="48">
         <v>72</v>
       </c>
@@ -23673,7 +23748,7 @@
         <v>330</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="331">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" s="48">
         <v>72</v>
       </c>
@@ -23705,7 +23780,7 @@
         <v>331</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="332">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332" s="48">
         <v>72</v>
       </c>
@@ -23737,7 +23812,7 @@
         <v>332</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="333">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333" s="48">
         <v>72</v>
       </c>
@@ -23769,7 +23844,7 @@
         <v>333</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="334">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334" s="48">
         <v>72</v>
       </c>
@@ -23793,7 +23868,7 @@
         <v>334</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="335">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" s="48">
         <v>73</v>
       </c>
@@ -23825,7 +23900,7 @@
         <v>335</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="336">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336" s="48">
         <v>73</v>
       </c>
@@ -23857,7 +23932,7 @@
         <v>336</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="337">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" s="48">
         <v>73</v>
       </c>
@@ -23881,7 +23956,7 @@
         <v>337</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="338">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" s="48">
         <v>74</v>
       </c>
@@ -23913,7 +23988,7 @@
         <v>338</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="339">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" s="48">
         <v>74</v>
       </c>
@@ -23947,7 +24022,7 @@
         <v>339</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="340">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340" s="48">
         <v>74</v>
       </c>
@@ -23981,7 +24056,7 @@
         <v>340</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="341">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341" s="48">
         <v>74</v>
       </c>
@@ -24015,7 +24090,7 @@
         <v>341</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="342">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" s="48">
         <v>74</v>
       </c>
@@ -24049,7 +24124,7 @@
         <v>342</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="343">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" s="48">
         <v>74</v>
       </c>
@@ -24073,7 +24148,7 @@
         <v>343</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="344">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344" s="48">
         <v>75</v>
       </c>
@@ -24105,7 +24180,7 @@
         <v>344</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="345">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345" s="48">
         <v>75</v>
       </c>
@@ -24137,7 +24212,7 @@
         <v>345</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="346">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A346" s="48">
         <v>75</v>
       </c>
@@ -24161,7 +24236,7 @@
         <v>346</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="347">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347" s="48">
         <v>76</v>
       </c>
@@ -24193,7 +24268,7 @@
         <v>347</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="348">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348" s="48">
         <v>76</v>
       </c>
@@ -24225,7 +24300,7 @@
         <v>348</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="349">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" s="48">
         <v>76</v>
       </c>
@@ -24249,7 +24324,7 @@
         <v>349</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="350">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350" s="48">
         <v>77</v>
       </c>
@@ -24281,7 +24356,7 @@
         <v>350</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="351">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A351" s="48">
         <v>77</v>
       </c>
@@ -24313,7 +24388,7 @@
         <v>351</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="352">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A352" s="48">
         <v>77</v>
       </c>
@@ -24345,7 +24420,7 @@
         <v>352</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="353">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A353" s="48">
         <v>77</v>
       </c>
@@ -24377,7 +24452,7 @@
         <v>353</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="354">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" s="48">
         <v>77</v>
       </c>
@@ -24403,7 +24478,7 @@
         <v>354</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="355">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" s="48">
         <v>78</v>
       </c>
@@ -24435,7 +24510,7 @@
         <v>355</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="356">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A356" s="48">
         <v>78</v>
       </c>
@@ -24467,7 +24542,7 @@
         <v>356</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="357">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A357" s="48">
         <v>78</v>
       </c>
@@ -24499,7 +24574,7 @@
         <v>357</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="358">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A358" s="48">
         <v>78</v>
       </c>
@@ -24531,7 +24606,7 @@
         <v>358</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="359">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A359" s="48">
         <v>78</v>
       </c>
@@ -24557,7 +24632,7 @@
         <v>359</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="360">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A360" s="48">
         <v>79</v>
       </c>
@@ -24589,7 +24664,7 @@
         <v>360</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="361">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A361" s="48">
         <v>79</v>
       </c>
@@ -24613,7 +24688,7 @@
       </c>
       <c r="H361" s="24"/>
       <c r="I361" s="24">
-        <v>9.95</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="J361" s="14"/>
       <c r="K361" s="48">
@@ -24621,7 +24696,7 @@
         <v>361</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="362">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A362" s="48">
         <v>79</v>
       </c>
@@ -24653,7 +24728,7 @@
         <v>362</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="363">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A363" s="48">
         <v>79</v>
       </c>
@@ -24683,7 +24758,7 @@
         <v>363</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="364">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A364" s="48">
         <v>79</v>
       </c>
@@ -24709,7 +24784,7 @@
         <v>364</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="365">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A365" s="48">
         <v>80</v>
       </c>
@@ -24738,7 +24813,7 @@
         <v>365</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="366">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" s="48">
         <v>80</v>
       </c>
@@ -24768,7 +24843,7 @@
         <v>366</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="367">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367" s="48">
         <v>80</v>
       </c>
@@ -24792,7 +24867,7 @@
         <v>367</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="368">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A368" s="48">
         <v>81</v>
       </c>
@@ -24813,7 +24888,7 @@
         <v>514</v>
       </c>
       <c r="H368" s="24">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I368" s="24"/>
       <c r="J368" s="14"/>
@@ -24822,7 +24897,7 @@
         <v>368</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="369">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" s="48">
         <v>81</v>
       </c>
@@ -24852,7 +24927,7 @@
         <v>369</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="370">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A370" s="48">
         <v>81</v>
       </c>
@@ -24882,7 +24957,7 @@
         <v>370</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="371">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A371" s="48">
         <v>81</v>
       </c>
@@ -24914,7 +24989,7 @@
         <v>371</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="372">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A372" s="48">
         <v>81</v>
       </c>
@@ -24938,7 +25013,7 @@
         <v>372</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="373">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A373" s="48">
         <v>82</v>
       </c>
@@ -24970,7 +25045,7 @@
         <v>373</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="374">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" s="48">
         <v>82</v>
       </c>
@@ -25002,7 +25077,7 @@
         <v>374</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="375">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A375" s="48">
         <v>82</v>
       </c>
@@ -25028,7 +25103,7 @@
         <v>375</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="376">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A376" s="48">
         <v>83</v>
       </c>
@@ -25057,7 +25132,7 @@
         <v>376</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="377">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" s="48">
         <v>83</v>
       </c>
@@ -25087,7 +25162,7 @@
         <v>377</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="378">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378" s="48">
         <v>83</v>
       </c>
@@ -25117,7 +25192,7 @@
         <v>378</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="379">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" s="48">
         <v>83</v>
       </c>
@@ -25147,7 +25222,7 @@
         <v>379</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="380">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" s="48">
         <v>83</v>
       </c>
@@ -25171,7 +25246,7 @@
         <v>380</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="381">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A381" s="48">
         <v>84</v>
       </c>
@@ -25203,7 +25278,7 @@
         <v>381</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="382">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382" s="48">
         <v>84</v>
       </c>
@@ -25235,7 +25310,7 @@
         <v>382</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="383">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A383" s="48">
         <v>84</v>
       </c>
@@ -25261,7 +25336,7 @@
         <v>383</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="384">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A384" s="48">
         <v>85</v>
       </c>
@@ -25281,7 +25356,7 @@
         <v>514</v>
       </c>
       <c r="H384" s="24">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I384" s="24"/>
       <c r="J384" s="14"/>
@@ -25290,7 +25365,7 @@
         <v>384</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="385">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A385" s="48">
         <v>85</v>
       </c>
@@ -25320,7 +25395,7 @@
         <v>385</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="386">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A386" s="48">
         <v>85</v>
       </c>
@@ -25350,7 +25425,7 @@
         <v>386</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="387">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A387" s="48">
         <v>85</v>
       </c>
@@ -25382,7 +25457,7 @@
         <v>387</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="388">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A388" s="48">
         <v>85</v>
       </c>
@@ -25406,7 +25481,7 @@
         <v>388</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="389">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A389" s="48">
         <v>86</v>
       </c>
@@ -25426,7 +25501,7 @@
         <v>514</v>
       </c>
       <c r="H389" s="24">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="I389" s="24"/>
       <c r="J389" s="14"/>
@@ -25435,7 +25510,7 @@
         <v>389</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="390">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A390" s="48">
         <v>86</v>
       </c>
@@ -25457,7 +25532,7 @@
       </c>
       <c r="H390" s="24"/>
       <c r="I390" s="24">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J390" s="14"/>
       <c r="K390" s="48">
@@ -25465,7 +25540,7 @@
         <v>390</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="391">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" s="48">
         <v>86</v>
       </c>
@@ -25489,7 +25564,7 @@
         <v>391</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="392">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A392" s="48">
         <v>87</v>
       </c>
@@ -25521,7 +25596,7 @@
         <v>392</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="393">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A393" s="48">
         <v>87</v>
       </c>
@@ -25553,7 +25628,7 @@
         <v>393</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="394">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A394" s="48">
         <v>87</v>
       </c>
@@ -25585,7 +25660,7 @@
         <v>394</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="395">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A395" s="48">
         <v>87</v>
       </c>
@@ -25617,7 +25692,7 @@
         <v>395</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="396">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" s="48">
         <v>87</v>
       </c>
@@ -25643,7 +25718,7 @@
         <v>396</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="397">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" s="48">
         <v>88</v>
       </c>
@@ -25675,7 +25750,7 @@
         <v>397</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="398">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A398" s="48">
         <v>88</v>
       </c>
@@ -25707,7 +25782,7 @@
         <v>398</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="399">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A399" s="48">
         <v>88</v>
       </c>
@@ -25733,7 +25808,7 @@
         <v>399</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="400">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A400" s="48">
         <v>89</v>
       </c>
@@ -25764,7 +25839,7 @@
         <v>400</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="401">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A401" s="48">
         <v>89</v>
       </c>
@@ -25795,7 +25870,7 @@
         <v>401</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="402">
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A402" s="48">
         <v>89</v>
       </c>
@@ -25819,7 +25894,7 @@
         <v>402</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="403">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A403" s="48">
         <v>90</v>
       </c>
@@ -25847,7 +25922,7 @@
         <v>403</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="404">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A404" s="48">
         <v>90</v>
       </c>
@@ -25876,7 +25951,7 @@
         <v>404</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="405">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A405" s="48">
         <v>90</v>
       </c>
@@ -25895,7 +25970,7 @@
         <v>405</v>
       </c>
     </row>
-    <row outlineLevel="0" r="406">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A406" s="87">
         <v>91</v>
       </c>
@@ -25905,31 +25980,23 @@
       <c r="C406" s="87">
         <v>91</v>
       </c>
-      <c r="D406" s="87" t="inlineStr">
-        <is>
-          <t>Test mercredi</t>
-        </is>
-      </c>
-      <c r="E406" s="87" t="inlineStr">
-        <is>
-          <t>Ceci est la description de l'entrée de journal</t>
-        </is>
-      </c>
-      <c r="F406" s="87" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="G406" s="87" t="inlineStr">
-        <is>
-          <t>Encaisse</t>
-        </is>
+      <c r="D406" s="87" t="s">
+        <v>568</v>
+      </c>
+      <c r="E406" s="87" t="s">
+        <v>569</v>
+      </c>
+      <c r="F406" s="87" t="s">
+        <v>401</v>
+      </c>
+      <c r="G406" s="87" t="s">
+        <v>399</v>
       </c>
       <c r="H406" s="84">
         <v>0.25</v>
       </c>
     </row>
-    <row outlineLevel="0" r="407">
+    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A407" s="87">
         <v>91</v>
       </c>
@@ -25939,31 +26006,23 @@
       <c r="C407" s="87">
         <v>91</v>
       </c>
-      <c r="D407" s="87" t="inlineStr">
-        <is>
-          <t>Test mercredi</t>
-        </is>
-      </c>
-      <c r="E407" s="87" t="inlineStr">
-        <is>
-          <t>Ceci est la description de l'entrée de journal</t>
-        </is>
-      </c>
-      <c r="F407" s="87" t="inlineStr">
-        <is>
-          <t>5008</t>
-        </is>
-      </c>
-      <c r="G407" s="87" t="inlineStr">
-        <is>
-          <t>Frais de communications</t>
-        </is>
+      <c r="D407" s="87" t="s">
+        <v>568</v>
+      </c>
+      <c r="E407" s="87" t="s">
+        <v>569</v>
+      </c>
+      <c r="F407" s="87" t="s">
+        <v>426</v>
+      </c>
+      <c r="G407" s="87" t="s">
+        <v>427</v>
       </c>
       <c r="I407" s="84">
         <v>0.25</v>
       </c>
     </row>
-    <row outlineLevel="0" r="408">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A408" s="87">
         <v>91</v>
       </c>
@@ -25973,15 +26032,11 @@
       <c r="C408" s="87">
         <v>91</v>
       </c>
-      <c r="D408" s="87" t="inlineStr">
-        <is>
-          <t>Test mercredi</t>
-        </is>
-      </c>
-      <c r="E408" s="87" t="inlineStr">
-        <is>
-          <t>Ceci est la description de l'entrée de journal</t>
-        </is>
+      <c r="D408" s="87" t="s">
+        <v>568</v>
+      </c>
+      <c r="E408" s="87" t="s">
+        <v>569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.8 - Avant intégration des encaissements
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86E1CBA-1588-42F3-8996-7FD88B8920A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18352A12-E438-4DB7-A07B-DA402823B133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2728" uniqueCount="630">
   <si>
     <t>TEC_ID</t>
   </si>
@@ -2278,7 +2278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2544,6 +2544,15 @@
     </xf>
     <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire 2" xfId="1" xr:uid="{7066D7D9-A0C5-4744-AD1B-CDB1C4228FB1}"/>
@@ -2774,6 +2783,87 @@
           <cell r="A31">
             <v>15</v>
           </cell>
+        </row>
+        <row r="32">
+          <cell r="A32"/>
+        </row>
+        <row r="33">
+          <cell r="A33"/>
+        </row>
+        <row r="34">
+          <cell r="A34"/>
+        </row>
+        <row r="35">
+          <cell r="A35"/>
+        </row>
+        <row r="36">
+          <cell r="A36"/>
+        </row>
+        <row r="37">
+          <cell r="A37"/>
+        </row>
+        <row r="38">
+          <cell r="A38"/>
+        </row>
+        <row r="39">
+          <cell r="A39"/>
+        </row>
+        <row r="40">
+          <cell r="A40"/>
+        </row>
+        <row r="41">
+          <cell r="A41"/>
+        </row>
+        <row r="42">
+          <cell r="A42"/>
+        </row>
+        <row r="43">
+          <cell r="A43"/>
+        </row>
+        <row r="44">
+          <cell r="A44"/>
+        </row>
+        <row r="45">
+          <cell r="A45"/>
+        </row>
+        <row r="46">
+          <cell r="A46"/>
+        </row>
+        <row r="47">
+          <cell r="A47"/>
+        </row>
+        <row r="48">
+          <cell r="A48"/>
+        </row>
+        <row r="49">
+          <cell r="A49"/>
+        </row>
+        <row r="50">
+          <cell r="A50"/>
+        </row>
+        <row r="51">
+          <cell r="A51"/>
+        </row>
+        <row r="52">
+          <cell r="A52"/>
+        </row>
+        <row r="53">
+          <cell r="A53"/>
+        </row>
+        <row r="54">
+          <cell r="A54"/>
+        </row>
+        <row r="55">
+          <cell r="A55"/>
+        </row>
+        <row r="56">
+          <cell r="A56"/>
+        </row>
+        <row r="57">
+          <cell r="A57"/>
+        </row>
+        <row r="58">
+          <cell r="A58"/>
         </row>
       </sheetData>
       <sheetData sheetId="4"/>
@@ -14394,12 +14484,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D58006-DE1D-488F-9BB7-8096C5818030}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{E0D58006-DE1D-488F-9BB7-8096C5818030}">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="A1:K456"/>
+  <dimension ref="A1:K465"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A427" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K453" sqref="K453:K456"/>
+    <sheetView tabSelected="1" topLeftCell="A427" zoomScale="90" zoomScaleNormal="90" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="B465" sqref="B465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14416,7 +14506,7 @@
     <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row spans="1:11" ht="25.5" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
       <c r="A1" s="28" t="s">
         <v>531</v>
       </c>
@@ -14451,7 +14541,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
       <c r="A2" s="46">
         <v>1</v>
       </c>
@@ -14483,7 +14573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row spans="1:11" ht="15.75" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
       <c r="A3" s="46">
         <v>1</v>
       </c>
@@ -14515,7 +14605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
       <c r="A4" s="46">
         <v>1</v>
       </c>
@@ -14536,7 +14626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
       <c r="A5" s="46">
         <v>2</v>
       </c>
@@ -14568,7 +14658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="6">
       <c r="A6" s="46">
         <v>2</v>
       </c>
@@ -14600,7 +14690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="7">
       <c r="A7" s="46">
         <v>2</v>
       </c>
@@ -14618,7 +14708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="8">
       <c r="A8" s="46">
         <v>3</v>
       </c>
@@ -14650,7 +14740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="9">
       <c r="A9" s="46">
         <v>3</v>
       </c>
@@ -14682,7 +14772,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="10">
       <c r="A10" s="46">
         <v>3</v>
       </c>
@@ -14702,7 +14792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="11">
       <c r="A11" s="46">
         <v>4</v>
       </c>
@@ -14734,7 +14824,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="12">
       <c r="A12" s="46">
         <v>4</v>
       </c>
@@ -14766,7 +14856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="13">
       <c r="A13" s="46">
         <v>4</v>
       </c>
@@ -14789,7 +14879,7 @@
         <v>415</v>
       </c>
       <c r="H13" s="86">
-        <v>570.91999999999996</v>
+        <v>570.92</v>
       </c>
       <c r="I13" s="86"/>
       <c r="J13" s="14"/>
@@ -14798,7 +14888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="14">
       <c r="A14" s="46">
         <v>4</v>
       </c>
@@ -14830,7 +14920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="15">
       <c r="A15" s="46">
         <v>4</v>
       </c>
@@ -14862,7 +14952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="16">
       <c r="A16" s="46">
         <v>4</v>
       </c>
@@ -14886,7 +14976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="17">
       <c r="A17" s="46">
         <v>5</v>
       </c>
@@ -14918,7 +15008,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="18">
       <c r="A18" s="46">
         <v>5</v>
       </c>
@@ -14950,7 +15040,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="19">
       <c r="A19" s="46">
         <v>5</v>
       </c>
@@ -14982,7 +15072,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="20">
       <c r="A20" s="46">
         <v>5</v>
       </c>
@@ -15014,7 +15104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="21">
       <c r="A21" s="46">
         <v>5</v>
       </c>
@@ -15046,7 +15136,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="22">
       <c r="A22" s="46">
         <v>5</v>
       </c>
@@ -15078,7 +15168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="23">
       <c r="A23" s="46">
         <v>5</v>
       </c>
@@ -15110,7 +15200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="24">
       <c r="A24" s="46">
         <v>5</v>
       </c>
@@ -15142,7 +15232,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="25">
       <c r="A25" s="46">
         <v>5</v>
       </c>
@@ -15166,7 +15256,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="26">
       <c r="A26" s="46">
         <v>6</v>
       </c>
@@ -15198,7 +15288,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="27">
       <c r="A27" s="46">
         <v>6</v>
       </c>
@@ -15230,7 +15320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="28">
       <c r="A28" s="46">
         <v>6</v>
       </c>
@@ -15262,7 +15352,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="29">
       <c r="A29" s="46">
         <v>6</v>
       </c>
@@ -15294,7 +15384,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="30">
       <c r="A30" s="46">
         <v>6</v>
       </c>
@@ -15326,7 +15416,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="31">
       <c r="A31" s="46">
         <v>6</v>
       </c>
@@ -15358,7 +15448,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="32">
       <c r="A32" s="46">
         <v>6</v>
       </c>
@@ -15390,7 +15480,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="33">
       <c r="A33" s="46">
         <v>6</v>
       </c>
@@ -15422,7 +15512,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="34">
       <c r="A34" s="46">
         <v>6</v>
       </c>
@@ -15446,7 +15536,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="35">
       <c r="A35" s="46">
         <v>7</v>
       </c>
@@ -15478,7 +15568,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="36">
       <c r="A36" s="46">
         <v>7</v>
       </c>
@@ -15510,7 +15600,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="37">
       <c r="A37" s="46">
         <v>7</v>
       </c>
@@ -15542,7 +15632,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="38">
       <c r="A38" s="46">
         <v>7</v>
       </c>
@@ -15574,7 +15664,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="39">
       <c r="A39" s="46">
         <v>7</v>
       </c>
@@ -15606,7 +15696,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="40">
       <c r="A40" s="46">
         <v>7</v>
       </c>
@@ -15638,7 +15728,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="41">
       <c r="A41" s="46">
         <v>7</v>
       </c>
@@ -15662,7 +15752,7 @@
       </c>
       <c r="H41" s="86"/>
       <c r="I41" s="86">
-        <v>67.680000000000007</v>
+        <v>67.68</v>
       </c>
       <c r="J41" s="14"/>
       <c r="K41" s="46">
@@ -15670,7 +15760,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="42">
       <c r="A42" s="46">
         <v>7</v>
       </c>
@@ -15702,7 +15792,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="43">
       <c r="A43" s="46">
         <v>7</v>
       </c>
@@ -15726,7 +15816,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="44">
       <c r="A44" s="46">
         <v>8</v>
       </c>
@@ -15749,7 +15839,7 @@
         <v>402</v>
       </c>
       <c r="H44" s="86">
-        <v>1248.6300000000001</v>
+        <v>1248.63</v>
       </c>
       <c r="I44" s="86"/>
       <c r="J44" s="14"/>
@@ -15758,7 +15848,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="45">
       <c r="A45" s="46">
         <v>8</v>
       </c>
@@ -15790,7 +15880,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="46">
       <c r="A46" s="46">
         <v>8</v>
       </c>
@@ -15822,7 +15912,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="47">
       <c r="A47" s="46">
         <v>8</v>
       </c>
@@ -15854,7 +15944,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="48">
       <c r="A48" s="46">
         <v>8</v>
       </c>
@@ -15886,7 +15976,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="49">
       <c r="A49" s="46">
         <v>8</v>
       </c>
@@ -15918,7 +16008,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="50">
       <c r="A50" s="46">
         <v>8</v>
       </c>
@@ -15950,7 +16040,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="51">
       <c r="A51" s="46">
         <v>8</v>
       </c>
@@ -15974,7 +16064,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="52">
       <c r="A52" s="46">
         <v>9</v>
       </c>
@@ -15997,7 +16087,7 @@
         <v>399</v>
       </c>
       <c r="H52" s="86">
-        <v>1248.6300000000001</v>
+        <v>1248.63</v>
       </c>
       <c r="I52" s="86"/>
       <c r="J52" s="14"/>
@@ -16006,7 +16096,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="53">
       <c r="A53" s="46">
         <v>9</v>
       </c>
@@ -16030,7 +16120,7 @@
       </c>
       <c r="H53" s="86"/>
       <c r="I53" s="86">
-        <v>1248.6300000000001</v>
+        <v>1248.63</v>
       </c>
       <c r="J53" s="14"/>
       <c r="K53" s="46">
@@ -16038,7 +16128,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="54">
       <c r="A54" s="46">
         <v>9</v>
       </c>
@@ -16062,7 +16152,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="55">
       <c r="A55" s="46">
         <v>10</v>
       </c>
@@ -16094,7 +16184,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="56">
       <c r="A56" s="46">
         <v>10</v>
       </c>
@@ -16126,7 +16216,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="57">
       <c r="A57" s="46">
         <v>10</v>
       </c>
@@ -16143,7 +16233,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="58">
       <c r="A58" s="46">
         <v>11</v>
       </c>
@@ -16175,7 +16265,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="59">
       <c r="A59" s="46">
         <v>11</v>
       </c>
@@ -16207,7 +16297,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="60">
       <c r="A60" s="46">
         <v>11</v>
       </c>
@@ -16231,7 +16321,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="61">
       <c r="A61" s="46">
         <v>12</v>
       </c>
@@ -16260,7 +16350,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="62">
       <c r="A62" s="46">
         <v>12</v>
       </c>
@@ -16290,7 +16380,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="63">
       <c r="A63" s="46">
         <v>12</v>
       </c>
@@ -16320,7 +16410,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="64">
       <c r="A64" s="46">
         <v>12</v>
       </c>
@@ -16342,7 +16432,7 @@
       </c>
       <c r="H64" s="86"/>
       <c r="I64" s="86">
-        <v>4585.3999999999996</v>
+        <v>4585.4</v>
       </c>
       <c r="J64" s="14"/>
       <c r="K64" s="46">
@@ -16350,7 +16440,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="65">
       <c r="A65" s="46">
         <v>12</v>
       </c>
@@ -16372,7 +16462,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="66">
       <c r="A66" s="46">
         <v>13</v>
       </c>
@@ -16404,7 +16494,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="67">
       <c r="A67" s="46">
         <v>13</v>
       </c>
@@ -16436,7 +16526,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="68">
       <c r="A68" s="46">
         <v>13</v>
       </c>
@@ -16468,7 +16558,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="69">
       <c r="A69" s="46">
         <v>13</v>
       </c>
@@ -16500,7 +16590,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="70">
       <c r="A70" s="46">
         <v>13</v>
       </c>
@@ -16524,7 +16614,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="71">
       <c r="A71" s="46">
         <v>14</v>
       </c>
@@ -16547,7 +16637,7 @@
         <v>402</v>
       </c>
       <c r="H71" s="86">
-        <v>1034.9100000000001</v>
+        <v>1034.91</v>
       </c>
       <c r="I71" s="86"/>
       <c r="J71" s="14"/>
@@ -16556,7 +16646,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="72">
       <c r="A72" s="46">
         <v>14</v>
       </c>
@@ -16588,7 +16678,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="73">
       <c r="A73" s="46">
         <v>14</v>
       </c>
@@ -16612,7 +16702,7 @@
       </c>
       <c r="H73" s="86"/>
       <c r="I73" s="86">
-        <v>153.72999999999999</v>
+        <v>153.73</v>
       </c>
       <c r="J73" s="14"/>
       <c r="K73" s="46">
@@ -16620,7 +16710,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="74">
       <c r="A74" s="46">
         <v>14</v>
       </c>
@@ -16652,7 +16742,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="75">
       <c r="A75" s="46">
         <v>14</v>
       </c>
@@ -16684,7 +16774,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="76">
       <c r="A76" s="46">
         <v>14</v>
       </c>
@@ -16716,7 +16806,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="77">
       <c r="A77" s="46">
         <v>14</v>
       </c>
@@ -16748,7 +16838,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="78">
       <c r="A78" s="46">
         <v>14</v>
       </c>
@@ -16780,7 +16870,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="79">
       <c r="A79" s="46">
         <v>14</v>
       </c>
@@ -16804,7 +16894,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="80">
       <c r="A80" s="46">
         <v>15</v>
       </c>
@@ -16836,7 +16926,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="81">
       <c r="A81" s="46">
         <v>15</v>
       </c>
@@ -16868,7 +16958,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="82">
       <c r="A82" s="46">
         <v>15</v>
       </c>
@@ -16900,7 +16990,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="83">
       <c r="A83" s="46">
         <v>15</v>
       </c>
@@ -16932,7 +17022,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="84">
       <c r="A84" s="46">
         <v>15</v>
       </c>
@@ -16964,7 +17054,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="85">
       <c r="A85" s="46">
         <v>15</v>
       </c>
@@ -16996,7 +17086,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="86">
       <c r="A86" s="46">
         <v>15</v>
       </c>
@@ -17028,7 +17118,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="87">
       <c r="A87" s="46">
         <v>15</v>
       </c>
@@ -17062,7 +17152,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="88">
       <c r="A88" s="46">
         <v>15</v>
       </c>
@@ -17086,7 +17176,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="89">
       <c r="A89" s="46">
         <v>16</v>
       </c>
@@ -17109,7 +17199,7 @@
         <v>399</v>
       </c>
       <c r="H89" s="86">
-        <v>1034.9100000000001</v>
+        <v>1034.91</v>
       </c>
       <c r="I89" s="86"/>
       <c r="J89" s="14"/>
@@ -17118,7 +17208,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="90">
       <c r="A90" s="46">
         <v>16</v>
       </c>
@@ -17142,7 +17232,7 @@
       </c>
       <c r="H90" s="86"/>
       <c r="I90" s="86">
-        <v>1034.9100000000001</v>
+        <v>1034.91</v>
       </c>
       <c r="J90" s="14"/>
       <c r="K90" s="46">
@@ -17150,7 +17240,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="91">
       <c r="A91" s="46">
         <v>16</v>
       </c>
@@ -17174,7 +17264,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="92">
       <c r="A92" s="46">
         <v>17</v>
       </c>
@@ -17208,7 +17298,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="93">
       <c r="A93" s="46">
         <v>17</v>
       </c>
@@ -17242,7 +17332,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="94">
       <c r="A94" s="46">
         <v>17</v>
       </c>
@@ -17266,7 +17356,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="95">
       <c r="A95" s="46">
         <v>18</v>
       </c>
@@ -17298,7 +17388,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="96">
       <c r="A96" s="46">
         <v>18</v>
       </c>
@@ -17330,7 +17420,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="97">
       <c r="A97" s="46">
         <v>18</v>
       </c>
@@ -17362,7 +17452,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="98">
       <c r="A98" s="46">
         <v>18</v>
       </c>
@@ -17394,7 +17484,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="99">
       <c r="A99" s="46">
         <v>18</v>
       </c>
@@ -17418,7 +17508,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="100">
       <c r="A100" s="46">
         <v>19</v>
       </c>
@@ -17450,7 +17540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="101">
       <c r="A101" s="46">
         <v>19</v>
       </c>
@@ -17482,7 +17572,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="102">
       <c r="A102" s="46">
         <v>19</v>
       </c>
@@ -17506,7 +17596,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="103">
       <c r="A103" s="46">
         <v>20</v>
       </c>
@@ -17538,7 +17628,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="104">
       <c r="A104" s="46">
         <v>20</v>
       </c>
@@ -17570,7 +17660,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="105">
       <c r="A105" s="46">
         <v>20</v>
       </c>
@@ -17594,7 +17684,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="106">
       <c r="A106" s="46">
         <v>21</v>
       </c>
@@ -17626,7 +17716,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="107">
       <c r="A107" s="46">
         <v>21</v>
       </c>
@@ -17658,7 +17748,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="108">
       <c r="A108" s="46">
         <v>21</v>
       </c>
@@ -17682,7 +17772,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="109">
       <c r="A109" s="46">
         <v>22</v>
       </c>
@@ -17716,7 +17806,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="110">
       <c r="A110" s="46">
         <v>22</v>
       </c>
@@ -17748,7 +17838,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="111">
       <c r="A111" s="46">
         <v>22</v>
       </c>
@@ -17772,7 +17862,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="112">
       <c r="A112" s="46">
         <v>23</v>
       </c>
@@ -17795,7 +17885,7 @@
         <v>399</v>
       </c>
       <c r="H112" s="86">
-        <v>159.94999999999999</v>
+        <v>159.95</v>
       </c>
       <c r="I112" s="86"/>
       <c r="J112" s="14"/>
@@ -17804,7 +17894,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="113">
       <c r="A113" s="46">
         <v>23</v>
       </c>
@@ -17828,7 +17918,7 @@
       </c>
       <c r="H113" s="86"/>
       <c r="I113" s="86">
-        <v>149.94999999999999</v>
+        <v>149.95</v>
       </c>
       <c r="J113" s="14"/>
       <c r="K113" s="46">
@@ -17836,7 +17926,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="114">
       <c r="A114" s="46">
         <v>23</v>
       </c>
@@ -17868,7 +17958,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="115">
       <c r="A115" s="46">
         <v>23</v>
       </c>
@@ -17900,7 +17990,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="116">
       <c r="A116" s="46">
         <v>23</v>
       </c>
@@ -17924,7 +18014,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="117">
       <c r="A117" s="46">
         <v>24</v>
       </c>
@@ -17956,7 +18046,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="118">
       <c r="A118" s="46">
         <v>24</v>
       </c>
@@ -17988,7 +18078,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="119">
       <c r="A119" s="46">
         <v>24</v>
       </c>
@@ -18012,7 +18102,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="120">
       <c r="A120" s="46">
         <v>25</v>
       </c>
@@ -18044,7 +18134,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="121">
       <c r="A121" s="46">
         <v>25</v>
       </c>
@@ -18076,7 +18166,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="122">
       <c r="A122" s="46">
         <v>25</v>
       </c>
@@ -18100,7 +18190,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="123">
       <c r="A123" s="46">
         <v>26</v>
       </c>
@@ -18132,7 +18222,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="124">
       <c r="A124" s="46">
         <v>26</v>
       </c>
@@ -18164,7 +18254,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="125">
       <c r="A125" s="46">
         <v>26</v>
       </c>
@@ -18188,7 +18278,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="126">
       <c r="A126" s="46">
         <v>27</v>
       </c>
@@ -18220,7 +18310,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="127">
       <c r="A127" s="46">
         <v>27</v>
       </c>
@@ -18252,7 +18342,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="128">
       <c r="A128" s="46">
         <v>27</v>
       </c>
@@ -18276,7 +18366,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="129">
       <c r="A129" s="46">
         <v>28</v>
       </c>
@@ -18308,7 +18398,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="130">
       <c r="A130" s="46">
         <v>28</v>
       </c>
@@ -18340,7 +18430,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="131">
       <c r="A131" s="46">
         <v>28</v>
       </c>
@@ -18364,7 +18454,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="132">
       <c r="A132" s="46">
         <v>29</v>
       </c>
@@ -18387,7 +18477,7 @@
         <v>402</v>
       </c>
       <c r="H132" s="86">
-        <v>2157.0700000000002</v>
+        <v>2157.07</v>
       </c>
       <c r="I132" s="86"/>
       <c r="J132" s="14"/>
@@ -18396,7 +18486,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="133">
       <c r="A133" s="46">
         <v>29</v>
       </c>
@@ -18428,7 +18518,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="134">
       <c r="A134" s="46">
         <v>29</v>
       </c>
@@ -18460,7 +18550,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="135">
       <c r="A135" s="46">
         <v>29</v>
       </c>
@@ -18492,7 +18582,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="136">
       <c r="A136" s="46">
         <v>29</v>
       </c>
@@ -18524,7 +18614,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="137">
       <c r="A137" s="46">
         <v>29</v>
       </c>
@@ -18556,7 +18646,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="138">
       <c r="A138" s="46">
         <v>29</v>
       </c>
@@ -18588,7 +18678,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="139">
       <c r="A139" s="46">
         <v>29</v>
       </c>
@@ -18620,7 +18710,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="140">
       <c r="A140" s="46">
         <v>29</v>
       </c>
@@ -18644,7 +18734,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="141">
       <c r="A141" s="46">
         <v>30</v>
       </c>
@@ -18676,7 +18766,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="142">
       <c r="A142" s="46">
         <v>30</v>
       </c>
@@ -18708,7 +18798,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="143">
       <c r="A143" s="46">
         <v>30</v>
       </c>
@@ -18740,7 +18830,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="144">
       <c r="A144" s="46">
         <v>30</v>
       </c>
@@ -18772,7 +18862,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="145">
       <c r="A145" s="46">
         <v>30</v>
       </c>
@@ -18804,7 +18894,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="146">
       <c r="A146" s="46">
         <v>30</v>
       </c>
@@ -18836,7 +18926,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="147">
       <c r="A147" s="46">
         <v>30</v>
       </c>
@@ -18868,7 +18958,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="148">
       <c r="A148" s="46">
         <v>30</v>
       </c>
@@ -18900,7 +18990,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="149">
       <c r="A149" s="46">
         <v>30</v>
       </c>
@@ -18924,7 +19014,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="150">
       <c r="A150" s="46">
         <v>31</v>
       </c>
@@ -18956,7 +19046,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="151">
       <c r="A151" s="46">
         <v>31</v>
       </c>
@@ -18988,7 +19078,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="152">
       <c r="A152" s="46">
         <v>31</v>
       </c>
@@ -19012,7 +19102,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="153">
       <c r="A153" s="46">
         <v>32</v>
       </c>
@@ -19044,7 +19134,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="154">
       <c r="A154" s="46">
         <v>32</v>
       </c>
@@ -19076,7 +19166,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="155">
       <c r="A155" s="46">
         <v>32</v>
       </c>
@@ -19100,7 +19190,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="156">
       <c r="A156" s="46">
         <v>33</v>
       </c>
@@ -19132,7 +19222,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="157">
       <c r="A157" s="46">
         <v>33</v>
       </c>
@@ -19166,7 +19256,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="158">
       <c r="A158" s="46">
         <v>33</v>
       </c>
@@ -19190,7 +19280,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="159">
       <c r="A159" s="46">
         <v>34</v>
       </c>
@@ -19222,7 +19312,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="160">
       <c r="A160" s="46">
         <v>34</v>
       </c>
@@ -19254,7 +19344,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="161">
       <c r="A161" s="46">
         <v>34</v>
       </c>
@@ -19278,7 +19368,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="162">
       <c r="A162" s="46">
         <v>35</v>
       </c>
@@ -19310,7 +19400,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="163">
       <c r="A163" s="46">
         <v>35</v>
       </c>
@@ -19342,7 +19432,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="164">
       <c r="A164" s="46">
         <v>35</v>
       </c>
@@ -19366,7 +19456,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="165">
       <c r="A165" s="46">
         <v>36</v>
       </c>
@@ -19395,7 +19485,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="166">
       <c r="A166" s="46">
         <v>36</v>
       </c>
@@ -19425,7 +19515,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="167">
       <c r="A167" s="46">
         <v>36</v>
       </c>
@@ -19447,7 +19537,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="168">
       <c r="A168" s="46">
         <v>37</v>
       </c>
@@ -19479,7 +19569,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="169">
       <c r="A169" s="46">
         <v>37</v>
       </c>
@@ -19511,7 +19601,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="170">
       <c r="A170" s="46">
         <v>37</v>
       </c>
@@ -19535,7 +19625,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="171">
       <c r="A171" s="46">
         <v>38</v>
       </c>
@@ -19567,7 +19657,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="172">
       <c r="A172" s="46">
         <v>38</v>
       </c>
@@ -19599,7 +19689,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="173">
       <c r="A173" s="46">
         <v>38</v>
       </c>
@@ -19623,7 +19713,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="174">
       <c r="A174" s="46">
         <v>39</v>
       </c>
@@ -19655,7 +19745,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="175">
       <c r="A175" s="46">
         <v>39</v>
       </c>
@@ -19687,7 +19777,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="176">
       <c r="A176" s="46">
         <v>39</v>
       </c>
@@ -19711,7 +19801,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="177">
       <c r="A177" s="46">
         <v>40</v>
       </c>
@@ -19743,7 +19833,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="178">
       <c r="A178" s="46">
         <v>40</v>
       </c>
@@ -19775,7 +19865,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="179">
       <c r="A179" s="46">
         <v>40</v>
       </c>
@@ -19799,7 +19889,7 @@
       </c>
       <c r="H179" s="86"/>
       <c r="I179" s="86">
-        <v>33.950000000000003</v>
+        <v>33.95</v>
       </c>
       <c r="J179" s="14"/>
       <c r="K179" s="46">
@@ -19807,7 +19897,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="180">
       <c r="A180" s="46">
         <v>40</v>
       </c>
@@ -19831,7 +19921,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="181">
       <c r="A181" s="46">
         <v>41</v>
       </c>
@@ -19863,7 +19953,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="182">
       <c r="A182" s="46">
         <v>41</v>
       </c>
@@ -19895,7 +19985,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="183">
       <c r="A183" s="46">
         <v>41</v>
       </c>
@@ -19919,7 +20009,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="184">
       <c r="A184" s="46">
         <v>42</v>
       </c>
@@ -19951,7 +20041,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="185">
       <c r="A185" s="46">
         <v>42</v>
       </c>
@@ -19983,7 +20073,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="186">
       <c r="A186" s="46">
         <v>42</v>
       </c>
@@ -20007,7 +20097,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="187">
       <c r="A187" s="46">
         <v>43</v>
       </c>
@@ -20039,7 +20129,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="188">
       <c r="A188" s="46">
         <v>43</v>
       </c>
@@ -20071,7 +20161,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="189">
       <c r="A189" s="46">
         <v>43</v>
       </c>
@@ -20095,7 +20185,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="190">
       <c r="A190" s="46">
         <v>44</v>
       </c>
@@ -20127,7 +20217,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="191">
       <c r="A191" s="46">
         <v>44</v>
       </c>
@@ -20159,7 +20249,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="192">
       <c r="A192" s="46">
         <v>44</v>
       </c>
@@ -20183,7 +20273,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="193">
       <c r="A193" s="46">
         <v>45</v>
       </c>
@@ -20215,7 +20305,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="194">
       <c r="A194" s="46">
         <v>45</v>
       </c>
@@ -20247,7 +20337,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="195">
       <c r="A195" s="46">
         <v>45</v>
       </c>
@@ -20279,7 +20369,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="196">
       <c r="A196" s="46">
         <v>45</v>
       </c>
@@ -20311,7 +20401,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="197">
       <c r="A197" s="46">
         <v>45</v>
       </c>
@@ -20335,7 +20425,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="198">
       <c r="A198" s="46">
         <v>46</v>
       </c>
@@ -20358,7 +20448,7 @@
         <v>469</v>
       </c>
       <c r="H198" s="86">
-        <v>9.9499999999999993</v>
+        <v>9.95</v>
       </c>
       <c r="I198" s="86"/>
       <c r="J198" s="14"/>
@@ -20367,7 +20457,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="199">
       <c r="A199" s="46">
         <v>46</v>
       </c>
@@ -20391,7 +20481,7 @@
       </c>
       <c r="H199" s="86"/>
       <c r="I199" s="86">
-        <v>9.9499999999999993</v>
+        <v>9.95</v>
       </c>
       <c r="J199" s="14"/>
       <c r="K199" s="46">
@@ -20399,7 +20489,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="200">
       <c r="A200" s="46">
         <v>46</v>
       </c>
@@ -20423,7 +20513,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="201">
       <c r="A201" s="46">
         <v>47</v>
       </c>
@@ -20452,7 +20542,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="202">
       <c r="A202" s="46">
         <v>47</v>
       </c>
@@ -20482,7 +20572,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="203">
       <c r="A203" s="46">
         <v>47</v>
       </c>
@@ -20504,7 +20594,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="204">
       <c r="A204" s="46">
         <v>48</v>
       </c>
@@ -20533,7 +20623,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="205">
       <c r="A205" s="46">
         <v>48</v>
       </c>
@@ -20563,7 +20653,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="206">
       <c r="A206" s="46">
         <v>48</v>
       </c>
@@ -20593,7 +20683,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="207">
       <c r="A207" s="46">
         <v>48</v>
       </c>
@@ -20623,7 +20713,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="208">
       <c r="A208" s="46">
         <v>48</v>
       </c>
@@ -20653,7 +20743,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="209">
       <c r="A209" s="46">
         <v>48</v>
       </c>
@@ -20675,7 +20765,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="210">
       <c r="A210" s="46">
         <v>49</v>
       </c>
@@ -20707,7 +20797,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="211">
       <c r="A211" s="46">
         <v>49</v>
       </c>
@@ -20739,7 +20829,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="212">
       <c r="A212" s="46">
         <v>49</v>
       </c>
@@ -20771,7 +20861,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="213">
       <c r="A213" s="46">
         <v>49</v>
       </c>
@@ -20803,7 +20893,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="214">
       <c r="A214" s="46">
         <v>49</v>
       </c>
@@ -20827,7 +20917,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="215">
       <c r="A215" s="46">
         <v>50</v>
       </c>
@@ -20859,7 +20949,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="216">
       <c r="A216" s="46">
         <v>50</v>
       </c>
@@ -20891,7 +20981,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="217">
       <c r="A217" s="46">
         <v>50</v>
       </c>
@@ -20923,7 +21013,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="218">
       <c r="A218" s="46">
         <v>50</v>
       </c>
@@ -20955,7 +21045,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="219">
       <c r="A219" s="46">
         <v>50</v>
       </c>
@@ -20979,7 +21069,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="220">
       <c r="A220" s="46">
         <v>51</v>
       </c>
@@ -21011,7 +21101,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="221">
       <c r="A221" s="46">
         <v>51</v>
       </c>
@@ -21043,7 +21133,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="222">
       <c r="A222" s="46">
         <v>51</v>
       </c>
@@ -21067,7 +21157,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="223">
       <c r="A223" s="46">
         <v>52</v>
       </c>
@@ -21090,7 +21180,7 @@
         <v>514</v>
       </c>
       <c r="H223" s="86">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="I223" s="86"/>
       <c r="J223" s="14"/>
@@ -21099,7 +21189,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="224">
       <c r="A224" s="46">
         <v>52</v>
       </c>
@@ -21131,7 +21221,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="225">
       <c r="A225" s="46">
         <v>52</v>
       </c>
@@ -21163,7 +21253,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="226">
       <c r="A226" s="46">
         <v>52</v>
       </c>
@@ -21197,7 +21287,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="227">
       <c r="A227" s="46">
         <v>52</v>
       </c>
@@ -21221,7 +21311,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="228">
       <c r="A228" s="46">
         <v>53</v>
       </c>
@@ -21241,7 +21331,7 @@
         <v>514</v>
       </c>
       <c r="H228" s="86">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="I228" s="86"/>
       <c r="J228" s="14"/>
@@ -21250,7 +21340,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="229">
       <c r="A229" s="46">
         <v>53</v>
       </c>
@@ -21280,7 +21370,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="230">
       <c r="A230" s="46">
         <v>53</v>
       </c>
@@ -21310,7 +21400,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="231">
       <c r="A231" s="46">
         <v>53</v>
       </c>
@@ -21342,7 +21432,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="232">
       <c r="A232" s="46">
         <v>53</v>
       </c>
@@ -21364,7 +21454,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="233">
       <c r="A233" s="46">
         <v>54</v>
       </c>
@@ -21384,7 +21474,7 @@
         <v>514</v>
       </c>
       <c r="H233" s="86">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="I233" s="86"/>
       <c r="J233" s="14"/>
@@ -21393,7 +21483,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="234">
       <c r="A234" s="46">
         <v>54</v>
       </c>
@@ -21423,7 +21513,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="235">
       <c r="A235" s="46">
         <v>54</v>
       </c>
@@ -21453,7 +21543,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="236">
       <c r="A236" s="46">
         <v>54</v>
       </c>
@@ -21485,7 +21575,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="237">
       <c r="A237" s="46">
         <v>54</v>
       </c>
@@ -21507,7 +21597,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="238">
       <c r="A238" s="46">
         <v>55</v>
       </c>
@@ -21527,7 +21617,7 @@
         <v>514</v>
       </c>
       <c r="H238" s="86">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="I238" s="86"/>
       <c r="J238" s="14"/>
@@ -21536,7 +21626,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="239">
       <c r="A239" s="46">
         <v>55</v>
       </c>
@@ -21566,7 +21656,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="240">
       <c r="A240" s="46">
         <v>55</v>
       </c>
@@ -21596,7 +21686,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="241">
       <c r="A241" s="46">
         <v>55</v>
       </c>
@@ -21628,7 +21718,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="242">
       <c r="A242" s="46">
         <v>55</v>
       </c>
@@ -21650,7 +21740,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="243">
       <c r="A243" s="46">
         <v>56</v>
       </c>
@@ -21679,7 +21769,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="244">
       <c r="A244" s="46">
         <v>56</v>
       </c>
@@ -21709,7 +21799,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="245">
       <c r="A245" s="46">
         <v>56</v>
       </c>
@@ -21731,7 +21821,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="246">
       <c r="A246" s="46">
         <v>57</v>
       </c>
@@ -21760,7 +21850,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="247">
       <c r="A247" s="46">
         <v>57</v>
       </c>
@@ -21790,7 +21880,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="248">
       <c r="A248" s="46">
         <v>57</v>
       </c>
@@ -21820,7 +21910,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="249">
       <c r="A249" s="46">
         <v>57</v>
       </c>
@@ -21850,7 +21940,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="250">
       <c r="A250" s="46">
         <v>57</v>
       </c>
@@ -21880,7 +21970,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="251">
       <c r="A251" s="46">
         <v>57</v>
       </c>
@@ -21902,7 +21992,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="252">
       <c r="A252" s="46">
         <v>58</v>
       </c>
@@ -21931,7 +22021,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="253">
       <c r="A253" s="46">
         <v>58</v>
       </c>
@@ -21961,7 +22051,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="254">
       <c r="A254" s="46">
         <v>58</v>
       </c>
@@ -21991,7 +22081,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="255">
       <c r="A255" s="46">
         <v>58</v>
       </c>
@@ -22021,7 +22111,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="256">
       <c r="A256" s="46">
         <v>58</v>
       </c>
@@ -22043,7 +22133,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="257">
       <c r="A257" s="46">
         <v>59</v>
       </c>
@@ -22072,7 +22162,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="258">
       <c r="A258" s="46">
         <v>59</v>
       </c>
@@ -22102,7 +22192,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="259">
       <c r="A259" s="46">
         <v>59</v>
       </c>
@@ -22132,7 +22222,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="260">
       <c r="A260" s="46">
         <v>59</v>
       </c>
@@ -22162,7 +22252,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="261">
       <c r="A261" s="46">
         <v>59</v>
       </c>
@@ -22184,7 +22274,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="262">
       <c r="A262" s="46">
         <v>60</v>
       </c>
@@ -22204,7 +22294,7 @@
         <v>514</v>
       </c>
       <c r="H262" s="86">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="I262" s="86"/>
       <c r="J262" s="14"/>
@@ -22213,7 +22303,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="263">
       <c r="A263" s="46">
         <v>60</v>
       </c>
@@ -22243,7 +22333,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="264">
       <c r="A264" s="46">
         <v>60</v>
       </c>
@@ -22273,7 +22363,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="265">
       <c r="A265" s="46">
         <v>60</v>
       </c>
@@ -22305,7 +22395,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="266">
       <c r="A266" s="46">
         <v>60</v>
       </c>
@@ -22327,7 +22417,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="267">
       <c r="A267" s="46">
         <v>61</v>
       </c>
@@ -22356,7 +22446,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="268">
       <c r="A268" s="46">
         <v>61</v>
       </c>
@@ -22386,7 +22476,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="269">
       <c r="A269" s="46">
         <v>61</v>
       </c>
@@ -22416,7 +22506,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="270">
       <c r="A270" s="46">
         <v>61</v>
       </c>
@@ -22446,7 +22536,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="271">
       <c r="A271" s="46">
         <v>61</v>
       </c>
@@ -22476,7 +22566,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="272">
       <c r="A272" s="46">
         <v>61</v>
       </c>
@@ -22498,7 +22588,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="273">
       <c r="A273" s="46">
         <v>62</v>
       </c>
@@ -22527,7 +22617,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="274">
       <c r="A274" s="46">
         <v>62</v>
       </c>
@@ -22557,7 +22647,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="275">
       <c r="A275" s="46">
         <v>62</v>
       </c>
@@ -22587,7 +22677,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="276">
       <c r="A276" s="46">
         <v>62</v>
       </c>
@@ -22617,7 +22707,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="277">
       <c r="A277" s="46">
         <v>62</v>
       </c>
@@ -22639,7 +22729,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="278">
       <c r="A278" s="46">
         <v>63</v>
       </c>
@@ -22668,7 +22758,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="279">
       <c r="A279" s="46">
         <v>63</v>
       </c>
@@ -22698,7 +22788,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="280">
       <c r="A280" s="46">
         <v>63</v>
       </c>
@@ -22728,7 +22818,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="281">
       <c r="A281" s="46">
         <v>63</v>
       </c>
@@ -22758,7 +22848,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="282">
       <c r="A282" s="46">
         <v>63</v>
       </c>
@@ -22780,7 +22870,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="283">
       <c r="A283" s="46">
         <v>64</v>
       </c>
@@ -22812,7 +22902,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="284">
       <c r="A284" s="46">
         <v>64</v>
       </c>
@@ -22844,7 +22934,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="285">
       <c r="A285" s="46">
         <v>64</v>
       </c>
@@ -22876,7 +22966,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="286">
       <c r="A286" s="46">
         <v>64</v>
       </c>
@@ -22908,7 +22998,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="287">
       <c r="A287" s="46">
         <v>64</v>
       </c>
@@ -22940,7 +23030,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="288">
       <c r="A288" s="46">
         <v>64</v>
       </c>
@@ -22972,7 +23062,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="289">
       <c r="A289" s="46">
         <v>64</v>
       </c>
@@ -22996,7 +23086,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="290">
       <c r="A290" s="46">
         <v>65</v>
       </c>
@@ -23025,7 +23115,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="291">
       <c r="A291" s="46">
         <v>65</v>
       </c>
@@ -23055,7 +23145,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="292">
       <c r="A292" s="46">
         <v>65</v>
       </c>
@@ -23085,7 +23175,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="293">
       <c r="A293" s="46">
         <v>65</v>
       </c>
@@ -23115,7 +23205,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="294">
       <c r="A294" s="46">
         <v>65</v>
       </c>
@@ -23137,7 +23227,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="295">
       <c r="A295" s="46">
         <v>66</v>
       </c>
@@ -23169,7 +23259,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="296">
       <c r="A296" s="46">
         <v>66</v>
       </c>
@@ -23201,7 +23291,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="297">
       <c r="A297" s="46">
         <v>66</v>
       </c>
@@ -23225,7 +23315,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="298">
       <c r="A298" s="46">
         <v>67</v>
       </c>
@@ -23257,7 +23347,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="299">
       <c r="A299" s="46">
         <v>67</v>
       </c>
@@ -23287,7 +23377,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="300">
       <c r="A300" s="46">
         <v>67</v>
       </c>
@@ -23309,7 +23399,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="301">
       <c r="A301" s="46">
         <v>68</v>
       </c>
@@ -23341,7 +23431,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="302">
       <c r="A302" s="46">
         <v>68</v>
       </c>
@@ -23373,7 +23463,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="303">
       <c r="A303" s="46">
         <v>68</v>
       </c>
@@ -23405,7 +23495,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="304">
       <c r="A304" s="46">
         <v>68</v>
       </c>
@@ -23429,7 +23519,7 @@
       </c>
       <c r="H304" s="86"/>
       <c r="I304" s="86">
-        <v>37.409999999999997</v>
+        <v>37.41</v>
       </c>
       <c r="J304" s="14"/>
       <c r="K304" s="46">
@@ -23437,7 +23527,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="305">
       <c r="A305" s="46">
         <v>68</v>
       </c>
@@ -23460,7 +23550,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="306">
       <c r="A306" s="46">
         <v>69</v>
       </c>
@@ -23492,7 +23582,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="307">
       <c r="A307" s="46">
         <v>69</v>
       </c>
@@ -23524,7 +23614,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="308">
       <c r="A308" s="46">
         <v>69</v>
       </c>
@@ -23556,7 +23646,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="309">
       <c r="A309" s="46">
         <v>69</v>
       </c>
@@ -23588,7 +23678,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="310">
       <c r="A310" s="46">
         <v>69</v>
       </c>
@@ -23620,7 +23710,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="311">
       <c r="A311" s="46">
         <v>69</v>
       </c>
@@ -23652,7 +23742,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="312">
       <c r="A312" s="46">
         <v>69</v>
       </c>
@@ -23684,7 +23774,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="313">
       <c r="A313" s="46">
         <v>69</v>
       </c>
@@ -23705,7 +23795,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="314">
       <c r="A314" s="46">
         <v>70</v>
       </c>
@@ -23737,7 +23827,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="315">
       <c r="A315" s="46">
         <v>70</v>
       </c>
@@ -23769,7 +23859,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="316">
       <c r="A316" s="46">
         <v>70</v>
       </c>
@@ -23801,7 +23891,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="317">
       <c r="A317" s="46">
         <v>70</v>
       </c>
@@ -23833,7 +23923,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="318">
       <c r="A318" s="46">
         <v>70</v>
       </c>
@@ -23865,7 +23955,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="319">
       <c r="A319" s="46">
         <v>70</v>
       </c>
@@ -23897,7 +23987,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="320">
       <c r="A320" s="46">
         <v>70</v>
       </c>
@@ -23929,7 +24019,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="321">
       <c r="A321" s="46">
         <v>70</v>
       </c>
@@ -23952,7 +24042,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="322">
       <c r="A322" s="46">
         <v>71</v>
       </c>
@@ -23984,7 +24074,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="323">
       <c r="A323" s="46">
         <v>71</v>
       </c>
@@ -24016,7 +24106,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="324">
       <c r="A324" s="46">
         <v>71</v>
       </c>
@@ -24048,7 +24138,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="325">
       <c r="A325" s="46">
         <v>71</v>
       </c>
@@ -24080,7 +24170,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="326">
       <c r="A326" s="46">
         <v>71</v>
       </c>
@@ -24112,7 +24202,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="327">
       <c r="A327" s="46">
         <v>71</v>
       </c>
@@ -24144,7 +24234,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="328">
       <c r="A328" s="46">
         <v>71</v>
       </c>
@@ -24176,7 +24266,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="329">
       <c r="A329" s="46">
         <v>71</v>
       </c>
@@ -24199,7 +24289,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="330">
       <c r="A330" s="46">
         <v>72</v>
       </c>
@@ -24231,7 +24321,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="331">
       <c r="A331" s="46">
         <v>72</v>
       </c>
@@ -24263,7 +24353,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="332">
       <c r="A332" s="46">
         <v>72</v>
       </c>
@@ -24295,7 +24385,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="333">
       <c r="A333" s="46">
         <v>72</v>
       </c>
@@ -24327,7 +24417,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="334">
       <c r="A334" s="46">
         <v>72</v>
       </c>
@@ -24350,7 +24440,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="335">
       <c r="A335" s="46">
         <v>73</v>
       </c>
@@ -24382,7 +24472,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="336">
       <c r="A336" s="46">
         <v>73</v>
       </c>
@@ -24414,7 +24504,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="337">
       <c r="A337" s="46">
         <v>73</v>
       </c>
@@ -24437,7 +24527,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="338">
       <c r="A338" s="46">
         <v>74</v>
       </c>
@@ -24469,7 +24559,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="339">
       <c r="A339" s="46">
         <v>74</v>
       </c>
@@ -24503,7 +24593,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="340">
       <c r="A340" s="46">
         <v>74</v>
       </c>
@@ -24537,7 +24627,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="341">
       <c r="A341" s="46">
         <v>74</v>
       </c>
@@ -24571,7 +24661,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="342">
       <c r="A342" s="46">
         <v>74</v>
       </c>
@@ -24605,7 +24695,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="343">
       <c r="A343" s="46">
         <v>74</v>
       </c>
@@ -24628,7 +24718,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="344">
       <c r="A344" s="46">
         <v>75</v>
       </c>
@@ -24660,7 +24750,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="345">
       <c r="A345" s="46">
         <v>75</v>
       </c>
@@ -24692,7 +24782,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="346">
       <c r="A346" s="46">
         <v>75</v>
       </c>
@@ -24715,7 +24805,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="347">
       <c r="A347" s="46">
         <v>76</v>
       </c>
@@ -24747,7 +24837,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="348">
       <c r="A348" s="46">
         <v>76</v>
       </c>
@@ -24779,7 +24869,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="349">
       <c r="A349" s="46">
         <v>76</v>
       </c>
@@ -24802,7 +24892,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="350">
       <c r="A350" s="46">
         <v>77</v>
       </c>
@@ -24834,7 +24924,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="351">
       <c r="A351" s="46">
         <v>77</v>
       </c>
@@ -24866,7 +24956,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="352">
       <c r="A352" s="46">
         <v>77</v>
       </c>
@@ -24898,7 +24988,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="353">
       <c r="A353" s="46">
         <v>77</v>
       </c>
@@ -24930,7 +25020,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="354">
       <c r="A354" s="46">
         <v>77</v>
       </c>
@@ -24955,7 +25045,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="355">
       <c r="A355" s="46">
         <v>78</v>
       </c>
@@ -24987,7 +25077,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="356">
       <c r="A356" s="46">
         <v>78</v>
       </c>
@@ -25019,7 +25109,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="357">
       <c r="A357" s="46">
         <v>78</v>
       </c>
@@ -25051,7 +25141,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="358">
       <c r="A358" s="46">
         <v>78</v>
       </c>
@@ -25083,7 +25173,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="359">
       <c r="A359" s="46">
         <v>78</v>
       </c>
@@ -25108,7 +25198,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="360">
       <c r="A360" s="46">
         <v>79</v>
       </c>
@@ -25140,7 +25230,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="361">
       <c r="A361" s="46">
         <v>79</v>
       </c>
@@ -25164,7 +25254,7 @@
       </c>
       <c r="H361" s="86"/>
       <c r="I361" s="86">
-        <v>9.9499999999999993</v>
+        <v>9.95</v>
       </c>
       <c r="J361" s="14"/>
       <c r="K361" s="46">
@@ -25172,7 +25262,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="362">
       <c r="A362" s="46">
         <v>79</v>
       </c>
@@ -25204,7 +25294,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="363">
       <c r="A363" s="46">
         <v>79</v>
       </c>
@@ -25234,7 +25324,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="364">
       <c r="A364" s="46">
         <v>79</v>
       </c>
@@ -25259,7 +25349,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="365">
       <c r="A365" s="46">
         <v>80</v>
       </c>
@@ -25288,7 +25378,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="366">
       <c r="A366" s="46">
         <v>80</v>
       </c>
@@ -25318,7 +25408,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="367">
       <c r="A367" s="46">
         <v>80</v>
       </c>
@@ -25341,7 +25431,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="368">
       <c r="A368" s="46">
         <v>81</v>
       </c>
@@ -25362,7 +25452,7 @@
         <v>514</v>
       </c>
       <c r="H368" s="86">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="I368" s="86"/>
       <c r="J368" s="14"/>
@@ -25371,7 +25461,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="369">
       <c r="A369" s="46">
         <v>81</v>
       </c>
@@ -25401,7 +25491,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="370">
       <c r="A370" s="46">
         <v>81</v>
       </c>
@@ -25431,7 +25521,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="371">
       <c r="A371" s="46">
         <v>81</v>
       </c>
@@ -25463,7 +25553,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="372">
       <c r="A372" s="46">
         <v>81</v>
       </c>
@@ -25486,7 +25576,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="373">
       <c r="A373" s="46">
         <v>82</v>
       </c>
@@ -25518,7 +25608,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="374">
       <c r="A374" s="46">
         <v>82</v>
       </c>
@@ -25550,7 +25640,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="375">
       <c r="A375" s="46">
         <v>82</v>
       </c>
@@ -25575,7 +25665,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="376">
       <c r="A376" s="46">
         <v>83</v>
       </c>
@@ -25604,7 +25694,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="377">
       <c r="A377" s="46">
         <v>83</v>
       </c>
@@ -25634,7 +25724,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="378">
       <c r="A378" s="46">
         <v>83</v>
       </c>
@@ -25664,7 +25754,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="379">
       <c r="A379" s="46">
         <v>83</v>
       </c>
@@ -25694,7 +25784,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="380">
       <c r="A380" s="46">
         <v>83</v>
       </c>
@@ -25717,7 +25807,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="381">
       <c r="A381" s="46">
         <v>84</v>
       </c>
@@ -25749,7 +25839,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="382">
       <c r="A382" s="46">
         <v>84</v>
       </c>
@@ -25781,7 +25871,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="383">
       <c r="A383" s="46">
         <v>84</v>
       </c>
@@ -25806,7 +25896,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="384">
       <c r="A384" s="46">
         <v>85</v>
       </c>
@@ -25826,7 +25916,7 @@
         <v>514</v>
       </c>
       <c r="H384" s="86">
-        <v>129.94999999999999</v>
+        <v>129.95</v>
       </c>
       <c r="I384" s="86"/>
       <c r="J384" s="14"/>
@@ -25835,7 +25925,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="385">
       <c r="A385" s="46">
         <v>85</v>
       </c>
@@ -25865,7 +25955,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="386">
       <c r="A386" s="46">
         <v>85</v>
       </c>
@@ -25895,7 +25985,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="387">
       <c r="A387" s="46">
         <v>85</v>
       </c>
@@ -25927,7 +26017,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="388">
       <c r="A388" s="46">
         <v>85</v>
       </c>
@@ -25950,7 +26040,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="389">
       <c r="A389" s="46">
         <v>86</v>
       </c>
@@ -25970,7 +26060,7 @@
         <v>514</v>
       </c>
       <c r="H389" s="86">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="I389" s="86"/>
       <c r="J389" s="14"/>
@@ -25979,7 +26069,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="390">
       <c r="A390" s="46">
         <v>86</v>
       </c>
@@ -26001,7 +26091,7 @@
       </c>
       <c r="H390" s="86"/>
       <c r="I390" s="86">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="J390" s="14"/>
       <c r="K390" s="46">
@@ -26009,7 +26099,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="391">
       <c r="A391" s="46">
         <v>86</v>
       </c>
@@ -26032,7 +26122,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="392">
       <c r="A392" s="46">
         <v>87</v>
       </c>
@@ -26064,7 +26154,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="393">
       <c r="A393" s="46">
         <v>87</v>
       </c>
@@ -26096,7 +26186,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="394">
       <c r="A394" s="46">
         <v>87</v>
       </c>
@@ -26128,7 +26218,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="395">
       <c r="A395" s="46">
         <v>87</v>
       </c>
@@ -26160,7 +26250,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="396">
       <c r="A396" s="46">
         <v>87</v>
       </c>
@@ -26185,7 +26275,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="397">
       <c r="A397" s="46">
         <v>88</v>
       </c>
@@ -26217,7 +26307,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="398">
       <c r="A398" s="46">
         <v>88</v>
       </c>
@@ -26249,7 +26339,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="399">
       <c r="A399" s="46">
         <v>88</v>
       </c>
@@ -26274,7 +26364,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="400">
       <c r="A400" s="46">
         <v>89</v>
       </c>
@@ -26305,7 +26395,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="401">
       <c r="A401" s="46">
         <v>89</v>
       </c>
@@ -26336,7 +26426,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="402">
       <c r="A402" s="46">
         <v>89</v>
       </c>
@@ -26359,7 +26449,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="403">
       <c r="A403" s="46">
         <v>90</v>
       </c>
@@ -26387,7 +26477,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="404">
       <c r="A404" s="46">
         <v>90</v>
       </c>
@@ -26416,7 +26506,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="405">
       <c r="A405" s="46">
         <v>90</v>
       </c>
@@ -26435,7 +26525,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="406">
       <c r="A406" s="46">
         <v>91</v>
       </c>
@@ -26465,7 +26555,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="407">
       <c r="A407" s="46">
         <v>91</v>
       </c>
@@ -26495,7 +26585,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="408">
       <c r="A408" s="46">
         <v>91</v>
       </c>
@@ -26516,7 +26606,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="409">
       <c r="A409" s="46">
         <v>92</v>
       </c>
@@ -26546,7 +26636,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="410">
       <c r="A410" s="46">
         <v>92</v>
       </c>
@@ -26576,7 +26666,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="411">
       <c r="A411" s="46">
         <v>92</v>
       </c>
@@ -26597,7 +26687,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="412">
       <c r="A412" s="46">
         <v>93</v>
       </c>
@@ -26627,7 +26717,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="413">
       <c r="A413" s="46">
         <v>93</v>
       </c>
@@ -26657,7 +26747,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="414">
       <c r="A414" s="46">
         <v>93</v>
       </c>
@@ -26678,7 +26768,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="415">
       <c r="A415" s="46">
         <v>94</v>
       </c>
@@ -26708,7 +26798,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="416">
       <c r="A416" s="46">
         <v>94</v>
       </c>
@@ -26738,7 +26828,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="417">
       <c r="A417" s="46">
         <v>94</v>
       </c>
@@ -26759,7 +26849,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="418">
       <c r="A418" s="46">
         <v>95</v>
       </c>
@@ -26789,7 +26879,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="419">
       <c r="A419" s="46">
         <v>95</v>
       </c>
@@ -26819,7 +26909,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="420">
       <c r="A420" s="46">
         <v>95</v>
       </c>
@@ -26840,7 +26930,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="421">
       <c r="A421" s="46">
         <v>96</v>
       </c>
@@ -26870,7 +26960,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="422">
       <c r="A422" s="46">
         <v>96</v>
       </c>
@@ -26900,7 +26990,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="423">
       <c r="A423" s="46">
         <v>96</v>
       </c>
@@ -26921,7 +27011,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="424">
       <c r="A424" s="46">
         <v>97</v>
       </c>
@@ -26951,7 +27041,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="425">
       <c r="A425" s="46">
         <v>97</v>
       </c>
@@ -26981,7 +27071,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="426">
       <c r="A426" s="46">
         <v>97</v>
       </c>
@@ -27002,7 +27092,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="427">
       <c r="A427" s="46">
         <v>98</v>
       </c>
@@ -27032,7 +27122,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="428">
       <c r="A428" s="46">
         <v>98</v>
       </c>
@@ -27062,7 +27152,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="429">
       <c r="A429" s="46">
         <v>98</v>
       </c>
@@ -27083,7 +27173,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="430">
       <c r="A430" s="46">
         <v>99</v>
       </c>
@@ -27113,7 +27203,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="431">
       <c r="A431" s="46">
         <v>99</v>
       </c>
@@ -27143,7 +27233,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="432">
       <c r="A432" s="46">
         <v>99</v>
       </c>
@@ -27164,7 +27254,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="433" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="433">
       <c r="A433" s="46">
         <v>100</v>
       </c>
@@ -27194,7 +27284,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="434">
       <c r="A434" s="46">
         <v>100</v>
       </c>
@@ -27224,7 +27314,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="435">
       <c r="A435" s="46">
         <v>100</v>
       </c>
@@ -27245,7 +27335,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="436" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="436">
       <c r="A436" s="46">
         <v>101</v>
       </c>
@@ -27275,7 +27365,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="437" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="437">
       <c r="A437" s="46">
         <v>101</v>
       </c>
@@ -27305,7 +27395,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="438">
       <c r="A438" s="46">
         <v>101</v>
       </c>
@@ -27326,7 +27416,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="439">
       <c r="A439" s="46">
         <v>102</v>
       </c>
@@ -27356,7 +27446,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="440" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="440">
       <c r="A440" s="46">
         <v>102</v>
       </c>
@@ -27386,7 +27476,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="441" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="441">
       <c r="A441" s="46">
         <v>102</v>
       </c>
@@ -27407,7 +27497,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="442" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="442">
       <c r="A442" s="46">
         <v>103</v>
       </c>
@@ -27437,7 +27527,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="443" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="443">
       <c r="A443" s="46">
         <v>103</v>
       </c>
@@ -27467,7 +27557,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="444" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="444">
       <c r="A444" s="46">
         <v>103</v>
       </c>
@@ -27488,7 +27578,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="445" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="445">
       <c r="A445" s="46">
         <v>104</v>
       </c>
@@ -27518,7 +27608,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="446" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="446">
       <c r="A446" s="46">
         <v>104</v>
       </c>
@@ -27548,7 +27638,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="447" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="447">
       <c r="A447" s="46">
         <v>104</v>
       </c>
@@ -27569,7 +27659,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="448" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="448">
       <c r="A448" s="46">
         <v>105</v>
       </c>
@@ -27599,7 +27689,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="449" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="449">
       <c r="A449" s="46">
         <v>105</v>
       </c>
@@ -27629,7 +27719,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="450" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="450">
       <c r="A450" s="46">
         <v>105</v>
       </c>
@@ -27650,7 +27740,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="451" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="451">
       <c r="A451" s="46">
         <v>106</v>
       </c>
@@ -27680,7 +27770,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="452" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="452">
       <c r="A452" s="46">
         <v>106</v>
       </c>
@@ -27710,7 +27800,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="453" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="453">
       <c r="A453" s="46">
         <v>106</v>
       </c>
@@ -27731,7 +27821,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="454" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="454">
       <c r="A454" s="46">
         <v>107</v>
       </c>
@@ -27761,7 +27851,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="455" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="455">
       <c r="A455" s="46">
         <v>107</v>
       </c>
@@ -27791,7 +27881,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="456" spans="1:11" x14ac:dyDescent="0.25">
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="456">
       <c r="A456" s="46">
         <v>107</v>
       </c>
@@ -27810,6 +27900,258 @@
       <c r="K456" s="46">
         <f>ROW()</f>
         <v>456</v>
+      </c>
+    </row>
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="457">
+      <c r="A457" s="46">
+        <v>108</v>
+      </c>
+      <c r="B457" s="41">
+        <v>45331</v>
+      </c>
+      <c r="C457" s="100">
+        <v>108</v>
+      </c>
+      <c r="E457" s="103" t="s">
+        <v>518</v>
+      </c>
+      <c r="F457" s="100" t="s">
+        <v>446</v>
+      </c>
+      <c r="G457" s="103" t="s">
+        <v>402</v>
+      </c>
+      <c r="H457" s="101">
+        <v>262.44</v>
+      </c>
+      <c r="I457" s="101"/>
+      <c r="K457" s="46">
+        <f>ROW()</f>
+        <v>457</v>
+      </c>
+    </row>
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="458">
+      <c r="A458" s="46">
+        <v>108</v>
+      </c>
+      <c r="B458" s="48">
+        <v>45331</v>
+      </c>
+      <c r="C458" s="104">
+        <v>108</v>
+      </c>
+      <c r="D458" s="42"/>
+      <c r="E458" s="105" t="s">
+        <v>518</v>
+      </c>
+      <c r="F458" s="100" t="s">
+        <v>422</v>
+      </c>
+      <c r="G458" s="103" t="s">
+        <v>423</v>
+      </c>
+      <c r="H458" s="101"/>
+      <c r="I458" s="101">
+        <v>250</v>
+      </c>
+      <c r="K458" s="46">
+        <f>ROW()</f>
+        <v>458</v>
+      </c>
+    </row>
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="459">
+      <c r="A459" s="46">
+        <v>108</v>
+      </c>
+      <c r="B459" s="48">
+        <v>45331</v>
+      </c>
+      <c r="C459" s="104">
+        <v>108</v>
+      </c>
+      <c r="D459" s="42"/>
+      <c r="E459" s="105" t="s">
+        <v>518</v>
+      </c>
+      <c r="F459" s="100" t="s">
+        <v>409</v>
+      </c>
+      <c r="G459" s="103" t="s">
+        <v>410</v>
+      </c>
+      <c r="H459" s="101"/>
+      <c r="I459" s="101">
+        <v>12.5</v>
+      </c>
+      <c r="K459" s="46">
+        <f>ROW()</f>
+        <v>459</v>
+      </c>
+    </row>
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="460">
+      <c r="A460" s="46">
+        <v>108</v>
+      </c>
+      <c r="B460" s="48">
+        <v>45331</v>
+      </c>
+      <c r="C460" s="104">
+        <v>108</v>
+      </c>
+      <c r="D460" s="42"/>
+      <c r="E460" s="105" t="s">
+        <v>518</v>
+      </c>
+      <c r="F460" s="100" t="s">
+        <v>417</v>
+      </c>
+      <c r="G460" s="103" t="s">
+        <v>418</v>
+      </c>
+      <c r="H460" s="101"/>
+      <c r="I460" s="101">
+        <v>24.94</v>
+      </c>
+      <c r="K460" s="46">
+        <f>ROW()</f>
+        <v>460</v>
+      </c>
+    </row>
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="461">
+      <c r="A461" s="46">
+        <v>108</v>
+      </c>
+      <c r="B461" s="48">
+        <v>45331</v>
+      </c>
+      <c r="C461" s="104">
+        <v>108</v>
+      </c>
+      <c r="D461" s="42"/>
+      <c r="E461" s="105" t="s">
+        <v>518</v>
+      </c>
+      <c r="F461" s="100" t="s">
+        <v>431</v>
+      </c>
+      <c r="G461" s="103" t="s">
+        <v>432</v>
+      </c>
+      <c r="H461" s="101">
+        <v>25</v>
+      </c>
+      <c r="I461" s="101"/>
+      <c r="K461" s="46">
+        <f>ROW()</f>
+        <v>461</v>
+      </c>
+    </row>
+    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="462">
+      <c r="A462" s="46">
+        <v>108</v>
+      </c>
+      <c r="B462" s="48">
+        <v>45331</v>
+      </c>
+      <c r="C462" s="104">
+        <v>108</v>
+      </c>
+      <c r="D462" s="42"/>
+      <c r="E462" s="105" t="s">
+        <v>518</v>
+      </c>
+      <c r="K462" s="46">
+        <f>ROW()</f>
+        <v>462</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="463">
+      <c r="A463" s="103">
+        <v>109</v>
+      </c>
+      <c r="B463" s="78">
+        <v>45331</v>
+      </c>
+      <c r="C463" s="103">
+        <v>109</v>
+      </c>
+      <c r="D463" s="103" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="E463" s="103" t="inlineStr">
+        <is>
+          <t>TEST - TEST - TEST</t>
+        </is>
+      </c>
+      <c r="F463" s="103" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="G463" s="103" t="inlineStr">
+        <is>
+          <t>Encaisse</t>
+        </is>
+      </c>
+      <c r="H463" s="76">
+        <v>199.99</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="464">
+      <c r="A464" s="103">
+        <v>109</v>
+      </c>
+      <c r="B464" s="78">
+        <v>45331</v>
+      </c>
+      <c r="C464" s="103">
+        <v>109</v>
+      </c>
+      <c r="D464" s="103" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="E464" s="103" t="inlineStr">
+        <is>
+          <t>TEST - TEST - TEST</t>
+        </is>
+      </c>
+      <c r="F464" s="103" t="inlineStr">
+        <is>
+          <t>5013</t>
+        </is>
+      </c>
+      <c r="G464" s="103" t="inlineStr">
+        <is>
+          <t>Frais financiers</t>
+        </is>
+      </c>
+      <c r="I464" s="76">
+        <v>199.99</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="465">
+      <c r="A465" s="103">
+        <v>109</v>
+      </c>
+      <c r="B465" s="78">
+        <v>45331</v>
+      </c>
+      <c r="C465" s="103">
+        <v>109</v>
+      </c>
+      <c r="D465" s="103" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="E465" s="103" t="inlineStr">
+        <is>
+          <t>TEST - TEST - TEST</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v2.0 - Encaissement intégré, mais pas testé à 100 %
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18352A12-E438-4DB7-A07B-DA402823B133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847F540B-EFB4-4517-B5BC-F01AD732AC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2728" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2766" uniqueCount="635">
   <si>
     <t>TEC_ID</t>
   </si>
@@ -1974,6 +1974,21 @@
   </si>
   <si>
     <t>Test d'écriture en BD (Sortie)</t>
+  </si>
+  <si>
+    <t>TEST - TEST - TEST</t>
+  </si>
+  <si>
+    <t>Encaissement # 16</t>
+  </si>
+  <si>
+    <t>Encaissement # 17</t>
+  </si>
+  <si>
+    <t>Encaissement # 18</t>
+  </si>
+  <si>
+    <t>Test avec comptabilisation</t>
   </si>
 </sst>
 </file>
@@ -2278,7 +2293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2553,6 +2568,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire 2" xfId="1" xr:uid="{7066D7D9-A0C5-4744-AD1B-CDB1C4228FB1}"/>
@@ -2627,6 +2651,7 @@
       <sheetName val="Encaissements_Détail"/>
       <sheetName val="Enc_Clients"/>
       <sheetName val="Enc_Admin"/>
+      <sheetName val="Invoice_Payment_Manager - v1.4"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -2868,6 +2893,7 @@
       </sheetData>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -14484,12 +14510,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{E0D58006-DE1D-488F-9BB7-8096C5818030}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D58006-DE1D-488F-9BB7-8096C5818030}">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="A1:K465"/>
+  <dimension ref="A1:K474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A427" zoomScale="90" zoomScaleNormal="90" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="B465" sqref="B465"/>
+    <sheetView tabSelected="1" topLeftCell="A445" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H480" sqref="H480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14506,7 +14532,7 @@
     <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:11" ht="25.5" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>531</v>
       </c>
@@ -14541,7 +14567,7 @@
         <v>397</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="46">
         <v>1</v>
       </c>
@@ -14573,7 +14599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row spans="1:11" ht="15.75" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="46">
         <v>1</v>
       </c>
@@ -14605,7 +14631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="46">
         <v>1</v>
       </c>
@@ -14626,7 +14652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="46">
         <v>2</v>
       </c>
@@ -14658,7 +14684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="46">
         <v>2</v>
       </c>
@@ -14690,7 +14716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="46">
         <v>2</v>
       </c>
@@ -14708,7 +14734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="46">
         <v>3</v>
       </c>
@@ -14740,7 +14766,7 @@
         <v>8</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="46">
         <v>3</v>
       </c>
@@ -14772,7 +14798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="46">
         <v>3</v>
       </c>
@@ -14792,7 +14818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="46">
         <v>4</v>
       </c>
@@ -14824,7 +14850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="46">
         <v>4</v>
       </c>
@@ -14856,7 +14882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="13">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="46">
         <v>4</v>
       </c>
@@ -14879,7 +14905,7 @@
         <v>415</v>
       </c>
       <c r="H13" s="86">
-        <v>570.92</v>
+        <v>570.91999999999996</v>
       </c>
       <c r="I13" s="86"/>
       <c r="J13" s="14"/>
@@ -14888,7 +14914,7 @@
         <v>13</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="14">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="46">
         <v>4</v>
       </c>
@@ -14920,7 +14946,7 @@
         <v>14</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="46">
         <v>4</v>
       </c>
@@ -14952,7 +14978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="16">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="46">
         <v>4</v>
       </c>
@@ -14976,7 +15002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="17">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="46">
         <v>5</v>
       </c>
@@ -15008,7 +15034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="18">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="46">
         <v>5</v>
       </c>
@@ -15040,7 +15066,7 @@
         <v>18</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="19">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="46">
         <v>5</v>
       </c>
@@ -15072,7 +15098,7 @@
         <v>19</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="20">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="46">
         <v>5</v>
       </c>
@@ -15104,7 +15130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="21">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="46">
         <v>5</v>
       </c>
@@ -15136,7 +15162,7 @@
         <v>21</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="22">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="46">
         <v>5</v>
       </c>
@@ -15168,7 +15194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="23">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="46">
         <v>5</v>
       </c>
@@ -15200,7 +15226,7 @@
         <v>23</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="24">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="46">
         <v>5</v>
       </c>
@@ -15232,7 +15258,7 @@
         <v>24</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="46">
         <v>5</v>
       </c>
@@ -15256,7 +15282,7 @@
         <v>25</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="26">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="46">
         <v>6</v>
       </c>
@@ -15288,7 +15314,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="27">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="46">
         <v>6</v>
       </c>
@@ -15320,7 +15346,7 @@
         <v>27</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="28">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="46">
         <v>6</v>
       </c>
@@ -15352,7 +15378,7 @@
         <v>28</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="29">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="46">
         <v>6</v>
       </c>
@@ -15384,7 +15410,7 @@
         <v>29</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="30">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="46">
         <v>6</v>
       </c>
@@ -15416,7 +15442,7 @@
         <v>30</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="31">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="46">
         <v>6</v>
       </c>
@@ -15448,7 +15474,7 @@
         <v>31</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="32">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="46">
         <v>6</v>
       </c>
@@ -15480,7 +15506,7 @@
         <v>32</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="33">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="46">
         <v>6</v>
       </c>
@@ -15512,7 +15538,7 @@
         <v>33</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="34">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="46">
         <v>6</v>
       </c>
@@ -15536,7 +15562,7 @@
         <v>34</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="46">
         <v>7</v>
       </c>
@@ -15568,7 +15594,7 @@
         <v>35</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="36">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="46">
         <v>7</v>
       </c>
@@ -15600,7 +15626,7 @@
         <v>36</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="37">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="46">
         <v>7</v>
       </c>
@@ -15632,7 +15658,7 @@
         <v>37</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="38">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="46">
         <v>7</v>
       </c>
@@ -15664,7 +15690,7 @@
         <v>38</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="39">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="46">
         <v>7</v>
       </c>
@@ -15696,7 +15722,7 @@
         <v>39</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="40">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="46">
         <v>7</v>
       </c>
@@ -15728,7 +15754,7 @@
         <v>40</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="41">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="46">
         <v>7</v>
       </c>
@@ -15752,7 +15778,7 @@
       </c>
       <c r="H41" s="86"/>
       <c r="I41" s="86">
-        <v>67.68</v>
+        <v>67.680000000000007</v>
       </c>
       <c r="J41" s="14"/>
       <c r="K41" s="46">
@@ -15760,7 +15786,7 @@
         <v>41</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="42">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="46">
         <v>7</v>
       </c>
@@ -15792,7 +15818,7 @@
         <v>42</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="43">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="46">
         <v>7</v>
       </c>
@@ -15816,7 +15842,7 @@
         <v>43</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="44">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="46">
         <v>8</v>
       </c>
@@ -15839,7 +15865,7 @@
         <v>402</v>
       </c>
       <c r="H44" s="86">
-        <v>1248.63</v>
+        <v>1248.6300000000001</v>
       </c>
       <c r="I44" s="86"/>
       <c r="J44" s="14"/>
@@ -15848,7 +15874,7 @@
         <v>44</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="46">
         <v>8</v>
       </c>
@@ -15880,7 +15906,7 @@
         <v>45</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="46">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="46">
         <v>8</v>
       </c>
@@ -15912,7 +15938,7 @@
         <v>46</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="47">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="46">
         <v>8</v>
       </c>
@@ -15944,7 +15970,7 @@
         <v>47</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="48">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="46">
         <v>8</v>
       </c>
@@ -15976,7 +16002,7 @@
         <v>48</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="49">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="46">
         <v>8</v>
       </c>
@@ -16008,7 +16034,7 @@
         <v>49</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="50">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="46">
         <v>8</v>
       </c>
@@ -16040,7 +16066,7 @@
         <v>50</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="51">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="46">
         <v>8</v>
       </c>
@@ -16064,7 +16090,7 @@
         <v>51</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="52">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="46">
         <v>9</v>
       </c>
@@ -16087,7 +16113,7 @@
         <v>399</v>
       </c>
       <c r="H52" s="86">
-        <v>1248.63</v>
+        <v>1248.6300000000001</v>
       </c>
       <c r="I52" s="86"/>
       <c r="J52" s="14"/>
@@ -16096,7 +16122,7 @@
         <v>52</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="53">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="46">
         <v>9</v>
       </c>
@@ -16120,7 +16146,7 @@
       </c>
       <c r="H53" s="86"/>
       <c r="I53" s="86">
-        <v>1248.63</v>
+        <v>1248.6300000000001</v>
       </c>
       <c r="J53" s="14"/>
       <c r="K53" s="46">
@@ -16128,7 +16154,7 @@
         <v>53</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="54">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="46">
         <v>9</v>
       </c>
@@ -16152,7 +16178,7 @@
         <v>54</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="55">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="46">
         <v>10</v>
       </c>
@@ -16184,7 +16210,7 @@
         <v>55</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="56">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="46">
         <v>10</v>
       </c>
@@ -16216,7 +16242,7 @@
         <v>56</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="57">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="46">
         <v>10</v>
       </c>
@@ -16233,7 +16259,7 @@
         <v>67</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="58">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="46">
         <v>11</v>
       </c>
@@ -16265,7 +16291,7 @@
         <v>58</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="59">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="46">
         <v>11</v>
       </c>
@@ -16297,7 +16323,7 @@
         <v>59</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="60">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="46">
         <v>11</v>
       </c>
@@ -16321,7 +16347,7 @@
         <v>60</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="61">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="46">
         <v>12</v>
       </c>
@@ -16350,7 +16376,7 @@
         <v>61</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="62">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="46">
         <v>12</v>
       </c>
@@ -16380,7 +16406,7 @@
         <v>62</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="63">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="46">
         <v>12</v>
       </c>
@@ -16410,7 +16436,7 @@
         <v>63</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="64">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="46">
         <v>12</v>
       </c>
@@ -16432,7 +16458,7 @@
       </c>
       <c r="H64" s="86"/>
       <c r="I64" s="86">
-        <v>4585.4</v>
+        <v>4585.3999999999996</v>
       </c>
       <c r="J64" s="14"/>
       <c r="K64" s="46">
@@ -16440,7 +16466,7 @@
         <v>64</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="65">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="46">
         <v>12</v>
       </c>
@@ -16462,7 +16488,7 @@
         <v>65</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="66">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="46">
         <v>13</v>
       </c>
@@ -16494,7 +16520,7 @@
         <v>66</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="67">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="46">
         <v>13</v>
       </c>
@@ -16526,7 +16552,7 @@
         <v>67</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="68">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="46">
         <v>13</v>
       </c>
@@ -16558,7 +16584,7 @@
         <v>68</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="69">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="46">
         <v>13</v>
       </c>
@@ -16590,7 +16616,7 @@
         <v>69</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="70">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="46">
         <v>13</v>
       </c>
@@ -16614,7 +16640,7 @@
         <v>70</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="71">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="46">
         <v>14</v>
       </c>
@@ -16637,7 +16663,7 @@
         <v>402</v>
       </c>
       <c r="H71" s="86">
-        <v>1034.91</v>
+        <v>1034.9100000000001</v>
       </c>
       <c r="I71" s="86"/>
       <c r="J71" s="14"/>
@@ -16646,7 +16672,7 @@
         <v>71</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="72">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="46">
         <v>14</v>
       </c>
@@ -16678,7 +16704,7 @@
         <v>72</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="73">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="46">
         <v>14</v>
       </c>
@@ -16702,7 +16728,7 @@
       </c>
       <c r="H73" s="86"/>
       <c r="I73" s="86">
-        <v>153.73</v>
+        <v>153.72999999999999</v>
       </c>
       <c r="J73" s="14"/>
       <c r="K73" s="46">
@@ -16710,7 +16736,7 @@
         <v>73</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="74">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="46">
         <v>14</v>
       </c>
@@ -16742,7 +16768,7 @@
         <v>74</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="75">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="46">
         <v>14</v>
       </c>
@@ -16774,7 +16800,7 @@
         <v>75</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="76">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="46">
         <v>14</v>
       </c>
@@ -16806,7 +16832,7 @@
         <v>76</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="77">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="46">
         <v>14</v>
       </c>
@@ -16838,7 +16864,7 @@
         <v>77</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="78">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="46">
         <v>14</v>
       </c>
@@ -16870,7 +16896,7 @@
         <v>78</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="79">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="46">
         <v>14</v>
       </c>
@@ -16894,7 +16920,7 @@
         <v>79</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="80">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="46">
         <v>15</v>
       </c>
@@ -16926,7 +16952,7 @@
         <v>80</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="81">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="46">
         <v>15</v>
       </c>
@@ -16958,7 +16984,7 @@
         <v>81</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="82">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="46">
         <v>15</v>
       </c>
@@ -16990,7 +17016,7 @@
         <v>82</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="83">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="46">
         <v>15</v>
       </c>
@@ -17022,7 +17048,7 @@
         <v>83</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="84">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="46">
         <v>15</v>
       </c>
@@ -17054,7 +17080,7 @@
         <v>84</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="85">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="46">
         <v>15</v>
       </c>
@@ -17086,7 +17112,7 @@
         <v>85</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="86">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="46">
         <v>15</v>
       </c>
@@ -17118,7 +17144,7 @@
         <v>86</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="87">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="46">
         <v>15</v>
       </c>
@@ -17152,7 +17178,7 @@
         <v>87</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="88">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="46">
         <v>15</v>
       </c>
@@ -17176,7 +17202,7 @@
         <v>88</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="89">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="46">
         <v>16</v>
       </c>
@@ -17199,7 +17225,7 @@
         <v>399</v>
       </c>
       <c r="H89" s="86">
-        <v>1034.91</v>
+        <v>1034.9100000000001</v>
       </c>
       <c r="I89" s="86"/>
       <c r="J89" s="14"/>
@@ -17208,7 +17234,7 @@
         <v>89</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="90">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="46">
         <v>16</v>
       </c>
@@ -17232,7 +17258,7 @@
       </c>
       <c r="H90" s="86"/>
       <c r="I90" s="86">
-        <v>1034.91</v>
+        <v>1034.9100000000001</v>
       </c>
       <c r="J90" s="14"/>
       <c r="K90" s="46">
@@ -17240,7 +17266,7 @@
         <v>90</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="91">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="46">
         <v>16</v>
       </c>
@@ -17264,7 +17290,7 @@
         <v>91</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="92">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="46">
         <v>17</v>
       </c>
@@ -17298,7 +17324,7 @@
         <v>92</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="93">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="46">
         <v>17</v>
       </c>
@@ -17332,7 +17358,7 @@
         <v>93</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="94">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="46">
         <v>17</v>
       </c>
@@ -17356,7 +17382,7 @@
         <v>94</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="95">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="46">
         <v>18</v>
       </c>
@@ -17388,7 +17414,7 @@
         <v>95</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="96">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="46">
         <v>18</v>
       </c>
@@ -17420,7 +17446,7 @@
         <v>96</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="97">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="46">
         <v>18</v>
       </c>
@@ -17452,7 +17478,7 @@
         <v>97</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="98">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="46">
         <v>18</v>
       </c>
@@ -17484,7 +17510,7 @@
         <v>98</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="99">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="46">
         <v>18</v>
       </c>
@@ -17508,7 +17534,7 @@
         <v>99</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="100">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="46">
         <v>19</v>
       </c>
@@ -17540,7 +17566,7 @@
         <v>100</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="101">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="46">
         <v>19</v>
       </c>
@@ -17572,7 +17598,7 @@
         <v>101</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="102">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="46">
         <v>19</v>
       </c>
@@ -17596,7 +17622,7 @@
         <v>102</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="103">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="46">
         <v>20</v>
       </c>
@@ -17628,7 +17654,7 @@
         <v>103</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="104">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="46">
         <v>20</v>
       </c>
@@ -17660,7 +17686,7 @@
         <v>104</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="105">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="46">
         <v>20</v>
       </c>
@@ -17684,7 +17710,7 @@
         <v>105</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="106">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="46">
         <v>21</v>
       </c>
@@ -17716,7 +17742,7 @@
         <v>106</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="107">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="46">
         <v>21</v>
       </c>
@@ -17748,7 +17774,7 @@
         <v>107</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="108">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="46">
         <v>21</v>
       </c>
@@ -17772,7 +17798,7 @@
         <v>108</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="109">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="46">
         <v>22</v>
       </c>
@@ -17806,7 +17832,7 @@
         <v>109</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="110">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="46">
         <v>22</v>
       </c>
@@ -17838,7 +17864,7 @@
         <v>110</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="111">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="46">
         <v>22</v>
       </c>
@@ -17862,7 +17888,7 @@
         <v>111</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="112">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="46">
         <v>23</v>
       </c>
@@ -17885,7 +17911,7 @@
         <v>399</v>
       </c>
       <c r="H112" s="86">
-        <v>159.95</v>
+        <v>159.94999999999999</v>
       </c>
       <c r="I112" s="86"/>
       <c r="J112" s="14"/>
@@ -17894,7 +17920,7 @@
         <v>112</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="113">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="46">
         <v>23</v>
       </c>
@@ -17918,7 +17944,7 @@
       </c>
       <c r="H113" s="86"/>
       <c r="I113" s="86">
-        <v>149.95</v>
+        <v>149.94999999999999</v>
       </c>
       <c r="J113" s="14"/>
       <c r="K113" s="46">
@@ -17926,7 +17952,7 @@
         <v>113</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="114">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="46">
         <v>23</v>
       </c>
@@ -17958,7 +17984,7 @@
         <v>114</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="115">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="46">
         <v>23</v>
       </c>
@@ -17990,7 +18016,7 @@
         <v>115</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="116">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="46">
         <v>23</v>
       </c>
@@ -18014,7 +18040,7 @@
         <v>116</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="117">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="46">
         <v>24</v>
       </c>
@@ -18046,7 +18072,7 @@
         <v>117</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="118">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="46">
         <v>24</v>
       </c>
@@ -18078,7 +18104,7 @@
         <v>118</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="119">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="46">
         <v>24</v>
       </c>
@@ -18102,7 +18128,7 @@
         <v>119</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="120">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="46">
         <v>25</v>
       </c>
@@ -18134,7 +18160,7 @@
         <v>120</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="121">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="46">
         <v>25</v>
       </c>
@@ -18166,7 +18192,7 @@
         <v>121</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="122">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="46">
         <v>25</v>
       </c>
@@ -18190,7 +18216,7 @@
         <v>122</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="123">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="46">
         <v>26</v>
       </c>
@@ -18222,7 +18248,7 @@
         <v>123</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="124">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="46">
         <v>26</v>
       </c>
@@ -18254,7 +18280,7 @@
         <v>124</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="125">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="46">
         <v>26</v>
       </c>
@@ -18278,7 +18304,7 @@
         <v>125</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="126">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="46">
         <v>27</v>
       </c>
@@ -18310,7 +18336,7 @@
         <v>126</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="127">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="46">
         <v>27</v>
       </c>
@@ -18342,7 +18368,7 @@
         <v>127</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="128">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="46">
         <v>27</v>
       </c>
@@ -18366,7 +18392,7 @@
         <v>128</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="129">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="46">
         <v>28</v>
       </c>
@@ -18398,7 +18424,7 @@
         <v>129</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="130">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="46">
         <v>28</v>
       </c>
@@ -18430,7 +18456,7 @@
         <v>130</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="131">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="46">
         <v>28</v>
       </c>
@@ -18454,7 +18480,7 @@
         <v>131</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="132">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="46">
         <v>29</v>
       </c>
@@ -18477,7 +18503,7 @@
         <v>402</v>
       </c>
       <c r="H132" s="86">
-        <v>2157.07</v>
+        <v>2157.0700000000002</v>
       </c>
       <c r="I132" s="86"/>
       <c r="J132" s="14"/>
@@ -18486,7 +18512,7 @@
         <v>132</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="133">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="46">
         <v>29</v>
       </c>
@@ -18518,7 +18544,7 @@
         <v>133</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="134">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="46">
         <v>29</v>
       </c>
@@ -18550,7 +18576,7 @@
         <v>134</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="135">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="46">
         <v>29</v>
       </c>
@@ -18582,7 +18608,7 @@
         <v>135</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="136">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="46">
         <v>29</v>
       </c>
@@ -18614,7 +18640,7 @@
         <v>136</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="137">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="46">
         <v>29</v>
       </c>
@@ -18646,7 +18672,7 @@
         <v>137</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="138">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="46">
         <v>29</v>
       </c>
@@ -18678,7 +18704,7 @@
         <v>138</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="139">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="46">
         <v>29</v>
       </c>
@@ -18710,7 +18736,7 @@
         <v>139</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="140">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="46">
         <v>29</v>
       </c>
@@ -18734,7 +18760,7 @@
         <v>140</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="141">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="46">
         <v>30</v>
       </c>
@@ -18766,7 +18792,7 @@
         <v>141</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="142">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="46">
         <v>30</v>
       </c>
@@ -18798,7 +18824,7 @@
         <v>142</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="143">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="46">
         <v>30</v>
       </c>
@@ -18830,7 +18856,7 @@
         <v>143</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="144">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="46">
         <v>30</v>
       </c>
@@ -18862,7 +18888,7 @@
         <v>144</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="145">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="46">
         <v>30</v>
       </c>
@@ -18894,7 +18920,7 @@
         <v>145</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="146">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="46">
         <v>30</v>
       </c>
@@ -18926,7 +18952,7 @@
         <v>146</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="147">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="46">
         <v>30</v>
       </c>
@@ -18958,7 +18984,7 @@
         <v>147</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="148">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="46">
         <v>30</v>
       </c>
@@ -18990,7 +19016,7 @@
         <v>148</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="149">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="46">
         <v>30</v>
       </c>
@@ -19014,7 +19040,7 @@
         <v>149</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="150">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="46">
         <v>31</v>
       </c>
@@ -19046,7 +19072,7 @@
         <v>150</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="151">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="46">
         <v>31</v>
       </c>
@@ -19078,7 +19104,7 @@
         <v>151</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="152">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="46">
         <v>31</v>
       </c>
@@ -19102,7 +19128,7 @@
         <v>152</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="153">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="46">
         <v>32</v>
       </c>
@@ -19134,7 +19160,7 @@
         <v>153</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="154">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="46">
         <v>32</v>
       </c>
@@ -19166,7 +19192,7 @@
         <v>154</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="155">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="46">
         <v>32</v>
       </c>
@@ -19190,7 +19216,7 @@
         <v>155</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="156">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="46">
         <v>33</v>
       </c>
@@ -19222,7 +19248,7 @@
         <v>156</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="157">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="46">
         <v>33</v>
       </c>
@@ -19256,7 +19282,7 @@
         <v>157</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="158">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="46">
         <v>33</v>
       </c>
@@ -19280,7 +19306,7 @@
         <v>158</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="159">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="46">
         <v>34</v>
       </c>
@@ -19312,7 +19338,7 @@
         <v>159</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="160">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="46">
         <v>34</v>
       </c>
@@ -19344,7 +19370,7 @@
         <v>160</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="161">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="46">
         <v>34</v>
       </c>
@@ -19368,7 +19394,7 @@
         <v>161</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="162">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="46">
         <v>35</v>
       </c>
@@ -19400,7 +19426,7 @@
         <v>162</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="163">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="46">
         <v>35</v>
       </c>
@@ -19432,7 +19458,7 @@
         <v>163</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="164">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="46">
         <v>35</v>
       </c>
@@ -19456,7 +19482,7 @@
         <v>164</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="165">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="46">
         <v>36</v>
       </c>
@@ -19485,7 +19511,7 @@
         <v>165</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="166">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="46">
         <v>36</v>
       </c>
@@ -19515,7 +19541,7 @@
         <v>166</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="167">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="46">
         <v>36</v>
       </c>
@@ -19537,7 +19563,7 @@
         <v>167</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="168">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="46">
         <v>37</v>
       </c>
@@ -19569,7 +19595,7 @@
         <v>168</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="169">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="46">
         <v>37</v>
       </c>
@@ -19601,7 +19627,7 @@
         <v>169</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="170">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="46">
         <v>37</v>
       </c>
@@ -19625,7 +19651,7 @@
         <v>170</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="171">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="46">
         <v>38</v>
       </c>
@@ -19657,7 +19683,7 @@
         <v>171</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="172">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="46">
         <v>38</v>
       </c>
@@ -19689,7 +19715,7 @@
         <v>172</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="173">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="46">
         <v>38</v>
       </c>
@@ -19713,7 +19739,7 @@
         <v>173</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="174">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="46">
         <v>39</v>
       </c>
@@ -19745,7 +19771,7 @@
         <v>174</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="175">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="46">
         <v>39</v>
       </c>
@@ -19777,7 +19803,7 @@
         <v>175</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="176">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="46">
         <v>39</v>
       </c>
@@ -19801,7 +19827,7 @@
         <v>176</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="177">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="46">
         <v>40</v>
       </c>
@@ -19833,7 +19859,7 @@
         <v>177</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="178">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="46">
         <v>40</v>
       </c>
@@ -19865,7 +19891,7 @@
         <v>178</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="179">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="46">
         <v>40</v>
       </c>
@@ -19889,7 +19915,7 @@
       </c>
       <c r="H179" s="86"/>
       <c r="I179" s="86">
-        <v>33.95</v>
+        <v>33.950000000000003</v>
       </c>
       <c r="J179" s="14"/>
       <c r="K179" s="46">
@@ -19897,7 +19923,7 @@
         <v>179</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="180">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="46">
         <v>40</v>
       </c>
@@ -19921,7 +19947,7 @@
         <v>180</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="181">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="46">
         <v>41</v>
       </c>
@@ -19953,7 +19979,7 @@
         <v>181</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="182">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="46">
         <v>41</v>
       </c>
@@ -19985,7 +20011,7 @@
         <v>182</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="183">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="46">
         <v>41</v>
       </c>
@@ -20009,7 +20035,7 @@
         <v>183</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="184">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="46">
         <v>42</v>
       </c>
@@ -20041,7 +20067,7 @@
         <v>184</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="185">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="46">
         <v>42</v>
       </c>
@@ -20073,7 +20099,7 @@
         <v>185</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="186">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="46">
         <v>42</v>
       </c>
@@ -20097,7 +20123,7 @@
         <v>186</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="187">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="46">
         <v>43</v>
       </c>
@@ -20129,7 +20155,7 @@
         <v>187</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="188">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="46">
         <v>43</v>
       </c>
@@ -20161,7 +20187,7 @@
         <v>188</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="189">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="46">
         <v>43</v>
       </c>
@@ -20185,7 +20211,7 @@
         <v>189</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="190">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="46">
         <v>44</v>
       </c>
@@ -20217,7 +20243,7 @@
         <v>190</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="191">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="46">
         <v>44</v>
       </c>
@@ -20249,7 +20275,7 @@
         <v>191</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="192">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="46">
         <v>44</v>
       </c>
@@ -20273,7 +20299,7 @@
         <v>192</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="193">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="46">
         <v>45</v>
       </c>
@@ -20305,7 +20331,7 @@
         <v>193</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="194">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="46">
         <v>45</v>
       </c>
@@ -20337,7 +20363,7 @@
         <v>194</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="195">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="46">
         <v>45</v>
       </c>
@@ -20369,7 +20395,7 @@
         <v>195</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="196">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="46">
         <v>45</v>
       </c>
@@ -20401,7 +20427,7 @@
         <v>196</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="197">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="46">
         <v>45</v>
       </c>
@@ -20425,7 +20451,7 @@
         <v>197</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="198">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="46">
         <v>46</v>
       </c>
@@ -20448,7 +20474,7 @@
         <v>469</v>
       </c>
       <c r="H198" s="86">
-        <v>9.95</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="I198" s="86"/>
       <c r="J198" s="14"/>
@@ -20457,7 +20483,7 @@
         <v>198</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="199">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="46">
         <v>46</v>
       </c>
@@ -20481,7 +20507,7 @@
       </c>
       <c r="H199" s="86"/>
       <c r="I199" s="86">
-        <v>9.95</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="J199" s="14"/>
       <c r="K199" s="46">
@@ -20489,7 +20515,7 @@
         <v>199</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="200">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="46">
         <v>46</v>
       </c>
@@ -20513,7 +20539,7 @@
         <v>200</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="201">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="46">
         <v>47</v>
       </c>
@@ -20542,7 +20568,7 @@
         <v>201</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="202">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="46">
         <v>47</v>
       </c>
@@ -20572,7 +20598,7 @@
         <v>202</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="203">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="46">
         <v>47</v>
       </c>
@@ -20594,7 +20620,7 @@
         <v>203</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="204">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="46">
         <v>48</v>
       </c>
@@ -20623,7 +20649,7 @@
         <v>204</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="205">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="46">
         <v>48</v>
       </c>
@@ -20653,7 +20679,7 @@
         <v>205</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="206">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="46">
         <v>48</v>
       </c>
@@ -20683,7 +20709,7 @@
         <v>206</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="207">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="46">
         <v>48</v>
       </c>
@@ -20713,7 +20739,7 @@
         <v>207</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="208">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="46">
         <v>48</v>
       </c>
@@ -20743,7 +20769,7 @@
         <v>208</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="209">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="46">
         <v>48</v>
       </c>
@@ -20765,7 +20791,7 @@
         <v>209</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="210">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="46">
         <v>49</v>
       </c>
@@ -20797,7 +20823,7 @@
         <v>210</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="211">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="46">
         <v>49</v>
       </c>
@@ -20829,7 +20855,7 @@
         <v>211</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="212">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="46">
         <v>49</v>
       </c>
@@ -20861,7 +20887,7 @@
         <v>212</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="213">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="46">
         <v>49</v>
       </c>
@@ -20893,7 +20919,7 @@
         <v>213</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="214">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="46">
         <v>49</v>
       </c>
@@ -20917,7 +20943,7 @@
         <v>214</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="215">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="46">
         <v>50</v>
       </c>
@@ -20949,7 +20975,7 @@
         <v>215</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="216">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="46">
         <v>50</v>
       </c>
@@ -20981,7 +21007,7 @@
         <v>216</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="217">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="46">
         <v>50</v>
       </c>
@@ -21013,7 +21039,7 @@
         <v>217</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="218">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="46">
         <v>50</v>
       </c>
@@ -21045,7 +21071,7 @@
         <v>218</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="219">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="46">
         <v>50</v>
       </c>
@@ -21069,7 +21095,7 @@
         <v>219</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="220">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="46">
         <v>51</v>
       </c>
@@ -21101,7 +21127,7 @@
         <v>220</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="221">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="46">
         <v>51</v>
       </c>
@@ -21133,7 +21159,7 @@
         <v>221</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="222">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="46">
         <v>51</v>
       </c>
@@ -21157,7 +21183,7 @@
         <v>222</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="223">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="46">
         <v>52</v>
       </c>
@@ -21180,7 +21206,7 @@
         <v>514</v>
       </c>
       <c r="H223" s="86">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I223" s="86"/>
       <c r="J223" s="14"/>
@@ -21189,7 +21215,7 @@
         <v>223</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="224">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="46">
         <v>52</v>
       </c>
@@ -21221,7 +21247,7 @@
         <v>224</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="225">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="46">
         <v>52</v>
       </c>
@@ -21253,7 +21279,7 @@
         <v>225</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="226">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="46">
         <v>52</v>
       </c>
@@ -21287,7 +21313,7 @@
         <v>226</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="227">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="46">
         <v>52</v>
       </c>
@@ -21311,7 +21337,7 @@
         <v>227</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="228">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="46">
         <v>53</v>
       </c>
@@ -21331,7 +21357,7 @@
         <v>514</v>
       </c>
       <c r="H228" s="86">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I228" s="86"/>
       <c r="J228" s="14"/>
@@ -21340,7 +21366,7 @@
         <v>228</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="229">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="46">
         <v>53</v>
       </c>
@@ -21370,7 +21396,7 @@
         <v>229</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="230">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="46">
         <v>53</v>
       </c>
@@ -21400,7 +21426,7 @@
         <v>230</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="231">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="46">
         <v>53</v>
       </c>
@@ -21432,7 +21458,7 @@
         <v>231</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="232">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="46">
         <v>53</v>
       </c>
@@ -21454,7 +21480,7 @@
         <v>232</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="233">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="46">
         <v>54</v>
       </c>
@@ -21474,7 +21500,7 @@
         <v>514</v>
       </c>
       <c r="H233" s="86">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I233" s="86"/>
       <c r="J233" s="14"/>
@@ -21483,7 +21509,7 @@
         <v>233</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="234">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="46">
         <v>54</v>
       </c>
@@ -21513,7 +21539,7 @@
         <v>234</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="235">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="46">
         <v>54</v>
       </c>
@@ -21543,7 +21569,7 @@
         <v>235</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="236">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="46">
         <v>54</v>
       </c>
@@ -21575,7 +21601,7 @@
         <v>236</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="237">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="46">
         <v>54</v>
       </c>
@@ -21597,7 +21623,7 @@
         <v>237</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="238">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="46">
         <v>55</v>
       </c>
@@ -21617,7 +21643,7 @@
         <v>514</v>
       </c>
       <c r="H238" s="86">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I238" s="86"/>
       <c r="J238" s="14"/>
@@ -21626,7 +21652,7 @@
         <v>238</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="239">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="46">
         <v>55</v>
       </c>
@@ -21656,7 +21682,7 @@
         <v>239</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="240">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="46">
         <v>55</v>
       </c>
@@ -21686,7 +21712,7 @@
         <v>240</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="241">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="46">
         <v>55</v>
       </c>
@@ -21718,7 +21744,7 @@
         <v>241</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="242">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="46">
         <v>55</v>
       </c>
@@ -21740,7 +21766,7 @@
         <v>242</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="243">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="46">
         <v>56</v>
       </c>
@@ -21769,7 +21795,7 @@
         <v>243</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="244">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="46">
         <v>56</v>
       </c>
@@ -21799,7 +21825,7 @@
         <v>244</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="245">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="46">
         <v>56</v>
       </c>
@@ -21821,7 +21847,7 @@
         <v>245</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="246">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="46">
         <v>57</v>
       </c>
@@ -21850,7 +21876,7 @@
         <v>246</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="247">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="46">
         <v>57</v>
       </c>
@@ -21880,7 +21906,7 @@
         <v>247</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="248">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="46">
         <v>57</v>
       </c>
@@ -21910,7 +21936,7 @@
         <v>248</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="249">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="46">
         <v>57</v>
       </c>
@@ -21940,7 +21966,7 @@
         <v>249</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="250">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="46">
         <v>57</v>
       </c>
@@ -21970,7 +21996,7 @@
         <v>250</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="251">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" s="46">
         <v>57</v>
       </c>
@@ -21992,7 +22018,7 @@
         <v>251</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="252">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" s="46">
         <v>58</v>
       </c>
@@ -22021,7 +22047,7 @@
         <v>252</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="253">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" s="46">
         <v>58</v>
       </c>
@@ -22051,7 +22077,7 @@
         <v>253</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="254">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="46">
         <v>58</v>
       </c>
@@ -22081,7 +22107,7 @@
         <v>254</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="255">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="46">
         <v>58</v>
       </c>
@@ -22111,7 +22137,7 @@
         <v>255</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="256">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" s="46">
         <v>58</v>
       </c>
@@ -22133,7 +22159,7 @@
         <v>256</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="257">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="46">
         <v>59</v>
       </c>
@@ -22162,7 +22188,7 @@
         <v>257</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="258">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="46">
         <v>59</v>
       </c>
@@ -22192,7 +22218,7 @@
         <v>258</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="259">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="46">
         <v>59</v>
       </c>
@@ -22222,7 +22248,7 @@
         <v>259</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="260">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="46">
         <v>59</v>
       </c>
@@ -22252,7 +22278,7 @@
         <v>260</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="261">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" s="46">
         <v>59</v>
       </c>
@@ -22274,7 +22300,7 @@
         <v>261</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="262">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="46">
         <v>60</v>
       </c>
@@ -22294,7 +22320,7 @@
         <v>514</v>
       </c>
       <c r="H262" s="86">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I262" s="86"/>
       <c r="J262" s="14"/>
@@ -22303,7 +22329,7 @@
         <v>262</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="263">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="46">
         <v>60</v>
       </c>
@@ -22333,7 +22359,7 @@
         <v>263</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="264">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="46">
         <v>60</v>
       </c>
@@ -22363,7 +22389,7 @@
         <v>264</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="265">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="46">
         <v>60</v>
       </c>
@@ -22395,7 +22421,7 @@
         <v>265</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="266">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="46">
         <v>60</v>
       </c>
@@ -22417,7 +22443,7 @@
         <v>266</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="267">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" s="46">
         <v>61</v>
       </c>
@@ -22446,7 +22472,7 @@
         <v>267</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="268">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" s="46">
         <v>61</v>
       </c>
@@ -22476,7 +22502,7 @@
         <v>268</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="269">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="46">
         <v>61</v>
       </c>
@@ -22506,7 +22532,7 @@
         <v>269</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="270">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="46">
         <v>61</v>
       </c>
@@ -22536,7 +22562,7 @@
         <v>270</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="271">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="46">
         <v>61</v>
       </c>
@@ -22566,7 +22592,7 @@
         <v>271</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="272">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="46">
         <v>61</v>
       </c>
@@ -22588,7 +22614,7 @@
         <v>272</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="273">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" s="46">
         <v>62</v>
       </c>
@@ -22617,7 +22643,7 @@
         <v>273</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="274">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="46">
         <v>62</v>
       </c>
@@ -22647,7 +22673,7 @@
         <v>274</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="275">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" s="46">
         <v>62</v>
       </c>
@@ -22677,7 +22703,7 @@
         <v>275</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="276">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="46">
         <v>62</v>
       </c>
@@ -22707,7 +22733,7 @@
         <v>276</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="277">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" s="46">
         <v>62</v>
       </c>
@@ -22729,7 +22755,7 @@
         <v>277</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="278">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="46">
         <v>63</v>
       </c>
@@ -22758,7 +22784,7 @@
         <v>278</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="279">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="46">
         <v>63</v>
       </c>
@@ -22788,7 +22814,7 @@
         <v>279</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="280">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="46">
         <v>63</v>
       </c>
@@ -22818,7 +22844,7 @@
         <v>280</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="281">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="46">
         <v>63</v>
       </c>
@@ -22848,7 +22874,7 @@
         <v>281</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="282">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="46">
         <v>63</v>
       </c>
@@ -22870,7 +22896,7 @@
         <v>282</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="283">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="46">
         <v>64</v>
       </c>
@@ -22902,7 +22928,7 @@
         <v>283</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="284">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="46">
         <v>64</v>
       </c>
@@ -22934,7 +22960,7 @@
         <v>284</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="285">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="46">
         <v>64</v>
       </c>
@@ -22966,7 +22992,7 @@
         <v>285</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="286">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" s="46">
         <v>64</v>
       </c>
@@ -22998,7 +23024,7 @@
         <v>286</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="287">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="46">
         <v>64</v>
       </c>
@@ -23030,7 +23056,7 @@
         <v>287</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="288">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" s="46">
         <v>64</v>
       </c>
@@ -23062,7 +23088,7 @@
         <v>288</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="289">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="46">
         <v>64</v>
       </c>
@@ -23086,7 +23112,7 @@
         <v>289</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="290">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" s="46">
         <v>65</v>
       </c>
@@ -23115,7 +23141,7 @@
         <v>290</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="291">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291" s="46">
         <v>65</v>
       </c>
@@ -23145,7 +23171,7 @@
         <v>291</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="292">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292" s="46">
         <v>65</v>
       </c>
@@ -23175,7 +23201,7 @@
         <v>292</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="293">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293" s="46">
         <v>65</v>
       </c>
@@ -23205,7 +23231,7 @@
         <v>293</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="294">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" s="46">
         <v>65</v>
       </c>
@@ -23227,7 +23253,7 @@
         <v>294</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="295">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A295" s="46">
         <v>66</v>
       </c>
@@ -23259,7 +23285,7 @@
         <v>295</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="296">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296" s="46">
         <v>66</v>
       </c>
@@ -23291,7 +23317,7 @@
         <v>296</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="297">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A297" s="46">
         <v>66</v>
       </c>
@@ -23315,7 +23341,7 @@
         <v>297</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="298">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" s="46">
         <v>67</v>
       </c>
@@ -23347,7 +23373,7 @@
         <v>298</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="299">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" s="46">
         <v>67</v>
       </c>
@@ -23377,7 +23403,7 @@
         <v>299</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="300">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" s="46">
         <v>67</v>
       </c>
@@ -23399,7 +23425,7 @@
         <v>300</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="301">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A301" s="46">
         <v>68</v>
       </c>
@@ -23431,7 +23457,7 @@
         <v>301</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="302">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" s="46">
         <v>68</v>
       </c>
@@ -23463,7 +23489,7 @@
         <v>302</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="303">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303" s="46">
         <v>68</v>
       </c>
@@ -23495,7 +23521,7 @@
         <v>303</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="304">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" s="46">
         <v>68</v>
       </c>
@@ -23519,7 +23545,7 @@
       </c>
       <c r="H304" s="86"/>
       <c r="I304" s="86">
-        <v>37.41</v>
+        <v>37.409999999999997</v>
       </c>
       <c r="J304" s="14"/>
       <c r="K304" s="46">
@@ -23527,7 +23553,7 @@
         <v>304</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="305">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305" s="46">
         <v>68</v>
       </c>
@@ -23550,7 +23576,7 @@
         <v>305</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="306">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="46">
         <v>69</v>
       </c>
@@ -23582,7 +23608,7 @@
         <v>306</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="307">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" s="46">
         <v>69</v>
       </c>
@@ -23614,7 +23640,7 @@
         <v>307</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="308">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="46">
         <v>69</v>
       </c>
@@ -23646,7 +23672,7 @@
         <v>308</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="309">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309" s="46">
         <v>69</v>
       </c>
@@ -23678,7 +23704,7 @@
         <v>309</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="310">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310" s="46">
         <v>69</v>
       </c>
@@ -23710,7 +23736,7 @@
         <v>310</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="311">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A311" s="46">
         <v>69</v>
       </c>
@@ -23742,7 +23768,7 @@
         <v>311</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="312">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A312" s="46">
         <v>69</v>
       </c>
@@ -23774,7 +23800,7 @@
         <v>312</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="313">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A313" s="46">
         <v>69</v>
       </c>
@@ -23795,7 +23821,7 @@
         <v>313</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="314">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314" s="46">
         <v>70</v>
       </c>
@@ -23827,7 +23853,7 @@
         <v>314</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="315">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A315" s="46">
         <v>70</v>
       </c>
@@ -23859,7 +23885,7 @@
         <v>315</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="316">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" s="46">
         <v>70</v>
       </c>
@@ -23891,7 +23917,7 @@
         <v>316</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="317">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="46">
         <v>70</v>
       </c>
@@ -23923,7 +23949,7 @@
         <v>317</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="318">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="46">
         <v>70</v>
       </c>
@@ -23955,7 +23981,7 @@
         <v>318</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="319">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" s="46">
         <v>70</v>
       </c>
@@ -23987,7 +24013,7 @@
         <v>319</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="320">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A320" s="46">
         <v>70</v>
       </c>
@@ -24019,7 +24045,7 @@
         <v>320</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="321">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" s="46">
         <v>70</v>
       </c>
@@ -24042,7 +24068,7 @@
         <v>321</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="322">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322" s="46">
         <v>71</v>
       </c>
@@ -24074,7 +24100,7 @@
         <v>322</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="323">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A323" s="46">
         <v>71</v>
       </c>
@@ -24106,7 +24132,7 @@
         <v>323</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="324">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" s="46">
         <v>71</v>
       </c>
@@ -24138,7 +24164,7 @@
         <v>324</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="325">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325" s="46">
         <v>71</v>
       </c>
@@ -24170,7 +24196,7 @@
         <v>325</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="326">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" s="46">
         <v>71</v>
       </c>
@@ -24202,7 +24228,7 @@
         <v>326</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="327">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="46">
         <v>71</v>
       </c>
@@ -24234,7 +24260,7 @@
         <v>327</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="328">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328" s="46">
         <v>71</v>
       </c>
@@ -24266,7 +24292,7 @@
         <v>328</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="329">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329" s="46">
         <v>71</v>
       </c>
@@ -24289,7 +24315,7 @@
         <v>329</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="330">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330" s="46">
         <v>72</v>
       </c>
@@ -24321,7 +24347,7 @@
         <v>330</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="331">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" s="46">
         <v>72</v>
       </c>
@@ -24353,7 +24379,7 @@
         <v>331</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="332">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332" s="46">
         <v>72</v>
       </c>
@@ -24385,7 +24411,7 @@
         <v>332</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="333">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333" s="46">
         <v>72</v>
       </c>
@@ -24417,7 +24443,7 @@
         <v>333</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="334">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334" s="46">
         <v>72</v>
       </c>
@@ -24440,7 +24466,7 @@
         <v>334</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="335">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" s="46">
         <v>73</v>
       </c>
@@ -24472,7 +24498,7 @@
         <v>335</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="336">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336" s="46">
         <v>73</v>
       </c>
@@ -24504,7 +24530,7 @@
         <v>336</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="337">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" s="46">
         <v>73</v>
       </c>
@@ -24527,7 +24553,7 @@
         <v>337</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="338">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" s="46">
         <v>74</v>
       </c>
@@ -24559,7 +24585,7 @@
         <v>338</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="339">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" s="46">
         <v>74</v>
       </c>
@@ -24593,7 +24619,7 @@
         <v>339</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="340">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340" s="46">
         <v>74</v>
       </c>
@@ -24627,7 +24653,7 @@
         <v>340</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="341">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341" s="46">
         <v>74</v>
       </c>
@@ -24661,7 +24687,7 @@
         <v>341</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="342">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" s="46">
         <v>74</v>
       </c>
@@ -24695,7 +24721,7 @@
         <v>342</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="343">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" s="46">
         <v>74</v>
       </c>
@@ -24718,7 +24744,7 @@
         <v>343</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="344">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344" s="46">
         <v>75</v>
       </c>
@@ -24750,7 +24776,7 @@
         <v>344</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="345">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345" s="46">
         <v>75</v>
       </c>
@@ -24782,7 +24808,7 @@
         <v>345</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="346">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A346" s="46">
         <v>75</v>
       </c>
@@ -24805,7 +24831,7 @@
         <v>346</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="347">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347" s="46">
         <v>76</v>
       </c>
@@ -24837,7 +24863,7 @@
         <v>347</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="348">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348" s="46">
         <v>76</v>
       </c>
@@ -24869,7 +24895,7 @@
         <v>348</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="349">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" s="46">
         <v>76</v>
       </c>
@@ -24892,7 +24918,7 @@
         <v>349</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="350">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350" s="46">
         <v>77</v>
       </c>
@@ -24924,7 +24950,7 @@
         <v>350</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="351">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A351" s="46">
         <v>77</v>
       </c>
@@ -24956,7 +24982,7 @@
         <v>351</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="352">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A352" s="46">
         <v>77</v>
       </c>
@@ -24988,7 +25014,7 @@
         <v>352</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="353">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A353" s="46">
         <v>77</v>
       </c>
@@ -25020,7 +25046,7 @@
         <v>353</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="354">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" s="46">
         <v>77</v>
       </c>
@@ -25045,7 +25071,7 @@
         <v>354</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="355">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" s="46">
         <v>78</v>
       </c>
@@ -25077,7 +25103,7 @@
         <v>355</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="356">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A356" s="46">
         <v>78</v>
       </c>
@@ -25109,7 +25135,7 @@
         <v>356</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="357">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A357" s="46">
         <v>78</v>
       </c>
@@ -25141,7 +25167,7 @@
         <v>357</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="358">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A358" s="46">
         <v>78</v>
       </c>
@@ -25173,7 +25199,7 @@
         <v>358</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="359">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A359" s="46">
         <v>78</v>
       </c>
@@ -25198,7 +25224,7 @@
         <v>359</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="360">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A360" s="46">
         <v>79</v>
       </c>
@@ -25230,7 +25256,7 @@
         <v>360</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="361">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A361" s="46">
         <v>79</v>
       </c>
@@ -25254,7 +25280,7 @@
       </c>
       <c r="H361" s="86"/>
       <c r="I361" s="86">
-        <v>9.95</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="J361" s="14"/>
       <c r="K361" s="46">
@@ -25262,7 +25288,7 @@
         <v>361</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="362">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A362" s="46">
         <v>79</v>
       </c>
@@ -25294,7 +25320,7 @@
         <v>362</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="363">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A363" s="46">
         <v>79</v>
       </c>
@@ -25324,7 +25350,7 @@
         <v>363</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="364">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A364" s="46">
         <v>79</v>
       </c>
@@ -25349,7 +25375,7 @@
         <v>364</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="365">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A365" s="46">
         <v>80</v>
       </c>
@@ -25378,7 +25404,7 @@
         <v>365</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="366">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" s="46">
         <v>80</v>
       </c>
@@ -25408,7 +25434,7 @@
         <v>366</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="367">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367" s="46">
         <v>80</v>
       </c>
@@ -25431,7 +25457,7 @@
         <v>367</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="368">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A368" s="46">
         <v>81</v>
       </c>
@@ -25452,7 +25478,7 @@
         <v>514</v>
       </c>
       <c r="H368" s="86">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I368" s="86"/>
       <c r="J368" s="14"/>
@@ -25461,7 +25487,7 @@
         <v>368</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="369">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" s="46">
         <v>81</v>
       </c>
@@ -25491,7 +25517,7 @@
         <v>369</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="370">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A370" s="46">
         <v>81</v>
       </c>
@@ -25521,7 +25547,7 @@
         <v>370</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="371">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A371" s="46">
         <v>81</v>
       </c>
@@ -25553,7 +25579,7 @@
         <v>371</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="372">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A372" s="46">
         <v>81</v>
       </c>
@@ -25576,7 +25602,7 @@
         <v>372</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="373">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A373" s="46">
         <v>82</v>
       </c>
@@ -25608,7 +25634,7 @@
         <v>373</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="374">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" s="46">
         <v>82</v>
       </c>
@@ -25640,7 +25666,7 @@
         <v>374</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="375">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A375" s="46">
         <v>82</v>
       </c>
@@ -25665,7 +25691,7 @@
         <v>375</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="376">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A376" s="46">
         <v>83</v>
       </c>
@@ -25694,7 +25720,7 @@
         <v>376</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="377">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" s="46">
         <v>83</v>
       </c>
@@ -25724,7 +25750,7 @@
         <v>377</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="378">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378" s="46">
         <v>83</v>
       </c>
@@ -25754,7 +25780,7 @@
         <v>378</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="379">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" s="46">
         <v>83</v>
       </c>
@@ -25784,7 +25810,7 @@
         <v>379</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="380">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" s="46">
         <v>83</v>
       </c>
@@ -25807,7 +25833,7 @@
         <v>380</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="381">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A381" s="46">
         <v>84</v>
       </c>
@@ -25839,7 +25865,7 @@
         <v>381</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="382">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382" s="46">
         <v>84</v>
       </c>
@@ -25871,7 +25897,7 @@
         <v>382</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="383">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A383" s="46">
         <v>84</v>
       </c>
@@ -25896,7 +25922,7 @@
         <v>383</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="384">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A384" s="46">
         <v>85</v>
       </c>
@@ -25916,7 +25942,7 @@
         <v>514</v>
       </c>
       <c r="H384" s="86">
-        <v>129.95</v>
+        <v>129.94999999999999</v>
       </c>
       <c r="I384" s="86"/>
       <c r="J384" s="14"/>
@@ -25925,7 +25951,7 @@
         <v>384</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="385">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A385" s="46">
         <v>85</v>
       </c>
@@ -25955,7 +25981,7 @@
         <v>385</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="386">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A386" s="46">
         <v>85</v>
       </c>
@@ -25985,7 +26011,7 @@
         <v>386</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="387">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A387" s="46">
         <v>85</v>
       </c>
@@ -26017,7 +26043,7 @@
         <v>387</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="388">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A388" s="46">
         <v>85</v>
       </c>
@@ -26040,7 +26066,7 @@
         <v>388</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="389">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A389" s="46">
         <v>86</v>
       </c>
@@ -26060,7 +26086,7 @@
         <v>514</v>
       </c>
       <c r="H389" s="86">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="I389" s="86"/>
       <c r="J389" s="14"/>
@@ -26069,7 +26095,7 @@
         <v>389</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="390">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A390" s="46">
         <v>86</v>
       </c>
@@ -26091,7 +26117,7 @@
       </c>
       <c r="H390" s="86"/>
       <c r="I390" s="86">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J390" s="14"/>
       <c r="K390" s="46">
@@ -26099,7 +26125,7 @@
         <v>390</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="391">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" s="46">
         <v>86</v>
       </c>
@@ -26122,7 +26148,7 @@
         <v>391</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="392">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A392" s="46">
         <v>87</v>
       </c>
@@ -26154,7 +26180,7 @@
         <v>392</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="393">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A393" s="46">
         <v>87</v>
       </c>
@@ -26186,7 +26212,7 @@
         <v>393</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="394">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A394" s="46">
         <v>87</v>
       </c>
@@ -26218,7 +26244,7 @@
         <v>394</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="395">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A395" s="46">
         <v>87</v>
       </c>
@@ -26250,7 +26276,7 @@
         <v>395</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="396">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" s="46">
         <v>87</v>
       </c>
@@ -26275,7 +26301,7 @@
         <v>396</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="397">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" s="46">
         <v>88</v>
       </c>
@@ -26307,7 +26333,7 @@
         <v>397</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="398">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A398" s="46">
         <v>88</v>
       </c>
@@ -26339,7 +26365,7 @@
         <v>398</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="399">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A399" s="46">
         <v>88</v>
       </c>
@@ -26364,7 +26390,7 @@
         <v>399</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="400">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A400" s="46">
         <v>89</v>
       </c>
@@ -26395,7 +26421,7 @@
         <v>400</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="401">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A401" s="46">
         <v>89</v>
       </c>
@@ -26426,7 +26452,7 @@
         <v>401</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="402">
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A402" s="46">
         <v>89</v>
       </c>
@@ -26449,7 +26475,7 @@
         <v>402</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="403">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A403" s="46">
         <v>90</v>
       </c>
@@ -26477,7 +26503,7 @@
         <v>403</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="404">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A404" s="46">
         <v>90</v>
       </c>
@@ -26506,7 +26532,7 @@
         <v>404</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="405">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A405" s="46">
         <v>90</v>
       </c>
@@ -26525,7 +26551,7 @@
         <v>405</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="406">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A406" s="46">
         <v>91</v>
       </c>
@@ -26555,7 +26581,7 @@
         <v>406</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="407">
+    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A407" s="46">
         <v>91</v>
       </c>
@@ -26585,7 +26611,7 @@
         <v>407</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="408">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A408" s="46">
         <v>91</v>
       </c>
@@ -26606,7 +26632,7 @@
         <v>408</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="409">
+    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A409" s="46">
         <v>92</v>
       </c>
@@ -26636,7 +26662,7 @@
         <v>409</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="410">
+    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A410" s="46">
         <v>92</v>
       </c>
@@ -26666,7 +26692,7 @@
         <v>410</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="411">
+    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A411" s="46">
         <v>92</v>
       </c>
@@ -26687,7 +26713,7 @@
         <v>411</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="412">
+    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A412" s="46">
         <v>93</v>
       </c>
@@ -26717,7 +26743,7 @@
         <v>412</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="413">
+    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A413" s="46">
         <v>93</v>
       </c>
@@ -26747,7 +26773,7 @@
         <v>413</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="414">
+    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A414" s="46">
         <v>93</v>
       </c>
@@ -26768,7 +26794,7 @@
         <v>414</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="415">
+    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A415" s="46">
         <v>94</v>
       </c>
@@ -26798,7 +26824,7 @@
         <v>415</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="416">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A416" s="46">
         <v>94</v>
       </c>
@@ -26828,7 +26854,7 @@
         <v>416</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="417">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A417" s="46">
         <v>94</v>
       </c>
@@ -26849,7 +26875,7 @@
         <v>417</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="418">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A418" s="46">
         <v>95</v>
       </c>
@@ -26879,7 +26905,7 @@
         <v>418</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="419">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A419" s="46">
         <v>95</v>
       </c>
@@ -26909,7 +26935,7 @@
         <v>419</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="420">
+    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A420" s="46">
         <v>95</v>
       </c>
@@ -26930,7 +26956,7 @@
         <v>420</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="421">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A421" s="46">
         <v>96</v>
       </c>
@@ -26960,7 +26986,7 @@
         <v>421</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="422">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A422" s="46">
         <v>96</v>
       </c>
@@ -26990,7 +27016,7 @@
         <v>422</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="423">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A423" s="46">
         <v>96</v>
       </c>
@@ -27011,7 +27037,7 @@
         <v>423</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="424">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A424" s="46">
         <v>97</v>
       </c>
@@ -27041,7 +27067,7 @@
         <v>424</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="425">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A425" s="46">
         <v>97</v>
       </c>
@@ -27071,7 +27097,7 @@
         <v>425</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="426">
+    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A426" s="46">
         <v>97</v>
       </c>
@@ -27092,7 +27118,7 @@
         <v>426</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="427">
+    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A427" s="46">
         <v>98</v>
       </c>
@@ -27122,7 +27148,7 @@
         <v>427</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="428">
+    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A428" s="46">
         <v>98</v>
       </c>
@@ -27152,7 +27178,7 @@
         <v>428</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="429">
+    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A429" s="46">
         <v>98</v>
       </c>
@@ -27173,7 +27199,7 @@
         <v>429</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="430">
+    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A430" s="46">
         <v>99</v>
       </c>
@@ -27203,7 +27229,7 @@
         <v>430</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="431">
+    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A431" s="46">
         <v>99</v>
       </c>
@@ -27233,7 +27259,7 @@
         <v>431</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="432">
+    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A432" s="46">
         <v>99</v>
       </c>
@@ -27254,7 +27280,7 @@
         <v>432</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="433">
+    <row r="433" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A433" s="46">
         <v>100</v>
       </c>
@@ -27284,7 +27310,7 @@
         <v>433</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="434">
+    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A434" s="46">
         <v>100</v>
       </c>
@@ -27314,7 +27340,7 @@
         <v>434</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="435">
+    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A435" s="46">
         <v>100</v>
       </c>
@@ -27335,7 +27361,7 @@
         <v>435</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="436">
+    <row r="436" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A436" s="46">
         <v>101</v>
       </c>
@@ -27365,7 +27391,7 @@
         <v>436</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="437">
+    <row r="437" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A437" s="46">
         <v>101</v>
       </c>
@@ -27395,7 +27421,7 @@
         <v>437</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="438">
+    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A438" s="46">
         <v>101</v>
       </c>
@@ -27416,7 +27442,7 @@
         <v>438</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="439">
+    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A439" s="46">
         <v>102</v>
       </c>
@@ -27446,7 +27472,7 @@
         <v>439</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="440">
+    <row r="440" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A440" s="46">
         <v>102</v>
       </c>
@@ -27476,7 +27502,7 @@
         <v>440</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="441">
+    <row r="441" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A441" s="46">
         <v>102</v>
       </c>
@@ -27497,7 +27523,7 @@
         <v>441</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="442">
+    <row r="442" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A442" s="46">
         <v>103</v>
       </c>
@@ -27527,7 +27553,7 @@
         <v>442</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="443">
+    <row r="443" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A443" s="46">
         <v>103</v>
       </c>
@@ -27557,7 +27583,7 @@
         <v>443</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="444">
+    <row r="444" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A444" s="46">
         <v>103</v>
       </c>
@@ -27578,7 +27604,7 @@
         <v>444</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="445">
+    <row r="445" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A445" s="46">
         <v>104</v>
       </c>
@@ -27608,7 +27634,7 @@
         <v>445</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="446">
+    <row r="446" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A446" s="46">
         <v>104</v>
       </c>
@@ -27638,7 +27664,7 @@
         <v>446</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="447">
+    <row r="447" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A447" s="46">
         <v>104</v>
       </c>
@@ -27659,7 +27685,7 @@
         <v>447</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="448">
+    <row r="448" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A448" s="46">
         <v>105</v>
       </c>
@@ -27689,7 +27715,7 @@
         <v>448</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="449">
+    <row r="449" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A449" s="46">
         <v>105</v>
       </c>
@@ -27719,7 +27745,7 @@
         <v>449</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="450">
+    <row r="450" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A450" s="46">
         <v>105</v>
       </c>
@@ -27740,7 +27766,7 @@
         <v>450</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="451">
+    <row r="451" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A451" s="46">
         <v>106</v>
       </c>
@@ -27770,7 +27796,7 @@
         <v>451</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="452">
+    <row r="452" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A452" s="46">
         <v>106</v>
       </c>
@@ -27800,7 +27826,7 @@
         <v>452</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="453">
+    <row r="453" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A453" s="46">
         <v>106</v>
       </c>
@@ -27821,7 +27847,7 @@
         <v>453</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="454">
+    <row r="454" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A454" s="46">
         <v>107</v>
       </c>
@@ -27851,7 +27877,7 @@
         <v>454</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="455">
+    <row r="455" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A455" s="46">
         <v>107</v>
       </c>
@@ -27881,7 +27907,7 @@
         <v>455</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="456">
+    <row r="456" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A456" s="46">
         <v>107</v>
       </c>
@@ -27902,7 +27928,7 @@
         <v>456</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="457">
+    <row r="457" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A457" s="46">
         <v>108</v>
       </c>
@@ -27930,7 +27956,7 @@
         <v>457</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="458">
+    <row r="458" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A458" s="46">
         <v>108</v>
       </c>
@@ -27959,7 +27985,7 @@
         <v>458</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="459">
+    <row r="459" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A459" s="46">
         <v>108</v>
       </c>
@@ -27988,7 +28014,7 @@
         <v>459</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="460">
+    <row r="460" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A460" s="46">
         <v>108</v>
       </c>
@@ -28017,7 +28043,7 @@
         <v>460</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="461">
+    <row r="461" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A461" s="46">
         <v>108</v>
       </c>
@@ -28046,7 +28072,7 @@
         <v>461</v>
       </c>
     </row>
-    <row spans="1:11" x14ac:dyDescent="0.25" outlineLevel="0" r="462">
+    <row r="462" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A462" s="46">
         <v>108</v>
       </c>
@@ -28065,93 +28091,336 @@
         <v>462</v>
       </c>
     </row>
-    <row outlineLevel="0" r="463">
-      <c r="A463" s="103">
+    <row r="463" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A463" s="46">
         <v>109</v>
       </c>
-      <c r="B463" s="78">
+      <c r="B463" s="41">
         <v>45331</v>
       </c>
-      <c r="C463" s="103">
+      <c r="C463" s="100">
         <v>109</v>
       </c>
-      <c r="D463" s="103" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="E463" s="103" t="inlineStr">
-        <is>
-          <t>TEST - TEST - TEST</t>
-        </is>
-      </c>
-      <c r="F463" s="103" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="G463" s="103" t="inlineStr">
-        <is>
-          <t>Encaisse</t>
-        </is>
-      </c>
-      <c r="H463" s="76">
+      <c r="D463" s="103" t="s">
+        <v>307</v>
+      </c>
+      <c r="E463" s="103" t="s">
+        <v>630</v>
+      </c>
+      <c r="F463" s="100" t="s">
+        <v>401</v>
+      </c>
+      <c r="G463" s="103" t="s">
+        <v>399</v>
+      </c>
+      <c r="H463" s="101">
         <v>199.99</v>
       </c>
-    </row>
-    <row outlineLevel="0" r="464">
-      <c r="A464" s="103">
+      <c r="I463" s="101"/>
+      <c r="K463" s="46">
+        <f>ROW()</f>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="464" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A464" s="46">
         <v>109</v>
       </c>
-      <c r="B464" s="78">
+      <c r="B464" s="31">
         <v>45331</v>
       </c>
-      <c r="C464" s="103">
+      <c r="C464" s="105">
         <v>109</v>
       </c>
-      <c r="D464" s="103" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="E464" s="103" t="inlineStr">
-        <is>
-          <t>TEST - TEST - TEST</t>
-        </is>
-      </c>
-      <c r="F464" s="103" t="inlineStr">
-        <is>
-          <t>5013</t>
-        </is>
-      </c>
-      <c r="G464" s="103" t="inlineStr">
-        <is>
-          <t>Frais financiers</t>
-        </is>
-      </c>
-      <c r="I464" s="76">
+      <c r="D464" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="E464" s="105" t="s">
+        <v>630</v>
+      </c>
+      <c r="F464" s="100" t="s">
+        <v>468</v>
+      </c>
+      <c r="G464" s="103" t="s">
+        <v>469</v>
+      </c>
+      <c r="H464" s="101"/>
+      <c r="I464" s="101">
         <v>199.99</v>
       </c>
-    </row>
-    <row outlineLevel="0" r="465">
-      <c r="A465" s="103">
+      <c r="K464" s="46">
+        <f>ROW()</f>
+        <v>464</v>
+      </c>
+    </row>
+    <row r="465" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A465" s="46">
         <v>109</v>
       </c>
-      <c r="B465" s="78">
+      <c r="B465" s="31">
         <v>45331</v>
       </c>
-      <c r="C465" s="103">
+      <c r="C465" s="105">
         <v>109</v>
       </c>
-      <c r="D465" s="103" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="E465" s="103" t="inlineStr">
-        <is>
-          <t>TEST - TEST - TEST</t>
-        </is>
+      <c r="D465" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="E465" s="105" t="s">
+        <v>630</v>
+      </c>
+      <c r="K465" s="46">
+        <f>ROW()</f>
+        <v>465</v>
+      </c>
+    </row>
+    <row r="466" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A466" s="46">
+        <v>110</v>
+      </c>
+      <c r="B466" s="41">
+        <v>45331</v>
+      </c>
+      <c r="C466" s="1">
+        <v>110</v>
+      </c>
+      <c r="D466" t="s">
+        <v>631</v>
+      </c>
+      <c r="E466" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F466" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G466" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="H466" s="83">
+        <v>45.2</v>
+      </c>
+      <c r="K466" s="46">
+        <f>ROW()</f>
+        <v>466</v>
+      </c>
+    </row>
+    <row r="467" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A467" s="46">
+        <v>110</v>
+      </c>
+      <c r="B467" s="48">
+        <v>45331</v>
+      </c>
+      <c r="C467" s="32">
+        <v>110</v>
+      </c>
+      <c r="D467" s="42" t="s">
+        <v>631</v>
+      </c>
+      <c r="E467" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="F467" s="1">
+        <v>1100</v>
+      </c>
+      <c r="G467" s="14" t="s">
+        <v>571</v>
+      </c>
+      <c r="I467" s="83">
+        <v>45.2</v>
+      </c>
+      <c r="K467" s="46">
+        <f>ROW()</f>
+        <v>467</v>
+      </c>
+    </row>
+    <row r="468" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A468" s="46">
+        <v>110</v>
+      </c>
+      <c r="B468" s="48">
+        <v>45331</v>
+      </c>
+      <c r="C468" s="32">
+        <v>110</v>
+      </c>
+      <c r="D468" s="42" t="s">
+        <v>631</v>
+      </c>
+      <c r="E468" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="K468" s="46">
+        <f>ROW()</f>
+        <v>468</v>
+      </c>
+    </row>
+    <row r="469" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A469" s="46">
+        <v>111</v>
+      </c>
+      <c r="B469" s="41">
+        <v>45331</v>
+      </c>
+      <c r="C469" s="1">
+        <v>111</v>
+      </c>
+      <c r="D469" t="s">
+        <v>632</v>
+      </c>
+      <c r="E469" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F469" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G469" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="H469" s="83">
+        <v>25</v>
+      </c>
+      <c r="K469" s="46">
+        <f>ROW()</f>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="470" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A470" s="46">
+        <v>111</v>
+      </c>
+      <c r="B470" s="48">
+        <v>45331</v>
+      </c>
+      <c r="C470" s="32">
+        <v>111</v>
+      </c>
+      <c r="D470" s="42" t="s">
+        <v>632</v>
+      </c>
+      <c r="E470" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="F470" s="1">
+        <v>1100</v>
+      </c>
+      <c r="G470" s="14" t="s">
+        <v>571</v>
+      </c>
+      <c r="I470" s="83">
+        <v>25</v>
+      </c>
+      <c r="K470" s="46">
+        <f>ROW()</f>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="471" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A471" s="46">
+        <v>111</v>
+      </c>
+      <c r="B471" s="48">
+        <v>45331</v>
+      </c>
+      <c r="C471" s="32">
+        <v>111</v>
+      </c>
+      <c r="D471" s="42" t="s">
+        <v>632</v>
+      </c>
+      <c r="E471" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="K471" s="46">
+        <f>ROW()</f>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="472" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A472" s="46">
+        <v>112</v>
+      </c>
+      <c r="B472" s="108">
+        <v>45331</v>
+      </c>
+      <c r="C472" s="100">
+        <v>112</v>
+      </c>
+      <c r="D472" s="103" t="s">
+        <v>633</v>
+      </c>
+      <c r="E472" s="103" t="s">
+        <v>53</v>
+      </c>
+      <c r="F472" s="100" t="s">
+        <v>401</v>
+      </c>
+      <c r="G472" s="103" t="s">
+        <v>399</v>
+      </c>
+      <c r="H472" s="83">
+        <v>25</v>
+      </c>
+      <c r="J472" s="103" t="s">
+        <v>634</v>
+      </c>
+      <c r="K472" s="46">
+        <f>ROW()</f>
+        <v>472</v>
+      </c>
+    </row>
+    <row r="473" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A473" s="46">
+        <v>112</v>
+      </c>
+      <c r="B473" s="106">
+        <v>45331</v>
+      </c>
+      <c r="C473" s="107">
+        <v>112</v>
+      </c>
+      <c r="D473" s="107" t="s">
+        <v>633</v>
+      </c>
+      <c r="E473" s="107" t="s">
+        <v>53</v>
+      </c>
+      <c r="F473" s="100" t="s">
+        <v>446</v>
+      </c>
+      <c r="G473" s="103" t="s">
+        <v>571</v>
+      </c>
+      <c r="I473" s="83">
+        <v>25</v>
+      </c>
+      <c r="J473" s="103" t="s">
+        <v>634</v>
+      </c>
+      <c r="K473" s="46">
+        <f>ROW()</f>
+        <v>473</v>
+      </c>
+    </row>
+    <row r="474" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A474" s="46">
+        <v>112</v>
+      </c>
+      <c r="B474" s="106">
+        <v>45331</v>
+      </c>
+      <c r="C474" s="107">
+        <v>112</v>
+      </c>
+      <c r="D474" s="107" t="s">
+        <v>633</v>
+      </c>
+      <c r="E474" s="107" t="s">
+        <v>53</v>
+      </c>
+      <c r="K474" s="46">
+        <f>ROW()</f>
+        <v>474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v2.0.1 - Changements aux noms de routines + Tests TEC
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE4BAC1-710E-4C55-A093-307A15F027ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B040CB43-7C68-4BB5-8EB9-7FC716B0BD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEC" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2670" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2708" uniqueCount="650">
   <si>
     <t>TEC_ID</t>
   </si>
@@ -2005,6 +2005,33 @@
   </si>
   <si>
     <t>Test avec Guillaume</t>
+  </si>
+  <si>
+    <t>Test en date du 14 février</t>
+  </si>
+  <si>
+    <t>Coomentaire en date du 14 février</t>
+  </si>
+  <si>
+    <t>v2.0.1</t>
+  </si>
+  <si>
+    <t>Commentaire en date du 14 février</t>
+  </si>
+  <si>
+    <t>Test avec nouvelle routine XLOOKUP pour retrouver le ID du client</t>
+  </si>
+  <si>
+    <t>Test avec la version 2.0.1</t>
+  </si>
+  <si>
+    <t>Révision du dossier</t>
+  </si>
+  <si>
+    <t>Tests multiples</t>
+  </si>
+  <si>
+    <t>Lone Star Technologies, Inc.</t>
   </si>
 </sst>
 </file>
@@ -2303,7 +2330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2488,9 +2515,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2544,16 +2568,43 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire 2" xfId="1" xr:uid="{7066D7D9-A0C5-4744-AD1B-CDB1C4228FB1}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFE5F4F7"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2581,7 +2632,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFE5F4F7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2869,12 +2920,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:P248"/>
+  <dimension ref="A1:P257"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A225" activePane="bottomLeft"/>
-      <selection sqref="A1:P1"/>
-      <selection pane="bottomLeft" activeCell="F252" sqref="F252"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A222" activePane="bottomLeft"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
+      <selection pane="bottomLeft" activeCell="F239" sqref="F239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2888,11 +2939,11 @@
     <col min="7" max="7" width="50.7109375" style="10" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.140625" style="9" bestFit="1" customWidth="1"/>
   </cols>
@@ -2919,7 +2970,7 @@
       <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="93" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
@@ -2984,7 +3035,7 @@
       <c r="L2" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M2" s="70"/>
+      <c r="M2" s="68"/>
       <c r="N2" s="68" t="b">
         <v>0</v>
       </c>
@@ -3028,7 +3079,7 @@
       <c r="L3" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M3" s="70"/>
+      <c r="M3" s="68"/>
       <c r="N3" s="68" t="b">
         <v>0</v>
       </c>
@@ -3070,7 +3121,7 @@
       <c r="L4" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M4" s="70"/>
+      <c r="M4" s="68"/>
       <c r="N4" s="68" t="b">
         <v>0</v>
       </c>
@@ -3114,7 +3165,7 @@
       <c r="L5" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M5" s="70"/>
+      <c r="M5" s="68"/>
       <c r="N5" s="68" t="b">
         <v>0</v>
       </c>
@@ -3158,7 +3209,7 @@
       <c r="L6" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M6" s="70"/>
+      <c r="M6" s="68"/>
       <c r="N6" s="68" t="b">
         <v>0</v>
       </c>
@@ -3202,7 +3253,7 @@
       <c r="L7" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M7" s="70"/>
+      <c r="M7" s="68"/>
       <c r="N7" s="68" t="b">
         <v>0</v>
       </c>
@@ -3246,7 +3297,7 @@
       <c r="L8" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="M8" s="70"/>
+      <c r="M8" s="68"/>
       <c r="N8" s="68" t="b">
         <v>0</v>
       </c>
@@ -3288,7 +3339,7 @@
       <c r="L9" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M9" s="70"/>
+      <c r="M9" s="68"/>
       <c r="N9" s="68" t="b">
         <v>0</v>
       </c>
@@ -3332,7 +3383,7 @@
       <c r="L10" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M10" s="70"/>
+      <c r="M10" s="68"/>
       <c r="N10" s="68" t="b">
         <v>0</v>
       </c>
@@ -3376,7 +3427,7 @@
       <c r="L11" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M11" s="70"/>
+      <c r="M11" s="68"/>
       <c r="N11" s="68" t="b">
         <v>0</v>
       </c>
@@ -3418,7 +3469,7 @@
       <c r="L12" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M12" s="70"/>
+      <c r="M12" s="68"/>
       <c r="N12" s="68" t="b">
         <v>0</v>
       </c>
@@ -3462,7 +3513,7 @@
       <c r="L13" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M13" s="70"/>
+      <c r="M13" s="68"/>
       <c r="N13" s="68" t="b">
         <v>0</v>
       </c>
@@ -3506,7 +3557,7 @@
       <c r="L14" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="M14" s="70"/>
+      <c r="M14" s="68"/>
       <c r="N14" s="68" t="b">
         <v>0</v>
       </c>
@@ -3550,7 +3601,7 @@
       <c r="L15" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M15" s="70"/>
+      <c r="M15" s="68"/>
       <c r="N15" s="68" t="b">
         <v>0</v>
       </c>
@@ -3594,7 +3645,7 @@
       <c r="L16" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="M16" s="70"/>
+      <c r="M16" s="68"/>
       <c r="N16" s="68" t="b">
         <v>0</v>
       </c>
@@ -3638,7 +3689,7 @@
       <c r="L17" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M17" s="70"/>
+      <c r="M17" s="68"/>
       <c r="N17" s="68" t="b">
         <v>0</v>
       </c>
@@ -3678,7 +3729,7 @@
       <c r="L18" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M18" s="70"/>
+      <c r="M18" s="68"/>
       <c r="N18" s="68" t="b">
         <v>0</v>
       </c>
@@ -3720,7 +3771,7 @@
       <c r="L19" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M19" s="70"/>
+      <c r="M19" s="68"/>
       <c r="N19" s="68" t="b">
         <v>0</v>
       </c>
@@ -3762,7 +3813,7 @@
       <c r="L20" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="M20" s="70"/>
+      <c r="M20" s="68"/>
       <c r="N20" s="68" t="b">
         <v>0</v>
       </c>
@@ -3804,7 +3855,7 @@
       <c r="L21" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M21" s="70"/>
+      <c r="M21" s="68"/>
       <c r="N21" s="68" t="b">
         <v>0</v>
       </c>
@@ -3846,7 +3897,7 @@
       <c r="L22" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="M22" s="70"/>
+      <c r="M22" s="68"/>
       <c r="N22" s="68" t="b">
         <v>0</v>
       </c>
@@ -3888,7 +3939,7 @@
       <c r="L23" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M23" s="70"/>
+      <c r="M23" s="68"/>
       <c r="N23" s="68" t="b">
         <v>0</v>
       </c>
@@ -3932,7 +3983,7 @@
       <c r="L24" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M24" s="70"/>
+      <c r="M24" s="68"/>
       <c r="N24" s="68" t="b">
         <v>0</v>
       </c>
@@ -3976,7 +4027,7 @@
       <c r="L25" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M25" s="70"/>
+      <c r="M25" s="68"/>
       <c r="N25" s="68" t="b">
         <v>0</v>
       </c>
@@ -4018,7 +4069,7 @@
       <c r="L26" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M26" s="70"/>
+      <c r="M26" s="68"/>
       <c r="N26" s="68" t="b">
         <v>0</v>
       </c>
@@ -4060,7 +4111,7 @@
       <c r="L27" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M27" s="70"/>
+      <c r="M27" s="68"/>
       <c r="N27" s="68" t="b">
         <v>0</v>
       </c>
@@ -4102,7 +4153,7 @@
       <c r="L28" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M28" s="70"/>
+      <c r="M28" s="68"/>
       <c r="N28" s="68" t="b">
         <v>0</v>
       </c>
@@ -4144,7 +4195,7 @@
       <c r="L29" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M29" s="70"/>
+      <c r="M29" s="68"/>
       <c r="N29" s="68" t="b">
         <v>0</v>
       </c>
@@ -4186,7 +4237,7 @@
       <c r="L30" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M30" s="70"/>
+      <c r="M30" s="68"/>
       <c r="N30" s="68" t="b">
         <v>0</v>
       </c>
@@ -4228,7 +4279,7 @@
       <c r="L31" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M31" s="70"/>
+      <c r="M31" s="68"/>
       <c r="N31" s="68" t="b">
         <v>0</v>
       </c>
@@ -4272,7 +4323,7 @@
       <c r="L32" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M32" s="70"/>
+      <c r="M32" s="68"/>
       <c r="N32" s="68" t="b">
         <v>0</v>
       </c>
@@ -4314,7 +4365,7 @@
       <c r="L33" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M33" s="70"/>
+      <c r="M33" s="68"/>
       <c r="N33" s="68" t="b">
         <v>0</v>
       </c>
@@ -4356,7 +4407,7 @@
       <c r="L34" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M34" s="70"/>
+      <c r="M34" s="68"/>
       <c r="N34" s="68" t="b">
         <v>0</v>
       </c>
@@ -4398,7 +4449,7 @@
       <c r="L35" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M35" s="70"/>
+      <c r="M35" s="68"/>
       <c r="N35" s="68" t="b">
         <v>0</v>
       </c>
@@ -4440,7 +4491,7 @@
       <c r="L36" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M36" s="70"/>
+      <c r="M36" s="68"/>
       <c r="N36" s="68" t="b">
         <v>0</v>
       </c>
@@ -4482,7 +4533,7 @@
       <c r="L37" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M37" s="70"/>
+      <c r="M37" s="68"/>
       <c r="N37" s="68" t="b">
         <v>0</v>
       </c>
@@ -4524,7 +4575,7 @@
       <c r="L38" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M38" s="70"/>
+      <c r="M38" s="68"/>
       <c r="N38" s="68" t="b">
         <v>0</v>
       </c>
@@ -4566,7 +4617,7 @@
       <c r="L39" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M39" s="70"/>
+      <c r="M39" s="68"/>
       <c r="N39" s="68" t="b">
         <v>0</v>
       </c>
@@ -4608,7 +4659,7 @@
       <c r="L40" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M40" s="70"/>
+      <c r="M40" s="68"/>
       <c r="N40" s="68" t="b">
         <v>0</v>
       </c>
@@ -4650,7 +4701,7 @@
       <c r="L41" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M41" s="70"/>
+      <c r="M41" s="68"/>
       <c r="N41" s="68" t="b">
         <v>0</v>
       </c>
@@ -4694,7 +4745,7 @@
       <c r="L42" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M42" s="70"/>
+      <c r="M42" s="68"/>
       <c r="N42" s="68" t="b">
         <v>0</v>
       </c>
@@ -4738,7 +4789,7 @@
       <c r="L43" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M43" s="70"/>
+      <c r="M43" s="68"/>
       <c r="N43" s="68" t="b">
         <v>0</v>
       </c>
@@ -4780,7 +4831,7 @@
       <c r="L44" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M44" s="70"/>
+      <c r="M44" s="68"/>
       <c r="N44" s="68" t="b">
         <v>0</v>
       </c>
@@ -4822,7 +4873,7 @@
       <c r="L45" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M45" s="70"/>
+      <c r="M45" s="68"/>
       <c r="N45" s="68" t="b">
         <v>0</v>
       </c>
@@ -4864,7 +4915,7 @@
       <c r="L46" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M46" s="70"/>
+      <c r="M46" s="68"/>
       <c r="N46" s="68" t="b">
         <v>0</v>
       </c>
@@ -4906,7 +4957,7 @@
       <c r="L47" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M47" s="70"/>
+      <c r="M47" s="68"/>
       <c r="N47" s="68" t="b">
         <v>0</v>
       </c>
@@ -4948,7 +4999,7 @@
       <c r="L48" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M48" s="70"/>
+      <c r="M48" s="68"/>
       <c r="N48" s="68" t="b">
         <v>0</v>
       </c>
@@ -4990,7 +5041,7 @@
       <c r="L49" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M49" s="70"/>
+      <c r="M49" s="68"/>
       <c r="N49" s="68" t="b">
         <v>0</v>
       </c>
@@ -5032,7 +5083,7 @@
       <c r="L50" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M50" s="70"/>
+      <c r="M50" s="68"/>
       <c r="N50" s="68" t="b">
         <v>0</v>
       </c>
@@ -5074,7 +5125,7 @@
       <c r="L51" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M51" s="70"/>
+      <c r="M51" s="68"/>
       <c r="N51" s="68" t="b">
         <v>0</v>
       </c>
@@ -5116,7 +5167,7 @@
       <c r="L52" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M52" s="70"/>
+      <c r="M52" s="68"/>
       <c r="N52" s="68" t="b">
         <v>0</v>
       </c>
@@ -5158,7 +5209,7 @@
       <c r="L53" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M53" s="70"/>
+      <c r="M53" s="68"/>
       <c r="N53" s="68" t="b">
         <v>0</v>
       </c>
@@ -5200,7 +5251,7 @@
       <c r="L54" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M54" s="70"/>
+      <c r="M54" s="68"/>
       <c r="N54" s="68" t="b">
         <v>0</v>
       </c>
@@ -5242,7 +5293,7 @@
       <c r="L55" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="M55" s="70"/>
+      <c r="M55" s="68"/>
       <c r="N55" s="68" t="b">
         <v>0</v>
       </c>
@@ -5284,7 +5335,7 @@
       <c r="L56" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="M56" s="70"/>
+      <c r="M56" s="68"/>
       <c r="N56" s="68" t="b">
         <v>0</v>
       </c>
@@ -5452,7 +5503,7 @@
       <c r="L60" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M60" s="70"/>
+      <c r="M60" s="68"/>
       <c r="N60" s="68" t="b">
         <v>0</v>
       </c>
@@ -5561,7 +5612,7 @@
       <c r="E63" s="64">
         <v>895</v>
       </c>
-      <c r="F63" s="71" t="s">
+      <c r="F63" s="70" t="s">
         <v>118</v>
       </c>
       <c r="G63" s="67" t="s">
@@ -5603,7 +5654,7 @@
       <c r="E64" s="64">
         <v>895</v>
       </c>
-      <c r="F64" s="71" t="s">
+      <c r="F64" s="70" t="s">
         <v>118</v>
       </c>
       <c r="G64" s="67" t="s">
@@ -5645,7 +5696,7 @@
       <c r="E65" s="64">
         <v>895</v>
       </c>
-      <c r="F65" s="71" t="s">
+      <c r="F65" s="70" t="s">
         <v>118</v>
       </c>
       <c r="G65" s="67" t="s">
@@ -6246,7 +6297,7 @@
       <c r="L79" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M79" s="70"/>
+      <c r="M79" s="68"/>
       <c r="N79" s="68" t="b">
         <v>0</v>
       </c>
@@ -6622,7 +6673,7 @@
       <c r="L88" s="68" t="b">
         <v>0</v>
       </c>
-      <c r="M88" s="70"/>
+      <c r="M88" s="68"/>
       <c r="N88" s="68" t="b">
         <v>0</v>
       </c>
@@ -7107,7 +7158,7 @@
       <c r="E100" s="64">
         <v>895</v>
       </c>
-      <c r="F100" s="71" t="s">
+      <c r="F100" s="70" t="s">
         <v>118</v>
       </c>
       <c r="G100" s="67" t="s">
@@ -8422,7 +8473,7 @@
       <c r="E132" s="64">
         <v>895</v>
       </c>
-      <c r="F132" s="71" t="s">
+      <c r="F132" s="70" t="s">
         <v>118</v>
       </c>
       <c r="G132" s="67" t="s">
@@ -9201,7 +9252,7 @@
       <c r="E151" s="64">
         <v>895</v>
       </c>
-      <c r="F151" s="71" t="s">
+      <c r="F151" s="70" t="s">
         <v>118</v>
       </c>
       <c r="G151" s="67" t="s">
@@ -9326,7 +9377,7 @@
       <c r="E154" s="64">
         <v>895</v>
       </c>
-      <c r="F154" s="71" t="s">
+      <c r="F154" s="70" t="s">
         <v>118</v>
       </c>
       <c r="G154" s="67" t="s">
@@ -9900,7 +9951,7 @@
       <c r="E168" s="64">
         <v>895</v>
       </c>
-      <c r="F168" s="71" t="s">
+      <c r="F168" s="70" t="s">
         <v>118</v>
       </c>
       <c r="G168" s="67" t="s">
@@ -10027,7 +10078,7 @@
       <c r="E171" s="64">
         <v>895</v>
       </c>
-      <c r="F171" s="71" t="s">
+      <c r="F171" s="70" t="s">
         <v>118</v>
       </c>
       <c r="G171" s="67" t="s">
@@ -10116,7 +10167,7 @@
       <c r="E173" s="64">
         <v>895</v>
       </c>
-      <c r="F173" s="71" t="s">
+      <c r="F173" s="70" t="s">
         <v>118</v>
       </c>
       <c r="G173" s="67" t="s">
@@ -10128,7 +10179,7 @@
       <c r="I173" s="67" t="s">
         <v>248</v>
       </c>
-      <c r="J173" t="b">
+      <c r="J173" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K173" s="69">
@@ -10138,7 +10189,7 @@
         <v>0</v>
       </c>
       <c r="M173" s="68"/>
-      <c r="N173" t="b">
+      <c r="N173" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O173" s="10" t="s">
@@ -10174,7 +10225,7 @@
       <c r="I174" s="67" t="s">
         <v>249</v>
       </c>
-      <c r="J174" t="b">
+      <c r="J174" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K174" s="69">
@@ -10184,7 +10235,7 @@
         <v>0</v>
       </c>
       <c r="M174" s="68"/>
-      <c r="N174" t="b">
+      <c r="N174" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O174" s="10" t="s">
@@ -10220,7 +10271,7 @@
       <c r="I175" s="67" t="s">
         <v>252</v>
       </c>
-      <c r="J175" t="b">
+      <c r="J175" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K175" s="69">
@@ -10230,7 +10281,7 @@
         <v>0</v>
       </c>
       <c r="M175" s="68"/>
-      <c r="N175" t="b">
+      <c r="N175" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O175" s="10" t="s">
@@ -10266,7 +10317,7 @@
       <c r="I176" s="67" t="s">
         <v>253</v>
       </c>
-      <c r="J176" t="b">
+      <c r="J176" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K176" s="69">
@@ -10276,7 +10327,7 @@
         <v>0</v>
       </c>
       <c r="M176" s="68"/>
-      <c r="N176" t="b">
+      <c r="N176" s="1" t="b">
         <v>1</v>
       </c>
       <c r="O176" s="10" t="s">
@@ -10312,7 +10363,7 @@
       <c r="I177" s="67" t="s">
         <v>255</v>
       </c>
-      <c r="J177" t="b">
+      <c r="J177" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K177" s="69">
@@ -10322,7 +10373,7 @@
         <v>0</v>
       </c>
       <c r="M177" s="68"/>
-      <c r="N177" t="b">
+      <c r="N177" s="1" t="b">
         <v>1</v>
       </c>
       <c r="O177" s="10" t="s">
@@ -10358,7 +10409,7 @@
       <c r="I178" s="67" t="s">
         <v>257</v>
       </c>
-      <c r="J178" t="b">
+      <c r="J178" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K178" s="69">
@@ -10368,7 +10419,7 @@
         <v>0</v>
       </c>
       <c r="M178" s="68"/>
-      <c r="N178" t="b">
+      <c r="N178" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O178" s="10" t="s">
@@ -10404,7 +10455,7 @@
       <c r="I179" s="67" t="s">
         <v>259</v>
       </c>
-      <c r="J179" t="b">
+      <c r="J179" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K179" s="69">
@@ -10414,7 +10465,7 @@
         <v>0</v>
       </c>
       <c r="M179" s="68"/>
-      <c r="N179" t="b">
+      <c r="N179" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O179" s="10" t="s">
@@ -10450,7 +10501,7 @@
       <c r="I180" s="67" t="s">
         <v>260</v>
       </c>
-      <c r="J180" t="b">
+      <c r="J180" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K180" s="69">
@@ -10460,7 +10511,7 @@
         <v>0</v>
       </c>
       <c r="M180" s="68"/>
-      <c r="N180" t="b">
+      <c r="N180" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O180" s="10" t="s">
@@ -10496,7 +10547,7 @@
       <c r="I181" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="J181" t="b">
+      <c r="J181" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K181" s="69">
@@ -10506,7 +10557,7 @@
         <v>0</v>
       </c>
       <c r="M181" s="68"/>
-      <c r="N181" t="b">
+      <c r="N181" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O181" s="10" t="s">
@@ -10540,7 +10591,7 @@
         <v>24</v>
       </c>
       <c r="I182" s="67"/>
-      <c r="J182" t="b">
+      <c r="J182" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K182" s="69">
@@ -10550,7 +10601,7 @@
         <v>0</v>
       </c>
       <c r="M182" s="68"/>
-      <c r="N182" t="b">
+      <c r="N182" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O182" s="10" t="s">
@@ -10584,7 +10635,7 @@
         <v>32</v>
       </c>
       <c r="I183" s="67"/>
-      <c r="J183" t="b">
+      <c r="J183" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K183" s="69">
@@ -10594,7 +10645,7 @@
         <v>0</v>
       </c>
       <c r="M183" s="68"/>
-      <c r="N183" t="b">
+      <c r="N183" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O183" s="10" t="s">
@@ -10628,7 +10679,7 @@
         <v>32</v>
       </c>
       <c r="I184" s="67"/>
-      <c r="J184" t="b">
+      <c r="J184" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K184" s="69">
@@ -10638,7 +10689,7 @@
         <v>0</v>
       </c>
       <c r="M184" s="68"/>
-      <c r="N184" t="b">
+      <c r="N184" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O184" s="10" t="s">
@@ -10674,7 +10725,7 @@
       <c r="I185" s="67">
         <v>45274.500486111101</v>
       </c>
-      <c r="J185" t="b">
+      <c r="J185" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K185" s="69">
@@ -10684,7 +10735,7 @@
         <v>0</v>
       </c>
       <c r="M185" s="68"/>
-      <c r="N185" t="b">
+      <c r="N185" s="1" t="b">
         <v>1</v>
       </c>
       <c r="O185" s="10" t="s">
@@ -10720,7 +10771,7 @@
       <c r="I186" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="J186" t="b">
+      <c r="J186" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K186" s="69">
@@ -10730,7 +10781,7 @@
         <v>0</v>
       </c>
       <c r="M186" s="68"/>
-      <c r="N186" t="b">
+      <c r="N186" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O186" s="10" t="s">
@@ -10766,7 +10817,7 @@
       <c r="I187" s="67" t="s">
         <v>268</v>
       </c>
-      <c r="J187" t="b">
+      <c r="J187" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K187" s="69">
@@ -10776,7 +10827,7 @@
         <v>0</v>
       </c>
       <c r="M187" s="68"/>
-      <c r="N187" t="b">
+      <c r="N187" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O187" s="10" t="s">
@@ -10812,7 +10863,7 @@
       <c r="I188" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="J188" t="b">
+      <c r="J188" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K188" s="69">
@@ -10822,7 +10873,7 @@
         <v>0</v>
       </c>
       <c r="M188" s="68"/>
-      <c r="N188" t="b">
+      <c r="N188" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O188" s="10" t="s">
@@ -10858,7 +10909,7 @@
       <c r="I189" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="J189" t="b">
+      <c r="J189" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K189" s="69">
@@ -10868,7 +10919,7 @@
         <v>0</v>
       </c>
       <c r="M189" s="68"/>
-      <c r="N189" t="b">
+      <c r="N189" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O189" s="10" t="s">
@@ -10900,7 +10951,7 @@
         <v>24</v>
       </c>
       <c r="I190" s="67"/>
-      <c r="J190" t="b">
+      <c r="J190" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K190" s="69">
@@ -10910,7 +10961,7 @@
         <v>0</v>
       </c>
       <c r="M190" s="68"/>
-      <c r="N190" t="b">
+      <c r="N190" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O190" s="10" t="s">
@@ -10942,7 +10993,7 @@
         <v>24</v>
       </c>
       <c r="I191" s="67"/>
-      <c r="J191" t="b">
+      <c r="J191" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K191" s="69">
@@ -10952,7 +11003,7 @@
         <v>0</v>
       </c>
       <c r="M191" s="68"/>
-      <c r="N191" t="b">
+      <c r="N191" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O191" s="10" t="s">
@@ -10984,7 +11035,7 @@
         <v>32</v>
       </c>
       <c r="I192" s="67"/>
-      <c r="J192" t="b">
+      <c r="J192" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K192" s="69">
@@ -10994,7 +11045,7 @@
         <v>0</v>
       </c>
       <c r="M192" s="68"/>
-      <c r="N192" t="b">
+      <c r="N192" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O192" s="10" t="s">
@@ -11026,7 +11077,7 @@
         <v>24</v>
       </c>
       <c r="I193" s="67"/>
-      <c r="J193" t="b">
+      <c r="J193" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K193" s="69">
@@ -11036,7 +11087,7 @@
         <v>0</v>
       </c>
       <c r="M193" s="68"/>
-      <c r="N193" t="b">
+      <c r="N193" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O193" s="10" t="s">
@@ -11070,7 +11121,7 @@
         <v>32</v>
       </c>
       <c r="I194" s="67"/>
-      <c r="J194" t="b">
+      <c r="J194" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K194" s="69">
@@ -11080,7 +11131,7 @@
         <v>0</v>
       </c>
       <c r="M194" s="68"/>
-      <c r="N194" t="b">
+      <c r="N194" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O194" s="10" t="s">
@@ -11114,7 +11165,7 @@
         <v>275</v>
       </c>
       <c r="I195" s="67"/>
-      <c r="J195" t="b">
+      <c r="J195" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K195" s="69">
@@ -11124,7 +11175,7 @@
         <v>0</v>
       </c>
       <c r="M195" s="68"/>
-      <c r="N195" t="b">
+      <c r="N195" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O195" s="10" t="s">
@@ -11166,7 +11217,7 @@
       <c r="K196" s="69">
         <v>45261.385486111103</v>
       </c>
-      <c r="L196" t="b">
+      <c r="L196" s="1" t="b">
         <v>0</v>
       </c>
       <c r="M196" s="68"/>
@@ -11204,7 +11255,7 @@
         <v>222</v>
       </c>
       <c r="I197" s="67"/>
-      <c r="J197" t="b">
+      <c r="J197" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K197" s="69">
@@ -11214,7 +11265,7 @@
         <v>0</v>
       </c>
       <c r="M197" s="68"/>
-      <c r="N197" t="b">
+      <c r="N197" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O197" s="10" t="s">
@@ -11250,7 +11301,7 @@
       <c r="I198" s="67" t="s">
         <v>282</v>
       </c>
-      <c r="J198" t="b">
+      <c r="J198" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K198" s="69">
@@ -11260,7 +11311,7 @@
         <v>0</v>
       </c>
       <c r="M198" s="68"/>
-      <c r="N198" t="b">
+      <c r="N198" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O198" s="10" t="s">
@@ -11294,7 +11345,7 @@
         <v>24</v>
       </c>
       <c r="I199" s="67"/>
-      <c r="J199" t="b">
+      <c r="J199" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K199" s="69">
@@ -11304,7 +11355,7 @@
         <v>0</v>
       </c>
       <c r="M199" s="68"/>
-      <c r="N199" t="b">
+      <c r="N199" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O199" s="10" t="s">
@@ -11338,7 +11389,7 @@
         <v>287</v>
       </c>
       <c r="I200" s="67"/>
-      <c r="J200" t="b">
+      <c r="J200" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K200" s="69">
@@ -11348,7 +11399,7 @@
         <v>0</v>
       </c>
       <c r="M200" s="68"/>
-      <c r="N200" t="b">
+      <c r="N200" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O200" s="10" t="s">
@@ -11382,7 +11433,7 @@
         <v>32</v>
       </c>
       <c r="I201" s="67"/>
-      <c r="J201" t="b">
+      <c r="J201" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K201" s="69">
@@ -11392,7 +11443,7 @@
         <v>0</v>
       </c>
       <c r="M201" s="68"/>
-      <c r="N201" t="b">
+      <c r="N201" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O201" s="10" t="s">
@@ -11426,7 +11477,7 @@
         <v>222</v>
       </c>
       <c r="I202" s="67"/>
-      <c r="J202" t="b">
+      <c r="J202" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K202" s="69">
@@ -11436,7 +11487,7 @@
         <v>0</v>
       </c>
       <c r="M202" s="68"/>
-      <c r="N202" t="b">
+      <c r="N202" s="1" t="b">
         <v>1</v>
       </c>
       <c r="O202" s="10" t="s">
@@ -11470,7 +11521,7 @@
         <v>294</v>
       </c>
       <c r="I203" s="67"/>
-      <c r="J203" t="b">
+      <c r="J203" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K203" s="69">
@@ -11480,7 +11531,7 @@
         <v>0</v>
       </c>
       <c r="M203" s="68"/>
-      <c r="N203" t="b">
+      <c r="N203" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O203" s="10" t="s">
@@ -11514,7 +11565,7 @@
         <v>24</v>
       </c>
       <c r="I204" s="67"/>
-      <c r="J204" t="b">
+      <c r="J204" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K204" s="69">
@@ -11524,7 +11575,7 @@
         <v>0</v>
       </c>
       <c r="M204" s="68"/>
-      <c r="N204" t="b">
+      <c r="N204" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O204" s="10" t="s">
@@ -11560,7 +11611,7 @@
       <c r="I205" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="J205" t="b">
+      <c r="J205" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K205" s="69">
@@ -11570,7 +11621,7 @@
         <v>0</v>
       </c>
       <c r="M205" s="68"/>
-      <c r="N205" t="b">
+      <c r="N205" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O205" s="10" t="s">
@@ -11604,7 +11655,7 @@
         <v>24</v>
       </c>
       <c r="I206" s="67"/>
-      <c r="J206" t="b">
+      <c r="J206" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K206" s="69">
@@ -11614,7 +11665,7 @@
         <v>0</v>
       </c>
       <c r="M206" s="68"/>
-      <c r="N206" t="b">
+      <c r="N206" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O206" s="10" t="s">
@@ -11648,7 +11699,7 @@
         <v>94</v>
       </c>
       <c r="I207" s="67"/>
-      <c r="J207" t="b">
+      <c r="J207" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K207" s="69">
@@ -11658,7 +11709,7 @@
         <v>0</v>
       </c>
       <c r="M207" s="68"/>
-      <c r="N207" t="b">
+      <c r="N207" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O207" s="10" t="s">
@@ -11692,7 +11743,7 @@
         <v>299</v>
       </c>
       <c r="I208" s="67"/>
-      <c r="J208" t="b">
+      <c r="J208" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K208" s="69">
@@ -11702,7 +11753,7 @@
         <v>0</v>
       </c>
       <c r="M208" s="68"/>
-      <c r="N208" t="b">
+      <c r="N208" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O208" s="10" t="s">
@@ -11736,7 +11787,7 @@
         <v>29</v>
       </c>
       <c r="I209" s="67"/>
-      <c r="J209" t="b">
+      <c r="J209" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K209" s="69">
@@ -11746,7 +11797,7 @@
         <v>0</v>
       </c>
       <c r="M209" s="68"/>
-      <c r="N209" t="b">
+      <c r="N209" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O209" s="10" t="s">
@@ -11780,7 +11831,7 @@
         <v>19</v>
       </c>
       <c r="I210" s="67"/>
-      <c r="J210" t="b">
+      <c r="J210" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K210" s="69">
@@ -11790,7 +11841,7 @@
         <v>0</v>
       </c>
       <c r="M210" s="68"/>
-      <c r="N210" t="b">
+      <c r="N210" s="1" t="b">
         <v>1</v>
       </c>
       <c r="O210" s="10" t="s">
@@ -11824,7 +11875,7 @@
         <v>199</v>
       </c>
       <c r="I211" s="67"/>
-      <c r="J211" t="b">
+      <c r="J211" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K211" s="69">
@@ -11834,7 +11885,7 @@
         <v>0</v>
       </c>
       <c r="M211" s="68"/>
-      <c r="N211" t="b">
+      <c r="N211" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O211" s="10" t="s">
@@ -11868,7 +11919,7 @@
         <v>305</v>
       </c>
       <c r="I212" s="67"/>
-      <c r="J212" t="b">
+      <c r="J212" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K212" s="69">
@@ -11878,7 +11929,7 @@
         <v>0</v>
       </c>
       <c r="M212" s="68"/>
-      <c r="N212" t="b">
+      <c r="N212" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O212" s="10" t="s">
@@ -11912,7 +11963,7 @@
         <v>97</v>
       </c>
       <c r="I213" s="67"/>
-      <c r="J213" t="b">
+      <c r="J213" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K213" s="69">
@@ -11922,7 +11973,7 @@
         <v>0</v>
       </c>
       <c r="M213" s="68"/>
-      <c r="N213" t="b">
+      <c r="N213" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O213" s="10" t="s">
@@ -11956,7 +12007,7 @@
         <v>305</v>
       </c>
       <c r="I214" s="67"/>
-      <c r="J214" t="b">
+      <c r="J214" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K214" s="69">
@@ -11966,7 +12017,7 @@
         <v>0</v>
       </c>
       <c r="M214" s="68"/>
-      <c r="N214" t="b">
+      <c r="N214" s="1" t="b">
         <v>1</v>
       </c>
       <c r="O214" s="10" t="s">
@@ -12000,7 +12051,7 @@
         <v>29</v>
       </c>
       <c r="I215" s="67"/>
-      <c r="J215" t="b">
+      <c r="J215" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K215" s="69">
@@ -12010,7 +12061,7 @@
         <v>0</v>
       </c>
       <c r="M215" s="68"/>
-      <c r="N215" t="b">
+      <c r="N215" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O215" s="10" t="s">
@@ -12044,7 +12095,7 @@
         <v>24</v>
       </c>
       <c r="I216" s="67"/>
-      <c r="J216" t="b">
+      <c r="J216" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K216" s="69">
@@ -12054,7 +12105,7 @@
         <v>0</v>
       </c>
       <c r="M216" s="68"/>
-      <c r="N216" t="b">
+      <c r="N216" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O216" s="10" t="s">
@@ -12088,7 +12139,7 @@
         <v>24</v>
       </c>
       <c r="I217" s="67"/>
-      <c r="J217" t="b">
+      <c r="J217" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K217" s="69">
@@ -12098,7 +12149,7 @@
         <v>0</v>
       </c>
       <c r="M217" s="68"/>
-      <c r="N217" t="b">
+      <c r="N217" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O217" s="10" t="s">
@@ -12132,7 +12183,7 @@
         <v>24</v>
       </c>
       <c r="I218" s="67"/>
-      <c r="J218" t="b">
+      <c r="J218" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K218" s="69">
@@ -12142,7 +12193,7 @@
         <v>0</v>
       </c>
       <c r="M218" s="68"/>
-      <c r="N218" t="b">
+      <c r="N218" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O218" s="10" t="s">
@@ -12176,7 +12227,7 @@
         <v>24</v>
       </c>
       <c r="I219" s="67"/>
-      <c r="J219" t="b">
+      <c r="J219" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K219" s="69">
@@ -12186,7 +12237,7 @@
         <v>0</v>
       </c>
       <c r="M219" s="68"/>
-      <c r="N219" t="b">
+      <c r="N219" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O219" s="10" t="s">
@@ -12220,7 +12271,7 @@
         <v>19</v>
       </c>
       <c r="I220" s="67"/>
-      <c r="J220" t="b">
+      <c r="J220" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K220" s="69">
@@ -12230,7 +12281,7 @@
         <v>0</v>
       </c>
       <c r="M220" s="68"/>
-      <c r="N220" t="b">
+      <c r="N220" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O220" s="10" t="s">
@@ -12264,7 +12315,7 @@
         <v>19</v>
       </c>
       <c r="I221" s="67"/>
-      <c r="J221" t="b">
+      <c r="J221" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K221" s="69">
@@ -12274,7 +12325,7 @@
         <v>0</v>
       </c>
       <c r="M221" s="68"/>
-      <c r="N221" t="b">
+      <c r="N221" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O221" s="10" t="s">
@@ -12310,7 +12361,7 @@
       <c r="I222" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="J222" t="b">
+      <c r="J222" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K222" s="69">
@@ -12320,7 +12371,7 @@
         <v>0</v>
       </c>
       <c r="M222" s="68"/>
-      <c r="N222" t="b">
+      <c r="N222" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O222" s="10" t="s">
@@ -12354,7 +12405,7 @@
         <v>19</v>
       </c>
       <c r="I223" s="67"/>
-      <c r="J223" t="b">
+      <c r="J223" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K223" s="69">
@@ -12364,7 +12415,7 @@
         <v>0</v>
       </c>
       <c r="M223" s="68"/>
-      <c r="N223" t="b">
+      <c r="N223" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O223" s="10" t="s">
@@ -12398,7 +12449,7 @@
         <v>29</v>
       </c>
       <c r="I224" s="67"/>
-      <c r="J224" t="b">
+      <c r="J224" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K224" s="69">
@@ -12408,7 +12459,7 @@
         <v>0</v>
       </c>
       <c r="M224" s="68"/>
-      <c r="N224" t="b">
+      <c r="N224" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O224" s="10" t="s">
@@ -12442,7 +12493,7 @@
         <v>32</v>
       </c>
       <c r="I225" s="67"/>
-      <c r="J225" t="b">
+      <c r="J225" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K225" s="69">
@@ -12452,7 +12503,7 @@
         <v>0</v>
       </c>
       <c r="M225" s="68"/>
-      <c r="N225" t="b">
+      <c r="N225" s="1" t="b">
         <v>1</v>
       </c>
       <c r="O225" s="10" t="s">
@@ -12486,7 +12537,7 @@
         <v>29</v>
       </c>
       <c r="I226" s="67"/>
-      <c r="J226" t="b">
+      <c r="J226" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K226" s="69">
@@ -12496,7 +12547,7 @@
         <v>0</v>
       </c>
       <c r="M226" s="68"/>
-      <c r="N226" t="b">
+      <c r="N226" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O226" s="10" t="s">
@@ -12528,7 +12579,7 @@
         <v>2</v>
       </c>
       <c r="I227" s="67"/>
-      <c r="J227" t="b">
+      <c r="J227" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K227" s="69">
@@ -12538,7 +12589,7 @@
         <v>0</v>
       </c>
       <c r="M227" s="68"/>
-      <c r="N227" t="b">
+      <c r="N227" s="1" t="b">
         <v>1</v>
       </c>
       <c r="O227" s="10" t="s">
@@ -12691,7 +12742,7 @@
       <c r="G231" s="14" t="s">
         <v>321</v>
       </c>
-      <c r="H231" s="1">
+      <c r="H231" s="71">
         <v>0.75</v>
       </c>
       <c r="J231" s="1" t="b">
@@ -12732,7 +12783,7 @@
       <c r="G232" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="H232" s="72">
+      <c r="H232" s="71">
         <v>2</v>
       </c>
       <c r="J232" s="1" t="b">
@@ -12773,7 +12824,7 @@
       <c r="G233" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="H233" s="72">
+      <c r="H233" s="71">
         <v>2.5</v>
       </c>
       <c r="J233" s="1" t="b">
@@ -12814,7 +12865,7 @@
       <c r="G234" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="H234" s="72">
+      <c r="H234" s="71">
         <v>1.75</v>
       </c>
       <c r="I234" s="10" t="s">
@@ -12858,7 +12909,7 @@
       <c r="G235" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="H235" s="72">
+      <c r="H235" s="71">
         <v>1</v>
       </c>
       <c r="J235" s="1" t="b">
@@ -12899,7 +12950,7 @@
       <c r="G236" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="H236" s="72">
+      <c r="H236" s="71">
         <v>2</v>
       </c>
       <c r="I236" s="10" t="s">
@@ -12943,7 +12994,7 @@
       <c r="G237" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="H237" s="72">
+      <c r="H237" s="71">
         <v>1</v>
       </c>
       <c r="J237" s="1" t="b">
@@ -12984,7 +13035,7 @@
       <c r="G238" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="H238" s="72">
+      <c r="H238" s="71">
         <v>1.25</v>
       </c>
       <c r="J238" s="1" t="b">
@@ -13025,7 +13076,7 @@
       <c r="G239" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="H239" s="72">
+      <c r="H239" s="71">
         <v>3.75</v>
       </c>
       <c r="J239" s="1" t="b">
@@ -13064,7 +13115,7 @@
         <v>337</v>
       </c>
       <c r="G240" s="14"/>
-      <c r="H240" s="72">
+      <c r="H240" s="71">
         <v>3</v>
       </c>
       <c r="J240" s="1" t="b">
@@ -13105,7 +13156,7 @@
       <c r="G241" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="H241" s="72">
+      <c r="H241" s="71">
         <v>2</v>
       </c>
       <c r="J241" s="1" t="b">
@@ -13146,7 +13197,7 @@
       <c r="G242" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="H242" s="72">
+      <c r="H242" s="71">
         <v>0.75</v>
       </c>
       <c r="J242" s="1" t="b">
@@ -13187,7 +13238,7 @@
       <c r="G243" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="H243" s="72">
+      <c r="H243" s="71">
         <v>0.25</v>
       </c>
       <c r="J243" s="1" t="b">
@@ -13228,7 +13279,7 @@
       <c r="G244" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="H244" s="72">
+      <c r="H244" s="71">
         <v>0.5</v>
       </c>
       <c r="J244" s="1" t="b">
@@ -13269,7 +13320,7 @@
       <c r="G245" s="14" t="s">
         <v>344</v>
       </c>
-      <c r="H245" s="72">
+      <c r="H245" s="71">
         <v>1</v>
       </c>
       <c r="J245" s="1" t="b">
@@ -13310,7 +13361,7 @@
       <c r="G246" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="H246" s="72">
+      <c r="H246" s="71">
         <v>1</v>
       </c>
       <c r="J246" s="1" t="b">
@@ -13351,7 +13402,7 @@
       <c r="G247" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="H247" s="72">
+      <c r="H247" s="71">
         <v>2.5</v>
       </c>
       <c r="J247" s="1" t="b">
@@ -13392,7 +13443,7 @@
       <c r="G248" s="14" t="s">
         <v>565</v>
       </c>
-      <c r="H248" s="72">
+      <c r="H248" s="71">
         <v>3</v>
       </c>
       <c r="J248" s="1" t="b">
@@ -13411,12 +13462,395 @@
         <v>633</v>
       </c>
     </row>
+    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A249" s="85">
+        <v>249</v>
+      </c>
+      <c r="B249" s="85">
+        <v>1</v>
+      </c>
+      <c r="C249" s="85" t="s">
+        <v>16</v>
+      </c>
+      <c r="D249" s="66">
+        <v>45336</v>
+      </c>
+      <c r="E249" s="4">
+        <v>1083</v>
+      </c>
+      <c r="F249" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="G249" s="87" t="s">
+        <v>641</v>
+      </c>
+      <c r="H249" s="94">
+        <v>1.5</v>
+      </c>
+      <c r="I249" s="87" t="s">
+        <v>642</v>
+      </c>
+      <c r="J249" s="85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K249" s="69">
+        <v>45336.309918981497</v>
+      </c>
+      <c r="L249" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N249" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="O249" s="87" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A250" s="85">
+        <v>250</v>
+      </c>
+      <c r="B250" s="85">
+        <v>1</v>
+      </c>
+      <c r="C250" s="85" t="s">
+        <v>16</v>
+      </c>
+      <c r="D250" s="66">
+        <v>45336</v>
+      </c>
+      <c r="E250" s="4">
+        <v>895</v>
+      </c>
+      <c r="F250" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="G250" s="87" t="s">
+        <v>641</v>
+      </c>
+      <c r="H250" s="94">
+        <v>2.5</v>
+      </c>
+      <c r="I250" s="87" t="s">
+        <v>644</v>
+      </c>
+      <c r="J250" s="85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K250" s="69">
+        <v>45336.310034722199</v>
+      </c>
+      <c r="L250" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N250" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="O250" s="87" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A251" s="85">
+        <v>251</v>
+      </c>
+      <c r="B251" s="85">
+        <v>1</v>
+      </c>
+      <c r="C251" s="85" t="s">
+        <v>16</v>
+      </c>
+      <c r="D251" s="66">
+        <v>45336</v>
+      </c>
+      <c r="E251" s="85">
+        <v>895</v>
+      </c>
+      <c r="F251" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="G251" s="87" t="s">
+        <v>645</v>
+      </c>
+      <c r="H251" s="94">
+        <v>2</v>
+      </c>
+      <c r="J251" s="85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K251" s="69">
+        <v>45336.324351851901</v>
+      </c>
+      <c r="L251" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N251" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="O251" s="87" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A252" s="85">
+        <v>252</v>
+      </c>
+      <c r="B252" s="85">
+        <v>1</v>
+      </c>
+      <c r="C252" s="85" t="s">
+        <v>16</v>
+      </c>
+      <c r="D252" s="66">
+        <v>45336</v>
+      </c>
+      <c r="E252" s="85">
+        <v>344</v>
+      </c>
+      <c r="F252" s="87" t="s">
+        <v>172</v>
+      </c>
+      <c r="G252" s="87" t="s">
+        <v>646</v>
+      </c>
+      <c r="H252" s="94">
+        <v>1</v>
+      </c>
+      <c r="J252" s="85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K252" s="69">
+        <v>45336.3262384259</v>
+      </c>
+      <c r="L252" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N252" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="O252" s="87" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A253" s="85">
+        <v>253</v>
+      </c>
+      <c r="B253" s="85">
+        <v>2</v>
+      </c>
+      <c r="C253" s="85" t="s">
+        <v>247</v>
+      </c>
+      <c r="D253" s="66">
+        <v>45336</v>
+      </c>
+      <c r="E253" s="85">
+        <v>895</v>
+      </c>
+      <c r="F253" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="G253" s="87" t="s">
+        <v>647</v>
+      </c>
+      <c r="H253" s="94">
+        <v>1</v>
+      </c>
+      <c r="J253" s="85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K253" s="69">
+        <v>45336.326446759304</v>
+      </c>
+      <c r="L253" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N253" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="O253" s="87" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A254" s="85">
+        <v>254</v>
+      </c>
+      <c r="B254" s="85">
+        <v>2</v>
+      </c>
+      <c r="C254" s="85" t="s">
+        <v>247</v>
+      </c>
+      <c r="D254" s="66">
+        <v>45336</v>
+      </c>
+      <c r="E254" s="85">
+        <v>344</v>
+      </c>
+      <c r="F254" s="87" t="s">
+        <v>172</v>
+      </c>
+      <c r="G254" s="87" t="s">
+        <v>646</v>
+      </c>
+      <c r="H254" s="94">
+        <v>2</v>
+      </c>
+      <c r="J254" s="85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K254" s="69">
+        <v>45336.326631944401</v>
+      </c>
+      <c r="L254" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N254" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="O254" s="87" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A255" s="85">
+        <v>255</v>
+      </c>
+      <c r="B255" s="85">
+        <v>3</v>
+      </c>
+      <c r="C255" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="D255" s="66">
+        <v>45335</v>
+      </c>
+      <c r="E255" s="85">
+        <v>1083</v>
+      </c>
+      <c r="F255" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="G255" s="87" t="s">
+        <v>646</v>
+      </c>
+      <c r="H255" s="94">
+        <v>2</v>
+      </c>
+      <c r="J255" s="85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K255" s="69">
+        <v>45336.326932870397</v>
+      </c>
+      <c r="L255" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N255" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="O255" s="87" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A256" s="85">
+        <v>256</v>
+      </c>
+      <c r="B256" s="85">
+        <v>4</v>
+      </c>
+      <c r="C256" s="85" t="s">
+        <v>21</v>
+      </c>
+      <c r="D256" s="66">
+        <v>45335</v>
+      </c>
+      <c r="E256" s="85">
+        <v>921</v>
+      </c>
+      <c r="F256" s="87" t="s">
+        <v>192</v>
+      </c>
+      <c r="G256" s="87" t="s">
+        <v>648</v>
+      </c>
+      <c r="H256" s="94">
+        <v>5</v>
+      </c>
+      <c r="J256" s="85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K256" s="69">
+        <v>45336.3274074074</v>
+      </c>
+      <c r="L256" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N256" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="O256" s="87" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="257" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A257" s="85">
+        <v>257</v>
+      </c>
+      <c r="B257" s="85">
+        <v>1</v>
+      </c>
+      <c r="C257" s="85" t="s">
+        <v>16</v>
+      </c>
+      <c r="D257" s="66">
+        <v>45336</v>
+      </c>
+      <c r="E257" s="85">
+        <v>1109</v>
+      </c>
+      <c r="F257" s="87" t="s">
+        <v>649</v>
+      </c>
+      <c r="G257" s="87" t="s">
+        <v>64</v>
+      </c>
+      <c r="H257" s="94">
+        <v>1</v>
+      </c>
+      <c r="J257" s="85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K257" s="69">
+        <v>45336.327800925901</v>
+      </c>
+      <c r="L257" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N257" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="O257" s="87" t="s">
+        <v>643</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:P248">
-    <cfRule type="expression" dxfId="5" priority="1">
+  <conditionalFormatting sqref="K249:K257">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
     <cfRule type="expression" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:P100002">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+    <cfRule type="expression" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14204,7 +14638,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:T12">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
     <cfRule type="expression" priority="2">
@@ -14222,7 +14656,7 @@
   </sheetPr>
   <dimension ref="A1:J369"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
@@ -14258,10 +14692,10 @@
       <c r="F1" s="43" t="s">
         <v>392</v>
       </c>
-      <c r="G1" s="90" t="s">
+      <c r="G1" s="89" t="s">
         <v>393</v>
       </c>
-      <c r="H1" s="90" t="s">
+      <c r="H1" s="89" t="s">
         <v>394</v>
       </c>
       <c r="I1" s="30" t="s">
@@ -21010,10 +21444,10 @@
       <c r="F238" s="14" t="s">
         <v>401</v>
       </c>
-      <c r="G238" s="91">
+      <c r="G238" s="90">
         <v>696.75</v>
       </c>
-      <c r="H238" s="91"/>
+      <c r="H238" s="90"/>
       <c r="I238" s="14"/>
       <c r="J238" s="42">
         <f>ROW()</f>
@@ -21039,8 +21473,8 @@
       <c r="F239" s="14" t="s">
         <v>488</v>
       </c>
-      <c r="G239" s="91"/>
-      <c r="H239" s="91">
+      <c r="G239" s="90"/>
+      <c r="H239" s="90">
         <v>600</v>
       </c>
       <c r="I239" s="14"/>
@@ -21068,8 +21502,8 @@
       <c r="F240" s="14" t="s">
         <v>504</v>
       </c>
-      <c r="G240" s="91"/>
-      <c r="H240" s="91">
+      <c r="G240" s="90"/>
+      <c r="H240" s="90">
         <v>1</v>
       </c>
       <c r="I240" s="14"/>
@@ -21097,8 +21531,8 @@
       <c r="F241" s="14" t="s">
         <v>501</v>
       </c>
-      <c r="G241" s="91"/>
-      <c r="H241" s="91">
+      <c r="G241" s="90"/>
+      <c r="H241" s="90">
         <v>2</v>
       </c>
       <c r="I241" s="14"/>
@@ -21126,8 +21560,8 @@
       <c r="F242" s="14" t="s">
         <v>494</v>
       </c>
-      <c r="G242" s="91"/>
-      <c r="H242" s="91">
+      <c r="G242" s="90"/>
+      <c r="H242" s="90">
         <v>3</v>
       </c>
       <c r="I242" s="14"/>
@@ -21155,8 +21589,8 @@
       <c r="F243" s="14" t="s">
         <v>486</v>
       </c>
-      <c r="G243" s="91"/>
-      <c r="H243" s="91">
+      <c r="G243" s="90"/>
+      <c r="H243" s="90">
         <v>30.3</v>
       </c>
       <c r="I243" s="14"/>
@@ -21184,8 +21618,8 @@
       <c r="F244" s="14" t="s">
         <v>487</v>
       </c>
-      <c r="G244" s="91"/>
-      <c r="H244" s="91">
+      <c r="G244" s="90"/>
+      <c r="H244" s="90">
         <v>60.45</v>
       </c>
       <c r="I244" s="14"/>
@@ -23237,7 +23671,7 @@
       <c r="F316" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="G316" s="92">
+      <c r="G316" s="91">
         <v>0.25</v>
       </c>
       <c r="J316" s="42">
@@ -23264,7 +23698,7 @@
       <c r="F317" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="H317" s="92">
+      <c r="H317" s="91">
         <v>0.25</v>
       </c>
       <c r="J317" s="42">
@@ -24089,16 +24523,16 @@
       <c r="B348" s="37">
         <v>45330</v>
       </c>
-      <c r="C348" s="85" t="s">
+      <c r="C348" s="84" t="s">
         <v>627</v>
       </c>
-      <c r="D348" s="85" t="s">
+      <c r="D348" s="84" t="s">
         <v>307</v>
       </c>
-      <c r="E348" s="86" t="s">
+      <c r="E348" s="85" t="s">
         <v>467</v>
       </c>
-      <c r="F348" s="85" t="s">
+      <c r="F348" s="84" t="s">
         <v>468</v>
       </c>
       <c r="G348" s="25">
@@ -24116,16 +24550,16 @@
       <c r="B349" s="57">
         <v>45330</v>
       </c>
-      <c r="C349" s="87" t="s">
+      <c r="C349" s="86" t="s">
         <v>627</v>
       </c>
-      <c r="D349" s="87" t="s">
+      <c r="D349" s="86" t="s">
         <v>307</v>
       </c>
-      <c r="E349" s="86" t="s">
+      <c r="E349" s="85" t="s">
         <v>400</v>
       </c>
-      <c r="F349" s="85" t="s">
+      <c r="F349" s="84" t="s">
         <v>398</v>
       </c>
       <c r="H349" s="25">
@@ -24143,13 +24577,13 @@
       <c r="B350" s="37">
         <v>45331</v>
       </c>
-      <c r="C350" s="88" t="s">
+      <c r="C350" s="87" t="s">
         <v>517</v>
       </c>
-      <c r="E350" s="86" t="s">
+      <c r="E350" s="85" t="s">
         <v>445</v>
       </c>
-      <c r="F350" s="88" t="s">
+      <c r="F350" s="87" t="s">
         <v>401</v>
       </c>
       <c r="G350" s="25">
@@ -24167,14 +24601,14 @@
       <c r="B351" s="44">
         <v>45331</v>
       </c>
-      <c r="C351" s="89" t="s">
+      <c r="C351" s="88" t="s">
         <v>517</v>
       </c>
       <c r="D351" s="38"/>
-      <c r="E351" s="86" t="s">
+      <c r="E351" s="85" t="s">
         <v>421</v>
       </c>
-      <c r="F351" s="88" t="s">
+      <c r="F351" s="87" t="s">
         <v>422</v>
       </c>
       <c r="H351" s="25">
@@ -24192,14 +24626,14 @@
       <c r="B352" s="44">
         <v>45331</v>
       </c>
-      <c r="C352" s="89" t="s">
+      <c r="C352" s="88" t="s">
         <v>517</v>
       </c>
       <c r="D352" s="38"/>
-      <c r="E352" s="86" t="s">
+      <c r="E352" s="85" t="s">
         <v>408</v>
       </c>
-      <c r="F352" s="88" t="s">
+      <c r="F352" s="87" t="s">
         <v>409</v>
       </c>
       <c r="H352" s="25">
@@ -24217,14 +24651,14 @@
       <c r="B353" s="44">
         <v>45331</v>
       </c>
-      <c r="C353" s="89" t="s">
+      <c r="C353" s="88" t="s">
         <v>517</v>
       </c>
       <c r="D353" s="38"/>
-      <c r="E353" s="86" t="s">
+      <c r="E353" s="85" t="s">
         <v>416</v>
       </c>
-      <c r="F353" s="88" t="s">
+      <c r="F353" s="87" t="s">
         <v>417</v>
       </c>
       <c r="H353" s="25">
@@ -24242,14 +24676,14 @@
       <c r="B354" s="44">
         <v>45331</v>
       </c>
-      <c r="C354" s="89" t="s">
+      <c r="C354" s="88" t="s">
         <v>517</v>
       </c>
       <c r="D354" s="38"/>
-      <c r="E354" s="86" t="s">
+      <c r="E354" s="85" t="s">
         <v>430</v>
       </c>
-      <c r="F354" s="88" t="s">
+      <c r="F354" s="87" t="s">
         <v>431</v>
       </c>
       <c r="G354" s="25">
@@ -24267,16 +24701,16 @@
       <c r="B355" s="37">
         <v>45331</v>
       </c>
-      <c r="C355" s="88" t="s">
+      <c r="C355" s="87" t="s">
         <v>628</v>
       </c>
-      <c r="D355" s="88" t="s">
+      <c r="D355" s="87" t="s">
         <v>307</v>
       </c>
-      <c r="E355" s="86" t="s">
+      <c r="E355" s="85" t="s">
         <v>400</v>
       </c>
-      <c r="F355" s="88" t="s">
+      <c r="F355" s="87" t="s">
         <v>398</v>
       </c>
       <c r="G355" s="25">
@@ -24294,16 +24728,16 @@
       <c r="B356" s="31">
         <v>45331</v>
       </c>
-      <c r="C356" s="89" t="s">
+      <c r="C356" s="88" t="s">
         <v>628</v>
       </c>
-      <c r="D356" s="89" t="s">
+      <c r="D356" s="88" t="s">
         <v>307</v>
       </c>
-      <c r="E356" s="86" t="s">
+      <c r="E356" s="85" t="s">
         <v>467</v>
       </c>
-      <c r="F356" s="88" t="s">
+      <c r="F356" s="87" t="s">
         <v>468</v>
       </c>
       <c r="H356" s="25">
@@ -24429,22 +24863,22 @@
       <c r="B361" s="22">
         <v>45331</v>
       </c>
-      <c r="C361" s="88" t="s">
+      <c r="C361" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="D361" s="88" t="s">
+      <c r="D361" s="87" t="s">
         <v>631</v>
       </c>
-      <c r="E361" s="86" t="s">
+      <c r="E361" s="85" t="s">
         <v>400</v>
       </c>
-      <c r="F361" s="88" t="s">
+      <c r="F361" s="87" t="s">
         <v>398</v>
       </c>
       <c r="G361" s="25">
         <v>25</v>
       </c>
-      <c r="I361" s="88" t="s">
+      <c r="I361" s="87" t="s">
         <v>632</v>
       </c>
       <c r="J361" s="42">
@@ -24459,22 +24893,22 @@
       <c r="B362" s="31">
         <v>45331</v>
       </c>
-      <c r="C362" s="89" t="s">
+      <c r="C362" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="D362" s="89" t="s">
+      <c r="D362" s="88" t="s">
         <v>631</v>
       </c>
-      <c r="E362" s="86" t="s">
+      <c r="E362" s="85" t="s">
         <v>445</v>
       </c>
-      <c r="F362" s="88" t="s">
+      <c r="F362" s="87" t="s">
         <v>569</v>
       </c>
       <c r="H362" s="25">
         <v>25</v>
       </c>
-      <c r="I362" s="88" t="s">
+      <c r="I362" s="87" t="s">
         <v>632</v>
       </c>
       <c r="J362" s="42">
@@ -24489,13 +24923,13 @@
       <c r="B363" s="22">
         <v>45331</v>
       </c>
-      <c r="C363" s="88" t="s">
+      <c r="C363" s="87" t="s">
         <v>634</v>
       </c>
-      <c r="E363" s="86" t="s">
+      <c r="E363" s="85" t="s">
         <v>467</v>
       </c>
-      <c r="F363" s="88" t="s">
+      <c r="F363" s="87" t="s">
         <v>468</v>
       </c>
       <c r="G363" s="25">
@@ -24513,14 +24947,14 @@
       <c r="B364" s="31">
         <v>45331</v>
       </c>
-      <c r="C364" s="89" t="s">
+      <c r="C364" s="88" t="s">
         <v>634</v>
       </c>
       <c r="D364" s="38"/>
-      <c r="E364" s="86" t="s">
+      <c r="E364" s="85" t="s">
         <v>400</v>
       </c>
-      <c r="F364" s="88" t="s">
+      <c r="F364" s="87" t="s">
         <v>398</v>
       </c>
       <c r="H364" s="25">
@@ -24538,16 +24972,16 @@
       <c r="B365" s="22">
         <v>45331</v>
       </c>
-      <c r="C365" s="88" t="s">
+      <c r="C365" s="87" t="s">
         <v>636</v>
       </c>
-      <c r="D365" s="88" t="s">
+      <c r="D365" s="87" t="s">
         <v>635</v>
       </c>
-      <c r="E365" s="86" t="s">
+      <c r="E365" s="85" t="s">
         <v>637</v>
       </c>
-      <c r="F365" s="88" t="s">
+      <c r="F365" s="87" t="s">
         <v>638</v>
       </c>
       <c r="G365" s="25">
@@ -24565,16 +24999,16 @@
       <c r="B366" s="31">
         <v>45331</v>
       </c>
-      <c r="C366" s="89" t="s">
+      <c r="C366" s="88" t="s">
         <v>636</v>
       </c>
-      <c r="D366" s="89" t="s">
+      <c r="D366" s="88" t="s">
         <v>635</v>
       </c>
-      <c r="E366" s="86" t="s">
+      <c r="E366" s="85" t="s">
         <v>430</v>
       </c>
-      <c r="F366" s="88" t="s">
+      <c r="F366" s="87" t="s">
         <v>431</v>
       </c>
       <c r="H366" s="25">
@@ -24592,22 +25026,22 @@
       <c r="B367" s="22">
         <v>45331</v>
       </c>
-      <c r="C367" s="88" t="s">
+      <c r="C367" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="D367" s="88" t="s">
+      <c r="D367" s="87" t="s">
         <v>639</v>
       </c>
-      <c r="E367" s="86" t="s">
+      <c r="E367" s="85" t="s">
         <v>400</v>
       </c>
-      <c r="F367" s="88" t="s">
+      <c r="F367" s="87" t="s">
         <v>398</v>
       </c>
       <c r="G367" s="25">
         <v>100</v>
       </c>
-      <c r="I367" s="88" t="s">
+      <c r="I367" s="87" t="s">
         <v>640</v>
       </c>
       <c r="J367" s="42">
@@ -24622,22 +25056,22 @@
       <c r="B368" s="31">
         <v>45331</v>
       </c>
-      <c r="C368" s="89" t="s">
+      <c r="C368" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="D368" s="89" t="s">
+      <c r="D368" s="88" t="s">
         <v>639</v>
       </c>
-      <c r="E368" s="86" t="s">
+      <c r="E368" s="85" t="s">
         <v>445</v>
       </c>
-      <c r="F368" s="88" t="s">
+      <c r="F368" s="87" t="s">
         <v>569</v>
       </c>
       <c r="H368" s="25">
         <v>100</v>
       </c>
-      <c r="I368" s="88" t="s">
+      <c r="I368" s="87" t="s">
         <v>640</v>
       </c>
       <c r="J368" s="42">
@@ -24646,8 +25080,8 @@
       </c>
     </row>
     <row r="369" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G369" s="93"/>
-      <c r="H369" s="93"/>
+      <c r="G369" s="92"/>
+      <c r="H369" s="92"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J369" xr:uid="{E0D58006-DE1D-488F-9BB7-8096C5818030}"/>
@@ -24671,7 +25105,7 @@
     <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.7109375" style="73" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="72" customWidth="1"/>
     <col min="7" max="7" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" customWidth="1"/>
   </cols>
@@ -24689,10 +25123,10 @@
       <c r="D1" s="43" t="s">
         <v>392</v>
       </c>
-      <c r="E1" s="82" t="s">
+      <c r="E1" s="81" t="s">
         <v>393</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="81" t="s">
         <v>394</v>
       </c>
       <c r="G1" s="30" t="s">
@@ -24715,10 +25149,10 @@
       <c r="D2" s="47" t="s">
         <v>468</v>
       </c>
-      <c r="E2" s="83">
+      <c r="E2" s="82">
         <v>29.95</v>
       </c>
-      <c r="F2" s="83"/>
+      <c r="F2" s="82"/>
       <c r="G2" s="48"/>
       <c r="H2" s="42">
         <f>ROW()</f>
@@ -24738,8 +25172,8 @@
       <c r="D3" s="51" t="s">
         <v>398</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84">
+      <c r="E3" s="83"/>
+      <c r="F3" s="83">
         <v>29.95</v>
       </c>
       <c r="G3" s="52"/>
@@ -24773,10 +25207,10 @@
       <c r="D5" s="47" t="s">
         <v>401</v>
       </c>
-      <c r="E5" s="83">
+      <c r="E5" s="82">
         <v>262.44</v>
       </c>
-      <c r="F5" s="83"/>
+      <c r="F5" s="82"/>
       <c r="G5" s="48"/>
       <c r="H5" s="42">
         <f>ROW()</f>
@@ -24796,7 +25230,7 @@
       <c r="D6" s="14" t="s">
         <v>422</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="72">
         <v>250</v>
       </c>
       <c r="G6" s="54"/>
@@ -24818,7 +25252,7 @@
       <c r="D7" s="14" t="s">
         <v>409</v>
       </c>
-      <c r="F7" s="73">
+      <c r="F7" s="72">
         <v>12.5</v>
       </c>
       <c r="G7" s="54"/>
@@ -24840,7 +25274,7 @@
       <c r="D8" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="F8" s="73">
+      <c r="F8" s="72">
         <v>24.94</v>
       </c>
       <c r="G8" s="54"/>
@@ -24862,10 +25296,10 @@
       <c r="D9" s="51" t="s">
         <v>431</v>
       </c>
-      <c r="E9" s="84">
+      <c r="E9" s="83">
         <v>25</v>
       </c>
-      <c r="F9" s="84"/>
+      <c r="F9" s="83"/>
       <c r="G9" s="52"/>
       <c r="H9" s="42">
         <f>ROW()</f>
@@ -24897,10 +25331,10 @@
       <c r="D11" s="47" t="s">
         <v>497</v>
       </c>
-      <c r="E11" s="83">
+      <c r="E11" s="82">
         <v>2400</v>
       </c>
-      <c r="F11" s="83"/>
+      <c r="F11" s="82"/>
       <c r="G11" s="48"/>
       <c r="H11" s="42">
         <f>ROW()</f>
@@ -24920,7 +25354,7 @@
       <c r="D12" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="E12" s="73">
+      <c r="E12" s="72">
         <v>120</v>
       </c>
       <c r="G12" s="54"/>
@@ -24942,7 +25376,7 @@
       <c r="D13" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="E13" s="73">
+      <c r="E13" s="72">
         <v>239.4</v>
       </c>
       <c r="G13" s="54"/>
@@ -24964,8 +25398,8 @@
       <c r="D14" s="51" t="s">
         <v>398</v>
       </c>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84">
+      <c r="E14" s="83"/>
+      <c r="F14" s="83">
         <v>2759.4</v>
       </c>
       <c r="G14" s="52"/>
@@ -24999,10 +25433,10 @@
       <c r="D16" s="47" t="s">
         <v>510</v>
       </c>
-      <c r="E16" s="83">
+      <c r="E16" s="82">
         <v>650</v>
       </c>
-      <c r="F16" s="83"/>
+      <c r="F16" s="82"/>
       <c r="G16" s="48"/>
       <c r="H16" s="42">
         <f>ROW()</f>
@@ -25022,7 +25456,7 @@
       <c r="D17" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="E17" s="73">
+      <c r="E17" s="72">
         <v>32.5</v>
       </c>
       <c r="G17" s="54"/>
@@ -25044,7 +25478,7 @@
       <c r="D18" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="E18" s="73">
+      <c r="E18" s="72">
         <v>64.84</v>
       </c>
       <c r="G18" s="54"/>
@@ -25066,8 +25500,8 @@
       <c r="D19" s="51" t="s">
         <v>398</v>
       </c>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84">
+      <c r="E19" s="83"/>
+      <c r="F19" s="83">
         <v>747.34</v>
       </c>
       <c r="G19" s="52"/>
@@ -25101,10 +25535,10 @@
       <c r="D21" s="47" t="s">
         <v>513</v>
       </c>
-      <c r="E21" s="83">
+      <c r="E21" s="82">
         <v>129.94999999999999</v>
       </c>
-      <c r="F21" s="83"/>
+      <c r="F21" s="82"/>
       <c r="G21" s="48"/>
       <c r="H21" s="42">
         <f>ROW()</f>
@@ -25124,7 +25558,7 @@
       <c r="D22" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="E22" s="73">
+      <c r="E22" s="72">
         <v>6.5</v>
       </c>
       <c r="G22" s="54"/>
@@ -25146,7 +25580,7 @@
       <c r="D23" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="E23" s="73">
+      <c r="E23" s="72">
         <v>12.96</v>
       </c>
       <c r="G23" s="54"/>
@@ -25168,8 +25602,8 @@
       <c r="D24" s="51" t="s">
         <v>462</v>
       </c>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84">
+      <c r="E24" s="83"/>
+      <c r="F24" s="83">
         <v>149.41</v>
       </c>
       <c r="G24" s="52" t="s">
@@ -25205,10 +25639,10 @@
       <c r="D26" s="47" t="s">
         <v>468</v>
       </c>
-      <c r="E26" s="83">
+      <c r="E26" s="82">
         <v>29.95</v>
       </c>
-      <c r="F26" s="83"/>
+      <c r="F26" s="82"/>
       <c r="G26" s="48"/>
       <c r="H26" s="42">
         <f>ROW()</f>
@@ -25228,8 +25662,8 @@
       <c r="D27" s="51" t="s">
         <v>398</v>
       </c>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84">
+      <c r="E27" s="83"/>
+      <c r="F27" s="83">
         <v>29.95</v>
       </c>
       <c r="G27" s="52"/>
@@ -25263,10 +25697,10 @@
       <c r="D29" s="59" t="s">
         <v>468</v>
       </c>
-      <c r="E29" s="83">
+      <c r="E29" s="82">
         <v>29.95</v>
       </c>
-      <c r="F29" s="83"/>
+      <c r="F29" s="82"/>
       <c r="G29" s="48"/>
       <c r="H29" s="42">
         <f>ROW()</f>
@@ -25286,8 +25720,8 @@
       <c r="D30" s="61" t="s">
         <v>398</v>
       </c>
-      <c r="E30" s="84"/>
-      <c r="F30" s="84">
+      <c r="E30" s="83"/>
+      <c r="F30" s="83">
         <v>29.95</v>
       </c>
       <c r="G30" s="52"/>
@@ -25321,39 +25755,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11.42578125" style="73"/>
-    <col min="10" max="10" width="11.42578125" style="73"/>
+    <col min="8" max="8" width="11.42578125" style="72"/>
+    <col min="10" max="10" width="11.42578125" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="73" t="s">
         <v>592</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="73" t="s">
         <v>593</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="73" t="s">
         <v>594</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="73" t="s">
         <v>595</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="73" t="s">
         <v>596</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="73" t="s">
         <v>597</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="73" t="s">
         <v>598</v>
       </c>
-      <c r="H1" s="80" t="s">
+      <c r="H1" s="79" t="s">
         <v>599</v>
       </c>
-      <c r="I1" s="75" t="s">
+      <c r="I1" s="74" t="s">
         <v>600</v>
       </c>
-      <c r="J1" s="81" t="s">
+      <c r="J1" s="80" t="s">
         <v>601</v>
       </c>
     </row>
@@ -25379,13 +25813,13 @@
       <c r="G2" t="s">
         <v>604</v>
       </c>
-      <c r="H2" s="73">
+      <c r="H2" s="72">
         <v>9128.4500000000007</v>
       </c>
       <c r="I2" s="1">
         <v>6</v>
       </c>
-      <c r="J2" s="76" cm="1">
+      <c r="J2" s="75" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">H2-IFERROR(SUMIF(PayItem_InvID,A2,PayItem_Amount),0)</f>
         <v>3646.6600000000008</v>
       </c>
@@ -25409,13 +25843,13 @@
       <c r="F3" s="23">
         <v>44729</v>
       </c>
-      <c r="H3" s="73">
+      <c r="H3" s="72">
         <v>1653.73</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="76" cm="1">
+      <c r="J3" s="75" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">H3-IFERROR(SUMIF(PayItem_InvID,A3,PayItem_Amount),0)</f>
         <v>1653.73</v>
       </c>
@@ -25439,13 +25873,13 @@
       <c r="F4" s="23">
         <v>44729</v>
       </c>
-      <c r="H4" s="73">
+      <c r="H4" s="72">
         <v>474.39</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
       </c>
-      <c r="J4" s="76" cm="1">
+      <c r="J4" s="75" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">H4-IFERROR(SUMIF(PayItem_InvID,A4,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
@@ -25463,19 +25897,19 @@
       <c r="D5" t="s">
         <v>607</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="76" t="s">
         <v>608</v>
       </c>
       <c r="F5" s="23">
         <v>44714</v>
       </c>
-      <c r="H5" s="73">
+      <c r="H5" s="72">
         <v>346.46</v>
       </c>
       <c r="I5" s="1">
         <v>1</v>
       </c>
-      <c r="J5" s="76" cm="1">
+      <c r="J5" s="75" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">H5-IFERROR(SUMIF(PayItem_InvID,A5,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
@@ -25493,22 +25927,22 @@
       <c r="D6" t="s">
         <v>602</v>
       </c>
-      <c r="E6" s="77" t="s">
+      <c r="E6" s="76" t="s">
         <v>606</v>
       </c>
       <c r="F6" s="23">
         <v>44953</v>
       </c>
-      <c r="G6" s="77" t="s">
+      <c r="G6" s="76" t="s">
         <v>609</v>
       </c>
-      <c r="H6" s="73">
+      <c r="H6" s="72">
         <v>3251.61</v>
       </c>
       <c r="I6" s="1">
         <v>2</v>
       </c>
-      <c r="J6" s="76" cm="1">
+      <c r="J6" s="75" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">H6-IFERROR(SUMIF(PayItem_InvID,A6,PayItem_Amount),0)</f>
         <v>3251.61</v>
       </c>
@@ -25533,14 +25967,14 @@
         <f t="shared" ref="F7:F16" si="0">B7+15</f>
         <v>44960</v>
       </c>
-      <c r="G7" s="77"/>
-      <c r="H7" s="73">
+      <c r="G7" s="76"/>
+      <c r="H7" s="72">
         <v>974.39</v>
       </c>
       <c r="I7" s="1">
         <v>1</v>
       </c>
-      <c r="J7" s="76" cm="1">
+      <c r="J7" s="75" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">H7-IFERROR(SUMIF(PayItem_InvID,A7,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
@@ -25565,13 +25999,13 @@
         <f t="shared" si="0"/>
         <v>44961</v>
       </c>
-      <c r="H8" s="73">
+      <c r="H8" s="72">
         <v>623.69000000000005</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>
       </c>
-      <c r="J8" s="76" cm="1">
+      <c r="J8" s="75" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">H8-IFERROR(SUMIF(PayItem_InvID,A8,PayItem_Amount),0)</f>
         <v>500.00000000000006</v>
       </c>
@@ -25596,13 +26030,13 @@
         <f t="shared" si="0"/>
         <v>44962</v>
       </c>
-      <c r="H9" s="73">
+      <c r="H9" s="72">
         <v>34.630000000000003</v>
       </c>
       <c r="I9" s="1">
         <v>1</v>
       </c>
-      <c r="J9" s="76" cm="1">
+      <c r="J9" s="75" cm="1">
         <f t="array" aca="1" ref="J9" ca="1">H9-IFERROR(SUMIF(PayItem_InvID,A9,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
@@ -25630,13 +26064,13 @@
       <c r="G10" t="s">
         <v>609</v>
       </c>
-      <c r="H10" s="73">
+      <c r="H10" s="72">
         <v>26.25</v>
       </c>
       <c r="I10" s="1">
         <v>1</v>
       </c>
-      <c r="J10" s="76" cm="1">
+      <c r="J10" s="75" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">H10-IFERROR(SUMIF(PayItem_InvID,A10,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
@@ -25661,13 +26095,13 @@
         <f t="shared" si="0"/>
         <v>44964</v>
       </c>
-      <c r="H11" s="73">
+      <c r="H11" s="72">
         <v>262.5</v>
       </c>
       <c r="I11" s="1">
         <v>1</v>
       </c>
-      <c r="J11" s="76" cm="1">
+      <c r="J11" s="75" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">H11-IFERROR(SUMIF(PayItem_InvID,A11,PayItem_Amount),0)</f>
         <v>162.5</v>
       </c>
@@ -25692,13 +26126,13 @@
         <f t="shared" si="0"/>
         <v>44965</v>
       </c>
-      <c r="H12" s="73">
+      <c r="H12" s="72">
         <v>445.2</v>
       </c>
       <c r="I12" s="1">
         <v>1</v>
       </c>
-      <c r="J12" s="76" cm="1">
+      <c r="J12" s="75" cm="1">
         <f t="array" aca="1" ref="J12" ca="1">H12-IFERROR(SUMIF(PayItem_InvID,A12,PayItem_Amount),0)</f>
         <v>445.2</v>
       </c>
@@ -25724,13 +26158,13 @@
         <f t="shared" si="0"/>
         <v>44968</v>
       </c>
-      <c r="H13" s="73">
+      <c r="H13" s="72">
         <v>26.25</v>
       </c>
       <c r="I13" s="1">
         <v>1</v>
       </c>
-      <c r="J13" s="76">
+      <c r="J13" s="75">
         <f t="shared" ref="J13:J31" ca="1" si="1">H13-IFERROR(SUMIF(PayItem_InvID,A13,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
@@ -25756,13 +26190,13 @@
         <f t="shared" si="0"/>
         <v>44971</v>
       </c>
-      <c r="H14" s="73">
+      <c r="H14" s="72">
         <v>500</v>
       </c>
       <c r="I14" s="1">
         <v>1</v>
       </c>
-      <c r="J14" s="76">
+      <c r="J14" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>500</v>
       </c>
@@ -25788,13 +26222,13 @@
         <f t="shared" si="0"/>
         <v>44974</v>
       </c>
-      <c r="H15" s="73">
+      <c r="H15" s="72">
         <v>600</v>
       </c>
       <c r="I15" s="1">
         <v>1</v>
       </c>
-      <c r="J15" s="76">
+      <c r="J15" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
@@ -25820,13 +26254,13 @@
         <f t="shared" si="0"/>
         <v>44982</v>
       </c>
-      <c r="H16" s="73">
+      <c r="H16" s="72">
         <v>700</v>
       </c>
       <c r="I16" s="1">
         <v>1</v>
       </c>
-      <c r="J16" s="76">
+      <c r="J16" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
@@ -25852,13 +26286,13 @@
         <f>B17+30</f>
         <v>45005</v>
       </c>
-      <c r="H17" s="73">
+      <c r="H17" s="72">
         <v>725</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
       </c>
-      <c r="J17" s="76">
+      <c r="J17" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
@@ -25884,13 +26318,13 @@
         <f t="shared" ref="F18:F23" si="3">B18+15</f>
         <v>44998</v>
       </c>
-      <c r="H18" s="73">
+      <c r="H18" s="72">
         <v>750</v>
       </c>
       <c r="I18" s="1">
         <v>1</v>
       </c>
-      <c r="J18" s="76">
+      <c r="J18" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
@@ -25916,13 +26350,13 @@
         <f t="shared" si="3"/>
         <v>45006</v>
       </c>
-      <c r="H19" s="73">
+      <c r="H19" s="72">
         <v>775</v>
       </c>
       <c r="I19" s="1">
         <v>1</v>
       </c>
-      <c r="J19" s="76">
+      <c r="J19" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
@@ -25948,13 +26382,13 @@
         <f t="shared" si="3"/>
         <v>45014</v>
       </c>
-      <c r="H20" s="73">
+      <c r="H20" s="72">
         <v>800</v>
       </c>
       <c r="I20" s="1">
         <v>1</v>
       </c>
-      <c r="J20" s="76">
+      <c r="J20" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>520</v>
       </c>
@@ -25980,13 +26414,13 @@
         <f t="shared" si="3"/>
         <v>45022</v>
       </c>
-      <c r="H21" s="73">
+      <c r="H21" s="72">
         <v>774</v>
       </c>
       <c r="I21" s="1">
         <v>1</v>
       </c>
-      <c r="J21" s="76">
+      <c r="J21" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>376.01</v>
       </c>
@@ -26012,13 +26446,13 @@
         <f t="shared" si="3"/>
         <v>45030</v>
       </c>
-      <c r="H22" s="73">
+      <c r="H22" s="72">
         <v>749</v>
       </c>
       <c r="I22" s="1">
         <v>1</v>
       </c>
-      <c r="J22" s="76">
+      <c r="J22" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>749</v>
       </c>
@@ -26044,13 +26478,13 @@
         <f t="shared" si="3"/>
         <v>45038</v>
       </c>
-      <c r="H23" s="73">
+      <c r="H23" s="72">
         <v>724</v>
       </c>
       <c r="I23" s="1">
         <v>1</v>
       </c>
-      <c r="J23" s="76">
+      <c r="J23" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>724</v>
       </c>
@@ -26076,13 +26510,13 @@
         <f>B24+45</f>
         <v>45083</v>
       </c>
-      <c r="H24" s="73">
+      <c r="H24" s="72">
         <v>699.99</v>
       </c>
       <c r="I24" s="1">
         <v>1</v>
       </c>
-      <c r="J24" s="76">
+      <c r="J24" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>626.66</v>
       </c>
@@ -26108,13 +26542,13 @@
         <f t="shared" ref="F25:F31" si="4">B25+15</f>
         <v>45068</v>
       </c>
-      <c r="H25" s="73">
+      <c r="H25" s="72">
         <v>599.99</v>
       </c>
       <c r="I25" s="1">
         <v>1</v>
       </c>
-      <c r="J25" s="76">
+      <c r="J25" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>599.99</v>
       </c>
@@ -26140,13 +26574,13 @@
         <f t="shared" si="4"/>
         <v>45083</v>
       </c>
-      <c r="H26" s="73">
+      <c r="H26" s="72">
         <v>499.99</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
       </c>
-      <c r="J26" s="76">
+      <c r="J26" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>499.99</v>
       </c>
@@ -26172,13 +26606,13 @@
         <f t="shared" si="4"/>
         <v>45098</v>
       </c>
-      <c r="H27" s="73">
+      <c r="H27" s="72">
         <v>399.99</v>
       </c>
       <c r="I27" s="1">
         <v>1</v>
       </c>
-      <c r="J27" s="76">
+      <c r="J27" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>399.99</v>
       </c>
@@ -26204,13 +26638,13 @@
         <f t="shared" si="4"/>
         <v>45113</v>
       </c>
-      <c r="H28" s="73">
+      <c r="H28" s="72">
         <v>299.99</v>
       </c>
       <c r="I28" s="1">
         <v>1</v>
       </c>
-      <c r="J28" s="76">
+      <c r="J28" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
@@ -26235,13 +26669,13 @@
         <f t="shared" si="4"/>
         <v>45214</v>
       </c>
-      <c r="H29" s="73">
+      <c r="H29" s="72">
         <v>8999.99</v>
       </c>
       <c r="I29" s="1">
         <v>1</v>
       </c>
-      <c r="J29" s="76">
+      <c r="J29" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>8700</v>
       </c>
@@ -26267,13 +26701,13 @@
         <f t="shared" si="4"/>
         <v>45245</v>
       </c>
-      <c r="H30" s="73">
+      <c r="H30" s="72">
         <v>7888.88</v>
       </c>
       <c r="I30" s="1">
         <v>1</v>
       </c>
-      <c r="J30" s="76">
+      <c r="J30" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>7888.88</v>
       </c>
@@ -26298,35 +26732,35 @@
         <f t="shared" si="4"/>
         <v>45307</v>
       </c>
-      <c r="H31" s="73">
+      <c r="H31" s="72">
         <v>6777.77</v>
       </c>
       <c r="I31" s="1">
         <v>1</v>
       </c>
-      <c r="J31" s="76">
+      <c r="J31" s="75">
         <f t="shared" ca="1" si="1"/>
         <v>6777.77</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C17:C21">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>AND($A17&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>AND($A23&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C28">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND($A27&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C31">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND($A30&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26349,27 +26783,27 @@
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="73" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="72" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="77" t="s">
         <v>613</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="77" t="s">
         <v>614</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="77" t="s">
         <v>594</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="77" t="s">
         <v>615</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="78" t="s">
         <v>616</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="77" t="s">
         <v>263</v>
       </c>
     </row>
@@ -26386,7 +26820,7 @@
       <c r="D2" t="s">
         <v>619</v>
       </c>
-      <c r="E2" s="76">
+      <c r="E2" s="75">
         <v>5066.22</v>
       </c>
       <c r="F2" t="s">
@@ -26406,7 +26840,7 @@
       <c r="D3" t="s">
         <v>619</v>
       </c>
-      <c r="E3" s="76">
+      <c r="E3" s="75">
         <v>5474.39</v>
       </c>
     </row>
@@ -26423,7 +26857,7 @@
       <c r="D4" t="s">
         <v>621</v>
       </c>
-      <c r="E4" s="76">
+      <c r="E4" s="75">
         <v>346.46</v>
       </c>
     </row>
@@ -26437,7 +26871,7 @@
       <c r="C5" t="s">
         <v>575</v>
       </c>
-      <c r="E5" s="73">
+      <c r="E5" s="72">
         <v>250</v>
       </c>
     </row>
@@ -26451,7 +26885,7 @@
       <c r="C6" t="s">
         <v>576</v>
       </c>
-      <c r="E6" s="73">
+      <c r="E6" s="72">
         <v>750</v>
       </c>
     </row>
@@ -26468,7 +26902,7 @@
       <c r="D7" t="s">
         <v>622</v>
       </c>
-      <c r="E7" s="73">
+      <c r="E7" s="72">
         <v>348.08</v>
       </c>
       <c r="F7" t="s">
@@ -26488,7 +26922,7 @@
       <c r="D8" t="s">
         <v>622</v>
       </c>
-      <c r="E8" s="73">
+      <c r="E8" s="72">
         <v>500</v>
       </c>
       <c r="F8" t="s">
@@ -26508,7 +26942,7 @@
       <c r="D9" t="s">
         <v>622</v>
       </c>
-      <c r="E9" s="73">
+      <c r="E9" s="72">
         <v>329.99</v>
       </c>
     </row>
@@ -26525,7 +26959,7 @@
       <c r="D10" t="s">
         <v>622</v>
       </c>
-      <c r="E10" s="73">
+      <c r="E10" s="72">
         <v>1397.99</v>
       </c>
     </row>
@@ -26542,7 +26976,7 @@
       <c r="D11" t="s">
         <v>622</v>
       </c>
-      <c r="E11" s="73">
+      <c r="E11" s="72">
         <v>500</v>
       </c>
     </row>
@@ -26559,7 +26993,7 @@
       <c r="D12" t="s">
         <v>622</v>
       </c>
-      <c r="E12" s="73">
+      <c r="E12" s="72">
         <v>1881.37</v>
       </c>
       <c r="F12" t="s">
@@ -26579,7 +27013,7 @@
       <c r="D13" t="s">
         <v>622</v>
       </c>
-      <c r="E13" s="73">
+      <c r="E13" s="72">
         <v>0</v>
       </c>
     </row>
@@ -26596,7 +27030,7 @@
       <c r="D14" t="s">
         <v>622</v>
       </c>
-      <c r="E14" s="73">
+      <c r="E14" s="72">
         <v>250</v>
       </c>
     </row>
@@ -26613,7 +27047,7 @@
       <c r="D15" t="s">
         <v>622</v>
       </c>
-      <c r="E15" s="73">
+      <c r="E15" s="72">
         <v>99.99</v>
       </c>
       <c r="F15" t="s">
@@ -26633,7 +27067,7 @@
       <c r="D16" t="s">
         <v>622</v>
       </c>
-      <c r="E16" s="73">
+      <c r="E16" s="72">
         <v>200</v>
       </c>
     </row>
@@ -26657,7 +27091,7 @@
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="73" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="72" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
@@ -26666,22 +27100,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="77" t="s">
         <v>613</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="77" t="s">
         <v>592</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="77" t="s">
         <v>594</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="77" t="s">
         <v>614</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="78" t="s">
         <v>617</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="77" t="s">
         <v>618</v>
       </c>
     </row>
@@ -26698,7 +27132,7 @@
       <c r="D2" s="22">
         <v>44931</v>
       </c>
-      <c r="E2" s="73">
+      <c r="E2" s="72">
         <v>1653.73</v>
       </c>
       <c r="F2" s="1">
@@ -26719,7 +27153,7 @@
       <c r="D3" s="22">
         <v>44931</v>
       </c>
-      <c r="E3" s="73">
+      <c r="E3" s="72">
         <v>3251.61</v>
       </c>
       <c r="F3" s="1">
@@ -26740,7 +27174,7 @@
       <c r="D4" s="22">
         <v>44931</v>
       </c>
-      <c r="E4" s="73">
+      <c r="E4" s="72">
         <v>34.630000000000003</v>
       </c>
       <c r="F4" s="1">
@@ -26761,7 +27195,7 @@
       <c r="D5" s="22">
         <v>44931</v>
       </c>
-      <c r="E5" s="73">
+      <c r="E5" s="72">
         <v>26.25</v>
       </c>
       <c r="F5" s="1">
@@ -26782,7 +27216,7 @@
       <c r="D6" s="22">
         <v>44931</v>
       </c>
-      <c r="E6" s="73">
+      <c r="E6" s="72">
         <v>100</v>
       </c>
       <c r="F6" s="1">
@@ -26803,7 +27237,7 @@
       <c r="D7" s="22">
         <v>44931</v>
       </c>
-      <c r="E7" s="73">
+      <c r="E7" s="72">
         <v>5000</v>
       </c>
       <c r="F7" s="1">
@@ -26824,7 +27258,7 @@
       <c r="D8" s="22">
         <v>44931</v>
       </c>
-      <c r="E8" s="73">
+      <c r="E8" s="72">
         <v>474.39</v>
       </c>
       <c r="F8" s="1">
@@ -26845,7 +27279,7 @@
       <c r="D9" s="22">
         <v>44931</v>
       </c>
-      <c r="E9" s="73">
+      <c r="E9" s="72">
         <v>346.46</v>
       </c>
       <c r="F9" s="1">
@@ -26866,7 +27300,7 @@
       <c r="D10" s="22">
         <v>45329</v>
       </c>
-      <c r="E10" s="73">
+      <c r="E10" s="72">
         <v>250</v>
       </c>
       <c r="F10" s="1">
@@ -26887,7 +27321,7 @@
       <c r="D11" s="22">
         <v>45329</v>
       </c>
-      <c r="E11" s="73">
+      <c r="E11" s="72">
         <v>750</v>
       </c>
       <c r="F11" s="1">
@@ -26908,7 +27342,7 @@
       <c r="D12" s="22">
         <v>45328</v>
       </c>
-      <c r="E12" s="73">
+      <c r="E12" s="72">
         <v>348.08</v>
       </c>
       <c r="F12" s="1">
@@ -26929,7 +27363,7 @@
       <c r="D13" s="22">
         <v>45329</v>
       </c>
-      <c r="E13" s="73">
+      <c r="E13" s="72">
         <v>376.31</v>
       </c>
       <c r="F13" s="1">
@@ -26950,7 +27384,7 @@
       <c r="D14" s="22">
         <v>45329</v>
       </c>
-      <c r="E14" s="73">
+      <c r="E14" s="72">
         <v>123.69</v>
       </c>
       <c r="F14" s="1">
@@ -26971,7 +27405,7 @@
       <c r="D15" s="22">
         <v>45329</v>
       </c>
-      <c r="E15" s="73">
+      <c r="E15" s="72">
         <v>30</v>
       </c>
       <c r="F15" s="1">
@@ -26992,7 +27426,7 @@
       <c r="D16" s="22">
         <v>45329</v>
       </c>
-      <c r="E16" s="73">
+      <c r="E16" s="72">
         <v>299.99</v>
       </c>
       <c r="F16" s="1">
@@ -27013,7 +27447,7 @@
       <c r="D17" s="22">
         <v>45329</v>
       </c>
-      <c r="E17" s="73">
+      <c r="E17" s="72">
         <v>725</v>
       </c>
       <c r="F17" s="1">
@@ -27034,7 +27468,7 @@
       <c r="D18" s="22">
         <v>45329</v>
       </c>
-      <c r="E18" s="73">
+      <c r="E18" s="72">
         <v>672.99</v>
       </c>
       <c r="F18" s="1">
@@ -27055,7 +27489,7 @@
       <c r="D19" s="22">
         <v>45329</v>
       </c>
-      <c r="E19" s="73">
+      <c r="E19" s="72">
         <v>102.01</v>
       </c>
       <c r="F19" s="1">
@@ -27076,7 +27510,7 @@
       <c r="D20" s="22">
         <v>45329</v>
       </c>
-      <c r="E20" s="73">
+      <c r="E20" s="72">
         <v>397.99</v>
       </c>
       <c r="F20" s="1">
@@ -27097,7 +27531,7 @@
       <c r="D21" s="22">
         <v>45330</v>
       </c>
-      <c r="E21" s="73">
+      <c r="E21" s="72">
         <v>555.12</v>
       </c>
       <c r="F21" s="1">
@@ -27118,7 +27552,7 @@
       <c r="D22" s="22">
         <v>45330</v>
       </c>
-      <c r="E22" s="73">
+      <c r="E22" s="72">
         <v>26.25</v>
       </c>
       <c r="F22" s="1">
@@ -27139,7 +27573,7 @@
       <c r="D23" s="22">
         <v>45330</v>
       </c>
-      <c r="E23" s="73">
+      <c r="E23" s="72">
         <v>600</v>
       </c>
       <c r="F23" s="1">
@@ -27160,7 +27594,7 @@
       <c r="D24" s="22">
         <v>45330</v>
       </c>
-      <c r="E24" s="73">
+      <c r="E24" s="72">
         <v>700</v>
       </c>
       <c r="F24" s="1">
@@ -27181,7 +27615,7 @@
       <c r="D25" s="22">
         <v>45330</v>
       </c>
-      <c r="E25" s="73">
+      <c r="E25" s="72">
         <v>-73.33</v>
       </c>
       <c r="F25" s="1">
@@ -27202,7 +27636,7 @@
       <c r="D26" s="22">
         <v>45330</v>
       </c>
-      <c r="E26" s="73">
+      <c r="E26" s="72">
         <v>73.33</v>
       </c>
       <c r="F26" s="1">
@@ -27223,7 +27657,7 @@
       <c r="D27" s="22">
         <v>45330</v>
       </c>
-      <c r="E27" s="73">
+      <c r="E27" s="72">
         <v>250</v>
       </c>
       <c r="F27" s="1">
@@ -27244,7 +27678,7 @@
       <c r="D28" s="22">
         <v>45330</v>
       </c>
-      <c r="E28" s="73">
+      <c r="E28" s="72">
         <v>99.99</v>
       </c>
       <c r="F28" s="1">
@@ -27265,7 +27699,7 @@
       <c r="D29" s="22">
         <v>45330</v>
       </c>
-      <c r="E29" s="73">
+      <c r="E29" s="72">
         <v>200</v>
       </c>
       <c r="F29" s="1">

</xml_diff>

<commit_message>
v2.0.2 - Avant d'intégrer le tableau de bord des C/C
Après avoir ajusté les tables de C/C
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B040CB43-7C68-4BB5-8EB9-7FC716B0BD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478DD5A2-B65B-454C-9746-7F6EA57B5C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28830" windowHeight="15600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEC" sheetId="1" r:id="rId1"/>
     <sheet name="FACTURES" sheetId="2" r:id="rId2"/>
     <sheet name="GL_Trans" sheetId="6" r:id="rId3"/>
-    <sheet name="EJAuto" sheetId="5" r:id="rId4"/>
+    <sheet name="EJ_Auto" sheetId="5" r:id="rId4"/>
     <sheet name="Comptes_Clients" sheetId="7" r:id="rId5"/>
     <sheet name="Encaissements_Entête" sheetId="8" r:id="rId6"/>
     <sheet name="Encaissements_Détail" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Comptes_Clients!$A$1:$J$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">GL_Trans!$A$1:$J$369</definedName>
-    <definedName name="dnrDescriptionEJAuto">OFFSET(EJAuto!#REF!,1,0,COUNTA(EJAuto!#REF!)-1,2)</definedName>
-    <definedName name="PayItem_Amount">OFFSET(Encaissements_Détail!$E$3,1,,COUNTA(Encaissements_Détail!$A$3:$A$981)-1,1)</definedName>
-    <definedName name="PayItem_InvID">OFFSET(Encaissements_Détail!$B$3,1,,COUNTA(Encaissements_Détail!$A$3:$A$981)-1,1)</definedName>
+    <definedName name="PayItem_Amount">OFFSET(Encaissements_Détail!$E$1,1,,COUNTA(Encaissements_Détail!$A$3:$A$999999)+1,1)</definedName>
+    <definedName name="PayItem_Inv_No">OFFSET(Encaissements_Détail!$B$1,1,,COUNTA(Encaissements_Détail!$A$3:$A$999999)+1,1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2708" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="648">
   <si>
     <t>TEC_ID</t>
   </si>
@@ -1860,9 +1860,6 @@
     <t>Betty White</t>
   </si>
   <si>
-    <t>Inv. ID</t>
-  </si>
-  <si>
     <t>Invoice Date</t>
   </si>
   <si>
@@ -1878,15 +1875,9 @@
     <t>Due Date</t>
   </si>
   <si>
-    <t>Footer Message</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Total Pages</t>
-  </si>
-  <si>
     <t>Balance</t>
   </si>
   <si>
@@ -1896,9 +1887,6 @@
     <t>Billed</t>
   </si>
   <si>
-    <t>Sumer Sale</t>
-  </si>
-  <si>
     <t>Dolores Richman</t>
   </si>
   <si>
@@ -1911,9 +1899,6 @@
     <t>Net 15</t>
   </si>
   <si>
-    <t>Black Friday</t>
-  </si>
-  <si>
     <t>Fred Fredders</t>
   </si>
   <si>
@@ -2032,6 +2017,15 @@
   </si>
   <si>
     <t>Lone Star Technologies, Inc.</t>
+  </si>
+  <si>
+    <t>Inco Ltd.</t>
+  </si>
+  <si>
+    <t>Inv_No</t>
+  </si>
+  <si>
+    <t>23-23039</t>
   </si>
 </sst>
 </file>
@@ -2046,7 +2040,7 @@
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2135,6 +2129,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2174,7 +2174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2299,19 +2299,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="5" tint="-0.249977111117893"/>
       </left>
       <right style="thin">
@@ -2326,11 +2313,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2525,21 +2513,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="1" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2574,37 +2552,31 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="6" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="1" fillId="5" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="5" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Monétaire" xfId="2" builtinId="4"/>
     <cellStyle name="Monétaire 2" xfId="1" xr:uid="{7066D7D9-A0C5-4744-AD1B-CDB1C4228FB1}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFE2F0FA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2633,6 +2605,44 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFE5F4F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2F0FA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2F0FA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2922,7 +2932,7 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:P257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="600" topLeftCell="A222" activePane="bottomLeft"/>
       <selection activeCell="P1" sqref="P1:P1048576"/>
       <selection pane="bottomLeft" activeCell="F239" sqref="F239"/>
@@ -2970,7 +2980,7 @@
       <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="93" t="s">
+      <c r="H1" s="89" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
@@ -13459,17 +13469,17 @@
         <v>0</v>
       </c>
       <c r="O248" s="14" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
     </row>
     <row r="249" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A249" s="85">
+      <c r="A249" s="81">
         <v>249</v>
       </c>
-      <c r="B249" s="85">
-        <v>1</v>
-      </c>
-      <c r="C249" s="85" t="s">
+      <c r="B249" s="81">
+        <v>1</v>
+      </c>
+      <c r="C249" s="81" t="s">
         <v>16</v>
       </c>
       <c r="D249" s="66">
@@ -13478,42 +13488,42 @@
       <c r="E249" s="4">
         <v>1083</v>
       </c>
-      <c r="F249" s="87" t="s">
+      <c r="F249" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="G249" s="87" t="s">
-        <v>641</v>
-      </c>
-      <c r="H249" s="94">
+      <c r="G249" s="83" t="s">
+        <v>636</v>
+      </c>
+      <c r="H249" s="90">
         <v>1.5</v>
       </c>
-      <c r="I249" s="87" t="s">
-        <v>642</v>
-      </c>
-      <c r="J249" s="85" t="b">
+      <c r="I249" s="83" t="s">
+        <v>637</v>
+      </c>
+      <c r="J249" s="81" t="b">
         <v>1</v>
       </c>
       <c r="K249" s="69">
         <v>45336.309918981497</v>
       </c>
-      <c r="L249" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="N249" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="O249" s="87" t="s">
-        <v>643</v>
+      <c r="L249" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="N249" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="O249" s="83" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="250" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A250" s="85">
+      <c r="A250" s="81">
         <v>250</v>
       </c>
-      <c r="B250" s="85">
-        <v>1</v>
-      </c>
-      <c r="C250" s="85" t="s">
+      <c r="B250" s="81">
+        <v>1</v>
+      </c>
+      <c r="C250" s="81" t="s">
         <v>16</v>
       </c>
       <c r="D250" s="66">
@@ -13522,335 +13532,335 @@
       <c r="E250" s="4">
         <v>895</v>
       </c>
-      <c r="F250" s="87" t="s">
+      <c r="F250" s="83" t="s">
         <v>118</v>
       </c>
-      <c r="G250" s="87" t="s">
-        <v>641</v>
-      </c>
-      <c r="H250" s="94">
+      <c r="G250" s="83" t="s">
+        <v>636</v>
+      </c>
+      <c r="H250" s="90">
         <v>2.5</v>
       </c>
-      <c r="I250" s="87" t="s">
-        <v>644</v>
-      </c>
-      <c r="J250" s="85" t="b">
+      <c r="I250" s="83" t="s">
+        <v>639</v>
+      </c>
+      <c r="J250" s="81" t="b">
         <v>1</v>
       </c>
       <c r="K250" s="69">
         <v>45336.310034722199</v>
       </c>
-      <c r="L250" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="N250" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="O250" s="87" t="s">
-        <v>643</v>
+      <c r="L250" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="N250" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="O250" s="83" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="251" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A251" s="85">
+      <c r="A251" s="81">
         <v>251</v>
       </c>
-      <c r="B251" s="85">
-        <v>1</v>
-      </c>
-      <c r="C251" s="85" t="s">
+      <c r="B251" s="81">
+        <v>1</v>
+      </c>
+      <c r="C251" s="81" t="s">
         <v>16</v>
       </c>
       <c r="D251" s="66">
         <v>45336</v>
       </c>
-      <c r="E251" s="85">
+      <c r="E251" s="81">
         <v>895</v>
       </c>
-      <c r="F251" s="87" t="s">
+      <c r="F251" s="83" t="s">
         <v>118</v>
       </c>
-      <c r="G251" s="87" t="s">
-        <v>645</v>
-      </c>
-      <c r="H251" s="94">
+      <c r="G251" s="83" t="s">
+        <v>640</v>
+      </c>
+      <c r="H251" s="90">
         <v>2</v>
       </c>
-      <c r="J251" s="85" t="b">
+      <c r="J251" s="81" t="b">
         <v>1</v>
       </c>
       <c r="K251" s="69">
         <v>45336.324351851901</v>
       </c>
-      <c r="L251" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="N251" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="O251" s="87" t="s">
-        <v>643</v>
+      <c r="L251" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="N251" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="O251" s="83" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="252" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A252" s="85">
+      <c r="A252" s="81">
         <v>252</v>
       </c>
-      <c r="B252" s="85">
-        <v>1</v>
-      </c>
-      <c r="C252" s="85" t="s">
+      <c r="B252" s="81">
+        <v>1</v>
+      </c>
+      <c r="C252" s="81" t="s">
         <v>16</v>
       </c>
       <c r="D252" s="66">
         <v>45336</v>
       </c>
-      <c r="E252" s="85">
+      <c r="E252" s="81">
         <v>344</v>
       </c>
-      <c r="F252" s="87" t="s">
+      <c r="F252" s="83" t="s">
         <v>172</v>
       </c>
-      <c r="G252" s="87" t="s">
-        <v>646</v>
-      </c>
-      <c r="H252" s="94">
-        <v>1</v>
-      </c>
-      <c r="J252" s="85" t="b">
+      <c r="G252" s="83" t="s">
+        <v>641</v>
+      </c>
+      <c r="H252" s="90">
+        <v>1</v>
+      </c>
+      <c r="J252" s="81" t="b">
         <v>1</v>
       </c>
       <c r="K252" s="69">
         <v>45336.3262384259</v>
       </c>
-      <c r="L252" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="N252" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="O252" s="87" t="s">
-        <v>643</v>
+      <c r="L252" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="N252" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="O252" s="83" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="253" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A253" s="85">
+      <c r="A253" s="81">
         <v>253</v>
       </c>
-      <c r="B253" s="85">
+      <c r="B253" s="81">
         <v>2</v>
       </c>
-      <c r="C253" s="85" t="s">
+      <c r="C253" s="81" t="s">
         <v>247</v>
       </c>
       <c r="D253" s="66">
         <v>45336</v>
       </c>
-      <c r="E253" s="85">
+      <c r="E253" s="81">
         <v>895</v>
       </c>
-      <c r="F253" s="87" t="s">
+      <c r="F253" s="83" t="s">
         <v>118</v>
       </c>
-      <c r="G253" s="87" t="s">
-        <v>647</v>
-      </c>
-      <c r="H253" s="94">
-        <v>1</v>
-      </c>
-      <c r="J253" s="85" t="b">
+      <c r="G253" s="83" t="s">
+        <v>642</v>
+      </c>
+      <c r="H253" s="90">
+        <v>1</v>
+      </c>
+      <c r="J253" s="81" t="b">
         <v>1</v>
       </c>
       <c r="K253" s="69">
         <v>45336.326446759304</v>
       </c>
-      <c r="L253" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="N253" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="O253" s="87" t="s">
-        <v>643</v>
+      <c r="L253" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="N253" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="O253" s="83" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="254" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A254" s="85">
+      <c r="A254" s="81">
         <v>254</v>
       </c>
-      <c r="B254" s="85">
+      <c r="B254" s="81">
         <v>2</v>
       </c>
-      <c r="C254" s="85" t="s">
+      <c r="C254" s="81" t="s">
         <v>247</v>
       </c>
       <c r="D254" s="66">
         <v>45336</v>
       </c>
-      <c r="E254" s="85">
+      <c r="E254" s="81">
         <v>344</v>
       </c>
-      <c r="F254" s="87" t="s">
+      <c r="F254" s="83" t="s">
         <v>172</v>
       </c>
-      <c r="G254" s="87" t="s">
-        <v>646</v>
-      </c>
-      <c r="H254" s="94">
+      <c r="G254" s="83" t="s">
+        <v>641</v>
+      </c>
+      <c r="H254" s="90">
         <v>2</v>
       </c>
-      <c r="J254" s="85" t="b">
+      <c r="J254" s="81" t="b">
         <v>1</v>
       </c>
       <c r="K254" s="69">
         <v>45336.326631944401</v>
       </c>
-      <c r="L254" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="N254" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="O254" s="87" t="s">
-        <v>643</v>
+      <c r="L254" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="N254" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="O254" s="83" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="255" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A255" s="85">
+      <c r="A255" s="81">
         <v>255</v>
       </c>
-      <c r="B255" s="85">
+      <c r="B255" s="81">
         <v>3</v>
       </c>
-      <c r="C255" s="85" t="s">
+      <c r="C255" s="81" t="s">
         <v>59</v>
       </c>
       <c r="D255" s="66">
         <v>45335</v>
       </c>
-      <c r="E255" s="85">
+      <c r="E255" s="81">
         <v>1083</v>
       </c>
-      <c r="F255" s="87" t="s">
+      <c r="F255" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="G255" s="87" t="s">
-        <v>646</v>
-      </c>
-      <c r="H255" s="94">
+      <c r="G255" s="83" t="s">
+        <v>641</v>
+      </c>
+      <c r="H255" s="90">
         <v>2</v>
       </c>
-      <c r="J255" s="85" t="b">
+      <c r="J255" s="81" t="b">
         <v>1</v>
       </c>
       <c r="K255" s="69">
         <v>45336.326932870397</v>
       </c>
-      <c r="L255" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="N255" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="O255" s="87" t="s">
-        <v>643</v>
+      <c r="L255" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="N255" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="O255" s="83" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A256" s="85">
+      <c r="A256" s="81">
         <v>256</v>
       </c>
-      <c r="B256" s="85">
+      <c r="B256" s="81">
         <v>4</v>
       </c>
-      <c r="C256" s="85" t="s">
+      <c r="C256" s="81" t="s">
         <v>21</v>
       </c>
       <c r="D256" s="66">
         <v>45335</v>
       </c>
-      <c r="E256" s="85">
+      <c r="E256" s="81">
         <v>921</v>
       </c>
-      <c r="F256" s="87" t="s">
+      <c r="F256" s="83" t="s">
         <v>192</v>
       </c>
-      <c r="G256" s="87" t="s">
-        <v>648</v>
-      </c>
-      <c r="H256" s="94">
+      <c r="G256" s="83" t="s">
+        <v>643</v>
+      </c>
+      <c r="H256" s="90">
         <v>5</v>
       </c>
-      <c r="J256" s="85" t="b">
+      <c r="J256" s="81" t="b">
         <v>1</v>
       </c>
       <c r="K256" s="69">
         <v>45336.3274074074</v>
       </c>
-      <c r="L256" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="N256" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="O256" s="87" t="s">
-        <v>643</v>
+      <c r="L256" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="N256" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="O256" s="83" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="257" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A257" s="85">
+      <c r="A257" s="81">
         <v>257</v>
       </c>
-      <c r="B257" s="85">
-        <v>1</v>
-      </c>
-      <c r="C257" s="85" t="s">
+      <c r="B257" s="81">
+        <v>1</v>
+      </c>
+      <c r="C257" s="81" t="s">
         <v>16</v>
       </c>
       <c r="D257" s="66">
         <v>45336</v>
       </c>
-      <c r="E257" s="85">
+      <c r="E257" s="81">
         <v>1109</v>
       </c>
-      <c r="F257" s="87" t="s">
-        <v>649</v>
-      </c>
-      <c r="G257" s="87" t="s">
+      <c r="F257" s="83" t="s">
+        <v>644</v>
+      </c>
+      <c r="G257" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="H257" s="94">
-        <v>1</v>
-      </c>
-      <c r="J257" s="85" t="b">
+      <c r="H257" s="90">
+        <v>1</v>
+      </c>
+      <c r="J257" s="81" t="b">
         <v>1</v>
       </c>
       <c r="K257" s="69">
         <v>45336.327800925901</v>
       </c>
-      <c r="L257" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="N257" s="85" t="b">
-        <v>0</v>
-      </c>
-      <c r="O257" s="87" t="s">
-        <v>643</v>
+      <c r="L257" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="N257" s="81" t="b">
+        <v>0</v>
+      </c>
+      <c r="O257" s="83" t="s">
+        <v>638</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:P100002">
+    <cfRule type="expression" dxfId="10" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+    <cfRule type="expression" priority="4">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K249:K257">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
     <cfRule type="expression" priority="2">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:P100002">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-    <cfRule type="expression" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14692,10 +14702,10 @@
       <c r="F1" s="43" t="s">
         <v>392</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="85" t="s">
         <v>393</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="85" t="s">
         <v>394</v>
       </c>
       <c r="I1" s="30" t="s">
@@ -21444,10 +21454,10 @@
       <c r="F238" s="14" t="s">
         <v>401</v>
       </c>
-      <c r="G238" s="90">
+      <c r="G238" s="86">
         <v>696.75</v>
       </c>
-      <c r="H238" s="90"/>
+      <c r="H238" s="86"/>
       <c r="I238" s="14"/>
       <c r="J238" s="42">
         <f>ROW()</f>
@@ -21473,8 +21483,8 @@
       <c r="F239" s="14" t="s">
         <v>488</v>
       </c>
-      <c r="G239" s="90"/>
-      <c r="H239" s="90">
+      <c r="G239" s="86"/>
+      <c r="H239" s="86">
         <v>600</v>
       </c>
       <c r="I239" s="14"/>
@@ -21502,8 +21512,8 @@
       <c r="F240" s="14" t="s">
         <v>504</v>
       </c>
-      <c r="G240" s="90"/>
-      <c r="H240" s="90">
+      <c r="G240" s="86"/>
+      <c r="H240" s="86">
         <v>1</v>
       </c>
       <c r="I240" s="14"/>
@@ -21531,8 +21541,8 @@
       <c r="F241" s="14" t="s">
         <v>501</v>
       </c>
-      <c r="G241" s="90"/>
-      <c r="H241" s="90">
+      <c r="G241" s="86"/>
+      <c r="H241" s="86">
         <v>2</v>
       </c>
       <c r="I241" s="14"/>
@@ -21560,8 +21570,8 @@
       <c r="F242" s="14" t="s">
         <v>494</v>
       </c>
-      <c r="G242" s="90"/>
-      <c r="H242" s="90">
+      <c r="G242" s="86"/>
+      <c r="H242" s="86">
         <v>3</v>
       </c>
       <c r="I242" s="14"/>
@@ -21589,8 +21599,8 @@
       <c r="F243" s="14" t="s">
         <v>486</v>
       </c>
-      <c r="G243" s="90"/>
-      <c r="H243" s="90">
+      <c r="G243" s="86"/>
+      <c r="H243" s="86">
         <v>30.3</v>
       </c>
       <c r="I243" s="14"/>
@@ -21618,8 +21628,8 @@
       <c r="F244" s="14" t="s">
         <v>487</v>
       </c>
-      <c r="G244" s="90"/>
-      <c r="H244" s="90">
+      <c r="G244" s="86"/>
+      <c r="H244" s="86">
         <v>60.45</v>
       </c>
       <c r="I244" s="14"/>
@@ -23671,7 +23681,7 @@
       <c r="F316" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="G316" s="91">
+      <c r="G316" s="87">
         <v>0.25</v>
       </c>
       <c r="J316" s="42">
@@ -23698,7 +23708,7 @@
       <c r="F317" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="H317" s="91">
+      <c r="H317" s="87">
         <v>0.25</v>
       </c>
       <c r="J317" s="42">
@@ -24523,16 +24533,16 @@
       <c r="B348" s="37">
         <v>45330</v>
       </c>
-      <c r="C348" s="84" t="s">
-        <v>627</v>
-      </c>
-      <c r="D348" s="84" t="s">
+      <c r="C348" s="80" t="s">
+        <v>622</v>
+      </c>
+      <c r="D348" s="80" t="s">
         <v>307</v>
       </c>
-      <c r="E348" s="85" t="s">
+      <c r="E348" s="81" t="s">
         <v>467</v>
       </c>
-      <c r="F348" s="84" t="s">
+      <c r="F348" s="80" t="s">
         <v>468</v>
       </c>
       <c r="G348" s="25">
@@ -24550,16 +24560,16 @@
       <c r="B349" s="57">
         <v>45330</v>
       </c>
-      <c r="C349" s="86" t="s">
-        <v>627</v>
-      </c>
-      <c r="D349" s="86" t="s">
+      <c r="C349" s="82" t="s">
+        <v>622</v>
+      </c>
+      <c r="D349" s="82" t="s">
         <v>307</v>
       </c>
-      <c r="E349" s="85" t="s">
+      <c r="E349" s="81" t="s">
         <v>400</v>
       </c>
-      <c r="F349" s="84" t="s">
+      <c r="F349" s="80" t="s">
         <v>398</v>
       </c>
       <c r="H349" s="25">
@@ -24577,13 +24587,13 @@
       <c r="B350" s="37">
         <v>45331</v>
       </c>
-      <c r="C350" s="87" t="s">
+      <c r="C350" s="83" t="s">
         <v>517</v>
       </c>
-      <c r="E350" s="85" t="s">
+      <c r="E350" s="81" t="s">
         <v>445</v>
       </c>
-      <c r="F350" s="87" t="s">
+      <c r="F350" s="83" t="s">
         <v>401</v>
       </c>
       <c r="G350" s="25">
@@ -24601,14 +24611,14 @@
       <c r="B351" s="44">
         <v>45331</v>
       </c>
-      <c r="C351" s="88" t="s">
+      <c r="C351" s="84" t="s">
         <v>517</v>
       </c>
       <c r="D351" s="38"/>
-      <c r="E351" s="85" t="s">
+      <c r="E351" s="81" t="s">
         <v>421</v>
       </c>
-      <c r="F351" s="87" t="s">
+      <c r="F351" s="83" t="s">
         <v>422</v>
       </c>
       <c r="H351" s="25">
@@ -24626,14 +24636,14 @@
       <c r="B352" s="44">
         <v>45331</v>
       </c>
-      <c r="C352" s="88" t="s">
+      <c r="C352" s="84" t="s">
         <v>517</v>
       </c>
       <c r="D352" s="38"/>
-      <c r="E352" s="85" t="s">
+      <c r="E352" s="81" t="s">
         <v>408</v>
       </c>
-      <c r="F352" s="87" t="s">
+      <c r="F352" s="83" t="s">
         <v>409</v>
       </c>
       <c r="H352" s="25">
@@ -24651,14 +24661,14 @@
       <c r="B353" s="44">
         <v>45331</v>
       </c>
-      <c r="C353" s="88" t="s">
+      <c r="C353" s="84" t="s">
         <v>517</v>
       </c>
       <c r="D353" s="38"/>
-      <c r="E353" s="85" t="s">
+      <c r="E353" s="81" t="s">
         <v>416</v>
       </c>
-      <c r="F353" s="87" t="s">
+      <c r="F353" s="83" t="s">
         <v>417</v>
       </c>
       <c r="H353" s="25">
@@ -24676,14 +24686,14 @@
       <c r="B354" s="44">
         <v>45331</v>
       </c>
-      <c r="C354" s="88" t="s">
+      <c r="C354" s="84" t="s">
         <v>517</v>
       </c>
       <c r="D354" s="38"/>
-      <c r="E354" s="85" t="s">
+      <c r="E354" s="81" t="s">
         <v>430</v>
       </c>
-      <c r="F354" s="87" t="s">
+      <c r="F354" s="83" t="s">
         <v>431</v>
       </c>
       <c r="G354" s="25">
@@ -24701,16 +24711,16 @@
       <c r="B355" s="37">
         <v>45331</v>
       </c>
-      <c r="C355" s="87" t="s">
-        <v>628</v>
-      </c>
-      <c r="D355" s="87" t="s">
+      <c r="C355" s="83" t="s">
+        <v>623</v>
+      </c>
+      <c r="D355" s="83" t="s">
         <v>307</v>
       </c>
-      <c r="E355" s="85" t="s">
+      <c r="E355" s="81" t="s">
         <v>400</v>
       </c>
-      <c r="F355" s="87" t="s">
+      <c r="F355" s="83" t="s">
         <v>398</v>
       </c>
       <c r="G355" s="25">
@@ -24728,16 +24738,16 @@
       <c r="B356" s="31">
         <v>45331</v>
       </c>
-      <c r="C356" s="88" t="s">
-        <v>628</v>
-      </c>
-      <c r="D356" s="88" t="s">
+      <c r="C356" s="84" t="s">
+        <v>623</v>
+      </c>
+      <c r="D356" s="84" t="s">
         <v>307</v>
       </c>
-      <c r="E356" s="85" t="s">
+      <c r="E356" s="81" t="s">
         <v>467</v>
       </c>
-      <c r="F356" s="87" t="s">
+      <c r="F356" s="83" t="s">
         <v>468</v>
       </c>
       <c r="H356" s="25">
@@ -24759,7 +24769,7 @@
         <v>53</v>
       </c>
       <c r="D357" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="E357" s="1">
         <v>1000</v>
@@ -24786,7 +24796,7 @@
         <v>53</v>
       </c>
       <c r="D358" s="38" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="E358" s="1">
         <v>1100</v>
@@ -24813,7 +24823,7 @@
         <v>53</v>
       </c>
       <c r="D359" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="E359" s="1">
         <v>1000</v>
@@ -24840,7 +24850,7 @@
         <v>53</v>
       </c>
       <c r="D360" s="38" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="E360" s="1">
         <v>1100</v>
@@ -24863,23 +24873,23 @@
       <c r="B361" s="22">
         <v>45331</v>
       </c>
-      <c r="C361" s="87" t="s">
+      <c r="C361" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="D361" s="87" t="s">
-        <v>631</v>
-      </c>
-      <c r="E361" s="85" t="s">
+      <c r="D361" s="83" t="s">
+        <v>626</v>
+      </c>
+      <c r="E361" s="81" t="s">
         <v>400</v>
       </c>
-      <c r="F361" s="87" t="s">
+      <c r="F361" s="83" t="s">
         <v>398</v>
       </c>
       <c r="G361" s="25">
         <v>25</v>
       </c>
-      <c r="I361" s="87" t="s">
-        <v>632</v>
+      <c r="I361" s="83" t="s">
+        <v>627</v>
       </c>
       <c r="J361" s="42">
         <f>ROW()</f>
@@ -24893,23 +24903,23 @@
       <c r="B362" s="31">
         <v>45331</v>
       </c>
-      <c r="C362" s="88" t="s">
+      <c r="C362" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="D362" s="88" t="s">
-        <v>631</v>
-      </c>
-      <c r="E362" s="85" t="s">
+      <c r="D362" s="84" t="s">
+        <v>626</v>
+      </c>
+      <c r="E362" s="81" t="s">
         <v>445</v>
       </c>
-      <c r="F362" s="87" t="s">
+      <c r="F362" s="83" t="s">
         <v>569</v>
       </c>
       <c r="H362" s="25">
         <v>25</v>
       </c>
-      <c r="I362" s="87" t="s">
-        <v>632</v>
+      <c r="I362" s="83" t="s">
+        <v>627</v>
       </c>
       <c r="J362" s="42">
         <f>ROW()</f>
@@ -24923,13 +24933,13 @@
       <c r="B363" s="22">
         <v>45331</v>
       </c>
-      <c r="C363" s="87" t="s">
-        <v>634</v>
-      </c>
-      <c r="E363" s="85" t="s">
+      <c r="C363" s="83" t="s">
+        <v>629</v>
+      </c>
+      <c r="E363" s="81" t="s">
         <v>467</v>
       </c>
-      <c r="F363" s="87" t="s">
+      <c r="F363" s="83" t="s">
         <v>468</v>
       </c>
       <c r="G363" s="25">
@@ -24947,14 +24957,14 @@
       <c r="B364" s="31">
         <v>45331</v>
       </c>
-      <c r="C364" s="88" t="s">
-        <v>634</v>
+      <c r="C364" s="84" t="s">
+        <v>629</v>
       </c>
       <c r="D364" s="38"/>
-      <c r="E364" s="85" t="s">
+      <c r="E364" s="81" t="s">
         <v>400</v>
       </c>
-      <c r="F364" s="87" t="s">
+      <c r="F364" s="83" t="s">
         <v>398</v>
       </c>
       <c r="H364" s="25">
@@ -24972,17 +24982,17 @@
       <c r="B365" s="22">
         <v>45331</v>
       </c>
-      <c r="C365" s="87" t="s">
-        <v>636</v>
-      </c>
-      <c r="D365" s="87" t="s">
-        <v>635</v>
-      </c>
-      <c r="E365" s="85" t="s">
-        <v>637</v>
-      </c>
-      <c r="F365" s="87" t="s">
-        <v>638</v>
+      <c r="C365" s="83" t="s">
+        <v>631</v>
+      </c>
+      <c r="D365" s="83" t="s">
+        <v>630</v>
+      </c>
+      <c r="E365" s="81" t="s">
+        <v>632</v>
+      </c>
+      <c r="F365" s="83" t="s">
+        <v>633</v>
       </c>
       <c r="G365" s="25">
         <v>195.95</v>
@@ -24999,16 +25009,16 @@
       <c r="B366" s="31">
         <v>45331</v>
       </c>
-      <c r="C366" s="88" t="s">
-        <v>636</v>
-      </c>
-      <c r="D366" s="88" t="s">
-        <v>635</v>
-      </c>
-      <c r="E366" s="85" t="s">
+      <c r="C366" s="84" t="s">
+        <v>631</v>
+      </c>
+      <c r="D366" s="84" t="s">
+        <v>630</v>
+      </c>
+      <c r="E366" s="81" t="s">
         <v>430</v>
       </c>
-      <c r="F366" s="87" t="s">
+      <c r="F366" s="83" t="s">
         <v>431</v>
       </c>
       <c r="H366" s="25">
@@ -25026,23 +25036,23 @@
       <c r="B367" s="22">
         <v>45331</v>
       </c>
-      <c r="C367" s="87" t="s">
+      <c r="C367" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="D367" s="87" t="s">
-        <v>639</v>
-      </c>
-      <c r="E367" s="85" t="s">
+      <c r="D367" s="83" t="s">
+        <v>634</v>
+      </c>
+      <c r="E367" s="81" t="s">
         <v>400</v>
       </c>
-      <c r="F367" s="87" t="s">
+      <c r="F367" s="83" t="s">
         <v>398</v>
       </c>
       <c r="G367" s="25">
         <v>100</v>
       </c>
-      <c r="I367" s="87" t="s">
-        <v>640</v>
+      <c r="I367" s="83" t="s">
+        <v>635</v>
       </c>
       <c r="J367" s="42">
         <f>ROW()</f>
@@ -25056,23 +25066,23 @@
       <c r="B368" s="31">
         <v>45331</v>
       </c>
-      <c r="C368" s="88" t="s">
+      <c r="C368" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="D368" s="88" t="s">
-        <v>639</v>
-      </c>
-      <c r="E368" s="85" t="s">
+      <c r="D368" s="84" t="s">
+        <v>634</v>
+      </c>
+      <c r="E368" s="81" t="s">
         <v>445</v>
       </c>
-      <c r="F368" s="87" t="s">
+      <c r="F368" s="83" t="s">
         <v>569</v>
       </c>
       <c r="H368" s="25">
         <v>100</v>
       </c>
-      <c r="I368" s="87" t="s">
-        <v>640</v>
+      <c r="I368" s="83" t="s">
+        <v>635</v>
       </c>
       <c r="J368" s="42">
         <f>ROW()</f>
@@ -25080,8 +25090,8 @@
       </c>
     </row>
     <row r="369" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G369" s="92"/>
-      <c r="H369" s="92"/>
+      <c r="G369" s="88"/>
+      <c r="H369" s="88"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J369" xr:uid="{E0D58006-DE1D-488F-9BB7-8096C5818030}"/>
@@ -25096,7 +25106,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1048576"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25123,10 +25133,10 @@
       <c r="D1" s="43" t="s">
         <v>392</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="77" t="s">
         <v>393</v>
       </c>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="77" t="s">
         <v>394</v>
       </c>
       <c r="G1" s="30" t="s">
@@ -25149,10 +25159,10 @@
       <c r="D2" s="47" t="s">
         <v>468</v>
       </c>
-      <c r="E2" s="82">
+      <c r="E2" s="78">
         <v>29.95</v>
       </c>
-      <c r="F2" s="82"/>
+      <c r="F2" s="78"/>
       <c r="G2" s="48"/>
       <c r="H2" s="42">
         <f>ROW()</f>
@@ -25172,8 +25182,8 @@
       <c r="D3" s="51" t="s">
         <v>398</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83">
+      <c r="E3" s="79"/>
+      <c r="F3" s="79">
         <v>29.95</v>
       </c>
       <c r="G3" s="52"/>
@@ -25207,10 +25217,10 @@
       <c r="D5" s="47" t="s">
         <v>401</v>
       </c>
-      <c r="E5" s="82">
+      <c r="E5" s="78">
         <v>262.44</v>
       </c>
-      <c r="F5" s="82"/>
+      <c r="F5" s="78"/>
       <c r="G5" s="48"/>
       <c r="H5" s="42">
         <f>ROW()</f>
@@ -25296,10 +25306,10 @@
       <c r="D9" s="51" t="s">
         <v>431</v>
       </c>
-      <c r="E9" s="83">
+      <c r="E9" s="79">
         <v>25</v>
       </c>
-      <c r="F9" s="83"/>
+      <c r="F9" s="79"/>
       <c r="G9" s="52"/>
       <c r="H9" s="42">
         <f>ROW()</f>
@@ -25331,10 +25341,10 @@
       <c r="D11" s="47" t="s">
         <v>497</v>
       </c>
-      <c r="E11" s="82">
+      <c r="E11" s="78">
         <v>2400</v>
       </c>
-      <c r="F11" s="82"/>
+      <c r="F11" s="78"/>
       <c r="G11" s="48"/>
       <c r="H11" s="42">
         <f>ROW()</f>
@@ -25398,8 +25408,8 @@
       <c r="D14" s="51" t="s">
         <v>398</v>
       </c>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83">
+      <c r="E14" s="79"/>
+      <c r="F14" s="79">
         <v>2759.4</v>
       </c>
       <c r="G14" s="52"/>
@@ -25433,10 +25443,10 @@
       <c r="D16" s="47" t="s">
         <v>510</v>
       </c>
-      <c r="E16" s="82">
+      <c r="E16" s="78">
         <v>650</v>
       </c>
-      <c r="F16" s="82"/>
+      <c r="F16" s="78"/>
       <c r="G16" s="48"/>
       <c r="H16" s="42">
         <f>ROW()</f>
@@ -25500,8 +25510,8 @@
       <c r="D19" s="51" t="s">
         <v>398</v>
       </c>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83">
+      <c r="E19" s="79"/>
+      <c r="F19" s="79">
         <v>747.34</v>
       </c>
       <c r="G19" s="52"/>
@@ -25535,10 +25545,10 @@
       <c r="D21" s="47" t="s">
         <v>513</v>
       </c>
-      <c r="E21" s="82">
+      <c r="E21" s="78">
         <v>129.94999999999999</v>
       </c>
-      <c r="F21" s="82"/>
+      <c r="F21" s="78"/>
       <c r="G21" s="48"/>
       <c r="H21" s="42">
         <f>ROW()</f>
@@ -25602,8 +25612,8 @@
       <c r="D24" s="51" t="s">
         <v>462</v>
       </c>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83">
+      <c r="E24" s="79"/>
+      <c r="F24" s="79">
         <v>149.41</v>
       </c>
       <c r="G24" s="52" t="s">
@@ -25639,10 +25649,10 @@
       <c r="D26" s="47" t="s">
         <v>468</v>
       </c>
-      <c r="E26" s="82">
+      <c r="E26" s="78">
         <v>29.95</v>
       </c>
-      <c r="F26" s="82"/>
+      <c r="F26" s="78"/>
       <c r="G26" s="48"/>
       <c r="H26" s="42">
         <f>ROW()</f>
@@ -25662,8 +25672,8 @@
       <c r="D27" s="51" t="s">
         <v>398</v>
       </c>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83">
+      <c r="E27" s="79"/>
+      <c r="F27" s="79">
         <v>29.95</v>
       </c>
       <c r="G27" s="52"/>
@@ -25697,10 +25707,10 @@
       <c r="D29" s="59" t="s">
         <v>468</v>
       </c>
-      <c r="E29" s="82">
+      <c r="E29" s="78">
         <v>29.95</v>
       </c>
-      <c r="F29" s="82"/>
+      <c r="F29" s="78"/>
       <c r="G29" s="48"/>
       <c r="H29" s="42">
         <f>ROW()</f>
@@ -25720,8 +25730,8 @@
       <c r="D30" s="61" t="s">
         <v>398</v>
       </c>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83">
+      <c r="E30" s="79"/>
+      <c r="F30" s="79">
         <v>29.95</v>
       </c>
       <c r="G30" s="52"/>
@@ -25747,81 +25757,78 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0BDE8C-C0CD-4E75-A0A0-916CFADCF838}">
   <sheetPr codeName="Feuil4"/>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11.42578125" style="72"/>
-    <col min="10" max="10" width="11.42578125" style="72"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="91" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="91" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12" style="91" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1" s="73" t="s">
         <v>592</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="C1" s="73" t="s">
         <v>593</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="D1" s="73" t="s">
         <v>594</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="E1" s="73" t="s">
         <v>595</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="F1" s="73" t="s">
         <v>596</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="G1" s="94" t="s">
         <v>597</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="H1" s="95" t="s">
         <v>598</v>
-      </c>
-      <c r="H1" s="79" t="s">
-        <v>599</v>
-      </c>
-      <c r="I1" s="74" t="s">
-        <v>600</v>
-      </c>
-      <c r="J1" s="80" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="37">
-        <v>44562</v>
+      <c r="B2" s="22">
+        <v>44927</v>
       </c>
       <c r="C2" t="s">
         <v>571</v>
       </c>
       <c r="D2" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E2" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F2" s="23">
         <v>44592</v>
       </c>
-      <c r="G2" t="s">
-        <v>604</v>
-      </c>
-      <c r="H2" s="72">
+      <c r="G2" s="91">
         <v>9128.4500000000007</v>
       </c>
-      <c r="I2" s="1">
-        <v>6</v>
-      </c>
-      <c r="J2" s="75" cm="1">
-        <f t="array" aca="1" ref="J2" ca="1">H2-IFERROR(SUMIF(PayItem_InvID,A2,PayItem_Amount),0)</f>
+      <c r="H2" s="91" cm="1">
+        <f t="array" aca="1" ref="H2" ca="1">G2-IFERROR(SUMIF(PayItem_Inv_No,A2,PayItem_Amount),0)</f>
         <v>3646.6600000000008</v>
+      </c>
+      <c r="J2" s="91">
+        <f ca="1">G2-H2</f>
+        <v>5481.79</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -25829,28 +25836,29 @@
         <v>2</v>
       </c>
       <c r="B3" s="22">
-        <v>44699</v>
+        <v>45064</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D3" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E3" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="F3" s="23">
         <v>44729</v>
       </c>
-      <c r="H3" s="72">
+      <c r="G3" s="91">
         <v>1653.73</v>
       </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="75" cm="1">
-        <f t="array" aca="1" ref="J3" ca="1">H3-IFERROR(SUMIF(PayItem_InvID,A3,PayItem_Amount),0)</f>
+      <c r="H3" s="91" cm="1">
+        <f t="array" aca="1" ref="H3" ca="1">G3-IFERROR(SUMIF(PayItem_Inv_No,A3,PayItem_Amount),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="91">
+        <f t="shared" ref="J3:J46" ca="1" si="0">G3-H3</f>
         <v>1653.73</v>
       </c>
     </row>
@@ -25858,92 +25866,92 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="37">
-        <v>44699</v>
+      <c r="B4" s="22">
+        <v>45064</v>
       </c>
       <c r="C4" t="s">
         <v>571</v>
       </c>
       <c r="D4" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E4" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="F4" s="23">
         <v>44729</v>
       </c>
-      <c r="H4" s="72">
+      <c r="G4" s="91">
         <v>474.39</v>
       </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-      <c r="J4" s="75" cm="1">
-        <f t="array" aca="1" ref="J4" ca="1">H4-IFERROR(SUMIF(PayItem_InvID,A4,PayItem_Amount),0)</f>
-        <v>0</v>
+      <c r="H4" s="91" cm="1">
+        <f t="array" aca="1" ref="H4" ca="1">G4-IFERROR(SUMIF(PayItem_Inv_No,A4,PayItem_Amount),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>474.39</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="37">
-        <v>44699</v>
+      <c r="B5" s="22">
+        <v>45064</v>
       </c>
       <c r="C5" t="s">
         <v>575</v>
       </c>
       <c r="D5" t="s">
-        <v>607</v>
-      </c>
-      <c r="E5" s="76" t="s">
-        <v>608</v>
+        <v>603</v>
+      </c>
+      <c r="E5" s="74" t="s">
+        <v>604</v>
       </c>
       <c r="F5" s="23">
         <v>44714</v>
       </c>
-      <c r="H5" s="72">
+      <c r="G5" s="91">
         <v>346.46</v>
       </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="75" cm="1">
-        <f t="array" aca="1" ref="J5" ca="1">H5-IFERROR(SUMIF(PayItem_InvID,A5,PayItem_Amount),0)</f>
-        <v>0</v>
+      <c r="H5" s="91" cm="1">
+        <f t="array" aca="1" ref="H5" ca="1">G5-IFERROR(SUMIF(PayItem_Inv_No,A5,PayItem_Amount),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>346.46</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="37">
-        <v>44923</v>
+      <c r="B6" s="22">
+        <v>45288</v>
       </c>
       <c r="C6" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D6" t="s">
+        <v>599</v>
+      </c>
+      <c r="E6" s="74" t="s">
         <v>602</v>
-      </c>
-      <c r="E6" s="76" t="s">
-        <v>606</v>
       </c>
       <c r="F6" s="23">
         <v>44953</v>
       </c>
-      <c r="G6" s="76" t="s">
-        <v>609</v>
-      </c>
-      <c r="H6" s="72">
+      <c r="G6" s="91">
         <v>3251.61</v>
       </c>
-      <c r="I6" s="1">
-        <v>2</v>
-      </c>
-      <c r="J6" s="75" cm="1">
-        <f t="array" aca="1" ref="J6" ca="1">H6-IFERROR(SUMIF(PayItem_InvID,A6,PayItem_Amount),0)</f>
+      <c r="H6" s="91" cm="1">
+        <f t="array" aca="1" ref="H6" ca="1">G6-IFERROR(SUMIF(PayItem_Inv_No,A6,PayItem_Amount),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="91">
+        <f t="shared" ca="1" si="0"/>
         <v>3251.61</v>
       </c>
     </row>
@@ -25958,25 +25966,25 @@
         <v>575</v>
       </c>
       <c r="D7" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="E7" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F7" s="23">
-        <f t="shared" ref="F7:F16" si="0">B7+15</f>
+        <f t="shared" ref="F7:F16" si="1">B7+15</f>
         <v>44960</v>
       </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="72">
+      <c r="G7" s="91">
         <v>974.39</v>
       </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="75" cm="1">
-        <f t="array" aca="1" ref="J7" ca="1">H7-IFERROR(SUMIF(PayItem_InvID,A7,PayItem_Amount),0)</f>
-        <v>0</v>
+      <c r="H7" s="91" cm="1">
+        <f t="array" aca="1" ref="H7" ca="1">G7-IFERROR(SUMIF(PayItem_Inv_No,A7,PayItem_Amount),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>974.39</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -25990,24 +25998,25 @@
         <v>575</v>
       </c>
       <c r="D8" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E8" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F8" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44961</v>
       </c>
-      <c r="H8" s="72">
+      <c r="G8" s="91">
         <v>623.69000000000005</v>
       </c>
-      <c r="I8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="75" cm="1">
-        <f t="array" aca="1" ref="J8" ca="1">H8-IFERROR(SUMIF(PayItem_InvID,A8,PayItem_Amount),0)</f>
+      <c r="H8" s="91" cm="1">
+        <f t="array" aca="1" ref="H8" ca="1">G8-IFERROR(SUMIF(PayItem_Inv_No,A8,PayItem_Amount),0)</f>
         <v>500.00000000000006</v>
+      </c>
+      <c r="J8" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>123.69</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -26018,27 +26027,28 @@
         <v>44947</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D9" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E9" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F9" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44962</v>
       </c>
-      <c r="H9" s="72">
+      <c r="G9" s="91">
         <v>34.630000000000003</v>
       </c>
-      <c r="I9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="75" cm="1">
-        <f t="array" aca="1" ref="J9" ca="1">H9-IFERROR(SUMIF(PayItem_InvID,A9,PayItem_Amount),0)</f>
-        <v>0</v>
+      <c r="H9" s="91" cm="1">
+        <f t="array" aca="1" ref="H9" ca="1">G9-IFERROR(SUMIF(PayItem_Inv_No,A9,PayItem_Amount),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>34.630000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -26049,30 +26059,28 @@
         <v>44948</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D10" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E10" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F10" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44963</v>
       </c>
-      <c r="G10" t="s">
-        <v>609</v>
-      </c>
-      <c r="H10" s="72">
+      <c r="G10" s="91">
         <v>26.25</v>
       </c>
-      <c r="I10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="75" cm="1">
-        <f t="array" aca="1" ref="J10" ca="1">H10-IFERROR(SUMIF(PayItem_InvID,A10,PayItem_Amount),0)</f>
-        <v>0</v>
+      <c r="H10" s="91" cm="1">
+        <f t="array" aca="1" ref="H10" ca="1">G10-IFERROR(SUMIF(PayItem_Inv_No,A10,PayItem_Amount),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>26.25</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -26083,27 +26091,28 @@
         <v>44949</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="D11" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E11" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F11" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44964</v>
       </c>
-      <c r="H11" s="72">
+      <c r="G11" s="91">
         <v>262.5</v>
       </c>
-      <c r="I11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="75" cm="1">
-        <f t="array" aca="1" ref="J11" ca="1">H11-IFERROR(SUMIF(PayItem_InvID,A11,PayItem_Amount),0)</f>
+      <c r="H11" s="91" cm="1">
+        <f t="array" aca="1" ref="H11" ca="1">G11-IFERROR(SUMIF(PayItem_Inv_No,A11,PayItem_Amount),0)</f>
         <v>162.5</v>
+      </c>
+      <c r="J11" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -26114,27 +26123,28 @@
         <v>44950</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D12" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E12" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F12" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44965</v>
       </c>
-      <c r="H12" s="72">
+      <c r="G12" s="91">
         <v>445.2</v>
       </c>
-      <c r="I12" s="1">
-        <v>1</v>
-      </c>
-      <c r="J12" s="75" cm="1">
-        <f t="array" aca="1" ref="J12" ca="1">H12-IFERROR(SUMIF(PayItem_InvID,A12,PayItem_Amount),0)</f>
+      <c r="H12" s="91" cm="1">
+        <f t="array" aca="1" ref="H12" ca="1">G12-IFERROR(SUMIF(PayItem_Inv_No,A12,PayItem_Amount),0)</f>
         <v>445.2</v>
+      </c>
+      <c r="J12" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -26146,27 +26156,28 @@
         <v>44953</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="D13" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E13" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F13" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44968</v>
       </c>
-      <c r="H13" s="72">
+      <c r="G13" s="91">
         <v>26.25</v>
       </c>
-      <c r="I13" s="1">
-        <v>1</v>
-      </c>
-      <c r="J13" s="75">
-        <f t="shared" ref="J13:J31" ca="1" si="1">H13-IFERROR(SUMIF(PayItem_InvID,A13,PayItem_Amount),0)</f>
-        <v>0</v>
+      <c r="H13" s="91">
+        <f t="shared" ref="H13:H46" ca="1" si="2">G13-IFERROR(SUMIF(PayItem_Inv_No,A13,PayItem_Amount),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>26.25</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -26178,27 +26189,28 @@
         <v>44956</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D14" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E14" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F14" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44971</v>
       </c>
-      <c r="H14" s="72">
+      <c r="G14" s="91">
         <v>500</v>
       </c>
-      <c r="I14" s="1">
-        <v>1</v>
-      </c>
-      <c r="J14" s="75">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H14" s="91">
+        <f t="shared" ca="1" si="2"/>
         <v>500</v>
+      </c>
+      <c r="J14" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -26213,24 +26225,25 @@
         <v>571</v>
       </c>
       <c r="D15" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E15" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F15" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44974</v>
       </c>
-      <c r="H15" s="72">
+      <c r="G15" s="91">
         <v>600</v>
       </c>
-      <c r="I15" s="1">
-        <v>1</v>
-      </c>
-      <c r="J15" s="75">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+      <c r="H15" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>600</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -26238,31 +26251,32 @@
         <v>15</v>
       </c>
       <c r="B16" s="22">
-        <f t="shared" ref="B16:B23" si="2">B15+8</f>
+        <f t="shared" ref="B16:B23" si="3">B15+8</f>
         <v>44967</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="D16" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E16" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F16" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44982</v>
       </c>
-      <c r="H16" s="72">
+      <c r="G16" s="91">
         <v>700</v>
       </c>
-      <c r="I16" s="1">
-        <v>1</v>
-      </c>
-      <c r="J16" s="75">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+      <c r="H16" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>700</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -26270,31 +26284,32 @@
         <v>16</v>
       </c>
       <c r="B17" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44975</v>
       </c>
       <c r="C17" t="s">
         <v>584</v>
       </c>
       <c r="D17" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E17" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F17" s="23">
         <f>B17+30</f>
         <v>45005</v>
       </c>
-      <c r="H17" s="72">
+      <c r="G17" s="91">
         <v>725</v>
       </c>
-      <c r="I17" s="1">
-        <v>1</v>
-      </c>
-      <c r="J17" s="75">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+      <c r="H17" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>725</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -26302,31 +26317,32 @@
         <v>17</v>
       </c>
       <c r="B18" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44983</v>
       </c>
       <c r="C18" t="s">
         <v>576</v>
       </c>
       <c r="D18" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E18" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F18" s="23">
-        <f t="shared" ref="F18:F23" si="3">B18+15</f>
+        <f t="shared" ref="F18:F23" si="4">B18+15</f>
         <v>44998</v>
       </c>
-      <c r="H18" s="72">
+      <c r="G18" s="91">
         <v>750</v>
       </c>
-      <c r="I18" s="1">
-        <v>1</v>
-      </c>
-      <c r="J18" s="75">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+      <c r="H18" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>750</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -26334,31 +26350,32 @@
         <v>18</v>
       </c>
       <c r="B19" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44991</v>
       </c>
       <c r="C19" t="s">
         <v>584</v>
       </c>
       <c r="D19" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E19" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F19" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45006</v>
       </c>
-      <c r="H19" s="72">
+      <c r="G19" s="91">
         <v>775</v>
       </c>
-      <c r="I19" s="1">
-        <v>1</v>
-      </c>
-      <c r="J19" s="75">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+      <c r="H19" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>775</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -26366,31 +26383,32 @@
         <v>19</v>
       </c>
       <c r="B20" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44999</v>
       </c>
       <c r="C20" t="s">
         <v>576</v>
       </c>
       <c r="D20" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E20" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F20" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45014</v>
       </c>
-      <c r="H20" s="72">
+      <c r="G20" s="91">
         <v>800</v>
       </c>
-      <c r="I20" s="1">
-        <v>1</v>
-      </c>
-      <c r="J20" s="75">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H20" s="91">
+        <f t="shared" ca="1" si="2"/>
         <v>520</v>
+      </c>
+      <c r="J20" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -26398,31 +26416,32 @@
         <v>20</v>
       </c>
       <c r="B21" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45007</v>
       </c>
       <c r="C21" t="s">
         <v>584</v>
       </c>
       <c r="D21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F21" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
-      <c r="H21" s="72">
+      <c r="G21" s="91">
         <v>774</v>
       </c>
-      <c r="I21" s="1">
-        <v>1</v>
-      </c>
-      <c r="J21" s="75">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H21" s="91">
+        <f t="shared" ca="1" si="2"/>
         <v>376.01</v>
+      </c>
+      <c r="J21" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>397.99</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -26430,31 +26449,32 @@
         <v>21</v>
       </c>
       <c r="B22" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45015</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="D22" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E22" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F22" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45030</v>
       </c>
-      <c r="H22" s="72">
+      <c r="G22" s="91">
         <v>749</v>
       </c>
-      <c r="I22" s="1">
-        <v>1</v>
-      </c>
-      <c r="J22" s="75">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H22" s="91">
+        <f t="shared" ca="1" si="2"/>
         <v>749</v>
+      </c>
+      <c r="J22" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -26462,31 +26482,32 @@
         <v>22</v>
       </c>
       <c r="B23" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45023</v>
       </c>
       <c r="C23" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="D23" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E23" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F23" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45038</v>
       </c>
-      <c r="H23" s="72">
+      <c r="G23" s="91">
         <v>724</v>
       </c>
-      <c r="I23" s="1">
-        <v>1</v>
-      </c>
-      <c r="J23" s="75">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H23" s="91">
+        <f t="shared" ca="1" si="2"/>
         <v>724</v>
+      </c>
+      <c r="J23" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -26501,24 +26522,25 @@
         <v>571</v>
       </c>
       <c r="D24" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E24" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F24" s="23">
         <f>B24+45</f>
         <v>45083</v>
       </c>
-      <c r="H24" s="72">
+      <c r="G24" s="91">
         <v>699.99</v>
       </c>
-      <c r="I24" s="1">
-        <v>1</v>
-      </c>
-      <c r="J24" s="75">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H24" s="91">
+        <f t="shared" ca="1" si="2"/>
         <v>626.66</v>
+      </c>
+      <c r="J24" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>73.330000000000041</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -26530,27 +26552,28 @@
         <v>45053</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="D25" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E25" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F25" s="23">
-        <f t="shared" ref="F25:F31" si="4">B25+15</f>
+        <f t="shared" ref="F25:F30" si="5">B25+15</f>
         <v>45068</v>
       </c>
-      <c r="H25" s="72">
+      <c r="G25" s="91">
         <v>599.99</v>
       </c>
-      <c r="I25" s="1">
-        <v>1</v>
-      </c>
-      <c r="J25" s="75">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H25" s="91">
+        <f t="shared" ca="1" si="2"/>
         <v>599.99</v>
+      </c>
+      <c r="J25" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -26562,27 +26585,28 @@
         <v>45068</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="D26" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E26" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F26" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45083</v>
       </c>
-      <c r="H26" s="72">
+      <c r="G26" s="91">
         <v>499.99</v>
       </c>
-      <c r="I26" s="1">
-        <v>1</v>
-      </c>
-      <c r="J26" s="75">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H26" s="91">
+        <f t="shared" ca="1" si="2"/>
         <v>499.99</v>
+      </c>
+      <c r="J26" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -26597,24 +26621,25 @@
         <v>584</v>
       </c>
       <c r="D27" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E27" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F27" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45098</v>
       </c>
-      <c r="H27" s="72">
+      <c r="G27" s="91">
         <v>399.99</v>
       </c>
-      <c r="I27" s="1">
-        <v>1</v>
-      </c>
-      <c r="J27" s="75">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H27" s="91">
+        <f t="shared" ca="1" si="2"/>
         <v>399.99</v>
+      </c>
+      <c r="J27" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -26629,24 +26654,25 @@
         <v>576</v>
       </c>
       <c r="D28" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E28" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F28" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45113</v>
       </c>
-      <c r="H28" s="72">
+      <c r="G28" s="91">
         <v>299.99</v>
       </c>
-      <c r="I28" s="1">
-        <v>1</v>
-      </c>
-      <c r="J28" s="75">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+      <c r="H28" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>299.99</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -26660,24 +26686,25 @@
         <v>591</v>
       </c>
       <c r="D29" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E29" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F29" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45214</v>
       </c>
-      <c r="H29" s="72">
+      <c r="G29" s="91">
         <v>8999.99</v>
       </c>
-      <c r="I29" s="1">
-        <v>1</v>
-      </c>
-      <c r="J29" s="75">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H29" s="91">
+        <f t="shared" ca="1" si="2"/>
         <v>8700</v>
+      </c>
+      <c r="J29" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>299.98999999999978</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -26692,24 +26719,25 @@
         <v>584</v>
       </c>
       <c r="D30" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E30" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F30" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45245</v>
       </c>
-      <c r="H30" s="72">
+      <c r="G30" s="91">
         <v>7888.88</v>
       </c>
-      <c r="I30" s="1">
-        <v>1</v>
-      </c>
-      <c r="J30" s="75">
-        <f t="shared" ca="1" si="1"/>
+      <c r="H30" s="91">
+        <f t="shared" ca="1" si="2"/>
         <v>7888.88</v>
+      </c>
+      <c r="J30" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -26717,51 +26745,554 @@
         <v>30</v>
       </c>
       <c r="B31" s="22">
-        <v>45292</v>
-      </c>
-      <c r="C31" t="s">
-        <v>576</v>
+        <v>45205</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>367</v>
       </c>
       <c r="D31" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E31" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F31" s="23">
-        <f t="shared" si="4"/>
-        <v>45307</v>
-      </c>
-      <c r="H31" s="72">
-        <v>6777.77</v>
-      </c>
-      <c r="I31" s="1">
-        <v>1</v>
-      </c>
-      <c r="J31" s="75">
-        <f t="shared" ca="1" si="1"/>
-        <v>6777.77</v>
+        <f>B31+30</f>
+        <v>45235</v>
+      </c>
+      <c r="G31" s="91">
+        <v>1207.24</v>
+      </c>
+      <c r="H31" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>1207.24</v>
+      </c>
+      <c r="J31" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>23031</v>
+      </c>
+      <c r="B32" s="22">
+        <v>45211</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E32" t="s">
+        <v>603</v>
+      </c>
+      <c r="F32" s="23">
+        <f t="shared" ref="F32:F46" si="6">B32+30</f>
+        <v>45241</v>
+      </c>
+      <c r="G32" s="96">
+        <v>18874.3</v>
+      </c>
+      <c r="H32" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>16374.3</v>
+      </c>
+      <c r="J32" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B33" s="22">
+        <v>45273</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>599</v>
+      </c>
+      <c r="E33" t="s">
+        <v>603</v>
+      </c>
+      <c r="F33" s="23">
+        <f t="shared" si="6"/>
+        <v>45303</v>
+      </c>
+      <c r="G33" s="96">
+        <v>2585.17</v>
+      </c>
+      <c r="H33" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>2085.17</v>
+      </c>
+      <c r="J33" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B34" s="22">
+        <v>45275</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>303</v>
+      </c>
+      <c r="D34" t="s">
+        <v>599</v>
+      </c>
+      <c r="E34" t="s">
+        <v>603</v>
+      </c>
+      <c r="F34" s="23">
+        <f t="shared" si="6"/>
+        <v>45305</v>
+      </c>
+      <c r="G34" s="96">
+        <v>2112.09</v>
+      </c>
+      <c r="H34" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>1612.0900000000001</v>
+      </c>
+      <c r="J34" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B35" s="22">
+        <v>45280</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" t="s">
+        <v>599</v>
+      </c>
+      <c r="E35" t="s">
+        <v>603</v>
+      </c>
+      <c r="F35" s="23">
+        <f t="shared" si="6"/>
+        <v>45310</v>
+      </c>
+      <c r="G35" s="96">
+        <v>1063.52</v>
+      </c>
+      <c r="H35" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>563.52</v>
+      </c>
+      <c r="J35" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B36" s="22">
+        <v>45279</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>599</v>
+      </c>
+      <c r="E36" t="s">
+        <v>603</v>
+      </c>
+      <c r="F36" s="23">
+        <f t="shared" si="6"/>
+        <v>45309</v>
+      </c>
+      <c r="G36" s="96">
+        <v>3111.2200000000003</v>
+      </c>
+      <c r="H36" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>3086.2200000000003</v>
+      </c>
+      <c r="J36" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B37" s="22">
+        <v>45280</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="D37" t="s">
+        <v>599</v>
+      </c>
+      <c r="E37" t="s">
+        <v>603</v>
+      </c>
+      <c r="F37" s="23">
+        <f t="shared" si="6"/>
+        <v>45310</v>
+      </c>
+      <c r="G37" s="96">
+        <v>413.90999999999997</v>
+      </c>
+      <c r="H37" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>163.90999999999997</v>
+      </c>
+      <c r="J37" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B38" s="22">
+        <v>45280</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="D38" t="s">
+        <v>599</v>
+      </c>
+      <c r="E38" t="s">
+        <v>603</v>
+      </c>
+      <c r="F38" s="23">
+        <f t="shared" si="6"/>
+        <v>45310</v>
+      </c>
+      <c r="G38" s="96">
+        <v>1046.27</v>
+      </c>
+      <c r="H38" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>1046.27</v>
+      </c>
+      <c r="J38" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B39" s="22">
+        <v>45280</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="D39" t="s">
+        <v>599</v>
+      </c>
+      <c r="E39" t="s">
+        <v>603</v>
+      </c>
+      <c r="F39" s="23">
+        <f t="shared" si="6"/>
+        <v>45310</v>
+      </c>
+      <c r="G39" s="96">
+        <v>1456.34</v>
+      </c>
+      <c r="H39" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>1306.3399999999999</v>
+      </c>
+      <c r="J39" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B40" s="22">
+        <v>45279</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" t="s">
+        <v>599</v>
+      </c>
+      <c r="E40" t="s">
+        <v>603</v>
+      </c>
+      <c r="F40" s="23">
+        <f t="shared" si="6"/>
+        <v>45309</v>
+      </c>
+      <c r="G40" s="96">
+        <v>-3111.22</v>
+      </c>
+      <c r="H40" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>-3136.22</v>
+      </c>
+      <c r="J40" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B41" s="22">
+        <v>45281</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="D41" t="s">
+        <v>599</v>
+      </c>
+      <c r="E41" t="s">
+        <v>603</v>
+      </c>
+      <c r="F41" s="23">
+        <f t="shared" si="6"/>
+        <v>45311</v>
+      </c>
+      <c r="G41" s="96">
+        <v>718.59</v>
+      </c>
+      <c r="H41" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>618.59</v>
+      </c>
+      <c r="J41" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B42" s="22">
+        <v>45281</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>645</v>
+      </c>
+      <c r="D42" t="s">
+        <v>599</v>
+      </c>
+      <c r="E42" t="s">
+        <v>603</v>
+      </c>
+      <c r="F42" s="23">
+        <f t="shared" si="6"/>
+        <v>45311</v>
+      </c>
+      <c r="G42" s="96">
+        <v>431.16</v>
+      </c>
+      <c r="H42" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>431.16</v>
+      </c>
+      <c r="J42" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B43" s="22">
+        <v>45281</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="D43" t="s">
+        <v>599</v>
+      </c>
+      <c r="E43" t="s">
+        <v>603</v>
+      </c>
+      <c r="F43" s="23">
+        <f t="shared" si="6"/>
+        <v>45311</v>
+      </c>
+      <c r="G43" s="96">
+        <v>696.75</v>
+      </c>
+      <c r="H43" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>671.75</v>
+      </c>
+      <c r="J43" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B44" s="22">
+        <v>45281</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="D44" t="s">
+        <v>599</v>
+      </c>
+      <c r="E44" t="s">
+        <v>603</v>
+      </c>
+      <c r="F44" s="23">
+        <f t="shared" si="6"/>
+        <v>45311</v>
+      </c>
+      <c r="G44" s="96">
+        <v>9388.86</v>
+      </c>
+      <c r="H44" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>6888.8600000000006</v>
+      </c>
+      <c r="J44" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B45" s="22">
+        <v>45281</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D45" t="s">
+        <v>599</v>
+      </c>
+      <c r="E45" t="s">
+        <v>603</v>
+      </c>
+      <c r="F45" s="23">
+        <f t="shared" si="6"/>
+        <v>45311</v>
+      </c>
+      <c r="G45" s="96">
+        <v>1766.02</v>
+      </c>
+      <c r="H45" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>1266.02</v>
+      </c>
+      <c r="J45" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B46" s="22">
+        <v>45281</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D46" t="s">
+        <v>599</v>
+      </c>
+      <c r="E46" t="s">
+        <v>603</v>
+      </c>
+      <c r="F46" s="23">
+        <f t="shared" si="6"/>
+        <v>45311</v>
+      </c>
+      <c r="G46" s="96">
+        <v>344.93</v>
+      </c>
+      <c r="H46" s="91">
+        <f t="shared" ca="1" si="2"/>
+        <v>344.93</v>
+      </c>
+      <c r="J46" s="91">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J46" xr:uid="{6A0BDE8C-C0CD-4E75-A0A0-916CFADCF838}"/>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <conditionalFormatting sqref="A32:B46">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>AND($A32&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:H999962">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>AND($A2&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:C31">
+    <cfRule type="expression" dxfId="5" priority="9">
+      <formula>AND($A31&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C17:C21">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="4" priority="14">
       <formula>AND($A17&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="3" priority="17">
       <formula>AND($A23&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C28">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="2" priority="13">
       <formula>AND($A27&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C31">
-    <cfRule type="expression" dxfId="4" priority="1">
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="1" priority="12">
       <formula>AND($A30&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32:G46">
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>AND($A32&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26770,44 +27301,48 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC0F112-F6F5-4729-8EA4-252A1080634A}">
-  <sheetPr codeName="Feuil5"/>
-  <dimension ref="A1:F16"/>
+  <sheetPr codeName="Feuil5">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A32" sqref="A32:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="72" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="91" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="91" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
-        <v>613</v>
-      </c>
-      <c r="B1" s="77" t="s">
-        <v>614</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>594</v>
-      </c>
-      <c r="D1" s="77" t="s">
-        <v>615</v>
-      </c>
-      <c r="E1" s="78" t="s">
-        <v>616</v>
-      </c>
-      <c r="F1" s="77" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
+        <v>608</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>609</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>593</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>610</v>
+      </c>
+      <c r="E1" s="92" t="s">
+        <v>611</v>
+      </c>
+      <c r="F1" s="75" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -26815,19 +27350,23 @@
         <v>44931</v>
       </c>
       <c r="C2" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D2" t="s">
-        <v>619</v>
-      </c>
-      <c r="E2" s="75">
+        <v>614</v>
+      </c>
+      <c r="E2" s="93">
         <v>5066.22</v>
       </c>
       <c r="F2" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>615</v>
+      </c>
+      <c r="H2" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A29,Encaissements_Entête!$A2,Encaissements_Détail!$E$2:$E29)</f>
+        <v>5066.22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -26838,13 +27377,17 @@
         <v>571</v>
       </c>
       <c r="D3" t="s">
-        <v>619</v>
-      </c>
-      <c r="E3" s="75">
+        <v>614</v>
+      </c>
+      <c r="E3" s="91">
         <v>5474.39</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A30,Encaissements_Entête!$A3,Encaissements_Détail!$E$2:$E30)</f>
+        <v>5474.39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -26855,13 +27398,17 @@
         <v>575</v>
       </c>
       <c r="D4" t="s">
-        <v>621</v>
-      </c>
-      <c r="E4" s="75">
+        <v>616</v>
+      </c>
+      <c r="E4" s="91">
         <v>346.46</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A31,Encaissements_Entête!$A4,Encaissements_Détail!$E$2:$E31)</f>
+        <v>346.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -26871,11 +27418,15 @@
       <c r="C5" t="s">
         <v>575</v>
       </c>
-      <c r="E5" s="72">
+      <c r="E5" s="91">
         <v>250</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A32,Encaissements_Entête!$A5,Encaissements_Détail!$E$2:$E32)</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -26885,11 +27436,15 @@
       <c r="C6" t="s">
         <v>576</v>
       </c>
-      <c r="E6" s="72">
+      <c r="E6" s="91">
         <v>750</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A33,Encaissements_Entête!$A6,Encaissements_Détail!$E$2:$E33)</f>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -26900,16 +27455,20 @@
         <v>575</v>
       </c>
       <c r="D7" t="s">
-        <v>622</v>
-      </c>
-      <c r="E7" s="72">
+        <v>617</v>
+      </c>
+      <c r="E7" s="91">
         <v>348.08</v>
       </c>
       <c r="F7" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>618</v>
+      </c>
+      <c r="H7" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A34,Encaissements_Entête!$A7,Encaissements_Détail!$E$2:$E34)</f>
+        <v>348.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -26920,16 +27479,20 @@
         <v>575</v>
       </c>
       <c r="D8" t="s">
-        <v>622</v>
-      </c>
-      <c r="E8" s="72">
+        <v>617</v>
+      </c>
+      <c r="E8" s="91">
         <v>500</v>
       </c>
       <c r="F8" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>619</v>
+      </c>
+      <c r="H8" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A35,Encaissements_Entête!$A8,Encaissements_Détail!$E$2:$E35)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -26940,13 +27503,17 @@
         <v>576</v>
       </c>
       <c r="D9" t="s">
-        <v>622</v>
-      </c>
-      <c r="E9" s="72">
+        <v>617</v>
+      </c>
+      <c r="E9" s="91">
         <v>329.99</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H9" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A36,Encaissements_Entête!$A9,Encaissements_Détail!$E$2:$E36)</f>
+        <v>329.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -26957,13 +27524,17 @@
         <v>584</v>
       </c>
       <c r="D10" t="s">
-        <v>622</v>
-      </c>
-      <c r="E10" s="72">
+        <v>617</v>
+      </c>
+      <c r="E10" s="91">
         <v>1397.99</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A37,Encaissements_Entête!$A10,Encaissements_Détail!$E$2:$E37)</f>
+        <v>1397.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -26974,13 +27545,17 @@
         <v>584</v>
       </c>
       <c r="D11" t="s">
-        <v>622</v>
-      </c>
-      <c r="E11" s="72">
+        <v>617</v>
+      </c>
+      <c r="E11" s="91">
         <v>500</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A38,Encaissements_Entête!$A11,Encaissements_Détail!$E$2:$E38)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -26991,16 +27566,20 @@
         <v>571</v>
       </c>
       <c r="D12" t="s">
-        <v>622</v>
-      </c>
-      <c r="E12" s="72">
+        <v>617</v>
+      </c>
+      <c r="E12" s="91">
         <v>1881.37</v>
       </c>
       <c r="F12" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>620</v>
+      </c>
+      <c r="H12" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A39,Encaissements_Entête!$A12,Encaissements_Détail!$E$2:$E39)</f>
+        <v>1881.37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -27011,13 +27590,17 @@
         <v>571</v>
       </c>
       <c r="D13" t="s">
-        <v>622</v>
-      </c>
-      <c r="E13" s="72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>617</v>
+      </c>
+      <c r="E13" s="91">
+        <v>0</v>
+      </c>
+      <c r="H13" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A40,Encaissements_Entête!$A13,Encaissements_Détail!$E$2:$E40)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -27028,13 +27611,17 @@
         <v>576</v>
       </c>
       <c r="D14" t="s">
-        <v>622</v>
-      </c>
-      <c r="E14" s="72">
+        <v>617</v>
+      </c>
+      <c r="E14" s="91">
         <v>250</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A41,Encaissements_Entête!$A14,Encaissements_Détail!$E$2:$E41)</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -27045,16 +27632,20 @@
         <v>591</v>
       </c>
       <c r="D15" t="s">
-        <v>622</v>
-      </c>
-      <c r="E15" s="72">
+        <v>617</v>
+      </c>
+      <c r="E15" s="91">
         <v>99.99</v>
       </c>
       <c r="F15" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>621</v>
+      </c>
+      <c r="H15" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A42,Encaissements_Entête!$A15,Encaissements_Détail!$E$2:$E42)</f>
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -27065,61 +27656,380 @@
         <v>591</v>
       </c>
       <c r="D16" t="s">
-        <v>622</v>
-      </c>
-      <c r="E16" s="72">
+        <v>617</v>
+      </c>
+      <c r="E16" s="91">
         <v>200</v>
       </c>
+      <c r="H16" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A43,Encaissements_Entête!$A16,Encaissements_Détail!$E$2:$E43)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>617</v>
+      </c>
+      <c r="E17" s="91">
+        <v>2500</v>
+      </c>
+      <c r="H17" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A44,Encaissements_Entête!$A17,Encaissements_Détail!$E$2:$E44)</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>617</v>
+      </c>
+      <c r="E18" s="91">
+        <v>500</v>
+      </c>
+      <c r="H18" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A45,Encaissements_Entête!$A18,Encaissements_Détail!$E$2:$E45)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C19" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" t="s">
+        <v>617</v>
+      </c>
+      <c r="E19" s="91">
+        <v>500</v>
+      </c>
+      <c r="H19" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A46,Encaissements_Entête!$A19,Encaissements_Détail!$E$2:$E46)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
+        <v>617</v>
+      </c>
+      <c r="E20" s="91">
+        <v>500</v>
+      </c>
+      <c r="H20" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A47,Encaissements_Entête!$A20,Encaissements_Détail!$E$2:$E47)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>617</v>
+      </c>
+      <c r="E21" s="91">
+        <v>25</v>
+      </c>
+      <c r="H21" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A48,Encaissements_Entête!$A21,Encaissements_Détail!$E$2:$E48)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C22" t="s">
+        <v>292</v>
+      </c>
+      <c r="D22" t="s">
+        <v>617</v>
+      </c>
+      <c r="E22" s="91">
+        <v>250</v>
+      </c>
+      <c r="H22" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A49,Encaissements_Entête!$A22,Encaissements_Détail!$E$2:$E49)</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C23" t="s">
+        <v>386</v>
+      </c>
+      <c r="D23" t="s">
+        <v>617</v>
+      </c>
+      <c r="E23" s="91">
+        <v>0</v>
+      </c>
+      <c r="H23" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A50,Encaissements_Entête!$A23,Encaissements_Détail!$E$2:$E50)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C24" t="s">
+        <v>192</v>
+      </c>
+      <c r="D24" t="s">
+        <v>617</v>
+      </c>
+      <c r="E24" s="91">
+        <v>150</v>
+      </c>
+      <c r="H24" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A51,Encaissements_Entête!$A24,Encaissements_Détail!$E$2:$E51)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>617</v>
+      </c>
+      <c r="E25" s="91">
+        <v>-25</v>
+      </c>
+      <c r="H25" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A52,Encaissements_Entête!$A25,Encaissements_Détail!$E$2:$E52)</f>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D26" t="s">
+        <v>617</v>
+      </c>
+      <c r="E26" s="91">
+        <v>100</v>
+      </c>
+      <c r="H26" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A53,Encaissements_Entête!$A26,Encaissements_Détail!$E$2:$E53)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C27" t="s">
+        <v>645</v>
+      </c>
+      <c r="D27" t="s">
+        <v>617</v>
+      </c>
+      <c r="E27" s="91">
+        <v>0</v>
+      </c>
+      <c r="H27" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A54,Encaissements_Entête!$A27,Encaissements_Détail!$E$2:$E54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C28" t="s">
+        <v>292</v>
+      </c>
+      <c r="D28" t="s">
+        <v>617</v>
+      </c>
+      <c r="E28" s="91">
+        <v>25</v>
+      </c>
+      <c r="H28" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A55,Encaissements_Entête!$A28,Encaissements_Détail!$E$2:$E55)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C29" t="s">
+        <v>262</v>
+      </c>
+      <c r="D29" t="s">
+        <v>617</v>
+      </c>
+      <c r="E29" s="91">
+        <v>2500</v>
+      </c>
+      <c r="H29" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A56,Encaissements_Entête!$A29,Encaissements_Détail!$E$2:$E56)</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" t="s">
+        <v>617</v>
+      </c>
+      <c r="E30" s="91">
+        <v>500</v>
+      </c>
+      <c r="H30" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A57,Encaissements_Entête!$A30,Encaissements_Détail!$E$2:$E57)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="22">
+        <v>45336</v>
+      </c>
+      <c r="C31" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" t="s">
+        <v>617</v>
+      </c>
+      <c r="E31" s="91">
+        <v>0</v>
+      </c>
+      <c r="H31" s="91">
+        <f>SUMIF(Encaissements_Détail!$A$2:$A58,Encaissements_Entête!$A31,Encaissements_Détail!$E$2:$E58)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="96" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E05112-4271-48D1-8A2E-8EB42F7BAB68}">
   <sheetPr codeName="Feuil6"/>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="72" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
+        <v>608</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>593</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>609</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>612</v>
+      </c>
+      <c r="F1" s="75" t="s">
         <v>613</v>
       </c>
-      <c r="B1" s="77" t="s">
-        <v>592</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>594</v>
-      </c>
-      <c r="D1" s="77" t="s">
-        <v>614</v>
-      </c>
-      <c r="E1" s="78" t="s">
-        <v>617</v>
-      </c>
-      <c r="F1" s="77" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -27127,7 +28037,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D2" s="22">
         <v>44931</v>
@@ -27140,7 +28050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -27148,7 +28058,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D3" s="22">
         <v>44931</v>
@@ -27161,7 +28071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -27169,7 +28079,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D4" s="22">
         <v>44931</v>
@@ -27182,7 +28092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -27190,7 +28100,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D5" s="22">
         <v>44931</v>
@@ -27203,7 +28113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -27211,7 +28121,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D6" s="22">
         <v>44931</v>
@@ -27223,8 +28133,9 @@
         <f>ROW()</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" s="72"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -27245,7 +28156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -27265,8 +28176,9 @@
         <f>ROW()</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8" s="72"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -27286,8 +28198,9 @@
         <f>ROW()</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H9" s="72"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -27307,8 +28220,9 @@
         <f>ROW()</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" s="72"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -27328,8 +28242,9 @@
         <f>ROW()</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11" s="72"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -27349,8 +28264,9 @@
         <f>ROW()</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" s="72"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>7</v>
       </c>
@@ -27371,7 +28287,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -27391,8 +28307,9 @@
         <f>ROW()</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" s="72"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>8</v>
       </c>
@@ -27413,7 +28330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -27433,8 +28350,9 @@
         <f>ROW()</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" s="72"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>9</v>
       </c>
@@ -27455,7 +28373,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -27475,8 +28393,9 @@
         <f>ROW()</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" s="72"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>10</v>
       </c>
@@ -27497,7 +28416,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>10</v>
       </c>
@@ -27517,8 +28436,9 @@
         <f>ROW()</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20" s="72"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>11</v>
       </c>
@@ -27539,7 +28459,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>11</v>
       </c>
@@ -27560,7 +28480,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>11</v>
       </c>
@@ -27581,7 +28501,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>11</v>
       </c>
@@ -27601,8 +28521,9 @@
         <f>ROW()</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24" s="72"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>12</v>
       </c>
@@ -27623,7 +28544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>12</v>
       </c>
@@ -27643,8 +28564,9 @@
         <f>ROW()</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26" s="72"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>13</v>
       </c>
@@ -27664,8 +28586,9 @@
         <f>ROW()</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H27" s="72"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>14</v>
       </c>
@@ -27685,8 +28608,9 @@
         <f>ROW()</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28" s="72"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>15</v>
       </c>
@@ -27706,8 +28630,341 @@
         <f>ROW()</f>
         <v>29</v>
       </c>
+      <c r="H29" s="72"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>16</v>
+      </c>
+      <c r="B30" s="1">
+        <v>23031</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E30" s="72">
+        <v>2500</v>
+      </c>
+      <c r="F30" s="1">
+        <f>ROW()</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>375</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E31" s="72">
+        <v>500</v>
+      </c>
+      <c r="F31" s="1">
+        <f>ROW()</f>
+        <v>31</v>
+      </c>
+      <c r="H31" s="72"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>377</v>
+      </c>
+      <c r="C32" t="s">
+        <v>303</v>
+      </c>
+      <c r="D32" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E32" s="72">
+        <v>500</v>
+      </c>
+      <c r="F32" s="1">
+        <f>ROW()</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>381</v>
+      </c>
+      <c r="C33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E33" s="72">
+        <v>500</v>
+      </c>
+      <c r="F33" s="1">
+        <f>ROW()</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>383</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E34" s="72">
+        <v>25</v>
+      </c>
+      <c r="F34" s="1">
+        <f>ROW()</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>21</v>
+      </c>
+      <c r="B35" t="s">
+        <v>384</v>
+      </c>
+      <c r="C35" t="s">
+        <v>292</v>
+      </c>
+      <c r="D35" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E35" s="72">
+        <v>250</v>
+      </c>
+      <c r="F35" s="1">
+        <f>ROW()</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>385</v>
+      </c>
+      <c r="C36" t="s">
+        <v>386</v>
+      </c>
+      <c r="D36" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E36" s="72">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <f>ROW()</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
+        <v>388</v>
+      </c>
+      <c r="C37" t="s">
+        <v>192</v>
+      </c>
+      <c r="D37" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E37" s="72">
+        <v>150</v>
+      </c>
+      <c r="F37" s="1">
+        <f>ROW()</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>24</v>
+      </c>
+      <c r="B38" t="s">
+        <v>647</v>
+      </c>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E38" s="72">
+        <v>-25</v>
+      </c>
+      <c r="F38" s="1">
+        <f>ROW()</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>389</v>
+      </c>
+      <c r="C39" t="s">
+        <v>283</v>
+      </c>
+      <c r="D39" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E39" s="72">
+        <v>100</v>
+      </c>
+      <c r="F39" s="1">
+        <f>ROW()</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>26</v>
+      </c>
+      <c r="B40" t="s">
+        <v>454</v>
+      </c>
+      <c r="C40" t="s">
+        <v>645</v>
+      </c>
+      <c r="D40" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E40" s="72">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <f>ROW()</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>27</v>
+      </c>
+      <c r="B41" t="s">
+        <v>455</v>
+      </c>
+      <c r="C41" t="s">
+        <v>292</v>
+      </c>
+      <c r="D41" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E41" s="72">
+        <v>25</v>
+      </c>
+      <c r="F41" s="1">
+        <f>ROW()</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>28</v>
+      </c>
+      <c r="B42" t="s">
+        <v>458</v>
+      </c>
+      <c r="C42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D42" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E42" s="72">
+        <v>2500</v>
+      </c>
+      <c r="F42" s="1">
+        <f>ROW()</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>29</v>
+      </c>
+      <c r="B43" t="s">
+        <v>459</v>
+      </c>
+      <c r="C43" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E43" s="72">
+        <v>500</v>
+      </c>
+      <c r="F43" s="1">
+        <f>ROW()</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>460</v>
+      </c>
+      <c r="C44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" s="22">
+        <v>45336</v>
+      </c>
+      <c r="E44" s="72">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <f>ROW()</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v2.1 - À la recherche d'un BUG dans les encaissements (Next/Previous)
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_BD_Sortie.xlsx
+++ b/DataFiles/GCF_BD_Sortie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478DD5A2-B65B-454C-9746-7F6EA57B5C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07ADA08D-B09E-4D49-9D06-B8F42A2A32E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28830" windowHeight="15600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEC" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,8 @@
     <sheet name="Encaissements_Détail" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Comptes_Clients!$A$1:$J$46</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">GL_Trans!$A$1:$J$369</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Comptes_Clients!$A$1:$H$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">GL_Trans!$A$1:$J$368</definedName>
     <definedName name="PayItem_Amount">OFFSET(Encaissements_Détail!$E$1,1,,COUNTA(Encaissements_Détail!$A$3:$A$999999)+1,1)</definedName>
     <definedName name="PayItem_Inv_No">OFFSET(Encaissements_Détail!$B$1,1,,COUNTA(Encaissements_Détail!$A$3:$A$999999)+1,1)</definedName>
   </definedNames>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2822" uniqueCount="648">
   <si>
     <t>TEC_ID</t>
   </si>
@@ -2040,7 +2040,7 @@
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2115,14 +2115,6 @@
     <font>
       <b/>
       <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2318,7 +2310,7 @@
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2545,7 +2537,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2980,7 +2971,7 @@
       <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="88" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
@@ -13494,7 +13485,7 @@
       <c r="G249" s="83" t="s">
         <v>636</v>
       </c>
-      <c r="H249" s="90">
+      <c r="H249" s="89">
         <v>1.5</v>
       </c>
       <c r="I249" s="83" t="s">
@@ -13538,7 +13529,7 @@
       <c r="G250" s="83" t="s">
         <v>636</v>
       </c>
-      <c r="H250" s="90">
+      <c r="H250" s="89">
         <v>2.5</v>
       </c>
       <c r="I250" s="83" t="s">
@@ -13582,7 +13573,7 @@
       <c r="G251" s="83" t="s">
         <v>640</v>
       </c>
-      <c r="H251" s="90">
+      <c r="H251" s="89">
         <v>2</v>
       </c>
       <c r="J251" s="81" t="b">
@@ -13623,7 +13614,7 @@
       <c r="G252" s="83" t="s">
         <v>641</v>
       </c>
-      <c r="H252" s="90">
+      <c r="H252" s="89">
         <v>1</v>
       </c>
       <c r="J252" s="81" t="b">
@@ -13664,7 +13655,7 @@
       <c r="G253" s="83" t="s">
         <v>642</v>
       </c>
-      <c r="H253" s="90">
+      <c r="H253" s="89">
         <v>1</v>
       </c>
       <c r="J253" s="81" t="b">
@@ -13705,7 +13696,7 @@
       <c r="G254" s="83" t="s">
         <v>641</v>
       </c>
-      <c r="H254" s="90">
+      <c r="H254" s="89">
         <v>2</v>
       </c>
       <c r="J254" s="81" t="b">
@@ -13746,7 +13737,7 @@
       <c r="G255" s="83" t="s">
         <v>641</v>
       </c>
-      <c r="H255" s="90">
+      <c r="H255" s="89">
         <v>2</v>
       </c>
       <c r="J255" s="81" t="b">
@@ -13787,7 +13778,7 @@
       <c r="G256" s="83" t="s">
         <v>643</v>
       </c>
-      <c r="H256" s="90">
+      <c r="H256" s="89">
         <v>5</v>
       </c>
       <c r="J256" s="81" t="b">
@@ -13828,7 +13819,7 @@
       <c r="G257" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="H257" s="90">
+      <c r="H257" s="89">
         <v>1</v>
       </c>
       <c r="J257" s="81" t="b">
@@ -14664,10 +14655,10 @@
   <sheetPr codeName="Feuil3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J369"/>
+  <dimension ref="A1:J368"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A330" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C358" sqref="C358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25089,12 +25080,8 @@
         <v>368</v>
       </c>
     </row>
-    <row r="369" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G369" s="88"/>
-      <c r="H369" s="88"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J369" xr:uid="{E0D58006-DE1D-488F-9BB7-8096C5818030}"/>
+  <autoFilter ref="A1:J368" xr:uid="{E0D58006-DE1D-488F-9BB7-8096C5818030}"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -25757,10 +25744,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0BDE8C-C0CD-4E75-A0A0-916CFADCF838}">
   <sheetPr codeName="Feuil4"/>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N51" sqref="N51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25768,13 +25755,11 @@
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="91" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="91" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12" style="91" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="90" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="90" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
         <v>646</v>
       </c>
@@ -25793,14 +25778,14 @@
       <c r="F1" s="73" t="s">
         <v>596</v>
       </c>
-      <c r="G1" s="94" t="s">
+      <c r="G1" s="93" t="s">
         <v>597</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="94" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -25819,19 +25804,15 @@
       <c r="F2" s="23">
         <v>44592</v>
       </c>
-      <c r="G2" s="91">
+      <c r="G2" s="90">
         <v>9128.4500000000007</v>
       </c>
-      <c r="H2" s="91" cm="1">
+      <c r="H2" s="90" cm="1">
         <f t="array" aca="1" ref="H2" ca="1">G2-IFERROR(SUMIF(PayItem_Inv_No,A2,PayItem_Amount),0)</f>
         <v>3646.6600000000008</v>
       </c>
-      <c r="J2" s="91">
-        <f ca="1">G2-H2</f>
-        <v>5481.79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -25850,19 +25831,15 @@
       <c r="F3" s="23">
         <v>44729</v>
       </c>
-      <c r="G3" s="91">
+      <c r="G3" s="90">
         <v>1653.73</v>
       </c>
-      <c r="H3" s="91" cm="1">
+      <c r="H3" s="90" cm="1">
         <f t="array" aca="1" ref="H3" ca="1">G3-IFERROR(SUMIF(PayItem_Inv_No,A3,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
-      <c r="J3" s="91">
-        <f t="shared" ref="J3:J46" ca="1" si="0">G3-H3</f>
-        <v>1653.73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -25881,19 +25858,15 @@
       <c r="F4" s="23">
         <v>44729</v>
       </c>
-      <c r="G4" s="91">
+      <c r="G4" s="90">
         <v>474.39</v>
       </c>
-      <c r="H4" s="91" cm="1">
+      <c r="H4" s="90" cm="1">
         <f t="array" aca="1" ref="H4" ca="1">G4-IFERROR(SUMIF(PayItem_Inv_No,A4,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>474.39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -25912,19 +25885,15 @@
       <c r="F5" s="23">
         <v>44714</v>
       </c>
-      <c r="G5" s="91">
+      <c r="G5" s="90">
         <v>346.46</v>
       </c>
-      <c r="H5" s="91" cm="1">
+      <c r="H5" s="90" cm="1">
         <f t="array" aca="1" ref="H5" ca="1">G5-IFERROR(SUMIF(PayItem_Inv_No,A5,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>346.46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -25943,19 +25912,15 @@
       <c r="F6" s="23">
         <v>44953</v>
       </c>
-      <c r="G6" s="91">
+      <c r="G6" s="90">
         <v>3251.61</v>
       </c>
-      <c r="H6" s="91" cm="1">
+      <c r="H6" s="90" cm="1">
         <f t="array" aca="1" ref="H6" ca="1">G6-IFERROR(SUMIF(PayItem_Inv_No,A6,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
-      <c r="J6" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>3251.61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -25972,22 +25937,18 @@
         <v>603</v>
       </c>
       <c r="F7" s="23">
-        <f t="shared" ref="F7:F16" si="1">B7+15</f>
+        <f t="shared" ref="F7:F16" si="0">B7+15</f>
         <v>44960</v>
       </c>
-      <c r="G7" s="91">
+      <c r="G7" s="90">
         <v>974.39</v>
       </c>
-      <c r="H7" s="91" cm="1">
+      <c r="H7" s="90" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">G7-IFERROR(SUMIF(PayItem_Inv_No,A7,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
-      <c r="J7" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>974.39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -26004,22 +25965,18 @@
         <v>603</v>
       </c>
       <c r="F8" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44961</v>
       </c>
-      <c r="G8" s="91">
+      <c r="G8" s="90">
         <v>623.69000000000005</v>
       </c>
-      <c r="H8" s="91" cm="1">
+      <c r="H8" s="90" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">G8-IFERROR(SUMIF(PayItem_Inv_No,A8,PayItem_Amount),0)</f>
         <v>500.00000000000006</v>
       </c>
-      <c r="J8" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>123.69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -26036,22 +25993,18 @@
         <v>603</v>
       </c>
       <c r="F9" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44962</v>
       </c>
-      <c r="G9" s="91">
+      <c r="G9" s="90">
         <v>34.630000000000003</v>
       </c>
-      <c r="H9" s="91" cm="1">
+      <c r="H9" s="90" cm="1">
         <f t="array" aca="1" ref="H9" ca="1">G9-IFERROR(SUMIF(PayItem_Inv_No,A9,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
-      <c r="J9" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>34.630000000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -26068,22 +26021,18 @@
         <v>603</v>
       </c>
       <c r="F10" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44963</v>
       </c>
-      <c r="G10" s="91">
+      <c r="G10" s="90">
         <v>26.25</v>
       </c>
-      <c r="H10" s="91" cm="1">
+      <c r="H10" s="90" cm="1">
         <f t="array" aca="1" ref="H10" ca="1">G10-IFERROR(SUMIF(PayItem_Inv_No,A10,PayItem_Amount),0)</f>
         <v>0</v>
       </c>
-      <c r="J10" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>26.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -26100,22 +26049,18 @@
         <v>603</v>
       </c>
       <c r="F11" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44964</v>
       </c>
-      <c r="G11" s="91">
+      <c r="G11" s="90">
         <v>262.5</v>
       </c>
-      <c r="H11" s="91" cm="1">
+      <c r="H11" s="90" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">G11-IFERROR(SUMIF(PayItem_Inv_No,A11,PayItem_Amount),0)</f>
         <v>162.5</v>
       </c>
-      <c r="J11" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -26132,22 +26077,18 @@
         <v>603</v>
       </c>
       <c r="F12" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44965</v>
       </c>
-      <c r="G12" s="91">
+      <c r="G12" s="90">
         <v>445.2</v>
       </c>
-      <c r="H12" s="91" cm="1">
+      <c r="H12" s="90" cm="1">
         <f t="array" aca="1" ref="H12" ca="1">G12-IFERROR(SUMIF(PayItem_Inv_No,A12,PayItem_Amount),0)</f>
         <v>445.2</v>
       </c>
-      <c r="J12" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -26165,22 +26106,18 @@
         <v>603</v>
       </c>
       <c r="F13" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44968</v>
       </c>
-      <c r="G13" s="91">
+      <c r="G13" s="90">
         <v>26.25</v>
       </c>
-      <c r="H13" s="91">
-        <f t="shared" ref="H13:H46" ca="1" si="2">G13-IFERROR(SUMIF(PayItem_Inv_No,A13,PayItem_Amount),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J13" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>26.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="90">
+        <f t="shared" ref="H13:H46" ca="1" si="1">G13-IFERROR(SUMIF(PayItem_Inv_No,A13,PayItem_Amount),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -26198,22 +26135,18 @@
         <v>603</v>
       </c>
       <c r="F14" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44971</v>
       </c>
-      <c r="G14" s="91">
+      <c r="G14" s="90">
         <v>500</v>
       </c>
-      <c r="H14" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H14" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>500</v>
       </c>
-      <c r="J14" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -26231,27 +26164,23 @@
         <v>603</v>
       </c>
       <c r="F15" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44974</v>
       </c>
-      <c r="G15" s="91">
+      <c r="G15" s="90">
         <v>600</v>
       </c>
-      <c r="H15" s="91">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="90">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="22">
-        <f t="shared" ref="B16:B23" si="3">B15+8</f>
+        <f t="shared" ref="B16:B23" si="2">B15+8</f>
         <v>44967</v>
       </c>
       <c r="C16" s="37" t="s">
@@ -26264,27 +26193,23 @@
         <v>603</v>
       </c>
       <c r="F16" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44982</v>
       </c>
-      <c r="G16" s="91">
+      <c r="G16" s="90">
         <v>700</v>
       </c>
-      <c r="H16" s="91">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>700</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H16" s="90">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44975</v>
       </c>
       <c r="C17" t="s">
@@ -26300,24 +26225,20 @@
         <f>B17+30</f>
         <v>45005</v>
       </c>
-      <c r="G17" s="91">
+      <c r="G17" s="90">
         <v>725</v>
       </c>
-      <c r="H17" s="91">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>725</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H17" s="90">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44983</v>
       </c>
       <c r="C18" t="s">
@@ -26330,27 +26251,23 @@
         <v>603</v>
       </c>
       <c r="F18" s="23">
-        <f t="shared" ref="F18:F23" si="4">B18+15</f>
+        <f t="shared" ref="F18:F23" si="3">B18+15</f>
         <v>44998</v>
       </c>
-      <c r="G18" s="91">
+      <c r="G18" s="90">
         <v>750</v>
       </c>
-      <c r="H18" s="91">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="90">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44991</v>
       </c>
       <c r="C19" t="s">
@@ -26363,27 +26280,23 @@
         <v>603</v>
       </c>
       <c r="F19" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>45006</v>
       </c>
-      <c r="G19" s="91">
+      <c r="G19" s="90">
         <v>775</v>
       </c>
-      <c r="H19" s="91">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>775</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="90">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44999</v>
       </c>
       <c r="C20" t="s">
@@ -26396,27 +26309,23 @@
         <v>603</v>
       </c>
       <c r="F20" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>45014</v>
       </c>
-      <c r="G20" s="91">
+      <c r="G20" s="90">
         <v>800</v>
       </c>
-      <c r="H20" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H20" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>520</v>
       </c>
-      <c r="J20" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>280</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45007</v>
       </c>
       <c r="C21" t="s">
@@ -26429,27 +26338,23 @@
         <v>603</v>
       </c>
       <c r="F21" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>45022</v>
       </c>
-      <c r="G21" s="91">
+      <c r="G21" s="90">
         <v>774</v>
       </c>
-      <c r="H21" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H21" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>376.01</v>
       </c>
-      <c r="J21" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>397.99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45015</v>
       </c>
       <c r="C22" s="37" t="s">
@@ -26462,27 +26367,23 @@
         <v>603</v>
       </c>
       <c r="F22" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>45030</v>
       </c>
-      <c r="G22" s="91">
+      <c r="G22" s="90">
         <v>749</v>
       </c>
-      <c r="H22" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H22" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>749</v>
       </c>
-      <c r="J22" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45023</v>
       </c>
       <c r="C23" t="s">
@@ -26495,22 +26396,18 @@
         <v>603</v>
       </c>
       <c r="F23" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>45038</v>
       </c>
-      <c r="G23" s="91">
+      <c r="G23" s="90">
         <v>724</v>
       </c>
-      <c r="H23" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H23" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>724</v>
       </c>
-      <c r="J23" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -26531,19 +26428,15 @@
         <f>B24+45</f>
         <v>45083</v>
       </c>
-      <c r="G24" s="91">
+      <c r="G24" s="90">
         <v>699.99</v>
       </c>
-      <c r="H24" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H24" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>626.66</v>
       </c>
-      <c r="J24" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>73.330000000000041</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -26561,22 +26454,18 @@
         <v>603</v>
       </c>
       <c r="F25" s="23">
-        <f t="shared" ref="F25:F30" si="5">B25+15</f>
+        <f t="shared" ref="F25:F30" si="4">B25+15</f>
         <v>45068</v>
       </c>
-      <c r="G25" s="91">
+      <c r="G25" s="90">
         <v>599.99</v>
       </c>
-      <c r="H25" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H25" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>599.99</v>
       </c>
-      <c r="J25" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -26594,22 +26483,18 @@
         <v>603</v>
       </c>
       <c r="F26" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>45083</v>
       </c>
-      <c r="G26" s="91">
+      <c r="G26" s="90">
         <v>499.99</v>
       </c>
-      <c r="H26" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H26" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>499.99</v>
       </c>
-      <c r="J26" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -26627,22 +26512,18 @@
         <v>603</v>
       </c>
       <c r="F27" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>45098</v>
       </c>
-      <c r="G27" s="91">
+      <c r="G27" s="90">
         <v>399.99</v>
       </c>
-      <c r="H27" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H27" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>399.99</v>
       </c>
-      <c r="J27" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -26660,22 +26541,18 @@
         <v>603</v>
       </c>
       <c r="F28" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>45113</v>
       </c>
-      <c r="G28" s="91">
+      <c r="G28" s="90">
         <v>299.99</v>
       </c>
-      <c r="H28" s="91">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>299.99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H28" s="90">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -26692,22 +26569,18 @@
         <v>603</v>
       </c>
       <c r="F29" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>45214</v>
       </c>
-      <c r="G29" s="91">
+      <c r="G29" s="90">
         <v>8999.99</v>
       </c>
-      <c r="H29" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H29" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>8700</v>
       </c>
-      <c r="J29" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>299.98999999999978</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -26725,22 +26598,18 @@
         <v>603</v>
       </c>
       <c r="F30" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>45245</v>
       </c>
-      <c r="G30" s="91">
+      <c r="G30" s="90">
         <v>7888.88</v>
       </c>
-      <c r="H30" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H30" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>7888.88</v>
       </c>
-      <c r="J30" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -26760,19 +26629,15 @@
         <f>B31+30</f>
         <v>45235</v>
       </c>
-      <c r="G31" s="91">
+      <c r="G31" s="90">
         <v>1207.24</v>
       </c>
-      <c r="H31" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H31" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>1207.24</v>
       </c>
-      <c r="J31" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>23031</v>
       </c>
@@ -26789,22 +26654,18 @@
         <v>603</v>
       </c>
       <c r="F32" s="23">
-        <f t="shared" ref="F32:F46" si="6">B32+30</f>
+        <f t="shared" ref="F32:F46" si="5">B32+30</f>
         <v>45241</v>
       </c>
-      <c r="G32" s="96">
+      <c r="G32" s="95">
         <v>18874.3</v>
       </c>
-      <c r="H32" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H32" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>16374.3</v>
       </c>
-      <c r="J32" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>375</v>
       </c>
@@ -26821,22 +26682,18 @@
         <v>603</v>
       </c>
       <c r="F33" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45303</v>
       </c>
-      <c r="G33" s="96">
+      <c r="G33" s="95">
         <v>2585.17</v>
       </c>
-      <c r="H33" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H33" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>2085.17</v>
       </c>
-      <c r="J33" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>377</v>
       </c>
@@ -26853,22 +26710,18 @@
         <v>603</v>
       </c>
       <c r="F34" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45305</v>
       </c>
-      <c r="G34" s="96">
+      <c r="G34" s="95">
         <v>2112.09</v>
       </c>
-      <c r="H34" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H34" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>1612.0900000000001</v>
       </c>
-      <c r="J34" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>381</v>
       </c>
@@ -26885,22 +26738,18 @@
         <v>603</v>
       </c>
       <c r="F35" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45310</v>
       </c>
-      <c r="G35" s="96">
+      <c r="G35" s="95">
         <v>1063.52</v>
       </c>
-      <c r="H35" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H35" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>563.52</v>
       </c>
-      <c r="J35" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>383</v>
       </c>
@@ -26917,22 +26766,18 @@
         <v>603</v>
       </c>
       <c r="F36" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45309</v>
       </c>
-      <c r="G36" s="96">
+      <c r="G36" s="95">
         <v>3111.2200000000003</v>
       </c>
-      <c r="H36" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H36" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>3086.2200000000003</v>
       </c>
-      <c r="J36" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>384</v>
       </c>
@@ -26949,22 +26794,18 @@
         <v>603</v>
       </c>
       <c r="F37" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45310</v>
       </c>
-      <c r="G37" s="96">
+      <c r="G37" s="95">
         <v>413.90999999999997</v>
       </c>
-      <c r="H37" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H37" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>163.90999999999997</v>
       </c>
-      <c r="J37" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>385</v>
       </c>
@@ -26981,22 +26822,18 @@
         <v>603</v>
       </c>
       <c r="F38" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45310</v>
       </c>
-      <c r="G38" s="96">
+      <c r="G38" s="95">
         <v>1046.27</v>
       </c>
-      <c r="H38" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H38" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>1046.27</v>
       </c>
-      <c r="J38" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>388</v>
       </c>
@@ -27013,22 +26850,18 @@
         <v>603</v>
       </c>
       <c r="F39" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45310</v>
       </c>
-      <c r="G39" s="96">
+      <c r="G39" s="95">
         <v>1456.34</v>
       </c>
-      <c r="H39" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H39" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>1306.3399999999999</v>
       </c>
-      <c r="J39" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>383</v>
       </c>
@@ -27045,22 +26878,18 @@
         <v>603</v>
       </c>
       <c r="F40" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45309</v>
       </c>
-      <c r="G40" s="96">
+      <c r="G40" s="95">
         <v>-3111.22</v>
       </c>
-      <c r="H40" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H40" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>-3136.22</v>
       </c>
-      <c r="J40" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>389</v>
       </c>
@@ -27077,22 +26906,18 @@
         <v>603</v>
       </c>
       <c r="F41" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45311</v>
       </c>
-      <c r="G41" s="96">
+      <c r="G41" s="95">
         <v>718.59</v>
       </c>
-      <c r="H41" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H41" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>618.59</v>
       </c>
-      <c r="J41" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>454</v>
       </c>
@@ -27109,22 +26934,18 @@
         <v>603</v>
       </c>
       <c r="F42" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45311</v>
       </c>
-      <c r="G42" s="96">
+      <c r="G42" s="95">
         <v>431.16</v>
       </c>
-      <c r="H42" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H42" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>431.16</v>
       </c>
-      <c r="J42" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>455</v>
       </c>
@@ -27141,22 +26962,18 @@
         <v>603</v>
       </c>
       <c r="F43" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45311</v>
       </c>
-      <c r="G43" s="96">
+      <c r="G43" s="95">
         <v>696.75</v>
       </c>
-      <c r="H43" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H43" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>671.75</v>
       </c>
-      <c r="J43" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>458</v>
       </c>
@@ -27173,22 +26990,18 @@
         <v>603</v>
       </c>
       <c r="F44" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45311</v>
       </c>
-      <c r="G44" s="96">
+      <c r="G44" s="95">
         <v>9388.86</v>
       </c>
-      <c r="H44" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H44" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>6888.8600000000006</v>
       </c>
-      <c r="J44" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>459</v>
       </c>
@@ -27205,22 +27018,18 @@
         <v>603</v>
       </c>
       <c r="F45" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45311</v>
       </c>
-      <c r="G45" s="96">
+      <c r="G45" s="95">
         <v>1766.02</v>
       </c>
-      <c r="H45" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H45" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>1266.02</v>
       </c>
-      <c r="J45" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>460</v>
       </c>
@@ -27237,24 +27046,20 @@
         <v>603</v>
       </c>
       <c r="F46" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>45311</v>
       </c>
-      <c r="G46" s="96">
+      <c r="G46" s="95">
         <v>344.93</v>
       </c>
-      <c r="H46" s="91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H46" s="90">
+        <f t="shared" ca="1" si="1"/>
         <v>344.93</v>
       </c>
-      <c r="J46" s="91">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J46" xr:uid="{6A0BDE8C-C0CD-4E75-A0A0-916CFADCF838}"/>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <autoFilter ref="A1:H46" xr:uid="{6A0BDE8C-C0CD-4E75-A0A0-916CFADCF838}"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="A32:B46">
     <cfRule type="expression" dxfId="7" priority="8">
       <formula>AND($A32&lt;&gt;"",MOD(ROW(),2)=0)</formula>
@@ -27304,10 +27109,10 @@
   <sheetPr codeName="Feuil5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD34"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27316,13 +27121,11 @@
     <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="91" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="91" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="90" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="75" t="s">
         <v>608</v>
       </c>
@@ -27335,14 +27138,14 @@
       <c r="D1" s="75" t="s">
         <v>610</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="E1" s="91" t="s">
         <v>611</v>
       </c>
       <c r="F1" s="75" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -27355,18 +27158,14 @@
       <c r="D2" t="s">
         <v>614</v>
       </c>
-      <c r="E2" s="93">
+      <c r="E2" s="92">
         <v>5066.22</v>
       </c>
       <c r="F2" t="s">
         <v>615</v>
       </c>
-      <c r="H2" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A29,Encaissements_Entête!$A2,Encaissements_Détail!$E$2:$E29)</f>
-        <v>5066.22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -27379,15 +27178,11 @@
       <c r="D3" t="s">
         <v>614</v>
       </c>
-      <c r="E3" s="91">
+      <c r="E3" s="90">
         <v>5474.39</v>
       </c>
-      <c r="H3" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A30,Encaissements_Entête!$A3,Encaissements_Détail!$E$2:$E30)</f>
-        <v>5474.39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -27400,15 +27195,11 @@
       <c r="D4" t="s">
         <v>616</v>
       </c>
-      <c r="E4" s="91">
+      <c r="E4" s="90">
         <v>346.46</v>
       </c>
-      <c r="H4" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A31,Encaissements_Entête!$A4,Encaissements_Détail!$E$2:$E31)</f>
-        <v>346.46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -27418,15 +27209,11 @@
       <c r="C5" t="s">
         <v>575</v>
       </c>
-      <c r="E5" s="91">
+      <c r="E5" s="90">
         <v>250</v>
       </c>
-      <c r="H5" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A32,Encaissements_Entête!$A5,Encaissements_Détail!$E$2:$E32)</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -27436,15 +27223,11 @@
       <c r="C6" t="s">
         <v>576</v>
       </c>
-      <c r="E6" s="91">
+      <c r="E6" s="90">
         <v>750</v>
       </c>
-      <c r="H6" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A33,Encaissements_Entête!$A6,Encaissements_Détail!$E$2:$E33)</f>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -27457,18 +27240,14 @@
       <c r="D7" t="s">
         <v>617</v>
       </c>
-      <c r="E7" s="91">
+      <c r="E7" s="90">
         <v>348.08</v>
       </c>
       <c r="F7" t="s">
         <v>618</v>
       </c>
-      <c r="H7" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A34,Encaissements_Entête!$A7,Encaissements_Détail!$E$2:$E34)</f>
-        <v>348.08</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -27481,18 +27260,14 @@
       <c r="D8" t="s">
         <v>617</v>
       </c>
-      <c r="E8" s="91">
+      <c r="E8" s="90">
         <v>500</v>
       </c>
       <c r="F8" t="s">
         <v>619</v>
       </c>
-      <c r="H8" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A35,Encaissements_Entête!$A8,Encaissements_Détail!$E$2:$E35)</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -27505,15 +27280,11 @@
       <c r="D9" t="s">
         <v>617</v>
       </c>
-      <c r="E9" s="91">
+      <c r="E9" s="90">
         <v>329.99</v>
       </c>
-      <c r="H9" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A36,Encaissements_Entête!$A9,Encaissements_Détail!$E$2:$E36)</f>
-        <v>329.99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -27526,15 +27297,11 @@
       <c r="D10" t="s">
         <v>617</v>
       </c>
-      <c r="E10" s="91">
+      <c r="E10" s="90">
         <v>1397.99</v>
       </c>
-      <c r="H10" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A37,Encaissements_Entête!$A10,Encaissements_Détail!$E$2:$E37)</f>
-        <v>1397.99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -27547,15 +27314,11 @@
       <c r="D11" t="s">
         <v>617</v>
       </c>
-      <c r="E11" s="91">
+      <c r="E11" s="90">
         <v>500</v>
       </c>
-      <c r="H11" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A38,Encaissements_Entête!$A11,Encaissements_Détail!$E$2:$E38)</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -27568,18 +27331,14 @@
       <c r="D12" t="s">
         <v>617</v>
       </c>
-      <c r="E12" s="91">
+      <c r="E12" s="90">
         <v>1881.37</v>
       </c>
       <c r="F12" t="s">
         <v>620</v>
       </c>
-      <c r="H12" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A39,Encaissements_Entête!$A12,Encaissements_Détail!$E$2:$E39)</f>
-        <v>1881.37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -27592,15 +27351,11 @@
       <c r="D13" t="s">
         <v>617</v>
       </c>
-      <c r="E13" s="91">
-        <v>0</v>
-      </c>
-      <c r="H13" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A40,Encaissements_Entête!$A13,Encaissements_Détail!$E$2:$E40)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -27613,15 +27368,11 @@
       <c r="D14" t="s">
         <v>617</v>
       </c>
-      <c r="E14" s="91">
+      <c r="E14" s="90">
         <v>250</v>
       </c>
-      <c r="H14" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A41,Encaissements_Entête!$A14,Encaissements_Détail!$E$2:$E41)</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -27634,18 +27385,14 @@
       <c r="D15" t="s">
         <v>617</v>
       </c>
-      <c r="E15" s="91">
+      <c r="E15" s="90">
         <v>99.99</v>
       </c>
       <c r="F15" t="s">
         <v>621</v>
       </c>
-      <c r="H15" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A42,Encaissements_Entête!$A15,Encaissements_Détail!$E$2:$E42)</f>
-        <v>99.99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -27658,15 +27405,11 @@
       <c r="D16" t="s">
         <v>617</v>
       </c>
-      <c r="E16" s="91">
+      <c r="E16" s="90">
         <v>200</v>
       </c>
-      <c r="H16" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A43,Encaissements_Entête!$A16,Encaissements_Détail!$E$2:$E43)</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -27679,15 +27422,11 @@
       <c r="D17" t="s">
         <v>617</v>
       </c>
-      <c r="E17" s="91">
+      <c r="E17" s="90">
         <v>2500</v>
       </c>
-      <c r="H17" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A44,Encaissements_Entête!$A17,Encaissements_Détail!$E$2:$E44)</f>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -27700,15 +27439,11 @@
       <c r="D18" t="s">
         <v>617</v>
       </c>
-      <c r="E18" s="91">
+      <c r="E18" s="90">
         <v>500</v>
       </c>
-      <c r="H18" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A45,Encaissements_Entête!$A18,Encaissements_Détail!$E$2:$E45)</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -27721,15 +27456,11 @@
       <c r="D19" t="s">
         <v>617</v>
       </c>
-      <c r="E19" s="91">
+      <c r="E19" s="90">
         <v>500</v>
       </c>
-      <c r="H19" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A46,Encaissements_Entête!$A19,Encaissements_Détail!$E$2:$E46)</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -27742,15 +27473,11 @@
       <c r="D20" t="s">
         <v>617</v>
       </c>
-      <c r="E20" s="91">
+      <c r="E20" s="90">
         <v>500</v>
       </c>
-      <c r="H20" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A47,Encaissements_Entête!$A20,Encaissements_Détail!$E$2:$E47)</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -27763,15 +27490,11 @@
       <c r="D21" t="s">
         <v>617</v>
       </c>
-      <c r="E21" s="91">
+      <c r="E21" s="90">
         <v>25</v>
       </c>
-      <c r="H21" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A48,Encaissements_Entête!$A21,Encaissements_Détail!$E$2:$E48)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -27784,15 +27507,11 @@
       <c r="D22" t="s">
         <v>617</v>
       </c>
-      <c r="E22" s="91">
+      <c r="E22" s="90">
         <v>250</v>
       </c>
-      <c r="H22" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A49,Encaissements_Entête!$A22,Encaissements_Détail!$E$2:$E49)</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -27805,15 +27524,11 @@
       <c r="D23" t="s">
         <v>617</v>
       </c>
-      <c r="E23" s="91">
-        <v>0</v>
-      </c>
-      <c r="H23" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A50,Encaissements_Entête!$A23,Encaissements_Détail!$E$2:$E50)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E23" s="90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -27826,15 +27541,11 @@
       <c r="D24" t="s">
         <v>617</v>
       </c>
-      <c r="E24" s="91">
+      <c r="E24" s="90">
         <v>150</v>
       </c>
-      <c r="H24" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A51,Encaissements_Entête!$A24,Encaissements_Détail!$E$2:$E51)</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -27847,15 +27558,11 @@
       <c r="D25" t="s">
         <v>617</v>
       </c>
-      <c r="E25" s="91">
+      <c r="E25" s="90">
         <v>-25</v>
       </c>
-      <c r="H25" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A52,Encaissements_Entête!$A25,Encaissements_Détail!$E$2:$E52)</f>
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -27868,15 +27575,11 @@
       <c r="D26" t="s">
         <v>617</v>
       </c>
-      <c r="E26" s="91">
+      <c r="E26" s="90">
         <v>100</v>
       </c>
-      <c r="H26" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A53,Encaissements_Entête!$A26,Encaissements_Détail!$E$2:$E53)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -27889,15 +27592,11 @@
       <c r="D27" t="s">
         <v>617</v>
       </c>
-      <c r="E27" s="91">
-        <v>0</v>
-      </c>
-      <c r="H27" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A54,Encaissements_Entête!$A27,Encaissements_Détail!$E$2:$E54)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E27" s="90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -27910,15 +27609,11 @@
       <c r="D28" t="s">
         <v>617</v>
       </c>
-      <c r="E28" s="91">
+      <c r="E28" s="90">
         <v>25</v>
       </c>
-      <c r="H28" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A55,Encaissements_Entête!$A28,Encaissements_Détail!$E$2:$E55)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -27931,15 +27626,11 @@
       <c r="D29" t="s">
         <v>617</v>
       </c>
-      <c r="E29" s="91">
+      <c r="E29" s="90">
         <v>2500</v>
       </c>
-      <c r="H29" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A56,Encaissements_Entête!$A29,Encaissements_Détail!$E$2:$E56)</f>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -27952,15 +27643,11 @@
       <c r="D30" t="s">
         <v>617</v>
       </c>
-      <c r="E30" s="91">
+      <c r="E30" s="90">
         <v>500</v>
       </c>
-      <c r="H30" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A57,Encaissements_Entête!$A30,Encaissements_Détail!$E$2:$E57)</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -27973,12 +27660,11 @@
       <c r="D31" t="s">
         <v>617</v>
       </c>
-      <c r="E31" s="91">
-        <v>0</v>
-      </c>
-      <c r="H31" s="91">
-        <f>SUMIF(Encaissements_Détail!$A$2:$A58,Encaissements_Entête!$A31,Encaissements_Détail!$E$2:$E58)</f>
-        <v>0</v>
+      <c r="E31" s="90">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -28964,7 +28650,7 @@
       <c r="A49" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>